<commit_message>
Motorraum in Oberraum war 0,5 mm zu eng
</commit_message>
<xml_diff>
--- a/theory/Kinematik.xlsx
+++ b/theory/Kinematik.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
   <si>
     <r>
       <t>Hüfte (T</t>
@@ -793,6 +793,12 @@
   <si>
     <t>http://kos.informatik.uni-osnabrueck.de/download/diplom/node26.html</t>
   </si>
+  <si>
+    <t>Modell zy'x''</t>
+  </si>
+  <si>
+    <t>http://www-home.htwg-konstanz.de/~bittel/ain_robo/Vorlesung/02_PositionUndOrientierung.pdf</t>
+  </si>
 </sst>
 </file>
 
@@ -1084,7 +1090,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1208,8 +1214,11 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="185" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -1314,10 +1323,10 @@
             <c:numRef>
               <c:f>Kinematik!$B$83</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>_-* #,##0.0\ _€_-;\-* #,##0.0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>196.20193825305205</c:v>
+                  <c:v>185.90126395942724</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1326,10 +1335,10 @@
             <c:numRef>
               <c:f>Kinematik!$B$84</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>43.412044416732584</c:v>
+                  <c:v>-32.779408583853218</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1382,7 +1391,7 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="_-* #,##0.0\ _€_-;\-* #,##0.0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1427,7 +1436,7 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1497,7 +1506,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.94727212553749</c:v>
+                  <c:v>188.76909060759877</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1512,7 +1521,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>300</c:v>
+                  <c:v>317.24839665526031</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -22518,21 +22527,21 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>36306</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>64993</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>127746</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="914400" cy="270843"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="40" name="Textfeld 39"/>
+            <xdr:cNvPr id="49" name="Textfeld 48"/>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="36306" y="11342593"/>
+              <a:off x="0" y="12140452"/>
               <a:ext cx="914400" cy="270843"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -22649,12 +22658,12 @@
       <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="40" name="Textfeld 39"/>
+            <xdr:cNvPr id="49" name="Textfeld 48"/>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="36306" y="11342593"/>
+              <a:off x="0" y="12140452"/>
               <a:ext cx="914400" cy="270843"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -22697,6 +22706,251 @@
               <a:r>
                 <a:rPr lang="de-DE" sz="1100"/>
                 <a:t>=</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>788892</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1093695" cy="270843"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="50" name="Textfeld 49"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5423645" y="12759017"/>
+              <a:ext cx="1093695" cy="270843"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:d>
+                    <m:dPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:dPr>
+                    <m:e>
+                      <m:sSubSup>
+                        <m:sSubSupPr>
+                          <m:ctrlPr>
+                            <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="Cambria Math"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:sSubSupPr>
+                        <m:e>
+                          <m:r>
+                            <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="Cambria Math"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                            <m:t>𝑇</m:t>
+                          </m:r>
+                        </m:e>
+                        <m:sub>
+                          <m:r>
+                            <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="Cambria Math"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                            <m:t>0</m:t>
+                          </m:r>
+                        </m:sub>
+                        <m:sup>
+                          <m:r>
+                            <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="Cambria Math"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                            <m:t>6</m:t>
+                          </m:r>
+                        </m:sup>
+                      </m:sSubSup>
+                    </m:e>
+                  </m:d>
+                  <m:r>
+                    <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t> </m:t>
+                  </m:r>
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>𝑊𝐶𝑃</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>𝑇𝐶𝑃</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100"/>
+                <a:t>= </a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="50" name="Textfeld 49"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5423645" y="12759017"/>
+              <a:ext cx="1093695" cy="270843"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>(𝑇_0^6 )  〖𝑊𝐶𝑃〗_𝑇𝐶𝑃</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100"/>
+                <a:t>= </a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -22959,6 +23213,43 @@
         <a:xfrm>
           <a:off x="170330" y="8552331"/>
           <a:ext cx="14631668" cy="5593976"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>134471</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>170328</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>8965</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Grafik 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:srcRect l="25794" t="23869" r="33401" b="39812"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="134471" y="14693152"/>
+          <a:ext cx="5970494" cy="2850777"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -23259,8 +23550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23279,7 +23570,7 @@
     <col min="13" max="13" width="11" customWidth="1"/>
     <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.44140625" customWidth="1"/>
     <col min="17" max="17" width="11.44140625" customWidth="1"/>
     <col min="18" max="18" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.77734375" customWidth="1"/>
@@ -23301,19 +23592,19 @@
       </c>
       <c r="G4" s="61">
         <f>B83</f>
-        <v>196.20193825305205</v>
+        <v>185.90126395942724</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G5" s="62">
         <f>B84</f>
-        <v>43.412044416732584</v>
+        <v>-32.779408583853218</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G6" s="63">
         <f>B85</f>
-        <v>600</v>
+        <v>617.24839665526031</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -23323,31 +23614,31 @@
       </c>
       <c r="G8" s="91">
         <f>V48</f>
-        <v>246.20193825305205</v>
+        <v>234.34170436810228</v>
       </c>
       <c r="H8" s="92">
         <f>X48</f>
-        <v>-169.99999999999997</v>
+        <v>-44.728060506391358</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G9" s="93">
         <f>V49</f>
-        <v>43.412044416732584</v>
+        <v>-41.629438490424469</v>
       </c>
       <c r="H9" s="94">
         <f>X49</f>
-        <v>-90</v>
+        <v>-75.870129985169925</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G10" s="95">
         <f>V50</f>
-        <v>600</v>
+        <v>625.92023058277505</v>
       </c>
       <c r="H10" s="96">
         <f>X50</f>
-        <v>0</v>
+        <v>-144.74556396082122</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
@@ -23377,19 +23668,19 @@
         <v>8</v>
       </c>
       <c r="B15" s="31">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="C15" s="24">
         <f>RADIANS(B15)</f>
-        <v>0.17453292519943295</v>
+        <v>-0.17453292519943295</v>
       </c>
       <c r="E15" s="23">
         <f>H85</f>
-        <v>12.476372505958198</v>
+        <v>-10.000000000000011</v>
       </c>
       <c r="I15" s="23">
         <f>H86</f>
-        <v>-167.52362749404179</v>
+        <v>169.99999999999997</v>
       </c>
       <c r="J15" s="29" t="s">
         <v>44</v>
@@ -23400,27 +23691,27 @@
         <v>5</v>
       </c>
       <c r="B16" s="33">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C16" s="24">
         <f t="shared" ref="C16:C20" si="0">RADIANS(B16)</f>
-        <v>0</v>
+        <v>-3.4906585039886591E-2</v>
       </c>
       <c r="D16" s="36">
         <f>N120</f>
-        <v>0.18091595117792342</v>
+        <v>-2.0000000000000284</v>
       </c>
       <c r="E16" s="36">
         <f>N126</f>
-        <v>67.449352764288065</v>
+        <v>63.506970256937187</v>
       </c>
       <c r="H16" s="36">
         <f>R120</f>
-        <v>-67.449352764288065</v>
+        <v>-63.506970256937187</v>
       </c>
       <c r="I16" s="36">
         <f>R126</f>
-        <v>-0.18091595117792342</v>
+        <v>2.0000000000000027</v>
       </c>
       <c r="V16" t="s">
         <v>18</v>
@@ -23431,27 +23722,27 @@
         <v>6</v>
       </c>
       <c r="B17" s="33">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="C17" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-5.235987755982989E-2</v>
       </c>
       <c r="D17" s="37">
         <f>N121</f>
-        <v>-0.18134439313047457</v>
+        <v>-2.9999999999999662</v>
       </c>
       <c r="E17" s="37">
         <f>N127</f>
-        <v>-179.81865560686953</v>
+        <v>-177.00000000000003</v>
       </c>
       <c r="H17" s="37">
         <f>R121</f>
-        <v>-0.18134439313047457</v>
+        <v>-2.9999999999999662</v>
       </c>
       <c r="I17" s="37">
         <f>R127</f>
-        <v>-179.81865560686953</v>
+        <v>-177.00000000000003</v>
       </c>
       <c r="V17">
         <v>0</v>
@@ -23462,19 +23753,19 @@
         <v>7</v>
       </c>
       <c r="B18" s="33">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C18" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9813170079773182E-2</v>
       </c>
       <c r="F18" s="97">
         <f>O142</f>
-        <v>-90</v>
+        <v>-175.99999999999997</v>
       </c>
       <c r="G18" s="31">
         <f>O143</f>
-        <v>90</v>
+        <v>175.99999999999997</v>
       </c>
       <c r="H18" s="23"/>
       <c r="V18">
@@ -23486,19 +23777,19 @@
         <v>9</v>
       </c>
       <c r="B19" s="33">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="C19" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-8.7266462599716474E-2</v>
       </c>
       <c r="F19" s="98">
         <f>H142</f>
-        <v>8.5377364625159387E-7</v>
+        <v>5.0000000000002105</v>
       </c>
       <c r="G19" s="33">
         <f>H143</f>
-        <v>-8.5377364625159387E-7</v>
+        <v>-5.0000000000002105</v>
       </c>
       <c r="V19">
         <v>0</v>
@@ -23509,19 +23800,19 @@
         <v>10</v>
       </c>
       <c r="B20" s="35">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C20" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.10471975511965978</v>
       </c>
       <c r="F20" s="99">
         <f>K142</f>
-        <v>-90</v>
+        <v>-173.99999999999997</v>
       </c>
       <c r="G20" s="35">
         <f>K143</f>
-        <v>90</v>
+        <v>173.99999999999997</v>
       </c>
       <c r="V20">
         <v>1</v>
@@ -23584,11 +23875,11 @@
       </c>
       <c r="G23" s="1">
         <f>B15</f>
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="H23" s="6">
         <f>RADIANS(G23)</f>
-        <v>0.17453292519943295</v>
+        <v>-0.17453292519943295</v>
       </c>
       <c r="N23" s="105">
         <f>COS(H23)</f>
@@ -23596,11 +23887,11 @@
       </c>
       <c r="O23" s="83">
         <f>-SIN(H23)*COS(D23)</f>
-        <v>-1.0637239828316862E-17</v>
+        <v>1.0637239828316862E-17</v>
       </c>
       <c r="P23" s="83">
         <f>SIN(H23)*SIN(D23)</f>
-        <v>-0.17364817766693033</v>
+        <v>0.17364817766693033</v>
       </c>
       <c r="Q23" s="106">
         <f>E23*COS(H23)</f>
@@ -23611,10 +23902,10 @@
         <v>0.98480775301220802</v>
       </c>
       <c r="S23" s="108">
-        <v>-1.0637239828316862E-17</v>
+        <v>1.0637239828316862E-17</v>
       </c>
       <c r="T23" s="108">
-        <v>-0.17364817766693033</v>
+        <v>0.17364817766693033</v>
       </c>
       <c r="U23" s="109">
         <v>0</v>
@@ -23635,7 +23926,7 @@
     <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="N24" s="105">
         <f>SIN(H23)</f>
-        <v>0.17364817766693033</v>
+        <v>-0.17364817766693033</v>
       </c>
       <c r="O24" s="83">
         <f>COS(H23)*COS(D23)</f>
@@ -23650,7 +23941,7 @@
         <v>0</v>
       </c>
       <c r="R24" s="107">
-        <v>0.17364817766693033</v>
+        <v>-0.17364817766693033</v>
       </c>
       <c r="S24" s="108">
         <v>6.032678484924683E-17</v>
@@ -23708,11 +23999,11 @@
       </c>
       <c r="W25" s="24">
         <f>IF(ABS(W24)=PI()/2,0,ATAN2(R23,R24))</f>
-        <v>0.17453292519943295</v>
+        <v>-0.17453292519943295</v>
       </c>
       <c r="X25" s="23">
         <f>DEGREES(W25)</f>
-        <v>10</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.3">
@@ -23768,19 +24059,19 @@
       </c>
       <c r="G28" s="1">
         <f>B16-90</f>
-        <v>-90</v>
+        <v>-92</v>
       </c>
       <c r="H28" s="6">
         <f>RADIANS(G28)</f>
-        <v>-1.5707963267948966</v>
+        <v>-1.6057029118347832</v>
       </c>
       <c r="N28" s="103">
         <f>COS(H28)</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-3.4899496702500955E-2</v>
       </c>
       <c r="O28" s="71">
         <f>-SIN(H28)*COS(D28)</f>
-        <v>1</v>
+        <v>0.99939082701909576</v>
       </c>
       <c r="P28" s="71">
         <f>SIN(H28)*SIN(D28)</f>
@@ -23788,42 +24079,42 @@
       </c>
       <c r="Q28" s="104">
         <f>E28*COS(H28)</f>
-        <v>1.83772268236293E-14</v>
+        <v>-10.469849010750286</v>
       </c>
       <c r="R28" s="107">
         <f t="array" ref="R28:U31">MMULT(R23:U26,N28:Q31)</f>
-        <v>7.0964024677563694E-17</v>
+        <v>-3.4369294928846945E-2</v>
       </c>
       <c r="S28" s="108">
-        <v>0.98480775301220802</v>
+        <v>0.98420783473768791</v>
       </c>
       <c r="T28" s="108">
-        <v>-0.17364817766693033</v>
+        <v>0.17364817766693033</v>
       </c>
       <c r="U28" s="109">
-        <v>2.1289207403269107E-14</v>
+        <v>-10.310788478654082</v>
       </c>
       <c r="V28" s="21">
         <f>$V$17*R28+$V$18*S28+$V$19*T28+$V$20*U28</f>
-        <v>2.1289207403269107E-14</v>
+        <v>-10.310788478654082</v>
       </c>
       <c r="W28" s="24">
         <f>IF(W29=PI()/2,ATAN2(S29,S28),IF(-W29=PI()/2,-ATAN2(S29,S28),ATAN2(T30,S30)))</f>
-        <v>-1.3962634015954636</v>
+        <v>1.5707963267948948</v>
       </c>
       <c r="X28" s="23">
         <f>DEGREES(W28)</f>
-        <v>-80</v>
+        <v>89.999999999999901</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="N29" s="103">
         <f>SIN(H28)</f>
-        <v>-1</v>
+        <v>-0.99939082701909576</v>
       </c>
       <c r="O29" s="71">
         <f>COS(H28)*COS(D28)</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-3.4899496702500955E-2</v>
       </c>
       <c r="P29" s="71">
         <f>-COS(H28)*SIN(D28)</f>
@@ -23831,31 +24122,31 @@
       </c>
       <c r="Q29" s="104">
         <f>E28*SIN(H28)</f>
-        <v>-300</v>
+        <v>-299.81724810572871</v>
       </c>
       <c r="R29" s="107">
-        <v>-4.9689545020929967E-17</v>
+        <v>6.0602340038822741E-3</v>
       </c>
       <c r="S29" s="108">
-        <v>0.17364817766693033</v>
+        <v>-0.17354239588891238</v>
       </c>
       <c r="T29" s="108">
         <v>0.98480775301220802</v>
       </c>
       <c r="U29" s="109">
-        <v>-1.4906863506278992E-14</v>
+        <v>1.8180702011646825</v>
       </c>
       <c r="V29" s="21">
         <f>$V$17*R29+$V$19*S29+$V$18*T29+$V$20*U29</f>
-        <v>-1.4906863506278992E-14</v>
+        <v>1.8180702011646825</v>
       </c>
       <c r="W29" s="24">
         <f>ATAN2(SQRT(R28^2+R29^2),-R30)</f>
-        <v>-1.5707963267948966</v>
+        <v>-1.5358897417550101</v>
       </c>
       <c r="X29" s="23">
         <f>DEGREES(W29)</f>
-        <v>-90</v>
+        <v>-88.000000000000014</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.3">
@@ -23875,28 +24166,28 @@
         <v>0</v>
       </c>
       <c r="R30" s="107">
-        <v>1</v>
+        <v>0.99939082701909576</v>
       </c>
       <c r="S30" s="108">
-        <v>-6.1257422745431001E-17</v>
+        <v>3.4899496702500955E-2</v>
       </c>
       <c r="T30" s="108">
         <v>6.1257422745431001E-17</v>
       </c>
       <c r="U30" s="109">
-        <v>600</v>
+        <v>599.81724810572871</v>
       </c>
       <c r="V30" s="21">
         <f>$V$17*R30+$V$18*S30+$V$19*T30+$V$20*U30</f>
-        <v>600</v>
+        <v>599.81724810572871</v>
       </c>
       <c r="W30" s="24">
         <f>IF(ABS(W29)=PI()/2,0,ATAN2(R28,R29))</f>
-        <v>0</v>
+        <v>2.9670597283903621</v>
       </c>
       <c r="X30" s="23">
         <f>DEGREES(W30)</f>
-        <v>0</v>
+        <v>170.00000000000011</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.3">
@@ -23952,23 +24243,23 @@
       </c>
       <c r="G33" s="1">
         <f>B17</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="H33" s="6">
         <f>RADIANS(G33)</f>
-        <v>0</v>
+        <v>-5.235987755982989E-2</v>
       </c>
       <c r="N33" s="11">
         <f>COS(H33)</f>
-        <v>1</v>
+        <v>0.99862953475457383</v>
       </c>
       <c r="O33" s="12">
         <f>-SIN(H33)*COS(D33)</f>
-        <v>0</v>
+        <v>3.2059657963603892E-18</v>
       </c>
       <c r="P33" s="12">
         <f>SIN(H33)*SIN(D33)</f>
-        <v>0</v>
+        <v>5.2335956242943835E-2</v>
       </c>
       <c r="Q33" s="13">
         <f>E33*COS(H33)</f>
@@ -23976,70 +24267,70 @@
       </c>
       <c r="R33" s="76">
         <f t="array" ref="R33:U36">MMULT(R28:U31,N33:Q36)</f>
-        <v>7.0964024677563694E-17</v>
+        <v>-8.5831651177431301E-2</v>
       </c>
       <c r="S33" s="77">
-        <v>0.17364817766693039</v>
+        <v>-0.17364817766693028</v>
       </c>
       <c r="T33" s="77">
-        <v>0.98480775301220802</v>
+        <v>0.98106026219040676</v>
       </c>
       <c r="U33" s="78">
-        <v>2.1289207403269107E-14</v>
+        <v>-10.310788478654082</v>
       </c>
       <c r="V33" s="21">
         <f>$V$17*R33+$V$18*S33+$V$19*T33+$V$20*U33</f>
-        <v>2.1289207403269107E-14</v>
+        <v>-10.310788478654082</v>
       </c>
       <c r="W33" s="24">
         <f>IF(W34=PI()/2,ATAN2(S34,S33),IF(-W34=PI()/2,-ATAN2(S34,S33),ATAN2(T35,S35)))</f>
-        <v>-2.9670597283903599</v>
+        <v>-6.4159268000441856E-16</v>
       </c>
       <c r="X33" s="23">
         <f>DEGREES(W33)</f>
-        <v>-169.99999999999997</v>
+        <v>-3.6760552730740746E-14</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="N34" s="11">
         <f>SIN(H33)</f>
-        <v>0</v>
+        <v>-5.2335956242943835E-2</v>
       </c>
       <c r="O34" s="12">
         <f>COS(H33)*COS(D33)</f>
-        <v>6.1257422745431001E-17</v>
+        <v>6.1173471576534015E-17</v>
       </c>
       <c r="P34" s="12">
         <f>-COS(H33)*SIN(D33)</f>
-        <v>1</v>
+        <v>0.99862953475457383</v>
       </c>
       <c r="Q34" s="13">
         <f>E33*SIN(H33)</f>
         <v>0</v>
       </c>
       <c r="R34" s="76">
-        <v>-4.9689545020929967E-17</v>
+        <v>1.5134435901338558E-2</v>
       </c>
       <c r="S34" s="77">
         <v>-0.98480775301220802</v>
       </c>
       <c r="T34" s="77">
-        <v>0.17364817766693039</v>
+        <v>-0.17298739392508941</v>
       </c>
       <c r="U34" s="78">
-        <v>-1.4906863506278992E-14</v>
+        <v>1.8180702011646825</v>
       </c>
       <c r="V34" s="21">
         <f>$V$17*R34+$V$19*S34+$V$18*T34+$V$20*U34</f>
-        <v>-1.4906863506278992E-14</v>
+        <v>1.8180702011646825</v>
       </c>
       <c r="W34" s="24">
         <f>ATAN2(SQRT(R33^2+R34^2),-R35)</f>
-        <v>-1.5707963267948966</v>
+        <v>-1.4835298641951802</v>
       </c>
       <c r="X34" s="23">
         <f>DEGREES(W34)</f>
-        <v>-90</v>
+        <v>-85</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.3">
@@ -24059,28 +24350,28 @@
         <v>0</v>
       </c>
       <c r="R35" s="76">
-        <v>1</v>
+        <v>0.99619469809174555</v>
       </c>
       <c r="S35" s="77">
-        <v>-6.1257422745431001E-17</v>
+        <v>-5.591848656724567E-17</v>
       </c>
       <c r="T35" s="77">
-        <v>-6.1257422745431001E-17</v>
+        <v>8.7155742747658166E-2</v>
       </c>
       <c r="U35" s="78">
-        <v>600</v>
+        <v>599.81724810572871</v>
       </c>
       <c r="V35" s="21">
         <f>$V$17*R35+$V$18*S35+$V$19*T35+$V$20*U35</f>
-        <v>600</v>
+        <v>599.81724810572871</v>
       </c>
       <c r="W35" s="24">
         <f>IF(ABS(W34)=PI()/2,0,ATAN2(R33,R34))</f>
-        <v>0</v>
+        <v>2.9670597283903608</v>
       </c>
       <c r="X35" s="23">
         <f>DEGREES(W35)</f>
-        <v>0</v>
+        <v>170.00000000000003</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.3">
@@ -24137,23 +24428,23 @@
       </c>
       <c r="G38" s="1">
         <f>B18</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H38" s="6">
         <f>RADIANS(G38)</f>
-        <v>0</v>
+        <v>6.9813170079773182E-2</v>
       </c>
       <c r="N38" s="11">
         <f>COS(H38)</f>
-        <v>1</v>
+        <v>0.9975640502598242</v>
       </c>
       <c r="O38" s="12">
         <f>-SIN(H38)*COS(D38)</f>
-        <v>0</v>
+        <v>-4.273101801374442E-18</v>
       </c>
       <c r="P38" s="12">
         <f>SIN(H38)*SIN(D38)</f>
-        <v>0</v>
+        <v>6.9756473744125302E-2</v>
       </c>
       <c r="Q38" s="13">
         <f>E38*COS(H38)</f>
@@ -24161,70 +24452,70 @@
       </c>
       <c r="R38" s="14">
         <f t="array" ref="R38:U41">MMULT(R33:U36,N38:Q41)</f>
-        <v>7.0964024677563694E-17</v>
+        <v>-9.7735654135185202E-2</v>
       </c>
       <c r="S38" s="15">
-        <v>0.98480775301220802</v>
+        <v>0.98106026219040676</v>
       </c>
       <c r="T38" s="15">
-        <v>-0.17364817766693033</v>
+        <v>0.16723786611188715</v>
       </c>
       <c r="U38" s="16">
-        <v>196.96155060244163</v>
+        <v>185.90126395942727</v>
       </c>
       <c r="V38" s="21">
         <f>$V$17*R38+$V$18*S38+$V$19*T38+$V$20*U38</f>
-        <v>196.96155060244163</v>
+        <v>185.90126395942727</v>
       </c>
       <c r="W38" s="24">
         <f>IF(W39=PI()/2,ATAN2(S39,S38),IF(-W39=PI()/2,-ATAN2(S39,S38),ATAN2(T40,S40)))</f>
-        <v>-1.3962634015954636</v>
+        <v>0.89769158095818025</v>
       </c>
       <c r="X38" s="7">
         <f>DEGREES(W38)</f>
-        <v>-80</v>
+        <v>51.433938893330186</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="N39" s="11">
         <f>SIN(H38)</f>
-        <v>0</v>
+        <v>6.9756473744125302E-2</v>
       </c>
       <c r="O39" s="12">
         <f>COS(H38)*COS(D38)</f>
-        <v>6.1257422745431001E-17</v>
+        <v>6.1108202742410423E-17</v>
       </c>
       <c r="P39" s="12">
         <f>-COS(H38)*SIN(D38)</f>
-        <v>-1</v>
+        <v>-0.9975640502598242</v>
       </c>
       <c r="Q39" s="13">
         <f>E38*SIN(H38)</f>
         <v>0</v>
       </c>
       <c r="R39" s="14">
-        <v>-4.9689545020929967E-17</v>
+        <v>-5.3599146989870144E-2</v>
       </c>
       <c r="S39" s="15">
-        <v>0.17364817766693033</v>
+        <v>-0.17298739392508947</v>
       </c>
       <c r="T39" s="15">
-        <v>0.98480775301220802</v>
+        <v>0.98346453570271875</v>
       </c>
       <c r="U39" s="16">
-        <v>34.729635533386066</v>
+        <v>-32.779408583853204</v>
       </c>
       <c r="V39" s="21">
         <f>$V$17*R39+$V$19*S39+$V$18*T39+$V$20*U39</f>
-        <v>34.729635533386066</v>
+        <v>-32.779408583853204</v>
       </c>
       <c r="W39" s="24">
         <f>ATAN2(SQRT(R38^2+R39^2),-R40)</f>
-        <v>-1.5707963267948966</v>
+        <v>-1.4590961402553408</v>
       </c>
       <c r="X39" s="7">
         <f>DEGREES(W39)</f>
-        <v>-90</v>
+        <v>-83.600050740459452</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.3">
@@ -24244,28 +24535,28 @@
         <v>200</v>
       </c>
       <c r="R40" s="14">
-        <v>1</v>
+        <v>0.99376801787576441</v>
       </c>
       <c r="S40" s="15">
-        <v>-6.1257422745431001E-17</v>
+        <v>8.7155742747658166E-2</v>
       </c>
       <c r="T40" s="15">
-        <v>6.1257422745431001E-17</v>
+        <v>6.9491029301473731E-2</v>
       </c>
       <c r="U40" s="16">
-        <v>600</v>
+        <v>617.24839665526031</v>
       </c>
       <c r="V40" s="21">
         <f>$V$17*R40+$V$18*S40+$V$19*T40+$V$20*U40</f>
-        <v>600</v>
+        <v>617.24839665526031</v>
       </c>
       <c r="W40" s="24">
         <f>IF(ABS(W39)=PI()/2,0,ATAN2(R38,R39))</f>
-        <v>0</v>
+        <v>-2.6399714878691736</v>
       </c>
       <c r="X40" s="23">
         <f>DEGREES(W40)</f>
-        <v>0</v>
+        <v>-151.25922428977606</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.3">
@@ -24319,23 +24610,23 @@
       </c>
       <c r="G43" s="1">
         <f>B19</f>
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="H43" s="6">
         <f>RADIANS(G43)</f>
-        <v>0</v>
+        <v>-8.7266462599716474E-2</v>
       </c>
       <c r="N43" s="11">
         <f>COS(H43)</f>
-        <v>1</v>
+        <v>0.99619469809174555</v>
       </c>
       <c r="O43" s="12">
         <f>-SIN(H43)*COS(D43)</f>
-        <v>0</v>
+        <v>5.3389361781853285E-18</v>
       </c>
       <c r="P43" s="12">
         <f>SIN(H43)*SIN(D43)</f>
-        <v>0</v>
+        <v>8.7155742747658166E-2</v>
       </c>
       <c r="Q43" s="13">
         <f>E43*COS(H43)</f>
@@ -24343,70 +24634,70 @@
       </c>
       <c r="R43" s="14">
         <f t="array" ref="R43:U46">MMULT(R38:U41,N43:Q46)</f>
-        <v>7.0964024677563694E-17</v>
+        <v>-0.18286877629541726</v>
       </c>
       <c r="S43" s="15">
-        <v>0.17364817766693039</v>
+        <v>-0.1672378661118871</v>
       </c>
       <c r="T43" s="15">
-        <v>0.98480775301220802</v>
+        <v>0.96880880817350068</v>
       </c>
       <c r="U43" s="16">
-        <v>196.96155060244163</v>
+        <v>185.90126395942727</v>
       </c>
       <c r="V43" s="21">
         <f>$V$17*R43+$V$18*S43+$V$19*T43+$V$20*U43</f>
-        <v>196.96155060244163</v>
+        <v>185.90126395942727</v>
       </c>
       <c r="W43" s="24">
         <f>IF(W44=PI()/2,ATAN2(S44,S43),IF(-W44=PI()/2,-ATAN2(S44,S43),ATAN2(T45,S45)))</f>
-        <v>-2.9670597283903599</v>
+        <v>-0.3810846014403374</v>
       </c>
       <c r="X43" s="7">
         <f>DEGREES(W43)</f>
-        <v>-169.99999999999997</v>
+        <v>-21.834539299956425</v>
       </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="N44" s="11">
         <f>SIN(H43)</f>
-        <v>0</v>
+        <v>-8.7155742747658166E-2</v>
       </c>
       <c r="O44" s="12">
         <f>COS(H43)*COS(D43)</f>
-        <v>6.1257422745431001E-17</v>
+        <v>6.1024319757763067E-17</v>
       </c>
       <c r="P44" s="12">
         <f>-COS(H43)*SIN(D43)</f>
-        <v>1</v>
+        <v>0.99619469809174555</v>
       </c>
       <c r="Q44" s="13">
         <f>E43*SIN(H43)</f>
         <v>0</v>
       </c>
       <c r="R44" s="14">
-        <v>-4.9689545020929967E-17</v>
+        <v>-3.8318341250025881E-2</v>
       </c>
       <c r="S44" s="15">
-        <v>-0.98480775301220802</v>
+        <v>-0.98346453570271875</v>
       </c>
       <c r="T44" s="15">
-        <v>0.17364817766693039</v>
+        <v>-0.17700059813142535</v>
       </c>
       <c r="U44" s="16">
-        <v>34.729635533386066</v>
+        <v>-32.779408583853204</v>
       </c>
       <c r="V44" s="21">
         <f>$V$17*R44+$V$19*S44+$V$18*T44+$V$20*U44</f>
-        <v>34.729635533386066</v>
+        <v>-32.779408583853204</v>
       </c>
       <c r="W44" s="24">
         <f>ATAN2(SQRT(R43^2+R44^2),-R45)</f>
-        <v>-1.5707963267948966</v>
+        <v>-1.3828515445598624</v>
       </c>
       <c r="X44" s="7">
         <f>DEGREES(W44)</f>
-        <v>-90</v>
+        <v>-79.231557196427204</v>
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.3">
@@ -24426,28 +24717,28 @@
         <v>0</v>
       </c>
       <c r="R45" s="14">
-        <v>1</v>
+        <v>0.98239030704708363</v>
       </c>
       <c r="S45" s="15">
-        <v>-6.1257422745431001E-17</v>
+        <v>-6.9491029301473717E-2</v>
       </c>
       <c r="T45" s="15">
-        <v>-6.1257422745431001E-17</v>
+        <v>0.17343667855029543</v>
       </c>
       <c r="U45" s="16">
-        <v>600</v>
+        <v>617.24839665526031</v>
       </c>
       <c r="V45" s="21">
         <f>$V$17*R45+$V$18*S45+$V$19*T45+$V$20*U45</f>
-        <v>600</v>
+        <v>617.24839665526031</v>
       </c>
       <c r="W45" s="24">
         <f>IF(ABS(W44)=PI()/2,0,ATAN2(R43,R44))</f>
-        <v>0</v>
+        <v>-2.9350409773488884</v>
       </c>
       <c r="X45" s="23">
         <f>DEGREES(W45)</f>
-        <v>0</v>
+        <v>-168.16546070004355</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.3">
@@ -24501,19 +24792,19 @@
       </c>
       <c r="G48" s="1">
         <f>B20</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H48" s="6">
         <f>RADIANS(G48)</f>
-        <v>0</v>
+        <v>0.10471975511965978</v>
       </c>
       <c r="N48" s="11">
         <f>COS(H48)</f>
-        <v>1</v>
+        <v>0.99452189536827329</v>
       </c>
       <c r="O48" s="12">
         <f>-SIN(H48)*COS(D48)</f>
-        <v>0</v>
+        <v>-0.10452846326765347</v>
       </c>
       <c r="P48" s="12">
         <f>SIN(H48)*SIN(D48)</f>
@@ -24523,40 +24814,40 @@
         <f>E48*COS(H48)</f>
         <v>0</v>
       </c>
-      <c r="R48" s="107">
+      <c r="R48" s="116">
         <f t="array" ref="R48:U51">MMULT(R43:U46,N48:Q51)</f>
-        <v>7.0964024677563694E-17</v>
-      </c>
-      <c r="S48" s="108">
-        <v>0.17364817766693039</v>
-      </c>
-      <c r="T48" s="108">
-        <v>0.98480775301220802</v>
+        <v>-0.19934811914983228</v>
+      </c>
+      <c r="S48" s="117">
+        <v>-0.14720672741714322</v>
+      </c>
+      <c r="T48" s="117">
+        <v>0.96880880817350068</v>
       </c>
       <c r="U48" s="109">
-        <v>246.20193825305205</v>
+        <v>234.34170436810228</v>
       </c>
       <c r="V48" s="21">
         <f>$V$17*R48+$V$18*S48+$V$19*T48+$V$20*U48</f>
-        <v>246.20193825305205</v>
+        <v>234.34170436810228</v>
       </c>
       <c r="W48" s="110">
         <f>IF(W49=PI()/2,ATAN2(S49,S48),IF(-W49=PI()/2,-ATAN2(S49,S48),ATAN2(T50,S50)))</f>
-        <v>-2.9670597283903599</v>
+        <v>-0.78065192386777138</v>
       </c>
       <c r="X48" s="7">
         <f>DEGREES(W48)</f>
-        <v>-169.99999999999997</v>
+        <v>-44.728060506391358</v>
       </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="N49" s="11">
         <f>SIN(H48)</f>
-        <v>0</v>
+        <v>0.10452846326765347</v>
       </c>
       <c r="O49" s="12">
         <f>COS(H48)*COS(D48)</f>
-        <v>1</v>
+        <v>0.99452189536827329</v>
       </c>
       <c r="P49" s="12">
         <f>-COS(H48)*SIN(D48)</f>
@@ -24566,29 +24857,29 @@
         <f>E48*SIN(H48)</f>
         <v>0</v>
       </c>
-      <c r="R49" s="107">
-        <v>-4.9689545020929967E-17</v>
-      </c>
-      <c r="S49" s="108">
-        <v>-0.98480775301220802</v>
-      </c>
-      <c r="T49" s="108">
-        <v>0.17364817766693039</v>
+      <c r="R49" s="116">
+        <v>-0.14090846596258555</v>
+      </c>
+      <c r="S49" s="117">
+        <v>-0.97407165674871599</v>
+      </c>
+      <c r="T49" s="117">
+        <v>-0.17700059813142535</v>
       </c>
       <c r="U49" s="109">
-        <v>43.412044416732584</v>
+        <v>-41.629438490424469</v>
       </c>
       <c r="V49" s="21">
         <f>$V$17*R49+$V$19*S49+$V$18*T49+$V$20*U49</f>
-        <v>43.412044416732584</v>
+        <v>-41.629438490424469</v>
       </c>
       <c r="W49" s="110">
         <f>ATAN2(SQRT(R48^2+R49^2),-R50)</f>
-        <v>-1.5707963267948966</v>
+        <v>-1.3241835721572917</v>
       </c>
       <c r="X49" s="7">
         <f>DEGREES(W49)</f>
-        <v>-90</v>
+        <v>-75.870129985169925</v>
       </c>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.3">
@@ -24607,29 +24898,29 @@
         <f>F48</f>
         <v>50</v>
       </c>
-      <c r="R50" s="107">
-        <v>1</v>
-      </c>
-      <c r="S50" s="108">
-        <v>-6.1257422745431001E-17</v>
-      </c>
-      <c r="T50" s="108">
-        <v>-6.1257422745431001E-17</v>
+      <c r="R50" s="116">
+        <v>0.96974487965211498</v>
+      </c>
+      <c r="S50" s="117">
+        <v>-0.17179809929666373</v>
+      </c>
+      <c r="T50" s="117">
+        <v>0.17343667855029543</v>
       </c>
       <c r="U50" s="109">
-        <v>600</v>
+        <v>625.92023058277505</v>
       </c>
       <c r="V50" s="21">
         <f>$V$17*R50+$V$18*S50+$V$19*T50+$V$20*U50</f>
-        <v>600</v>
+        <v>625.92023058277505</v>
       </c>
       <c r="W50" s="110">
         <f>IF(ABS(W49)=PI()/2,0,ATAN2(R48,R49))</f>
-        <v>0</v>
+        <v>-2.5262866687723746</v>
       </c>
       <c r="X50" s="23">
         <f>DEGREES(W50)</f>
-        <v>0</v>
+        <v>-144.74556396082122</v>
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.3">
@@ -24645,13 +24936,13 @@
       <c r="Q51" s="13">
         <v>1</v>
       </c>
-      <c r="R51" s="107">
+      <c r="R51" s="116">
         <v>0</v>
       </c>
-      <c r="S51" s="108">
+      <c r="S51" s="117">
         <v>0</v>
       </c>
-      <c r="T51" s="108">
+      <c r="T51" s="117">
         <v>0</v>
       </c>
       <c r="U51" s="109">
@@ -24700,75 +24991,75 @@
       </c>
       <c r="C56" s="7">
         <f t="array" ref="C56:C59">V48:V51</f>
-        <v>246.20193825305205</v>
+        <v>234.34170436810228</v>
       </c>
       <c r="D56" s="24">
         <f t="array" ref="D56:D58">W48:W50</f>
-        <v>-2.9670597283903599</v>
+        <v>-0.78065192386777138</v>
       </c>
       <c r="E56" s="23">
         <f>DEGREES(D56)</f>
-        <v>-169.99999999999997</v>
+        <v>-44.728060506391358</v>
       </c>
       <c r="F56" s="111">
         <f>D56+PI()</f>
-        <v>0.1745329251994332</v>
+        <v>2.3609407297220217</v>
       </c>
       <c r="G56" s="24">
         <f>IF(F56&gt;PI(),F56-2*PI(),F56)</f>
-        <v>0.1745329251994332</v>
+        <v>2.3609407297220217</v>
       </c>
       <c r="H56" s="23">
         <f>DEGREES(G56)</f>
-        <v>10.000000000000014</v>
+        <v>135.27193949360864</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C57" s="7">
-        <v>43.412044416732584</v>
+        <v>-41.629438490424469</v>
       </c>
       <c r="D57" s="24">
-        <v>-1.5707963267948966</v>
+        <v>-1.3241835721572917</v>
       </c>
       <c r="E57" s="23">
         <f>DEGREES(D57)</f>
-        <v>-90</v>
+        <v>-75.870129985169925</v>
       </c>
       <c r="F57" s="111">
         <f>D57+PI()/2</f>
-        <v>0</v>
+        <v>0.2466127546376049</v>
       </c>
       <c r="G57" s="24">
         <f>IF(F57&gt;PI(),F57-2*PI(),F57)</f>
-        <v>0</v>
+        <v>0.2466127546376049</v>
       </c>
       <c r="H57" s="23">
         <f>DEGREES(G57)</f>
-        <v>0</v>
+        <v>14.129870014830081</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C58" s="7">
-        <v>600</v>
+        <v>625.92023058277505</v>
       </c>
       <c r="D58" s="24">
-        <v>0</v>
+        <v>-2.5262866687723746</v>
       </c>
       <c r="E58" s="23">
         <f>DEGREES(D58)</f>
-        <v>0</v>
+        <v>-144.74556396082122</v>
       </c>
       <c r="F58" s="111">
         <f>D58</f>
-        <v>0</v>
+        <v>-2.5262866687723746</v>
       </c>
       <c r="G58" s="24">
         <f>IF(F58&gt;PI(),F58-2*PI(),F58)</f>
-        <v>0</v>
+        <v>-2.5262866687723746</v>
       </c>
       <c r="H58" s="23">
         <f>DEGREES(G58)</f>
-        <v>0</v>
+        <v>-144.74556396082122</v>
       </c>
       <c r="P58" s="110"/>
     </row>
@@ -24779,152 +25070,158 @@
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C60" s="7"/>
-      <c r="F60" t="s">
-        <v>67</v>
-      </c>
-      <c r="I60" t="s">
-        <v>65</v>
-      </c>
+      <c r="O60" s="7"/>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B61" s="113">
-        <f>COS(D58)*COS(D57)</f>
-        <v>6.1257422745431001E-17</v>
-      </c>
-      <c r="C61" s="113">
-        <f>-COS(D57)*SIN(D58)</f>
-        <v>0</v>
-      </c>
-      <c r="D61" s="113">
-        <f>-SIN(D57)</f>
-        <v>1</v>
-      </c>
-      <c r="E61" s="27">
-        <f>C56</f>
-        <v>246.20193825305205</v>
-      </c>
-      <c r="F61" s="110">
-        <f>IF(F62=PI()/2,ATAN2(C62,C61),IF(-F62=PI()/2,-ATAN2(C62,C61),ATAN2(D63,C63)))</f>
-        <v>-1.5707963267948968</v>
-      </c>
-      <c r="G61" s="7">
-        <f>DEGREES(F61)</f>
-        <v>-90.000000000000014</v>
-      </c>
-      <c r="H61" s="111">
-        <f>F61+PI()</f>
-        <v>1.5707963267948963</v>
-      </c>
-      <c r="I61" s="24">
-        <f>IF(H61&gt;PI(),H61-2*PI(),H61)</f>
-        <v>1.5707963267948963</v>
-      </c>
-      <c r="J61" s="23">
-        <f>DEGREES(I61)</f>
-        <v>89.999999999999986</v>
+      <c r="A61" t="s">
+        <v>69</v>
+      </c>
+      <c r="F61" t="s">
+        <v>67</v>
+      </c>
+      <c r="I61" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B62" s="113">
-        <f>-SIN(D56)*SIN(D57)*COS(D58)+COS(D56)*SIN(D58)</f>
-        <v>-0.17364817766693069</v>
+        <f>COS(D58)*COS(D57)</f>
+        <v>-0.19934811914983236</v>
       </c>
       <c r="C62" s="113">
-        <f>SIN(D56)*SIN(D57)*SIN(D58)+COS(D56)*COS(D58)</f>
-        <v>-0.98480775301220802</v>
+        <f>SIN(D56)*SIN(D57)*COS(D58)-COS(D56)*SIN(D58)</f>
+        <v>-0.14720672741714297</v>
       </c>
       <c r="D62" s="113">
-        <f>SIN(D56)*COS(D57)</f>
-        <v>-1.0637239828316884E-17</v>
-      </c>
-      <c r="E62" s="27">
-        <f>C57</f>
-        <v>43.412044416732584</v>
+        <f>COS(D56)*SIN(D57)*COS(D58)+SIN(D56)*SIN(D58)</f>
+        <v>0.9688088081735009</v>
+      </c>
+      <c r="E62" s="113">
+        <f>C56</f>
+        <v>234.34170436810228</v>
       </c>
       <c r="F62" s="110">
-        <f>ATAN2(SQRT(B61^2+B62^2),-B63)</f>
-        <v>-1.3962634015954634</v>
+        <f>IF(F63=PI()/2,ATAN2(C63,C62),IF(-F63=PI()/2,-ATAN2(C63,C62),ATAN2(D64,C64)))</f>
+        <v>-0.78065192386777138</v>
       </c>
       <c r="G62" s="7">
         <f>DEGREES(F62)</f>
-        <v>-79.999999999999986</v>
+        <v>-44.728060506391358</v>
       </c>
       <c r="H62" s="111">
-        <f>F62+PI()/2</f>
-        <v>0.1745329251994332</v>
+        <f>F62+PI()</f>
+        <v>2.3609407297220217</v>
       </c>
       <c r="I62" s="24">
         <f>IF(H62&gt;PI(),H62-2*PI(),H62)</f>
-        <v>0.1745329251994332</v>
+        <v>2.3609407297220217</v>
       </c>
       <c r="J62" s="23">
         <f>DEGREES(I62)</f>
-        <v>10.000000000000014</v>
+        <v>135.27193949360864</v>
       </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B63" s="113">
-        <f>COS(D56)*SIN(D57)*COS(D58)+SIN(D56)*SIN(D58)</f>
-        <v>0.98480775301220802</v>
-      </c>
-      <c r="C63" s="113">
-        <f>-COS(D56)*SIN(D57)*SIN(D58)+SIN(D56)*COS(D58)</f>
-        <v>-0.17364817766693069</v>
+      <c r="B63" s="114">
+        <f>COS(D57)*SIN(D58)</f>
+        <v>-0.14090846596258566</v>
+      </c>
+      <c r="C63" s="114">
+        <f>SIN(D56)*SIN(D57)*SIN(D58)+COS(D56)*COS(D58)</f>
+        <v>-0.97407165674871599</v>
       </c>
       <c r="D63" s="113">
-        <f>COS(D56)*COS(D57)</f>
-        <v>-6.032678484924683E-17</v>
-      </c>
-      <c r="E63" s="27">
-        <f>C58</f>
-        <v>600</v>
+        <f>COS(D56)*SIN(D57)*SIN(D58)-SIN(D56)*COS(D58)</f>
+        <v>-0.17700059813142499</v>
+      </c>
+      <c r="E63" s="113">
+        <f>C57</f>
+        <v>-41.629438490424469</v>
       </c>
       <c r="F63" s="110">
-        <f>IF(ABS(F62)=PI()/2,0,ATAN2(B61,B62))</f>
-        <v>-1.5707963267948963</v>
-      </c>
-      <c r="G63" s="23">
+        <f>ATAN2(SQRT(B62^2+B63^2),-B64)</f>
+        <v>-1.3241835721572917</v>
+      </c>
+      <c r="G63" s="7">
         <f>DEGREES(F63)</f>
-        <v>-89.999999999999986</v>
+        <v>-75.870129985169925</v>
       </c>
       <c r="H63" s="111">
-        <f>F63</f>
-        <v>-1.5707963267948963</v>
+        <f>F63+PI()/2</f>
+        <v>0.2466127546376049</v>
       </c>
       <c r="I63" s="24">
         <f>IF(H63&gt;PI(),H63-2*PI(),H63)</f>
-        <v>-1.5707963267948963</v>
+        <v>0.2466127546376049</v>
       </c>
       <c r="J63" s="23">
         <f>DEGREES(I63)</f>
-        <v>-89.999999999999986</v>
+        <v>14.129870014830081</v>
       </c>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B64">
+      <c r="B64" s="114">
+        <f>-SIN(D57)</f>
+        <v>0.96974487965211509</v>
+      </c>
+      <c r="C64" s="113">
+        <f>SIN(D56)*COS(D57)</f>
+        <v>-0.17179809929666384</v>
+      </c>
+      <c r="D64" s="113">
+        <f>COS(D56)*COS(D57)</f>
+        <v>0.17343667855029554</v>
+      </c>
+      <c r="E64" s="113">
+        <f>C58</f>
+        <v>625.92023058277505</v>
+      </c>
+      <c r="F64" s="110">
+        <f>IF(ABS(F63)=PI()/2,0,ATAN2(B62,B63))</f>
+        <v>-2.5262866687723746</v>
+      </c>
+      <c r="G64" s="7">
+        <f>DEGREES(F64)</f>
+        <v>-144.74556396082122</v>
+      </c>
+      <c r="H64" s="111">
+        <f>F64</f>
+        <v>-2.5262866687723746</v>
+      </c>
+      <c r="I64" s="24">
+        <f>IF(H64&gt;PI(),H64-2*PI(),H64)</f>
+        <v>-2.5262866687723746</v>
+      </c>
+      <c r="J64" s="23">
+        <f>DEGREES(I64)</f>
+        <v>-144.74556396082122</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B65" s="113">
         <v>0</v>
       </c>
-      <c r="C64" s="7">
+      <c r="C65" s="113">
         <v>0</v>
       </c>
-      <c r="D64">
+      <c r="D65" s="113">
         <v>0</v>
       </c>
-      <c r="E64">
+      <c r="E65" s="113">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A67" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>34</v>
       </c>
@@ -24932,29 +25229,78 @@
       <c r="F69">
         <v>0</v>
       </c>
+      <c r="I69" s="7">
+        <f t="array" ref="I69:L72">MMULT(B62:E65,F69:F72)</f>
+        <v>185.90126395942724</v>
+      </c>
+      <c r="J69" s="7">
+        <v>185.90126395942724</v>
+      </c>
+      <c r="K69" s="7">
+        <v>185.90126395942724</v>
+      </c>
+      <c r="L69" s="7">
+        <v>185.90126395942724</v>
+      </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F70">
         <v>0</v>
       </c>
+      <c r="I70" s="7">
+        <v>-32.779408583853218</v>
+      </c>
+      <c r="J70" s="7">
+        <v>-32.779408583853218</v>
+      </c>
+      <c r="K70" s="7">
+        <v>-32.779408583853218</v>
+      </c>
+      <c r="L70" s="7">
+        <v>-32.779408583853218</v>
+      </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F71">
         <f>-F48</f>
         <v>-50</v>
       </c>
+      <c r="I71" s="7">
+        <v>617.24839665526031</v>
+      </c>
+      <c r="J71" s="7">
+        <v>617.24839665526031</v>
+      </c>
+      <c r="K71" s="7">
+        <v>617.24839665526031</v>
+      </c>
+      <c r="L71" s="7">
+        <v>617.24839665526031</v>
+      </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F72">
         <v>1</v>
       </c>
+      <c r="I72" s="7">
+        <v>1</v>
+      </c>
+      <c r="J72" s="7">
+        <v>1</v>
+      </c>
+      <c r="K72" s="7">
+        <v>1</v>
+      </c>
+      <c r="L72" s="7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="73" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>35</v>
       </c>
@@ -24965,65 +25311,32 @@
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="5"/>
-      <c r="B76" s="8">
-        <f t="array" ref="B76:E79">MINVERSE(R48:U51)</f>
-        <v>7.0964024677563694E-17</v>
-      </c>
-      <c r="C76" s="8">
-        <v>-4.9689545020929967E-17</v>
-      </c>
-      <c r="D76" s="8">
-        <v>1</v>
-      </c>
-      <c r="E76" s="8">
-        <v>-600</v>
-      </c>
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B77" s="8">
-        <v>0.17364817766693041</v>
-      </c>
-      <c r="C77" s="8">
-        <v>-0.98480775301220813</v>
-      </c>
-      <c r="D77" s="8">
-        <v>-6.1257422745431001E-17</v>
-      </c>
-      <c r="E77" s="8">
-        <v>1.4430080055458136E-14</v>
-      </c>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B78" s="8">
-        <v>0.98480775301220813</v>
-      </c>
-      <c r="C78" s="8">
-        <v>0.17364817766693041</v>
-      </c>
-      <c r="D78" s="8">
-        <v>-6.1257422745431013E-17</v>
-      </c>
-      <c r="E78" s="8">
-        <v>-250.00000000000003</v>
-      </c>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B79" s="8">
-        <v>0</v>
-      </c>
-      <c r="C79" s="8">
-        <v>0</v>
-      </c>
-      <c r="D79" s="8">
-        <v>0</v>
-      </c>
-      <c r="E79" s="8">
-        <v>1</v>
-      </c>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
     </row>
-    <row r="80" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A80" s="18" t="s">
         <v>39</v>
       </c>
@@ -25041,62 +25354,60 @@
       <c r="A82" s="9"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B83" s="4">
-        <f>E61+F71*D61</f>
-        <v>196.20193825305205</v>
+      <c r="B83" s="27">
+        <f t="array" ref="B83:B86">L69:L72</f>
+        <v>185.90126395942724</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>36</v>
       </c>
       <c r="H83" s="24">
         <f>ATAN2(B83,B84)</f>
-        <v>0.2177537789342664</v>
+        <v>-0.17453292519943314</v>
       </c>
       <c r="I83" s="26">
         <f>DEGREES(H83)</f>
-        <v>12.476372505958198</v>
+        <v>-10.000000000000011</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>32</v>
       </c>
-      <c r="B84" s="4">
-        <f>E62+F71*D62</f>
-        <v>43.412044416732584</v>
+      <c r="B84">
+        <v>-32.779408583853218</v>
       </c>
       <c r="H84" s="24">
         <f>ATAN2(-B83,-B84)</f>
-        <v>-2.9238388746555266</v>
+        <v>2.9670597283903599</v>
       </c>
       <c r="I84" s="26">
         <f>DEGREES(H84)</f>
-        <v>-167.52362749404179</v>
+        <v>169.99999999999997</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B85" s="4">
-        <f>E63+F71*D63</f>
-        <v>600</v>
+      <c r="B85">
+        <v>617.24839665526031</v>
       </c>
       <c r="E85" t="s">
         <v>42</v>
       </c>
       <c r="G85" s="24">
         <f>IF(B87=1,H83,H84)</f>
-        <v>0.2177537789342664</v>
+        <v>-0.17453292519943314</v>
       </c>
       <c r="H85" s="26">
         <f>DEGREES(G85)</f>
-        <v>12.476372505958198</v>
+        <v>-10.000000000000011</v>
       </c>
       <c r="I85" s="18" t="str">
         <f>IF(ABS(H85-B15)&lt; 0.001,"OK","NOT OK!")</f>
-        <v>NOT OK!</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B86" s="4">
+      <c r="B86">
         <v>1</v>
       </c>
       <c r="E86" t="s">
@@ -25104,11 +25415,11 @@
       </c>
       <c r="G86" s="24">
         <f>IF(B87=-1,H83,H84)</f>
-        <v>-2.9238388746555266</v>
+        <v>2.9670597283903599</v>
       </c>
       <c r="H86" s="26">
         <f>DEGREES(G86)</f>
-        <v>-167.52362749404179</v>
+        <v>169.99999999999997</v>
       </c>
       <c r="I86" s="18" t="str">
         <f>IF(ABS(H86-B15)&lt; 0.001,"OK","NOT OK!")</f>
@@ -25143,7 +25454,7 @@
       </c>
       <c r="L96">
         <f>E112*B87</f>
-        <v>200.94727212553749</v>
+        <v>188.76909060759877</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.3">
@@ -25152,7 +25463,7 @@
       </c>
       <c r="L97" s="4">
         <f>E110</f>
-        <v>300</v>
+        <v>317.24839665526031</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.3">
@@ -25161,31 +25472,31 @@
     <row r="110" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E110" s="22">
         <f>B85-F23</f>
-        <v>300</v>
+        <v>317.24839665526031</v>
       </c>
       <c r="M110" s="24">
         <f>ACOS((E117*E117-E116*E116-E115*E115)/(-2*E116*E115))</f>
-        <v>0.58702785252926659</v>
+        <v>0.57165615699477501</v>
       </c>
       <c r="N110" s="23">
         <f>DEGREES(M110)</f>
-        <v>33.634218406555064</v>
+        <v>32.753485128468604</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E112" s="4">
         <f>SQRT(B83*B83+B84*B84)</f>
-        <v>200.94727212553749</v>
+        <v>188.76909060759877</v>
       </c>
       <c r="I112" s="22"/>
       <c r="J112" s="22"/>
       <c r="M112" s="24">
         <f>ACOS((E115*E115-E116*E116-E117*E117)/(-2*E116*E117))</f>
-        <v>1.5739613835350543</v>
+        <v>1.6231562043547259</v>
       </c>
       <c r="N112" s="25">
         <f>DEGREES(M112)</f>
-        <v>90.181344393130473</v>
+        <v>92.999999999999972</v>
       </c>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.3">
@@ -25209,7 +25520,7 @@
       </c>
       <c r="E115" s="7">
         <f>SQRT(E112*E112+E110*E110)</f>
-        <v>361.08143980921369</v>
+        <v>369.16163769973878</v>
       </c>
       <c r="L115" t="s">
         <v>48</v>
@@ -25242,21 +25553,21 @@
       </c>
       <c r="M116" s="42">
         <f>ATAN2(M115*E112,(B85-F23))</f>
-        <v>0.98061089524819778</v>
+        <v>1.0340467548400085</v>
       </c>
       <c r="N116" s="43">
         <f>DEGREES(M116)</f>
-        <v>56.184865642267006</v>
+        <v>59.246514871531417</v>
       </c>
       <c r="O116" s="44"/>
       <c r="P116" s="44"/>
       <c r="Q116" s="45">
         <f>ATAN2(Q115*E112,(B85-F23))</f>
-        <v>2.1609817583415953</v>
+        <v>2.1075458987497848</v>
       </c>
       <c r="R116" s="43">
         <f>DEGREES(Q116)</f>
-        <v>123.81513435773299</v>
+        <v>120.7534851284686</v>
       </c>
       <c r="S116" s="46"/>
     </row>
@@ -25304,24 +25615,24 @@
       <c r="G120" s="1"/>
       <c r="M120" s="48">
         <f>PI()/2-(M116+M110)</f>
-        <v>3.1575790174320773E-3</v>
+        <v>-3.4906585039887084E-2</v>
       </c>
       <c r="N120" s="49">
         <f>DEGREES(M120)</f>
-        <v>0.18091595117792342</v>
+        <v>-2.0000000000000284</v>
       </c>
       <c r="O120" s="50" t="str">
         <f>IF(ABS(N120-B16)&lt; 0.001,"OK","NOT OK!")</f>
-        <v>NOT OK!</v>
+        <v>OK</v>
       </c>
       <c r="P120" s="44"/>
       <c r="Q120" s="51">
         <f>PI()/2-(Q116+M110)</f>
-        <v>-1.1772132840759655</v>
+        <v>-1.1084057289496632</v>
       </c>
       <c r="R120" s="49">
         <f>DEGREES(Q120)</f>
-        <v>-67.449352764288065</v>
+        <v>-63.506970256937187</v>
       </c>
       <c r="S120" s="52" t="str">
         <f>IF(ABS(R120-H16)&lt; 0.001,"OK","NOT OK!")</f>
@@ -25332,24 +25643,24 @@
       <c r="G121" s="1"/>
       <c r="M121" s="48">
         <f>PI()/2-M112</f>
-        <v>-3.1650567401577678E-3</v>
+        <v>-5.2359877559829293E-2</v>
       </c>
       <c r="N121" s="49">
         <f>DEGREES(M121)</f>
-        <v>-0.18134439313047457</v>
+        <v>-2.9999999999999662</v>
       </c>
       <c r="O121" s="50" t="str">
         <f>IF(ABS(N121-B17)&lt; 0.001,"OK","NOT OK!")</f>
-        <v>NOT OK!</v>
+        <v>OK</v>
       </c>
       <c r="P121" s="44"/>
       <c r="Q121" s="51">
         <f>PI()/2-M112</f>
-        <v>-3.1650567401577678E-3</v>
+        <v>-5.2359877559829293E-2</v>
       </c>
       <c r="R121" s="49">
         <f>DEGREES(Q121)</f>
-        <v>-0.18134439313047457</v>
+        <v>-2.9999999999999662</v>
       </c>
       <c r="S121" s="52" t="str">
         <f>IF(ABS(R121-H17)&lt; 0.001,"OK","NOT OK!")</f>
@@ -25400,11 +25711,11 @@
       </c>
       <c r="M126" s="48">
         <f>PI()/2-(M116-M110)</f>
-        <v>1.1772132840759655</v>
+        <v>1.1084057289496632</v>
       </c>
       <c r="N126" s="49">
         <f>DEGREES(M126)</f>
-        <v>67.449352764288065</v>
+        <v>63.506970256937187</v>
       </c>
       <c r="O126" s="50" t="str">
         <f>IF(ABS(N126-B16)&lt; 0.001,"OK","NOT OK!")</f>
@@ -25413,11 +25724,11 @@
       <c r="P126" s="44"/>
       <c r="Q126" s="51">
         <f>PI()/2-(Q116-M110)</f>
-        <v>-3.1575790174320773E-3</v>
+        <v>3.490658503988664E-2</v>
       </c>
       <c r="R126" s="49">
         <f>DEGREES(Q126)</f>
-        <v>-0.18091595117792342</v>
+        <v>2.0000000000000027</v>
       </c>
       <c r="S126" s="52" t="str">
         <f>IF(ABS(R126-H16)&lt; 0.001,"OK","NOT OK!")</f>
@@ -25428,11 +25739,11 @@
       <c r="A127" s="18"/>
       <c r="M127" s="55">
         <f>(M112- PI()*3/2)</f>
-        <v>-3.1384275968496356</v>
+        <v>-3.0892327760299638</v>
       </c>
       <c r="N127" s="56">
         <f>DEGREES(M127)</f>
-        <v>-179.81865560686953</v>
+        <v>-177.00000000000003</v>
       </c>
       <c r="O127" s="57" t="str">
         <f>IF(ABS(N127-B17)&lt; 0.001,"OK","NOT OK!")</f>
@@ -25441,11 +25752,11 @@
       <c r="P127" s="58"/>
       <c r="Q127" s="59">
         <f>(M112- PI()*3/2)</f>
-        <v>-3.1384275968496356</v>
+        <v>-3.0892327760299638</v>
       </c>
       <c r="R127" s="56">
         <f>DEGREES(Q127)</f>
-        <v>-179.81865560686953</v>
+        <v>-177.00000000000003</v>
       </c>
       <c r="S127" s="60" t="str">
         <f>IF(ABS(R127-H17)&lt; 0.001,"OK","NOT OK!")</f>
@@ -25476,25 +25787,25 @@
       <c r="I131" s="64"/>
       <c r="J131" s="65">
         <f t="array" ref="J131:L133">MMULT(MMULT(N38:P40,N43:P45),N48:P50)</f>
-        <v>1</v>
+        <v>0.98103251569073346</v>
       </c>
       <c r="K131" s="65">
-        <v>0</v>
+        <v>-0.17325138423531034</v>
       </c>
       <c r="L131" s="65">
-        <v>0</v>
+        <v>8.694343573875718E-2</v>
       </c>
       <c r="M131" s="88">
         <f>COS(C18)*COS(C19)*COS(C20)-SIN(C18)*SIN(C20)</f>
-        <v>1</v>
+        <v>0.98103251569073346</v>
       </c>
       <c r="N131" s="88">
         <f>-COS(C18)*COS(C19)*SIN(C20)-SIN(C18)*COS(C20)</f>
-        <v>0</v>
+        <v>-0.17325138423531034</v>
       </c>
       <c r="O131" s="88">
         <f>-COS(C18)*SIN(C19)</f>
-        <v>0</v>
+        <v>8.694343573875718E-2</v>
       </c>
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.3">
@@ -25504,230 +25815,230 @@
       <c r="H132" s="64"/>
       <c r="I132" s="64"/>
       <c r="J132" s="65">
-        <v>0</v>
+        <v>0.17338418735670946</v>
       </c>
       <c r="K132" s="65">
-        <v>1</v>
+        <v>0.98483549951188121</v>
       </c>
       <c r="L132" s="65">
-        <v>0</v>
+        <v>6.0796772806267557E-3</v>
       </c>
       <c r="M132" s="88">
         <f>SIN(C18)*COS(C19)*COS(C20)+COS(C18)*SIN(C20)</f>
-        <v>0</v>
+        <v>0.17338418735670946</v>
       </c>
       <c r="N132" s="88">
         <f>-SIN(C18)*COS(C19)*SIN(C20)+COS(C18)*COS(C20)</f>
-        <v>1</v>
+        <v>0.98483549951188121</v>
       </c>
       <c r="O132" s="88">
         <f>-SIN(C18)*SIN(C19)</f>
-        <v>0</v>
+        <v>6.0796772806267557E-3</v>
       </c>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.3">
       <c r="J133" s="65">
-        <v>0</v>
+        <v>-8.6678294469630643E-2</v>
       </c>
       <c r="K133" s="65">
-        <v>0</v>
+        <v>9.1102558543636417E-3</v>
       </c>
       <c r="L133" s="65">
-        <v>1</v>
+        <v>0.99619469809174555</v>
       </c>
       <c r="M133" s="88">
         <f>SIN(C19)*COS(C20)</f>
-        <v>0</v>
+        <v>-8.6678294469630643E-2</v>
       </c>
       <c r="N133" s="88">
         <f>-SIN(C19)*SIN(C20)</f>
-        <v>0</v>
+        <v>9.1102558543636417E-3</v>
       </c>
       <c r="O133" s="88">
         <f>COS(C19)</f>
-        <v>1</v>
+        <v>0.99619469809174555</v>
       </c>
     </row>
     <row r="135" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="136" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B136" s="67">
         <f t="array" ref="B136:D138">MMULT(MMULT(N23:P25,N28:P30),N33:P35)</f>
-        <v>7.0964024677563694E-17</v>
+        <v>-8.5831651177431301E-2</v>
       </c>
       <c r="C136" s="68">
-        <v>0.17364817766693039</v>
+        <v>-0.17364817766693028</v>
       </c>
       <c r="D136" s="69">
-        <v>0.98480775301220802</v>
+        <v>0.98106026219040676</v>
       </c>
       <c r="H136" s="67">
         <f t="array" ref="H136:J138">TRANSPOSE(B136:D138)</f>
-        <v>7.0964024677563694E-17</v>
+        <v>-8.5831651177431301E-2</v>
       </c>
       <c r="I136" s="68">
-        <v>-4.9689545020929967E-17</v>
+        <v>1.5134435901338558E-2</v>
       </c>
       <c r="J136" s="69">
-        <v>1</v>
+        <v>0.99619469809174555</v>
       </c>
       <c r="M136" s="79">
         <f t="array" ref="M136:O138">R48:T50</f>
-        <v>7.0964024677563694E-17</v>
+        <v>-0.19934811914983228</v>
       </c>
       <c r="N136" s="80">
-        <v>0.17364817766693039</v>
+        <v>-0.14720672741714322</v>
       </c>
       <c r="O136" s="81">
-        <v>0.98480775301220802</v>
+        <v>0.96880880817350068</v>
       </c>
       <c r="S136" s="79">
         <f t="array" ref="S136:U138">MMULT(H136:J138,M136:O138)</f>
-        <v>1</v>
+        <v>0.98103251569073358</v>
       </c>
       <c r="T136" s="80">
-        <v>0</v>
+        <v>-0.17325138423531031</v>
       </c>
       <c r="U136" s="81">
-        <v>0</v>
+        <v>8.6943435738757166E-2</v>
       </c>
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B137" s="70">
-        <v>-4.9689545020929967E-17</v>
+        <v>1.5134435901338558E-2</v>
       </c>
       <c r="C137" s="71">
         <v>-0.98480775301220802</v>
       </c>
       <c r="D137" s="72">
-        <v>0.17364817766693039</v>
+        <v>-0.17298739392508941</v>
       </c>
       <c r="H137" s="70">
-        <v>0.17364817766693039</v>
+        <v>-0.17364817766693028</v>
       </c>
       <c r="I137" s="71">
         <v>-0.98480775301220802</v>
       </c>
       <c r="J137" s="72">
-        <v>-6.1257422745431001E-17</v>
+        <v>-5.591848656724567E-17</v>
       </c>
       <c r="M137" s="82">
-        <v>-4.9689545020929967E-17</v>
+        <v>-0.14090846596258555</v>
       </c>
       <c r="N137" s="83">
-        <v>-0.98480775301220802</v>
+        <v>-0.97407165674871599</v>
       </c>
       <c r="O137" s="84">
-        <v>0.17364817766693039</v>
+        <v>-0.17700059813142535</v>
       </c>
       <c r="S137" s="82">
-        <v>0</v>
+        <v>0.17338418735670949</v>
       </c>
       <c r="T137" s="83">
-        <v>0.99999999999999989</v>
+        <v>0.98483549951188132</v>
       </c>
       <c r="U137" s="84">
-        <v>3.7524718414124473E-33</v>
+        <v>6.0796772806267956E-3</v>
       </c>
     </row>
     <row r="138" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B138" s="73">
-        <v>1</v>
+        <v>0.99619469809174555</v>
       </c>
       <c r="C138" s="74">
-        <v>-6.1257422745431001E-17</v>
+        <v>-5.591848656724567E-17</v>
       </c>
       <c r="D138" s="75">
-        <v>-6.1257422745431001E-17</v>
+        <v>8.7155742747658166E-2</v>
       </c>
       <c r="H138" s="73">
-        <v>0.98480775301220802</v>
+        <v>0.98106026219040676</v>
       </c>
       <c r="I138" s="74">
-        <v>0.17364817766693039</v>
+        <v>-0.17298739392508941</v>
       </c>
       <c r="J138" s="75">
-        <v>-6.1257422745431001E-17</v>
+        <v>8.7155742747658166E-2</v>
       </c>
       <c r="M138" s="85">
-        <v>1</v>
+        <v>0.96974487965211498</v>
       </c>
       <c r="N138" s="86">
-        <v>-6.1257422745431001E-17</v>
+        <v>-0.17179809929666373</v>
       </c>
       <c r="O138" s="87">
-        <v>-6.1257422745431001E-17</v>
+        <v>0.17343667855029543</v>
       </c>
       <c r="S138" s="85">
-        <v>0</v>
+        <v>-8.6678294469630615E-2</v>
       </c>
       <c r="T138" s="86">
-        <v>3.7524718414124473E-33</v>
+        <v>9.1102558543636799E-3</v>
       </c>
       <c r="U138" s="87">
-        <v>0.99999999999999989</v>
+        <v>0.99619469809174521</v>
       </c>
     </row>
     <row r="142" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D142" s="66">
         <f>U138</f>
-        <v>0.99999999999999989</v>
+        <v>0.99619469809174521</v>
       </c>
       <c r="E142" s="5"/>
       <c r="G142" s="100">
         <f>ACOS(D142)</f>
-        <v>1.4901161193847656E-8</v>
+        <v>8.7266462599720152E-2</v>
       </c>
       <c r="H142" s="101">
         <f>DEGREES(G142)</f>
-        <v>8.5377364625159387E-7</v>
-      </c>
-      <c r="J142" s="114">
+        <v>5.0000000000002105</v>
+      </c>
+      <c r="J142" s="115">
         <f>ATAN2(D146,-D144)</f>
-        <v>-1.5707963267948966</v>
+        <v>-3.0368728984701328</v>
       </c>
       <c r="K142" s="101">
         <f>DEGREES(J142)</f>
-        <v>-90</v>
+        <v>-173.99999999999997</v>
       </c>
       <c r="N142" s="112">
         <f>ATAN2(-D150,-D148)</f>
-        <v>-1.5707963267948966</v>
+        <v>-3.0717794835100194</v>
       </c>
       <c r="O142" s="101">
         <f>DEGREES(N142)</f>
-        <v>-90</v>
+        <v>-175.99999999999997</v>
       </c>
     </row>
     <row r="143" spans="1:21" x14ac:dyDescent="0.3">
       <c r="G143" s="100">
         <f>-ACOS(D142)</f>
-        <v>-1.4901161193847656E-8</v>
+        <v>-8.7266462599720152E-2</v>
       </c>
       <c r="H143" s="101">
         <f>DEGREES(G143)</f>
-        <v>-8.5377364625159387E-7</v>
+        <v>-5.0000000000002105</v>
       </c>
       <c r="J143" s="100">
         <f>ATAN2(D146,D144)</f>
-        <v>1.5707963267948966</v>
+        <v>3.0368728984701328</v>
       </c>
       <c r="K143" s="101">
         <f>DEGREES(J143)</f>
-        <v>90</v>
+        <v>173.99999999999997</v>
       </c>
       <c r="N143" s="112">
         <f>ATAN2(-D150,D148)</f>
-        <v>1.5707963267948966</v>
+        <v>3.0717794835100194</v>
       </c>
       <c r="O143" s="101">
         <f>DEGREES(N143)</f>
-        <v>90</v>
+        <v>175.99999999999997</v>
       </c>
     </row>
     <row r="144" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D144" s="89">
         <f>T138</f>
-        <v>3.7524718414124473E-33</v>
+        <v>9.1102558543636799E-3</v>
       </c>
       <c r="G144" s="2"/>
       <c r="H144" s="2"/>
@@ -25753,7 +26064,7 @@
     <row r="146" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D146" s="90">
         <f>S138</f>
-        <v>0</v>
+        <v>-8.6678294469630615E-2</v>
       </c>
       <c r="I146" s="2"/>
       <c r="J146" s="2"/>
@@ -25775,7 +26086,7 @@
     <row r="148" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D148" s="64">
         <f>U137</f>
-        <v>3.7524718414124473E-33</v>
+        <v>6.0796772806267956E-3</v>
       </c>
       <c r="G148" s="2"/>
       <c r="H148" s="2"/>
@@ -25801,7 +26112,7 @@
     <row r="150" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D150" s="90">
         <f>U136</f>
-        <v>0</v>
+        <v>8.6943435738757166E-2</v>
       </c>
       <c r="I150" s="2"/>
       <c r="J150" s="2"/>
@@ -25834,10 +26145,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25860,6 +26171,11 @@
         <v>68</v>
       </c>
     </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
rotated gripper view to make it more handy
</commit_message>
<xml_diff>
--- a/theory/Kinematik.xlsx
+++ b/theory/Kinematik.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="84">
   <si>
     <r>
       <t>Hüfte (T</t>
@@ -820,6 +820,24 @@
   <si>
     <t>Nick/pitch</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
 </sst>
 </file>
 
@@ -1353,7 +1371,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Kinematik!$B$83</c:f>
+              <c:f>Kinematik!$B$89</c:f>
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1365,12 +1383,12 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Kinematik!$B$84</c:f>
+              <c:f>Kinematik!$B$90</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-1.4916679007785359E-14</c:v>
+                  <c:v>-1.3322676295501878E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1385,11 +1403,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="257299968"/>
-        <c:axId val="257323008"/>
+        <c:axId val="152384256"/>
+        <c:axId val="152386176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="257299968"/>
+        <c:axId val="152384256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1427,13 +1445,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="257323008"/>
+        <c:crossAx val="152386176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="257323008"/>
+        <c:axId val="152386176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1472,7 +1490,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="257299968"/>
+        <c:crossAx val="152384256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
@@ -1530,7 +1548,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Kinematik!$K$96:$L$96</c:f>
+              <c:f>Kinematik!$K$102:$L$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1545,7 +1563,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Kinematik!$K$97:$L$97</c:f>
+              <c:f>Kinematik!$K$103:$L$103</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1568,11 +1586,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="257467136"/>
-        <c:axId val="257468672"/>
+        <c:axId val="152410752"/>
+        <c:axId val="152703360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="257467136"/>
+        <c:axId val="152410752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -1584,13 +1602,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="257468672"/>
+        <c:crossAx val="152703360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="257468672"/>
+        <c:axId val="152703360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -1603,7 +1621,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="257467136"/>
+        <c:crossAx val="152410752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
@@ -1626,15 +1644,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>891600</xdr:colOff>
+      <xdr:colOff>981247</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>88100</xdr:rowOff>
+      <xdr:rowOff>79135</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>494844</xdr:colOff>
+      <xdr:colOff>584491</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>111385</xdr:rowOff>
+      <xdr:rowOff>84490</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1658,8 +1676,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6511350" y="316700"/>
-          <a:ext cx="5147690" cy="1871135"/>
+          <a:off x="7453765" y="312217"/>
+          <a:ext cx="5161361" cy="1852085"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2748,7 +2766,7 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="735106" cy="736292"/>
@@ -8789,7 +8807,7 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>233083</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>147917</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2259105" cy="277384"/>
@@ -9112,7 +9130,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>125504</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>116</xdr:row>
       <xdr:rowOff>40342</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2214283" cy="436786"/>
@@ -9497,7 +9515,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>367552</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>138953</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1918447" cy="267702"/>
@@ -9764,7 +9782,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>32270</xdr:colOff>
-      <xdr:row>108</xdr:row>
+      <xdr:row>114</xdr:row>
       <xdr:rowOff>84716</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2097743" cy="472694"/>
@@ -10159,7 +10177,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>546847</xdr:colOff>
-      <xdr:row>114</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>13447</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3021108" cy="472694"/>
@@ -10601,7 +10619,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>152399</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>129989</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1497106" cy="264560"/>
@@ -10864,7 +10882,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>573739</xdr:colOff>
-      <xdr:row>118</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>121023</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3021108" cy="264560"/>
@@ -11161,7 +11179,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>510986</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>116</xdr:row>
       <xdr:rowOff>113404</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3514166" cy="379399"/>
@@ -11798,7 +11816,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>597944</xdr:colOff>
-      <xdr:row>124</xdr:row>
+      <xdr:row>130</xdr:row>
       <xdr:rowOff>136713</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3021108" cy="264560"/>
@@ -12083,7 +12101,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>591671</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>26894</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3021108" cy="264560"/>
@@ -12344,7 +12362,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>595705</xdr:colOff>
-      <xdr:row>125</xdr:row>
+      <xdr:row>131</xdr:row>
       <xdr:rowOff>142989</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3021108" cy="264560"/>
@@ -12659,13 +12677,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>98611</xdr:colOff>
-      <xdr:row>92</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>62753</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>444947</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>136782</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -12697,13 +12715,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>744070</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>40342</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>295835</xdr:colOff>
-      <xdr:row>104</xdr:row>
+      <xdr:row>110</xdr:row>
       <xdr:rowOff>94130</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -12727,7 +12745,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>40341</xdr:colOff>
-      <xdr:row>129</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>102646</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6337599" cy="637290"/>
@@ -17094,7 +17112,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>22861</xdr:colOff>
-      <xdr:row>135</xdr:row>
+      <xdr:row>141</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="640080" cy="270843"/>
@@ -17280,7 +17298,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>135</xdr:row>
+      <xdr:row>141</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1562099" cy="323230"/>
@@ -17667,7 +17685,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>138</xdr:row>
+      <xdr:row>144</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1562099" cy="333809"/>
@@ -18140,7 +18158,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>34291</xdr:colOff>
-      <xdr:row>140</xdr:row>
+      <xdr:row>146</xdr:row>
       <xdr:rowOff>146685</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1325880" cy="311752"/>
@@ -18576,7 +18594,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>285751</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>147</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="739139" cy="269304"/>
@@ -18762,7 +18780,7 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>120833</xdr:colOff>
-      <xdr:row>135</xdr:row>
+      <xdr:row>141</xdr:row>
       <xdr:rowOff>145869</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="640080" cy="270843"/>
@@ -18948,7 +18966,7 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>433252</xdr:colOff>
-      <xdr:row>135</xdr:row>
+      <xdr:row>141</xdr:row>
       <xdr:rowOff>87086</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1562099" cy="333809"/>
@@ -19488,7 +19506,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>142</xdr:row>
+      <xdr:row>148</xdr:row>
       <xdr:rowOff>102870</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2000249" cy="312521"/>
@@ -20101,7 +20119,7 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>333376</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>147</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="739139" cy="269304"/>
@@ -20287,7 +20305,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>144</xdr:row>
+      <xdr:row>150</xdr:row>
       <xdr:rowOff>93345</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2000249" cy="312521"/>
@@ -20892,7 +20910,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>146</xdr:row>
+      <xdr:row>152</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2000249" cy="312521"/>
@@ -21512,7 +21530,7 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>295276</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>147</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="739139" cy="269304"/>
@@ -21698,7 +21716,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>148</xdr:row>
+      <xdr:row>154</xdr:row>
       <xdr:rowOff>102870</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2000249" cy="312521"/>
@@ -22315,7 +22333,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127746</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="914400" cy="270843"/>
@@ -22505,7 +22523,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>788892</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1093695" cy="270843"/>
@@ -22750,7 +22768,7 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>295276</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>147</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="739139" cy="269304"/>
@@ -22948,7 +22966,7 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>295276</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>147</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="739139" cy="269304"/>
@@ -23146,7 +23164,7 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>333376</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>147</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="739139" cy="269304"/>
@@ -23344,7 +23362,7 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>333376</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>147</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="739139" cy="269304"/>
@@ -23529,6 +23547,760 @@
                   <a:ea typeface="Cambria Math"/>
                 </a:rPr>
                 <a:t>=</a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>644177</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>78760</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2689413" cy="736292"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="48" name="Textfeld 47"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7116695" y="9760642"/>
+              <a:ext cx="2689413" cy="736292"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="left"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math"/>
+                          </a:rPr>
+                          <m:t>𝑇</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math"/>
+                          </a:rPr>
+                          <m:t>𝑉</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math"/>
+                          </a:rPr>
+                          <m:t>=</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math"/>
+                          </a:rPr>
+                          <m:t>𝑇</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math"/>
+                          </a:rPr>
+                          <m:t>6</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math"/>
+                          </a:rPr>
+                          <m:t>7</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                    <m:r>
+                      <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="de-DE" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:m>
+                          <m:mPr>
+                            <m:mcs>
+                              <m:mc>
+                                <m:mcPr>
+                                  <m:count m:val="4"/>
+                                  <m:mcJc m:val="center"/>
+                                </m:mcPr>
+                              </m:mc>
+                            </m:mcs>
+                            <m:ctrlPr>
+                              <a:rPr lang="de-DE" sz="1100" i="1">
+                                <a:latin typeface="Cambria Math"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:mPr>
+                          <m:mr>
+                            <m:e>
+                              <m:func>
+                                <m:funcPr>
+                                  <m:ctrlPr>
+                                    <a:rPr lang="de-DE" sz="1100" i="1">
+                                      <a:latin typeface="Cambria Math"/>
+                                    </a:rPr>
+                                  </m:ctrlPr>
+                                </m:funcPr>
+                                <m:fName>
+                                  <m:r>
+                                    <m:rPr>
+                                      <m:sty m:val="p"/>
+                                      <m:brk m:alnAt="7"/>
+                                    </m:rPr>
+                                    <a:rPr lang="de-DE" sz="1100" i="0">
+                                      <a:latin typeface="Cambria Math"/>
+                                    </a:rPr>
+                                    <m:t>c</m:t>
+                                  </m:r>
+                                  <m:r>
+                                    <m:rPr>
+                                      <m:sty m:val="p"/>
+                                    </m:rPr>
+                                    <a:rPr lang="de-DE" sz="1100" i="0">
+                                      <a:latin typeface="Cambria Math"/>
+                                    </a:rPr>
+                                    <m:t>os</m:t>
+                                  </m:r>
+                                </m:fName>
+                                <m:e>
+                                  <m:sSub>
+                                    <m:sSubPr>
+                                      <m:ctrlPr>
+                                        <a:rPr lang="de-DE" sz="1100" i="1">
+                                          <a:latin typeface="Cambria Math"/>
+                                        </a:rPr>
+                                      </m:ctrlPr>
+                                    </m:sSubPr>
+                                    <m:e>
+                                      <m:r>
+                                        <a:rPr lang="de-DE" sz="1100" i="1">
+                                          <a:latin typeface="Cambria Math"/>
+                                          <a:ea typeface="Cambria Math"/>
+                                        </a:rPr>
+                                        <m:t>𝜃</m:t>
+                                      </m:r>
+                                    </m:e>
+                                    <m:sub>
+                                      <m:r>
+                                        <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                          <a:latin typeface="Cambria Math"/>
+                                        </a:rPr>
+                                        <m:t>5</m:t>
+                                      </m:r>
+                                    </m:sub>
+                                  </m:sSub>
+                                </m:e>
+                              </m:func>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math"/>
+                                </a:rPr>
+                                <m:t>−</m:t>
+                              </m:r>
+                              <m:func>
+                                <m:funcPr>
+                                  <m:ctrlPr>
+                                    <a:rPr lang="de-DE" sz="1100" i="1">
+                                      <a:solidFill>
+                                        <a:schemeClr val="tx1"/>
+                                      </a:solidFill>
+                                      <a:effectLst/>
+                                      <a:latin typeface="Cambria Math"/>
+                                      <a:ea typeface="+mn-ea"/>
+                                      <a:cs typeface="+mn-cs"/>
+                                    </a:rPr>
+                                  </m:ctrlPr>
+                                </m:funcPr>
+                                <m:fName>
+                                  <m:r>
+                                    <m:rPr>
+                                      <m:sty m:val="p"/>
+                                    </m:rPr>
+                                    <a:rPr lang="de-DE" sz="1100" i="0">
+                                      <a:solidFill>
+                                        <a:schemeClr val="tx1"/>
+                                      </a:solidFill>
+                                      <a:effectLst/>
+                                      <a:latin typeface="Cambria Math"/>
+                                      <a:ea typeface="+mn-ea"/>
+                                      <a:cs typeface="+mn-cs"/>
+                                    </a:rPr>
+                                    <m:t>sin</m:t>
+                                  </m:r>
+                                </m:fName>
+                                <m:e>
+                                  <m:sSub>
+                                    <m:sSubPr>
+                                      <m:ctrlPr>
+                                        <a:rPr lang="de-DE" sz="1100" i="1">
+                                          <a:solidFill>
+                                            <a:schemeClr val="tx1"/>
+                                          </a:solidFill>
+                                          <a:effectLst/>
+                                          <a:latin typeface="Cambria Math"/>
+                                          <a:ea typeface="+mn-ea"/>
+                                          <a:cs typeface="+mn-cs"/>
+                                        </a:rPr>
+                                      </m:ctrlPr>
+                                    </m:sSubPr>
+                                    <m:e>
+                                      <m:r>
+                                        <a:rPr lang="de-DE" sz="1100" i="1">
+                                          <a:solidFill>
+                                            <a:schemeClr val="tx1"/>
+                                          </a:solidFill>
+                                          <a:effectLst/>
+                                          <a:latin typeface="Cambria Math"/>
+                                          <a:ea typeface="+mn-ea"/>
+                                          <a:cs typeface="+mn-cs"/>
+                                        </a:rPr>
+                                        <m:t>𝜃</m:t>
+                                      </m:r>
+                                    </m:e>
+                                    <m:sub>
+                                      <m:r>
+                                        <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                          <a:solidFill>
+                                            <a:schemeClr val="tx1"/>
+                                          </a:solidFill>
+                                          <a:effectLst/>
+                                          <a:latin typeface="Cambria Math"/>
+                                          <a:ea typeface="+mn-ea"/>
+                                          <a:cs typeface="+mn-cs"/>
+                                        </a:rPr>
+                                        <m:t>5</m:t>
+                                      </m:r>
+                                    </m:sub>
+                                  </m:sSub>
+                                </m:e>
+                              </m:func>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math"/>
+                                </a:rPr>
+                                <m:t>0</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math"/>
+                                </a:rPr>
+                                <m:t>0</m:t>
+                              </m:r>
+                            </m:e>
+                          </m:mr>
+                          <m:mr>
+                            <m:e>
+                              <m:func>
+                                <m:funcPr>
+                                  <m:ctrlPr>
+                                    <a:rPr lang="de-DE" sz="1100" i="1">
+                                      <a:solidFill>
+                                        <a:schemeClr val="tx1"/>
+                                      </a:solidFill>
+                                      <a:effectLst/>
+                                      <a:latin typeface="Cambria Math"/>
+                                      <a:ea typeface="+mn-ea"/>
+                                      <a:cs typeface="+mn-cs"/>
+                                    </a:rPr>
+                                  </m:ctrlPr>
+                                </m:funcPr>
+                                <m:fName>
+                                  <m:r>
+                                    <m:rPr>
+                                      <m:sty m:val="p"/>
+                                    </m:rPr>
+                                    <a:rPr lang="de-DE" sz="1100" i="0">
+                                      <a:solidFill>
+                                        <a:schemeClr val="tx1"/>
+                                      </a:solidFill>
+                                      <a:effectLst/>
+                                      <a:latin typeface="Cambria Math"/>
+                                      <a:ea typeface="+mn-ea"/>
+                                      <a:cs typeface="+mn-cs"/>
+                                    </a:rPr>
+                                    <m:t>sin</m:t>
+                                  </m:r>
+                                </m:fName>
+                                <m:e>
+                                  <m:sSub>
+                                    <m:sSubPr>
+                                      <m:ctrlPr>
+                                        <a:rPr lang="de-DE" sz="1100" i="1">
+                                          <a:solidFill>
+                                            <a:schemeClr val="tx1"/>
+                                          </a:solidFill>
+                                          <a:effectLst/>
+                                          <a:latin typeface="Cambria Math"/>
+                                          <a:ea typeface="+mn-ea"/>
+                                          <a:cs typeface="+mn-cs"/>
+                                        </a:rPr>
+                                      </m:ctrlPr>
+                                    </m:sSubPr>
+                                    <m:e>
+                                      <m:r>
+                                        <a:rPr lang="de-DE" sz="1100" i="1">
+                                          <a:solidFill>
+                                            <a:schemeClr val="tx1"/>
+                                          </a:solidFill>
+                                          <a:effectLst/>
+                                          <a:latin typeface="Cambria Math"/>
+                                          <a:ea typeface="+mn-ea"/>
+                                          <a:cs typeface="+mn-cs"/>
+                                        </a:rPr>
+                                        <m:t>𝜃</m:t>
+                                      </m:r>
+                                    </m:e>
+                                    <m:sub>
+                                      <m:r>
+                                        <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                          <a:solidFill>
+                                            <a:schemeClr val="tx1"/>
+                                          </a:solidFill>
+                                          <a:effectLst/>
+                                          <a:latin typeface="Cambria Math"/>
+                                          <a:ea typeface="+mn-ea"/>
+                                          <a:cs typeface="+mn-cs"/>
+                                        </a:rPr>
+                                        <m:t>5</m:t>
+                                      </m:r>
+                                    </m:sub>
+                                  </m:sSub>
+                                </m:e>
+                              </m:func>
+                            </m:e>
+                            <m:e>
+                              <m:func>
+                                <m:funcPr>
+                                  <m:ctrlPr>
+                                    <a:rPr lang="de-DE" sz="1100" i="1">
+                                      <a:solidFill>
+                                        <a:schemeClr val="tx1"/>
+                                      </a:solidFill>
+                                      <a:effectLst/>
+                                      <a:latin typeface="Cambria Math"/>
+                                      <a:ea typeface="+mn-ea"/>
+                                      <a:cs typeface="+mn-cs"/>
+                                    </a:rPr>
+                                  </m:ctrlPr>
+                                </m:funcPr>
+                                <m:fName>
+                                  <m:r>
+                                    <m:rPr>
+                                      <m:sty m:val="p"/>
+                                      <m:brk m:alnAt="7"/>
+                                    </m:rPr>
+                                    <a:rPr lang="de-DE" sz="1100" i="0">
+                                      <a:solidFill>
+                                        <a:schemeClr val="tx1"/>
+                                      </a:solidFill>
+                                      <a:effectLst/>
+                                      <a:latin typeface="Cambria Math"/>
+                                      <a:ea typeface="+mn-ea"/>
+                                      <a:cs typeface="+mn-cs"/>
+                                    </a:rPr>
+                                    <m:t>c</m:t>
+                                  </m:r>
+                                  <m:r>
+                                    <m:rPr>
+                                      <m:sty m:val="p"/>
+                                    </m:rPr>
+                                    <a:rPr lang="de-DE" sz="1100" i="0">
+                                      <a:solidFill>
+                                        <a:schemeClr val="tx1"/>
+                                      </a:solidFill>
+                                      <a:effectLst/>
+                                      <a:latin typeface="Cambria Math"/>
+                                      <a:ea typeface="+mn-ea"/>
+                                      <a:cs typeface="+mn-cs"/>
+                                    </a:rPr>
+                                    <m:t>os</m:t>
+                                  </m:r>
+                                </m:fName>
+                                <m:e>
+                                  <m:sSub>
+                                    <m:sSubPr>
+                                      <m:ctrlPr>
+                                        <a:rPr lang="de-DE" sz="1100" i="1">
+                                          <a:solidFill>
+                                            <a:schemeClr val="tx1"/>
+                                          </a:solidFill>
+                                          <a:effectLst/>
+                                          <a:latin typeface="Cambria Math"/>
+                                          <a:ea typeface="+mn-ea"/>
+                                          <a:cs typeface="+mn-cs"/>
+                                        </a:rPr>
+                                      </m:ctrlPr>
+                                    </m:sSubPr>
+                                    <m:e>
+                                      <m:r>
+                                        <a:rPr lang="de-DE" sz="1100" i="1">
+                                          <a:solidFill>
+                                            <a:schemeClr val="tx1"/>
+                                          </a:solidFill>
+                                          <a:effectLst/>
+                                          <a:latin typeface="Cambria Math"/>
+                                          <a:ea typeface="+mn-ea"/>
+                                          <a:cs typeface="+mn-cs"/>
+                                        </a:rPr>
+                                        <m:t>𝜃</m:t>
+                                      </m:r>
+                                    </m:e>
+                                    <m:sub>
+                                      <m:r>
+                                        <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                          <a:solidFill>
+                                            <a:schemeClr val="tx1"/>
+                                          </a:solidFill>
+                                          <a:effectLst/>
+                                          <a:latin typeface="Cambria Math"/>
+                                          <a:ea typeface="+mn-ea"/>
+                                          <a:cs typeface="+mn-cs"/>
+                                        </a:rPr>
+                                        <m:t>5</m:t>
+                                      </m:r>
+                                    </m:sub>
+                                  </m:sSub>
+                                </m:e>
+                              </m:func>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math"/>
+                                </a:rPr>
+                                <m:t>0</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math"/>
+                                </a:rPr>
+                                <m:t>0</m:t>
+                              </m:r>
+                            </m:e>
+                          </m:mr>
+                          <m:mr>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math"/>
+                                </a:rPr>
+                                <m:t>0</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math"/>
+                                </a:rPr>
+                                <m:t>0</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math"/>
+                                </a:rPr>
+                                <m:t>1</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:sSub>
+                                <m:sSubPr>
+                                  <m:ctrlPr>
+                                    <a:rPr lang="de-DE" sz="1100" i="1">
+                                      <a:latin typeface="Cambria Math"/>
+                                    </a:rPr>
+                                  </m:ctrlPr>
+                                </m:sSubPr>
+                                <m:e>
+                                  <m:r>
+                                    <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                      <a:latin typeface="Cambria Math"/>
+                                    </a:rPr>
+                                    <m:t>𝑑</m:t>
+                                  </m:r>
+                                </m:e>
+                                <m:sub>
+                                  <m:r>
+                                    <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                      <a:latin typeface="Cambria Math"/>
+                                    </a:rPr>
+                                    <m:t>5</m:t>
+                                  </m:r>
+                                </m:sub>
+                              </m:sSub>
+                            </m:e>
+                          </m:mr>
+                          <m:mr>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math"/>
+                                </a:rPr>
+                                <m:t>0</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math"/>
+                                </a:rPr>
+                                <m:t>0</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math"/>
+                                </a:rPr>
+                                <m:t>0</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math"/>
+                                </a:rPr>
+                                <m:t>1</m:t>
+                              </m:r>
+                            </m:e>
+                          </m:mr>
+                        </m:m>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="de-DE" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="48" name="Textfeld 47"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7116695" y="9760642"/>
+              <a:ext cx="2689413" cy="736292"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>𝑇_𝑉 〖=𝑇〗_6^7=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>(■8(cos⁡〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>𝜃_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>5 〗&amp;−</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>sin⁡〖𝜃_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>5 〗&amp;</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>0&amp;0@</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>sin⁡〖𝜃_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>5 〗&amp;</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>cos⁡〖𝜃_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>5 〗&amp;</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>0&amp;0@0&amp;0&amp;1&amp;𝑑_5@0&amp;0&amp;0&amp;1))</a:t>
               </a:r>
               <a:endParaRPr lang="de-DE" sz="1100"/>
             </a:p>
@@ -23837,6 +24609,61 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>286870</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>53787</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>145223</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Grafik 8" descr="https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcR6dqRK5iWrtixSWfDDKDUDawqDGnRKeHokFo4AI0OcJixWjlb3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="286870" y="17803905"/>
+          <a:ext cx="7173553" cy="2456330"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -24127,10 +24954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z152"/>
+  <dimension ref="A1:Z158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S67" sqref="S67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24171,44 +24998,51 @@
         <v>30</v>
       </c>
       <c r="G4" s="55">
-        <f>B83</f>
+        <f>B89</f>
         <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G5" s="56">
-        <f>B84</f>
-        <v>-1.4916679007785359E-14</v>
+        <f>B90</f>
+        <v>-1.3322676295501878E-14</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G6" s="57">
-        <f>B85</f>
+        <f>B91</f>
         <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F8" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="110">
         <f>V48</f>
-        <v>340</v>
+        <v>339.9147157826734</v>
       </c>
       <c r="H8" s="77">
         <f>X48</f>
-        <v>-90.000000000000057</v>
+        <v>-90</v>
+      </c>
+      <c r="I8" s="77">
+        <f t="array" ref="I8:I10">X53:X55</f>
+        <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G9" s="111">
         <f>V49</f>
-        <v>2.45029690981724E-15</v>
+        <v>4.8859295383501378</v>
       </c>
       <c r="H9" s="78">
         <f>X49</f>
-        <v>-86.9</v>
+        <v>3.0000000000000004</v>
+      </c>
+      <c r="I9" s="77">
+        <v>5.3390701230985497E-19</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -24218,7 +25052,10 @@
       </c>
       <c r="H10" s="79">
         <f>X50</f>
-        <v>-89.999999999999929</v>
+        <v>-88</v>
+      </c>
+      <c r="I10" s="77">
+        <v>2.0000000000000036</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
@@ -24255,11 +25092,11 @@
         <v>0</v>
       </c>
       <c r="E15" s="20">
-        <f>H85</f>
-        <v>-4.2733137574874679E-15</v>
+        <f>H91</f>
+        <v>-3.8166656177562198E-15</v>
       </c>
       <c r="I15" s="20">
-        <f>H86</f>
+        <f>H92</f>
         <v>180</v>
       </c>
       <c r="J15" s="26" t="s">
@@ -24273,24 +25110,24 @@
       <c r="B16" s="30">
         <v>0</v>
       </c>
-      <c r="C16" s="109">
+      <c r="C16" s="21">
         <f t="shared" ref="C16:C20" si="0">RADIANS(B16)</f>
         <v>0</v>
       </c>
       <c r="D16" s="116">
-        <f>N120</f>
+        <f>N126</f>
         <v>0</v>
       </c>
       <c r="E16" s="116">
-        <f>N126</f>
+        <f>N132</f>
         <v>67.380135051959556</v>
       </c>
       <c r="H16" s="116">
-        <f>R120</f>
+        <f>R126</f>
         <v>-67.380135051959556</v>
       </c>
       <c r="I16" s="116">
-        <f>R126</f>
+        <f>R132</f>
         <v>0</v>
       </c>
       <c r="V16" t="s">
@@ -24304,24 +25141,24 @@
       <c r="B17" s="30">
         <v>0</v>
       </c>
-      <c r="C17" s="109">
+      <c r="C17" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D17" s="117">
-        <f>N121</f>
+        <f>N127</f>
         <v>0</v>
       </c>
       <c r="E17" s="117">
-        <f>N127</f>
+        <f>N133</f>
         <v>-180</v>
       </c>
       <c r="H17" s="117">
-        <f>R121</f>
+        <f>R127</f>
         <v>0</v>
       </c>
       <c r="I17" s="117">
-        <f>R127</f>
+        <f>R133</f>
         <v>-180</v>
       </c>
       <c r="V17">
@@ -24333,19 +25170,19 @@
         <v>7</v>
       </c>
       <c r="B18" s="30">
-        <v>0.1</v>
+        <v>90</v>
       </c>
       <c r="C18" s="21">
         <f t="shared" si="0"/>
-        <v>1.7453292519943296E-3</v>
+        <v>1.5707963267948966</v>
       </c>
       <c r="F18" s="118">
-        <f>O142</f>
-        <v>94.126863195110516</v>
+        <f>O148</f>
+        <v>90.000000000000185</v>
       </c>
       <c r="G18" s="119">
-        <f>O143</f>
-        <v>94.126863195110516</v>
+        <f>O149</f>
+        <v>-89.999999999999815</v>
       </c>
       <c r="H18" s="20"/>
       <c r="V18">
@@ -24357,19 +25194,19 @@
         <v>9</v>
       </c>
       <c r="B19" s="30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C19" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.4906585039886591E-2</v>
       </c>
       <c r="F19" s="120">
-        <f>H142</f>
-        <v>0</v>
+        <f>H148</f>
+        <v>1.9999999999999392</v>
       </c>
       <c r="G19" s="121">
-        <f>H143</f>
-        <v>0</v>
+        <f>H149</f>
+        <v>-1.9999999999999392</v>
       </c>
       <c r="V19">
         <v>0</v>
@@ -24387,12 +25224,12 @@
         <v>5.235987755982989E-2</v>
       </c>
       <c r="F20" s="122">
-        <f>K142</f>
-        <v>-91.026863195110522</v>
+        <f>K148</f>
+        <v>2.9999999999998006</v>
       </c>
       <c r="G20" s="123">
-        <f>K143</f>
-        <v>-91.026863195110522</v>
+        <f>K149</f>
+        <v>-177.0000000000002</v>
       </c>
       <c r="V20">
         <v>1</v>
@@ -25008,23 +25845,23 @@
       </c>
       <c r="G38" s="1">
         <f>B18</f>
-        <v>0.1</v>
+        <v>90</v>
       </c>
       <c r="H38" s="6">
         <f>RADIANS(G38)</f>
-        <v>1.7453292519943296E-3</v>
+        <v>1.5707963267948966</v>
       </c>
       <c r="N38" s="11">
         <f>COS(H38)</f>
-        <v>0.99999847691328769</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="O38" s="12">
         <f>-SIN(H38)*COS(D38)</f>
-        <v>-1.0691431753942499E-19</v>
+        <v>-6.1257422745431001E-17</v>
       </c>
       <c r="P38" s="12">
         <f>SIN(H38)*SIN(D38)</f>
-        <v>1.7453283658983088E-3</v>
+        <v>1</v>
       </c>
       <c r="Q38" s="13">
         <f>E38*COS(H38)</f>
@@ -25032,13 +25869,13 @@
       </c>
       <c r="R38" s="62">
         <f t="array" ref="R38:U41">MMULT(R33:U36,N38:Q41)</f>
-        <v>6.1364243762603816E-17</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="S38" s="63">
         <v>1</v>
       </c>
       <c r="T38" s="63">
-        <v>1.0700761790603487E-19</v>
+        <v>1.22514845490862E-16</v>
       </c>
       <c r="U38" s="64">
         <v>200.00000000000003</v>
@@ -25049,38 +25886,38 @@
       </c>
       <c r="W38" s="21">
         <f>IF(W39=PI()/2,ATAN2(S39,S38),IF(-W39=PI()/2,-ATAN2(S39,S38),ATAN2(T40,S40)))</f>
-        <v>-3.5159193113431387E-14</v>
+        <v>-1.22514845490862E-16</v>
       </c>
       <c r="X38" s="20">
         <f>DEGREES(W38)</f>
-        <v>-2.0144733764850472E-12</v>
+        <v>-7.0195835743237771E-15</v>
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="N39" s="11">
         <f>SIN(H38)</f>
-        <v>1.7453283658983088E-3</v>
+        <v>1</v>
       </c>
       <c r="O39" s="12">
         <f>COS(H38)*COS(D38)</f>
-        <v>6.1257329445064391E-17</v>
+        <v>3.7524718414124473E-33</v>
       </c>
       <c r="P39" s="12">
         <f>-COS(H38)*SIN(D38)</f>
-        <v>-0.99999847691328769</v>
+        <v>-6.1257422745431001E-17</v>
       </c>
       <c r="Q39" s="13">
         <f>E38*SIN(H38)</f>
         <v>0</v>
       </c>
       <c r="R39" s="62">
-        <v>-1.74532836589837E-3</v>
+        <v>-1</v>
       </c>
       <c r="S39" s="63">
-        <v>9.3300366609759119E-23</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="T39" s="63">
-        <v>0.99999847691328769</v>
+        <v>3.7524718414124473E-33</v>
       </c>
       <c r="U39" s="64">
         <v>-6.1257422745431001E-15</v>
@@ -25091,11 +25928,11 @@
       </c>
       <c r="W39" s="21">
         <f>ATAN2(SQRT(R38^2+R39^2),-R40)</f>
-        <v>-1.5690509975429023</v>
+        <v>0</v>
       </c>
       <c r="X39" s="20">
         <f>DEGREES(W39)</f>
-        <v>-89.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.3">
@@ -25115,13 +25952,13 @@
         <v>200</v>
       </c>
       <c r="R40" s="62">
-        <v>0.99999847691328769</v>
+        <v>0</v>
       </c>
       <c r="S40" s="63">
-        <v>-6.1364337062970426E-17</v>
+        <v>-1.22514845490862E-16</v>
       </c>
       <c r="T40" s="63">
-        <v>1.74532836589837E-3</v>
+        <v>1</v>
       </c>
       <c r="U40" s="64">
         <v>400</v>
@@ -25132,11 +25969,11 @@
       </c>
       <c r="W40" s="21">
         <f>IF(ABS(W39)=PI()/2,0,ATAN2(R38,R39))</f>
-        <v>-1.5707963267948615</v>
+        <v>-1.5707963267948966</v>
       </c>
       <c r="X40" s="20">
         <f>DEGREES(W40)</f>
-        <v>-89.999999999997996</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.3">
@@ -25190,23 +26027,23 @@
       </c>
       <c r="G43" s="98">
         <f>B19</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H43" s="6">
         <f>RADIANS(G43)</f>
-        <v>0</v>
+        <v>3.4906585039886591E-2</v>
       </c>
       <c r="N43" s="11">
         <f>COS(H43)</f>
-        <v>1</v>
+        <v>0.99939082701909576</v>
       </c>
       <c r="O43" s="12">
         <f>-SIN(H43)*COS(D43)</f>
-        <v>0</v>
+        <v>-2.1378532231078771E-18</v>
       </c>
       <c r="P43" s="12">
         <f>SIN(H43)*SIN(D43)</f>
-        <v>0</v>
+        <v>-3.4899496702500969E-2</v>
       </c>
       <c r="Q43" s="13">
         <f>E43*COS(H43)</f>
@@ -25214,13 +26051,13 @@
       </c>
       <c r="R43" s="62">
         <f t="array" ref="R43:U46">MMULT(R38:U41,N43:Q46)</f>
-        <v>6.1364243762603816E-17</v>
+        <v>3.4899496702501032E-2</v>
       </c>
       <c r="S43" s="63">
-        <v>6.1150415127524966E-17</v>
+        <v>-6.1294739112247347E-17</v>
       </c>
       <c r="T43" s="63">
-        <v>1</v>
+        <v>0.99939082701909576</v>
       </c>
       <c r="U43" s="64">
         <v>200.00000000000003</v>
@@ -25231,38 +26068,38 @@
       </c>
       <c r="W43" s="21">
         <f>IF(W44=PI()/2,ATAN2(S44,S43),IF(-W44=PI()/2,-ATAN2(S44,S43),ATAN2(T45,S45)))</f>
-        <v>-1.5707963267949316</v>
+        <v>-1.5707963267948966</v>
       </c>
       <c r="X43" s="20">
         <f>DEGREES(W43)</f>
-        <v>-90.000000000002004</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="N44" s="11">
         <f>SIN(H43)</f>
-        <v>0</v>
+        <v>3.4899496702500969E-2</v>
       </c>
       <c r="O44" s="12">
         <f>COS(H43)*COS(D43)</f>
-        <v>6.1257422745431001E-17</v>
+        <v>6.1220106378614654E-17</v>
       </c>
       <c r="P44" s="12">
         <f>-COS(H43)*SIN(D43)</f>
-        <v>1</v>
+        <v>0.99939082701909576</v>
       </c>
       <c r="Q44" s="13">
         <f>E43*SIN(H43)</f>
         <v>0</v>
       </c>
       <c r="R44" s="62">
-        <v>-1.74532836589837E-3</v>
+        <v>-0.99939082701909576</v>
       </c>
       <c r="S44" s="63">
-        <v>-0.99999847691328769</v>
+        <v>2.1378532231078771E-18</v>
       </c>
       <c r="T44" s="63">
-        <v>6.1257422745431001E-17</v>
+        <v>3.4899496702501032E-2</v>
       </c>
       <c r="U44" s="64">
         <v>-6.1257422745431001E-15</v>
@@ -25273,11 +26110,11 @@
       </c>
       <c r="W44" s="21">
         <f>ATAN2(SQRT(R43^2+R44^2),-R45)</f>
-        <v>-1.5690509975429023</v>
+        <v>4.2757064462157541E-18</v>
       </c>
       <c r="X44" s="20">
         <f>DEGREES(W44)</f>
-        <v>-89.9</v>
+        <v>2.4497993380504262E-16</v>
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.3">
@@ -25297,13 +26134,13 @@
         <v>0</v>
       </c>
       <c r="R45" s="62">
-        <v>0.99999847691328769</v>
+        <v>-4.2757064462157541E-18</v>
       </c>
       <c r="S45" s="63">
-        <v>-1.74532836589837E-3</v>
+        <v>-1</v>
       </c>
       <c r="T45" s="63">
-        <v>-6.1257422745431001E-17</v>
+        <v>-6.1182790011798308E-17</v>
       </c>
       <c r="U45" s="64">
         <v>400</v>
@@ -25314,11 +26151,11 @@
       </c>
       <c r="W45" s="21">
         <f>IF(ABS(W44)=PI()/2,0,ATAN2(R43,R44))</f>
-        <v>-1.5707963267948615</v>
+        <v>-1.5358897417550099</v>
       </c>
       <c r="X45" s="20">
         <f>DEGREES(W45)</f>
-        <v>-89.999999999997996</v>
+        <v>-88</v>
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.3">
@@ -25396,28 +26233,28 @@
       </c>
       <c r="R48" s="95">
         <f t="array" ref="R48:U51">MMULT(R43:U46,N48:Q51)</f>
-        <v>6.4480511649567302E-17</v>
+        <v>3.4851668155187386E-2</v>
       </c>
       <c r="S48" s="96">
-        <v>5.7855054232408333E-17</v>
+        <v>-1.8264985323229177E-3</v>
       </c>
       <c r="T48" s="96">
-        <v>1</v>
+        <v>0.99939082701909576</v>
       </c>
       <c r="U48" s="89">
-        <v>340</v>
+        <v>339.9147157826734</v>
       </c>
       <c r="V48" s="18">
         <f>$V$17*R48+$V$18*S48+$V$19*T48+$V$20*U48</f>
-        <v>340</v>
+        <v>339.9147157826734</v>
       </c>
       <c r="W48" s="90">
         <f>IF(W49=PI()/2,ATAN2(S49,S48),IF(-W49=PI()/2,-ATAN2(S49,S48),ATAN2(T50,S50)))</f>
-        <v>-1.5707963267948977</v>
+        <v>-1.5707963267948966</v>
       </c>
       <c r="X48" s="20">
         <f>DEGREES(W48)</f>
-        <v>-90.000000000000057</v>
+        <v>-90</v>
       </c>
       <c r="Y48" s="1" t="s">
         <v>76</v>
@@ -25444,28 +26281,28 @@
         <v>0</v>
       </c>
       <c r="R49" s="95">
-        <v>-5.4078812984775355E-2</v>
+        <v>-0.99802119662406841</v>
       </c>
       <c r="S49" s="96">
-        <v>-0.99853667032621174</v>
+        <v>5.2304074592470849E-2</v>
       </c>
       <c r="T49" s="96">
-        <v>6.1257422745431001E-17</v>
+        <v>3.4899496702501032E-2</v>
       </c>
       <c r="U49" s="89">
-        <v>2.45029690981724E-15</v>
+        <v>4.8859295383501378</v>
       </c>
       <c r="V49" s="18">
         <f>$V$17*R49+$V$19*S49+$V$18*T49+$V$20*U49</f>
-        <v>2.45029690981724E-15</v>
+        <v>4.8859295383501378</v>
       </c>
       <c r="W49" s="90">
         <f>ATAN2(SQRT(R48^2+R49^2),-R50)</f>
-        <v>-1.5166911199830724</v>
+        <v>5.2359877559829897E-2</v>
       </c>
       <c r="X49" s="20">
         <f>DEGREES(W49)</f>
-        <v>-86.9</v>
+        <v>3.0000000000000004</v>
       </c>
       <c r="Y49" s="1" t="s">
         <v>73</v>
@@ -25491,13 +26328,13 @@
         <v>140</v>
       </c>
       <c r="R50" s="95">
-        <v>0.99853667032621174</v>
+        <v>-5.2335956242943842E-2</v>
       </c>
       <c r="S50" s="96">
-        <v>-5.4078812984775355E-2</v>
+        <v>-0.99862953475457383</v>
       </c>
       <c r="T50" s="96">
-        <v>-6.1257422745431001E-17</v>
+        <v>-6.1182790011798308E-17</v>
       </c>
       <c r="U50" s="89">
         <v>400</v>
@@ -25508,11 +26345,11 @@
       </c>
       <c r="W50" s="90">
         <f>IF(ABS(W49)=PI()/2,0,ATAN2(R48,R49))</f>
-        <v>-1.5707963267948954</v>
+        <v>-1.5358897417550099</v>
       </c>
       <c r="X50" s="20">
         <f>DEGREES(W50)</f>
-        <v>-89.999999999999929</v>
+        <v>-88</v>
       </c>
       <c r="Y50" s="1" t="s">
         <v>71</v>
@@ -25553,6 +26390,24 @@
       <c r="W51" s="8"/>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" t="s">
+        <v>83</v>
+      </c>
+      <c r="E52" t="s">
+        <v>79</v>
+      </c>
+      <c r="F52" t="s">
+        <v>82</v>
+      </c>
+      <c r="G52" t="s">
+        <v>80</v>
+      </c>
+      <c r="H52" t="s">
+        <v>81</v>
+      </c>
       <c r="N52" s="12"/>
       <c r="O52" s="12"/>
       <c r="P52" s="12"/>
@@ -25565,719 +26420,838 @@
       <c r="W52" s="8"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A53" s="15" t="s">
-        <v>26</v>
+      <c r="C53">
+        <v>-90</v>
+      </c>
+      <c r="D53" s="3">
+        <f>RADIANS(C53)</f>
+        <v>-1.5707963267948966</v>
+      </c>
+      <c r="E53">
+        <v>-90</v>
+      </c>
+      <c r="F53" s="6">
+        <f>RADIANS(E53)</f>
+        <v>-1.5707963267948966</v>
+      </c>
+      <c r="G53">
+        <v>-90</v>
+      </c>
+      <c r="H53" s="6">
+        <f>RADIANS(G53)</f>
+        <v>-1.5707963267948966</v>
+      </c>
+      <c r="N53" s="11">
+        <f>COS(H53)*COS(F53)</f>
+        <v>3.7524718414124473E-33</v>
+      </c>
+      <c r="O53" s="12">
+        <f>-SIN(H53)*COS(D53)+COS(H53)*SIN(F53)*SIN(D53)</f>
+        <v>1.22514845490862E-16</v>
+      </c>
+      <c r="P53" s="12">
+        <f>SIN(H53)*SIN(D53)+COS(H53)*SIN(F53)*COS(D53)</f>
+        <v>1</v>
+      </c>
+      <c r="Q53" s="13">
+        <v>0</v>
+      </c>
+      <c r="R53" s="95">
+        <f t="array" ref="R53:U56">MMULT(R48:U51,N53:Q56)</f>
+        <v>0.99939082701909576</v>
+      </c>
+      <c r="S53" s="96">
+        <v>1.8264985323228609E-3</v>
+      </c>
+      <c r="T53" s="96">
+        <v>3.4851668155187386E-2</v>
+      </c>
+      <c r="U53" s="89">
+        <v>0</v>
+      </c>
+      <c r="V53" s="18">
+        <f>$V$17*R53+$V$18*S53+$V$19*T53+$V$20*U53</f>
+        <v>0</v>
+      </c>
+      <c r="W53" s="90">
+        <f>IF(W54=PI()/2,ATAN2(S54,S53),IF(-W54=PI()/2,-ATAN2(S54,S53),ATAN2(T55,S55)))</f>
+        <v>1.6231562043547265</v>
+      </c>
+      <c r="X53" s="20">
+        <f>DEGREES(W53)</f>
+        <v>93</v>
+      </c>
+      <c r="Y53" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A54" s="15"/>
+      <c r="N54" s="11">
+        <f>SIN(H53)*COS(F53)</f>
+        <v>-6.1257422745431001E-17</v>
+      </c>
+      <c r="O54" s="12">
+        <f>COS(H53)*COS(D53)+SIN(H53)*SIN(F53)*SIN(D53)</f>
+        <v>-1</v>
+      </c>
+      <c r="P54" s="12">
+        <f>-COS(H53)*SIN(D53)+SIN(H53)*SIN(F53)*COS(D53)</f>
+        <v>1.22514845490862E-16</v>
+      </c>
+      <c r="Q54" s="13">
+        <v>0</v>
+      </c>
+      <c r="R54" s="95">
+        <v>3.4899496702501032E-2</v>
+      </c>
+      <c r="S54" s="96">
+        <v>-5.2304074592470974E-2</v>
+      </c>
+      <c r="T54" s="96">
+        <v>-0.99802119662406841</v>
+      </c>
+      <c r="U54" s="89">
+        <v>0</v>
+      </c>
+      <c r="V54" s="18">
+        <f>$V$17*R54+$V$19*S54+$V$18*T54+$V$20*U54</f>
+        <v>0</v>
+      </c>
+      <c r="W54" s="90">
+        <f>ATAN2(SQRT(R53^2+R54^2),-R55)</f>
+        <v>9.3184352642928652E-21</v>
+      </c>
+      <c r="X54" s="20">
+        <f>DEGREES(W54)</f>
+        <v>5.3390701230985497E-19</v>
+      </c>
+      <c r="Y54" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C55" t="s">
-        <v>13</v>
-      </c>
-      <c r="D55" t="s">
-        <v>64</v>
-      </c>
-      <c r="G55" t="s">
-        <v>62</v>
+      <c r="N55" s="11">
+        <f>-SIN(F53)</f>
+        <v>1</v>
+      </c>
+      <c r="O55" s="12">
+        <f>SIN(D53)*COS(F53)</f>
+        <v>-6.1257422745431001E-17</v>
+      </c>
+      <c r="P55" s="12">
+        <f>COS(D53)*COS(F53)</f>
+        <v>3.7524718414124473E-33</v>
+      </c>
+      <c r="Q55" s="13">
+        <v>0</v>
+      </c>
+      <c r="R55" s="95">
+        <v>-9.3184352642928652E-21</v>
+      </c>
+      <c r="S55" s="96">
+        <v>0.99862953475457383</v>
+      </c>
+      <c r="T55" s="96">
+        <v>-5.2335956242943966E-2</v>
+      </c>
+      <c r="U55" s="89">
+        <v>0</v>
+      </c>
+      <c r="V55" s="18">
+        <f>$V$17*R55+$V$19*S55+$V$18*T55+$V$20*U55</f>
+        <v>0</v>
+      </c>
+      <c r="W55" s="90">
+        <f>IF(ABS(W54)=PI()/2,0,ATAN2(R53,R54))</f>
+        <v>3.4906585039886653E-2</v>
+      </c>
+      <c r="X55" s="20">
+        <f>DEGREES(W55)</f>
+        <v>2.0000000000000036</v>
+      </c>
+      <c r="Y55" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>27</v>
-      </c>
-      <c r="C56" s="7">
-        <f t="array" ref="C56:C59">V48:V51</f>
-        <v>340</v>
-      </c>
-      <c r="D56" s="21">
-        <f t="array" ref="D56:D58">W48:W50</f>
-        <v>-1.5707963267948977</v>
-      </c>
-      <c r="E56" s="20">
-        <f>DEGREES(D56)</f>
-        <v>-90.000000000000057</v>
-      </c>
-      <c r="F56" s="91">
-        <f>D56+PI()</f>
-        <v>1.5707963267948954</v>
-      </c>
-      <c r="G56" s="21">
-        <f>IF(F56&gt;PI(),F56-2*PI(),F56)</f>
-        <v>1.5707963267948954</v>
-      </c>
-      <c r="H56" s="20">
-        <f>DEGREES(G56)</f>
-        <v>89.999999999999929</v>
-      </c>
+      <c r="N56" s="11">
+        <v>0</v>
+      </c>
+      <c r="O56" s="12">
+        <v>0</v>
+      </c>
+      <c r="P56" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="13">
+        <v>0</v>
+      </c>
+      <c r="R56" s="95">
+        <v>0</v>
+      </c>
+      <c r="S56" s="96">
+        <v>0</v>
+      </c>
+      <c r="T56" s="96">
+        <v>0</v>
+      </c>
+      <c r="U56" s="89">
+        <v>0</v>
+      </c>
+      <c r="V56" s="18">
+        <f>$V$17*R56+$V$18*S56+$V$19*T56+$V$20*U56</f>
+        <v>0</v>
+      </c>
+      <c r="W56" s="8"/>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C57" s="7">
-        <v>2.45029690981724E-15</v>
-      </c>
-      <c r="D57" s="21">
-        <v>-1.5166911199830724</v>
-      </c>
-      <c r="E57" s="20">
-        <f>DEGREES(D57)</f>
-        <v>-86.9</v>
-      </c>
-      <c r="F57" s="91">
-        <f>D57+PI()/2</f>
-        <v>5.410520681182418E-2</v>
-      </c>
-      <c r="G57" s="21">
-        <f>IF(F57&gt;PI(),F57-2*PI(),F57)</f>
-        <v>5.410520681182418E-2</v>
-      </c>
-      <c r="H57" s="20">
-        <f>DEGREES(G57)</f>
-        <v>3.0999999999999979</v>
-      </c>
+      <c r="N57" s="12"/>
+      <c r="O57" s="12"/>
+      <c r="P57" s="12"/>
+      <c r="Q57" s="12"/>
+      <c r="R57" s="88"/>
+      <c r="S57" s="88"/>
+      <c r="T57" s="88"/>
+      <c r="U57" s="88"/>
+      <c r="V57" s="18"/>
+      <c r="W57" s="8"/>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C58" s="7">
-        <v>400</v>
-      </c>
-      <c r="D58" s="21">
-        <v>-1.5707963267948954</v>
-      </c>
-      <c r="E58" s="20">
-        <f>DEGREES(D58)</f>
-        <v>-89.999999999999929</v>
-      </c>
-      <c r="F58" s="91">
-        <f>D58</f>
-        <v>-1.5707963267948954</v>
-      </c>
-      <c r="G58" s="21">
-        <f>IF(F58&gt;PI(),F58-2*PI(),F58)</f>
-        <v>-1.5707963267948954</v>
-      </c>
-      <c r="H58" s="20">
-        <f>DEGREES(G58)</f>
-        <v>-89.999999999999929</v>
-      </c>
-      <c r="P58" s="90"/>
+      <c r="N58" s="12"/>
+      <c r="O58" s="12"/>
+      <c r="P58" s="12"/>
+      <c r="Q58" s="12"/>
+      <c r="R58" s="88"/>
+      <c r="S58" s="88"/>
+      <c r="T58" s="88"/>
+      <c r="U58" s="88"/>
+      <c r="V58" s="18"/>
+      <c r="W58" s="8"/>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C59" s="7">
-        <v>1</v>
+      <c r="A59" s="15" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C60" s="7"/>
-      <c r="O60" s="7"/>
+      <c r="A60" s="15"/>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>66</v>
-      </c>
-      <c r="F61" t="s">
+      <c r="C61" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" t="s">
         <v>64</v>
       </c>
-      <c r="I61" t="s">
+      <c r="G61" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="B62" s="108">
-        <f>COS(D58)*COS(D57)</f>
-        <v>6.3352272028674918E-17</v>
-      </c>
-      <c r="C62" s="108">
-        <f>SIN(D56)*SIN(D57)*COS(D58)-COS(D56)*SIN(D58)</f>
-        <v>1.2080058338996191E-16</v>
-      </c>
-      <c r="D62" s="108">
-        <f>COS(D56)*SIN(D57)*COS(D58)+SIN(D56)*SIN(D58)</f>
-        <v>1</v>
-      </c>
-      <c r="E62" s="93">
-        <f>C56</f>
-        <v>340</v>
-      </c>
-      <c r="F62" s="90">
-        <f>IF(F63=PI()/2,ATAN2(C63,C62),IF(-F63=PI()/2,-ATAN2(C63,C62),ATAN2(D64,C64)))</f>
-        <v>-1.5707963267948974</v>
-      </c>
-      <c r="G62" s="7">
-        <f>DEGREES(F62)</f>
-        <v>-90.000000000000057</v>
-      </c>
-      <c r="H62" s="91">
-        <f>F62+PI()</f>
-        <v>1.5707963267948957</v>
-      </c>
-      <c r="I62" s="21">
-        <f>IF(H62&gt;PI(),H62-2*PI(),H62)</f>
-        <v>1.5707963267948957</v>
-      </c>
-      <c r="J62" s="20">
-        <f>DEGREES(I62)</f>
-        <v>89.999999999999943</v>
+      <c r="A62" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" s="7">
+        <f t="array" ref="C62:C65">V48:V51</f>
+        <v>339.9147157826734</v>
+      </c>
+      <c r="D62" s="21">
+        <f t="array" ref="D62:D64">W48:W50</f>
+        <v>-1.5707963267948966</v>
+      </c>
+      <c r="E62" s="20">
+        <f>DEGREES(D62)</f>
+        <v>-90</v>
+      </c>
+      <c r="F62" s="91">
+        <f>D62+PI()</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="G62" s="21">
+        <f>IF(F62&gt;PI(),F62-2*PI(),F62)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="H62" s="20">
+        <f>DEGREES(G62)</f>
+        <v>90</v>
       </c>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="B63" s="108">
-        <f>COS(D57)*SIN(D58)</f>
-        <v>-5.4078812984775314E-2</v>
-      </c>
-      <c r="C63" s="108">
-        <f>SIN(D56)*SIN(D57)*SIN(D58)+COS(D56)*COS(D58)</f>
-        <v>-0.99853667032621174</v>
-      </c>
-      <c r="D63" s="108">
-        <f>COS(D56)*SIN(D57)*SIN(D58)-SIN(D56)*COS(D58)</f>
-        <v>1.2404982798287571E-16</v>
-      </c>
-      <c r="E63" s="93">
-        <f>C57</f>
-        <v>2.45029690981724E-15</v>
-      </c>
-      <c r="F63" s="90">
-        <f>ATAN2(SQRT(B62^2+B63^2),-B64)</f>
-        <v>-1.5166911199830724</v>
-      </c>
-      <c r="G63" s="7">
-        <f>DEGREES(F63)</f>
-        <v>-86.9</v>
-      </c>
-      <c r="H63" s="91">
-        <f>F63+PI()/2</f>
-        <v>5.410520681182418E-2</v>
-      </c>
-      <c r="I63" s="21">
-        <f>IF(H63&gt;PI(),H63-2*PI(),H63)</f>
-        <v>5.410520681182418E-2</v>
-      </c>
-      <c r="J63" s="20">
-        <f>DEGREES(I63)</f>
-        <v>3.0999999999999979</v>
+      <c r="C63" s="7">
+        <v>4.8859295383501378</v>
+      </c>
+      <c r="D63" s="21">
+        <v>5.2359877559829897E-2</v>
+      </c>
+      <c r="E63" s="20">
+        <f>DEGREES(D63)</f>
+        <v>3.0000000000000004</v>
+      </c>
+      <c r="F63" s="91">
+        <f>D63+PI()/2</f>
+        <v>1.6231562043547265</v>
+      </c>
+      <c r="G63" s="21">
+        <f>IF(F63&gt;PI(),F63-2*PI(),F63)</f>
+        <v>1.6231562043547265</v>
+      </c>
+      <c r="H63" s="20">
+        <f>DEGREES(G63)</f>
+        <v>93</v>
       </c>
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="B64" s="108">
-        <f>-SIN(D57)</f>
-        <v>0.99853667032621174</v>
-      </c>
-      <c r="C64" s="108">
-        <f>SIN(D56)*COS(D57)</f>
-        <v>-5.4078812984775314E-2</v>
-      </c>
-      <c r="D64" s="108">
-        <f>COS(D56)*COS(D57)</f>
-        <v>-5.672681461151595E-17</v>
-      </c>
-      <c r="E64" s="93">
-        <f>C58</f>
+      <c r="C64" s="7">
         <v>400</v>
       </c>
-      <c r="F64" s="90">
-        <f>IF(ABS(F63)=PI()/2,0,ATAN2(B62,B63))</f>
-        <v>-1.5707963267948954</v>
-      </c>
-      <c r="G64" s="7">
-        <f>DEGREES(F64)</f>
-        <v>-89.999999999999929</v>
-      </c>
-      <c r="H64" s="91">
-        <f>F64</f>
-        <v>-1.5707963267948954</v>
-      </c>
-      <c r="I64" s="21">
-        <f>IF(H64&gt;PI(),H64-2*PI(),H64)</f>
-        <v>-1.5707963267948954</v>
-      </c>
-      <c r="J64" s="20">
-        <f>DEGREES(I64)</f>
-        <v>-89.999999999999929</v>
-      </c>
+      <c r="D64" s="21">
+        <v>-1.5358897417550099</v>
+      </c>
+      <c r="E64" s="20">
+        <f>DEGREES(D64)</f>
+        <v>-88</v>
+      </c>
+      <c r="F64" s="91">
+        <f>D64</f>
+        <v>-1.5358897417550099</v>
+      </c>
+      <c r="G64" s="21">
+        <f>IF(F64&gt;PI(),F64-2*PI(),F64)</f>
+        <v>-1.5358897417550099</v>
+      </c>
+      <c r="H64" s="20">
+        <f>DEGREES(G64)</f>
+        <v>-88</v>
+      </c>
+      <c r="P64" s="90"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B65" s="93">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C65" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C66" s="7"/>
+      <c r="O66" s="7"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+      <c r="F67" t="s">
+        <v>64</v>
+      </c>
+      <c r="I67" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B68" s="108">
+        <f>COS(D64)*COS(D63)</f>
+        <v>3.4851668155187435E-2</v>
+      </c>
+      <c r="C68" s="108">
+        <f>SIN(D62)*SIN(D63)*COS(D64)-COS(D62)*SIN(D64)</f>
+        <v>-1.8264985323227982E-3</v>
+      </c>
+      <c r="D68" s="108">
+        <f>COS(D62)*SIN(D63)*COS(D64)+SIN(D62)*SIN(D64)</f>
+        <v>0.99939082701909576</v>
+      </c>
+      <c r="E68" s="93">
+        <f>C62</f>
+        <v>339.9147157826734</v>
+      </c>
+      <c r="F68" s="90">
+        <f>IF(F69=PI()/2,ATAN2(C69,C68),IF(-F69=PI()/2,-ATAN2(C69,C68),ATAN2(D70,C70)))</f>
+        <v>-1.5707963267948966</v>
+      </c>
+      <c r="G68" s="7">
+        <f>DEGREES(F68)</f>
+        <v>-90</v>
+      </c>
+      <c r="H68" s="91">
+        <f>F68+PI()</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I68" s="21">
+        <f>IF(H68&gt;PI(),H68-2*PI(),H68)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="J68" s="20">
+        <f>DEGREES(I68)</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B69" s="108">
+        <f>COS(D63)*SIN(D64)</f>
+        <v>-0.99802119662406841</v>
+      </c>
+      <c r="C69" s="108">
+        <f>SIN(D62)*SIN(D63)*SIN(D64)+COS(D62)*COS(D64)</f>
+        <v>5.2304074592470856E-2</v>
+      </c>
+      <c r="D69" s="108">
+        <f>COS(D62)*SIN(D63)*SIN(D64)-SIN(D62)*COS(D64)</f>
+        <v>3.489949670250108E-2</v>
+      </c>
+      <c r="E69" s="93">
+        <f>C63</f>
+        <v>4.8859295383501378</v>
+      </c>
+      <c r="F69" s="90">
+        <f>ATAN2(SQRT(B68^2+B69^2),-B70)</f>
+        <v>5.2359877559829897E-2</v>
+      </c>
+      <c r="G69" s="7">
+        <f>DEGREES(F69)</f>
+        <v>3.0000000000000004</v>
+      </c>
+      <c r="H69" s="91">
+        <f>F69+PI()/2</f>
+        <v>1.6231562043547265</v>
+      </c>
+      <c r="I69" s="21">
+        <f>IF(H69&gt;PI(),H69-2*PI(),H69)</f>
+        <v>1.6231562043547265</v>
+      </c>
+      <c r="J69" s="20">
+        <f>DEGREES(I69)</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B70" s="108">
+        <f>-SIN(D63)</f>
+        <v>-5.2335956242943842E-2</v>
+      </c>
+      <c r="C70" s="108">
+        <f>SIN(D62)*COS(D63)</f>
+        <v>-0.99862953475457383</v>
+      </c>
+      <c r="D70" s="108">
+        <f>COS(D62)*COS(D63)</f>
+        <v>6.1173471576534015E-17</v>
+      </c>
+      <c r="E70" s="93">
+        <f>C64</f>
+        <v>400</v>
+      </c>
+      <c r="F70" s="90">
+        <f>IF(ABS(F69)=PI()/2,0,ATAN2(B68,B69))</f>
+        <v>-1.5358897417550099</v>
+      </c>
+      <c r="G70" s="7">
+        <f>DEGREES(F70)</f>
+        <v>-88</v>
+      </c>
+      <c r="H70" s="91">
+        <f>F70</f>
+        <v>-1.5358897417550099</v>
+      </c>
+      <c r="I70" s="21">
+        <f>IF(H70&gt;PI(),H70-2*PI(),H70)</f>
+        <v>-1.5358897417550099</v>
+      </c>
+      <c r="J70" s="20">
+        <f>DEGREES(I70)</f>
+        <v>-88</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B71" s="93">
         <v>0</v>
       </c>
-      <c r="C65" s="93">
+      <c r="C71" s="93">
         <v>0</v>
       </c>
-      <c r="D65" s="93">
+      <c r="D71" s="93">
         <v>0</v>
       </c>
-      <c r="E65" s="93">
+      <c r="E71" s="93">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A66" s="15" t="s">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A72" s="15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A67" s="9" t="s">
+    <row r="73" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A73" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
+    <row r="75" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>32</v>
       </c>
-      <c r="B69" s="16"/>
-      <c r="F69">
+      <c r="B75" s="16"/>
+      <c r="F75">
         <v>0</v>
       </c>
-      <c r="I69" s="7">
-        <f t="array" ref="I69:L72">MMULT(B62:E65,F69:F72)</f>
+      <c r="I75" s="7">
+        <f t="array" ref="I75:L78">MMULT(B68:E71,F75:F78)</f>
         <v>200</v>
       </c>
-      <c r="J69" s="7">
+      <c r="J75" s="7">
         <v>200</v>
       </c>
-      <c r="K69" s="7">
+      <c r="K75" s="7">
         <v>200</v>
       </c>
-      <c r="L69" s="7">
+      <c r="L75" s="7">
         <v>200</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F70">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F76">
         <v>0</v>
       </c>
-      <c r="I70" s="7">
-        <v>-1.4916679007785359E-14</v>
-      </c>
-      <c r="J70" s="7">
-        <v>-1.4916679007785359E-14</v>
-      </c>
-      <c r="K70" s="7">
-        <v>-1.4916679007785359E-14</v>
-      </c>
-      <c r="L70" s="7">
-        <v>-1.4916679007785359E-14</v>
+      <c r="I76" s="7">
+        <v>-1.3322676295501878E-14</v>
+      </c>
+      <c r="J76" s="7">
+        <v>-1.3322676295501878E-14</v>
+      </c>
+      <c r="K76" s="7">
+        <v>-1.3322676295501878E-14</v>
+      </c>
+      <c r="L76" s="7">
+        <v>-1.3322676295501878E-14</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F71">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F77">
         <f>-F48</f>
         <v>-140</v>
       </c>
-      <c r="I71" s="7">
+      <c r="I77" s="7">
         <v>400</v>
       </c>
-      <c r="J71" s="7">
+      <c r="J77" s="7">
         <v>400</v>
       </c>
-      <c r="K71" s="7">
+      <c r="K77" s="7">
         <v>400</v>
       </c>
-      <c r="L71" s="7">
+      <c r="L77" s="7">
         <v>400</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F72">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F78">
         <v>1</v>
       </c>
-      <c r="I72" s="7">
+      <c r="I78" s="7">
         <v>1</v>
       </c>
-      <c r="J72" s="7">
+      <c r="J78" s="7">
         <v>1</v>
       </c>
-      <c r="K72" s="7">
+      <c r="K78" s="7">
         <v>1</v>
       </c>
-      <c r="L72" s="7">
+      <c r="L78" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
+    <row r="79" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
+    <row r="80" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
         <v>33</v>
       </c>
-      <c r="B74" s="17" t="s">
+      <c r="B80" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C80" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A76" s="5"/>
-      <c r="B76" s="8"/>
-      <c r="C76" s="8"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="8"/>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="5"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B77" s="8"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="8"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B78" s="8"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="8"/>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B79" s="8"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
     </row>
-    <row r="80" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A80" s="15" t="s">
+    <row r="86" spans="1:9" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A86" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B80" s="8"/>
-      <c r="C80" s="8"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
+      <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A81" s="9" t="s">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A82" s="9"/>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" s="9"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B83" s="76">
-        <f t="array" ref="B83:B86">L69:L72</f>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B89" s="76">
+        <f t="array" ref="B89:B92">L75:L78</f>
         <v>200</v>
       </c>
-      <c r="E83" s="5" t="s">
+      <c r="E89" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H83" s="21">
-        <f>ATAN2(B83,B84)</f>
-        <v>-7.4583395038926799E-17</v>
-      </c>
-      <c r="I83" s="23">
-        <f>DEGREES(H83)</f>
-        <v>-4.2733137574874679E-15</v>
+      <c r="H89" s="21">
+        <f>ATAN2(B89,B90)</f>
+        <v>-6.661338147750939E-17</v>
+      </c>
+      <c r="I89" s="23">
+        <f>DEGREES(H89)</f>
+        <v>-3.8166656177562198E-15</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>30</v>
       </c>
-      <c r="B84" s="60">
-        <v>-1.4916679007785359E-14</v>
-      </c>
-      <c r="H84" s="21">
-        <f>ATAN2(-B83,-B84)</f>
+      <c r="B90" s="60">
+        <v>-1.3322676295501878E-14</v>
+      </c>
+      <c r="H90" s="21">
+        <f>ATAN2(-B89,-B90)</f>
         <v>3.1415926535897931</v>
       </c>
-      <c r="I84" s="23">
-        <f>DEGREES(H84)</f>
+      <c r="I90" s="23">
+        <f>DEGREES(H90)</f>
         <v>180</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B85" s="60">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B91" s="60">
         <v>400</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E91" t="s">
         <v>40</v>
       </c>
-      <c r="G85" s="21">
-        <f>IF(B87=1,H83,H84)</f>
-        <v>-7.4583395038926799E-17</v>
-      </c>
-      <c r="H85" s="23">
-        <f>DEGREES(G85)</f>
-        <v>-4.2733137574874679E-15</v>
-      </c>
-      <c r="I85" s="15" t="str">
-        <f>IF(ABS(H85-B15)&lt; 0.001,"OK","NOT OK!")</f>
+      <c r="G91" s="21">
+        <f>IF(B93=1,H89,H90)</f>
+        <v>-6.661338147750939E-17</v>
+      </c>
+      <c r="H91" s="23">
+        <f>DEGREES(G91)</f>
+        <v>-3.8166656177562198E-15</v>
+      </c>
+      <c r="I91" s="15" t="str">
+        <f>IF(ABS(H91-B15)&lt; 0.001,"OK","NOT OK!")</f>
         <v>OK</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B86">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B92">
         <v>1</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E92" t="s">
         <v>41</v>
       </c>
-      <c r="G86" s="21">
-        <f>IF(B87=-1,H83,H84)</f>
+      <c r="G92" s="21">
+        <f>IF(B93=-1,H89,H90)</f>
         <v>3.1415926535897931</v>
       </c>
-      <c r="H86" s="23">
-        <f>DEGREES(G86)</f>
+      <c r="H92" s="23">
+        <f>DEGREES(G92)</f>
         <v>180</v>
       </c>
-      <c r="I86" s="15" t="str">
-        <f>IF(ABS(H86-B15)&lt; 0.001,"OK","NOT OK!")</f>
+      <c r="I92" s="15" t="str">
+        <f>IF(ABS(H92-B15)&lt; 0.001,"OK","NOT OK!")</f>
         <v>NOT OK!</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>43</v>
       </c>
-      <c r="B87">
-        <f>SIGN(B83)</f>
+      <c r="B93">
+        <f>SIGN(B89)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A89" s="15" t="s">
+    <row r="95" spans="1:9" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A95" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A91" s="9" t="s">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A97" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="J96" t="s">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J102" t="s">
         <v>45</v>
       </c>
-      <c r="K96">
+      <c r="K102">
         <v>0</v>
       </c>
-      <c r="L96">
-        <f>E112*B87</f>
+      <c r="L102">
+        <f>E118*B93</f>
         <v>200</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="K97">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K103">
         <v>0</v>
       </c>
-      <c r="L97" s="4">
-        <f>E110</f>
+      <c r="L103" s="4">
+        <f>E116</f>
         <v>300</v>
-      </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A109" s="15"/>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E110" s="19">
-        <f>B85-F23</f>
-        <v>300</v>
-      </c>
-      <c r="M110" s="90">
-        <f>ACOS((E117*E117-E116*E116-E115*E115)/(-2*E116*E115))</f>
-        <v>0.58800260354756739</v>
-      </c>
-      <c r="N110" s="20">
-        <f>DEGREES(M110)</f>
-        <v>33.690067525979778</v>
-      </c>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E112" s="4">
-        <f>SQRT(B83*B83+B84*B84)</f>
-        <v>200</v>
-      </c>
-      <c r="I112" s="19"/>
-      <c r="J112" s="19"/>
-      <c r="M112" s="109">
-        <f>ACOS((E115*E115-E116*E116-E117*E117)/(-2*E116*E117))</f>
-        <v>1.5707963267948966</v>
-      </c>
-      <c r="N112" s="22">
-        <f>DEGREES(M112)</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="E113" s="4"/>
-      <c r="I113" s="19"/>
-      <c r="J113" s="19"/>
-      <c r="M113" s="21"/>
-      <c r="N113" s="22"/>
-    </row>
-    <row r="114" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M114" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q114" s="33" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B115" t="s">
-        <v>56</v>
-      </c>
-      <c r="E115" s="7">
-        <f>SQRT(E112*E112+E110*E110)</f>
-        <v>360.55512754639892</v>
-      </c>
-      <c r="L115" t="s">
-        <v>68</v>
-      </c>
-      <c r="M115" s="34">
-        <f>IF(B87=1,1,-1)</f>
-        <v>1</v>
-      </c>
-      <c r="N115" s="35"/>
-      <c r="O115" s="35"/>
-      <c r="P115" s="35"/>
-      <c r="Q115" s="35">
-        <f>IF(B87=1,-1,1)</f>
-        <v>-1</v>
-      </c>
-      <c r="R115" s="35"/>
-      <c r="S115" s="36"/>
+      <c r="A115" s="15"/>
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B116" t="s">
+      <c r="E116" s="19">
+        <f>B91-F23</f>
+        <v>300</v>
+      </c>
+      <c r="M116" s="90">
+        <f>ACOS((E123*E123-E122*E122-E121*E121)/(-2*E122*E121))</f>
+        <v>0.58800260354756739</v>
+      </c>
+      <c r="N116" s="20">
+        <f>DEGREES(M116)</f>
+        <v>33.690067525979778</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="E118" s="4">
+        <f>SQRT(B89*B89+B90*B90)</f>
+        <v>200</v>
+      </c>
+      <c r="I118" s="19"/>
+      <c r="J118" s="19"/>
+      <c r="M118" s="109">
+        <f>ACOS((E121*E121-E122*E122-E123*E123)/(-2*E122*E123))</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="N118" s="22">
+        <f>DEGREES(M118)</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="E119" s="4"/>
+      <c r="I119" s="19"/>
+      <c r="J119" s="19"/>
+      <c r="M119" s="21"/>
+      <c r="N119" s="22"/>
+    </row>
+    <row r="120" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M120" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q120" s="33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>56</v>
+      </c>
+      <c r="E121" s="7">
+        <f>SQRT(E118*E118+E116*E116)</f>
+        <v>360.55512754639892</v>
+      </c>
+      <c r="L121" t="s">
+        <v>68</v>
+      </c>
+      <c r="M121" s="34">
+        <f>IF(B93=1,1,-1)</f>
+        <v>1</v>
+      </c>
+      <c r="N121" s="35"/>
+      <c r="O121" s="35"/>
+      <c r="P121" s="35"/>
+      <c r="Q121" s="35">
+        <f>IF(B93=1,-1,1)</f>
+        <v>-1</v>
+      </c>
+      <c r="R121" s="35"/>
+      <c r="S121" s="36"/>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
         <v>54</v>
       </c>
-      <c r="E116" s="7">
+      <c r="E122" s="7">
         <f>E28</f>
         <v>300</v>
       </c>
-      <c r="F116" s="5"/>
-      <c r="L116" s="9" t="s">
+      <c r="F122" s="5"/>
+      <c r="L122" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M116" s="113">
-        <f>ATAN2(M115*E112,E110)</f>
+      <c r="M122" s="113">
+        <f>ATAN2(M121*E118,E116)</f>
         <v>0.98279372324732905</v>
       </c>
-      <c r="N116" s="37">
-        <f>DEGREES(M116)</f>
+      <c r="N122" s="37">
+        <f>DEGREES(M122)</f>
         <v>56.309932474020215</v>
       </c>
-      <c r="O116" s="38"/>
-      <c r="P116" s="38"/>
-      <c r="Q116" s="39">
-        <f>ATAN2(Q115*E112,E110)</f>
-        <v>2.158798930342464</v>
-      </c>
-      <c r="R116" s="37">
-        <f>DEGREES(Q116)</f>
-        <v>123.69006752597979</v>
-      </c>
-      <c r="S116" s="40"/>
-    </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B117" t="s">
-        <v>55</v>
-      </c>
-      <c r="E117" s="7">
-        <f>F38</f>
-        <v>200</v>
-      </c>
-      <c r="M117" s="41"/>
-      <c r="N117" s="38"/>
-      <c r="O117" s="38"/>
-      <c r="P117" s="38"/>
-      <c r="Q117" s="38"/>
-      <c r="R117" s="38"/>
-      <c r="S117" s="40"/>
-    </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="G118" s="1"/>
-      <c r="K118" s="115"/>
-      <c r="M118" s="41"/>
-      <c r="N118" s="38"/>
-      <c r="O118" s="38"/>
-      <c r="P118" s="38"/>
-      <c r="Q118" s="38"/>
-      <c r="R118" s="38"/>
-      <c r="S118" s="40"/>
-    </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="F119" s="5"/>
-      <c r="G119" s="1"/>
-      <c r="M119" s="41"/>
-      <c r="N119" s="38"/>
-      <c r="O119" s="38"/>
-      <c r="P119" s="38"/>
-      <c r="Q119" s="38"/>
-      <c r="R119" s="38"/>
-      <c r="S119" s="40"/>
-    </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="E120" t="s">
-        <v>46</v>
-      </c>
-      <c r="G120" s="1"/>
-      <c r="M120" s="114">
-        <f>PI()/2-(M116+M110)</f>
-        <v>0</v>
-      </c>
-      <c r="N120" s="43">
-        <f>DEGREES(M120)</f>
-        <v>0</v>
-      </c>
-      <c r="O120" s="44" t="str">
-        <f>IF(ABS(N120-B16)&lt; 0.001,"OK","NOT OK!")</f>
-        <v>OK</v>
-      </c>
-      <c r="P120" s="38"/>
-      <c r="Q120" s="45">
-        <f>PI()/2-(Q116+M110)</f>
-        <v>-1.1760052070951348</v>
-      </c>
-      <c r="R120" s="43">
-        <f>DEGREES(Q120)</f>
-        <v>-67.380135051959556</v>
-      </c>
-      <c r="S120" s="46" t="str">
-        <f>IF(ABS(R120-H16)&lt; 0.001,"OK","NOT OK!")</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="G121" s="1"/>
-      <c r="M121" s="42">
-        <f>PI()/2-M112</f>
-        <v>0</v>
-      </c>
-      <c r="N121" s="43">
-        <f>DEGREES(M121)</f>
-        <v>0</v>
-      </c>
-      <c r="O121" s="44" t="str">
-        <f>IF(ABS(N121-B17)&lt; 0.001,"OK","NOT OK!")</f>
-        <v>OK</v>
-      </c>
-      <c r="P121" s="38"/>
-      <c r="Q121" s="45">
-        <f>PI()/2-M112</f>
-        <v>0</v>
-      </c>
-      <c r="R121" s="43">
-        <f>DEGREES(Q121)</f>
-        <v>0</v>
-      </c>
-      <c r="S121" s="46" t="str">
-        <f>IF(ABS(R121-H17)&lt; 0.001,"OK","NOT OK!")</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="M122" s="41"/>
-      <c r="N122" s="38"/>
       <c r="O122" s="38"/>
       <c r="P122" s="38"/>
-      <c r="Q122" s="38"/>
-      <c r="R122" s="38"/>
+      <c r="Q122" s="39">
+        <f>ATAN2(Q121*E118,E116)</f>
+        <v>2.158798930342464</v>
+      </c>
+      <c r="R122" s="37">
+        <f>DEGREES(Q122)</f>
+        <v>123.69006752597979</v>
+      </c>
       <c r="S122" s="40"/>
     </row>
     <row r="123" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="M123" s="47"/>
-      <c r="N123" s="48"/>
+      <c r="B123" t="s">
+        <v>55</v>
+      </c>
+      <c r="E123" s="7">
+        <f>F38</f>
+        <v>200</v>
+      </c>
+      <c r="M123" s="41"/>
+      <c r="N123" s="38"/>
       <c r="O123" s="38"/>
       <c r="P123" s="38"/>
       <c r="Q123" s="38"/>
@@ -26285,8 +27259,8 @@
       <c r="S123" s="40"/>
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="F124" s="9"/>
       <c r="G124" s="1"/>
+      <c r="K124" s="115"/>
       <c r="M124" s="41"/>
       <c r="N124" s="38"/>
       <c r="O124" s="38"/>
@@ -26296,6 +27270,8 @@
       <c r="S124" s="40"/>
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F125" s="5"/>
+      <c r="G125" s="1"/>
       <c r="M125" s="41"/>
       <c r="N125" s="38"/>
       <c r="O125" s="38"/>
@@ -26306,432 +27282,529 @@
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.3">
       <c r="E126" t="s">
-        <v>47</v>
-      </c>
-      <c r="M126" s="42">
-        <f>PI()/2-(M116-M110)</f>
-        <v>1.1760052070951348</v>
+        <v>46</v>
+      </c>
+      <c r="G126" s="1"/>
+      <c r="M126" s="114">
+        <f>PI()/2-(M122+M116)</f>
+        <v>0</v>
       </c>
       <c r="N126" s="43">
         <f>DEGREES(M126)</f>
-        <v>67.380135051959556</v>
+        <v>0</v>
       </c>
       <c r="O126" s="44" t="str">
         <f>IF(ABS(N126-B16)&lt; 0.001,"OK","NOT OK!")</f>
-        <v>NOT OK!</v>
+        <v>OK</v>
       </c>
       <c r="P126" s="38"/>
       <c r="Q126" s="45">
-        <f>PI()/2-(Q116-M110)</f>
-        <v>0</v>
+        <f>PI()/2-(Q122+M116)</f>
+        <v>-1.1760052070951348</v>
       </c>
       <c r="R126" s="43">
         <f>DEGREES(Q126)</f>
-        <v>0</v>
+        <v>-67.380135051959556</v>
       </c>
       <c r="S126" s="46" t="str">
         <f>IF(ABS(R126-H16)&lt; 0.001,"OK","NOT OK!")</f>
-        <v>NOT OK!</v>
+        <v>OK</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A127" s="15"/>
-      <c r="M127" s="49">
-        <f>(M112- PI()*3/2)</f>
-        <v>-3.1415926535897931</v>
-      </c>
-      <c r="N127" s="50">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G127" s="1"/>
+      <c r="M127" s="42">
+        <f>PI()/2-M118</f>
+        <v>0</v>
+      </c>
+      <c r="N127" s="43">
         <f>DEGREES(M127)</f>
-        <v>-180</v>
-      </c>
-      <c r="O127" s="51" t="str">
+        <v>0</v>
+      </c>
+      <c r="O127" s="44" t="str">
         <f>IF(ABS(N127-B17)&lt; 0.001,"OK","NOT OK!")</f>
-        <v>NOT OK!</v>
-      </c>
-      <c r="P127" s="52"/>
-      <c r="Q127" s="53">
-        <f>(M112- PI()*3/2)</f>
-        <v>-3.1415926535897931</v>
-      </c>
-      <c r="R127" s="50">
+        <v>OK</v>
+      </c>
+      <c r="P127" s="38"/>
+      <c r="Q127" s="45">
+        <f>PI()/2-M118</f>
+        <v>0</v>
+      </c>
+      <c r="R127" s="43">
         <f>DEGREES(Q127)</f>
-        <v>-180</v>
-      </c>
-      <c r="S127" s="54" t="str">
+        <v>0</v>
+      </c>
+      <c r="S127" s="46" t="str">
         <f>IF(ABS(R127-H17)&lt; 0.001,"OK","NOT OK!")</f>
-        <v>NOT OK!</v>
+        <v>OK</v>
       </c>
     </row>
-    <row r="129" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A129" s="15" t="s">
-        <v>53</v>
-      </c>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="M128" s="41"/>
+      <c r="N128" s="38"/>
+      <c r="O128" s="38"/>
+      <c r="P128" s="38"/>
+      <c r="Q128" s="38"/>
+      <c r="R128" s="38"/>
+      <c r="S128" s="40"/>
+    </row>
+    <row r="129" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="M129" s="47"/>
+      <c r="N129" s="48"/>
+      <c r="O129" s="38"/>
+      <c r="P129" s="38"/>
+      <c r="Q129" s="38"/>
+      <c r="R129" s="38"/>
+      <c r="S129" s="40"/>
     </row>
     <row r="130" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="E130" s="58"/>
-      <c r="F130" s="58"/>
-      <c r="G130" s="58"/>
-      <c r="J130" t="s">
-        <v>51</v>
-      </c>
-      <c r="M130" t="s">
-        <v>52</v>
-      </c>
+      <c r="F130" s="9"/>
+      <c r="G130" s="1"/>
+      <c r="M130" s="41"/>
+      <c r="N130" s="38"/>
+      <c r="O130" s="38"/>
+      <c r="P130" s="38"/>
+      <c r="Q130" s="38"/>
+      <c r="R130" s="38"/>
+      <c r="S130" s="40"/>
     </row>
     <row r="131" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="E131" s="58"/>
-      <c r="F131" s="58"/>
-      <c r="G131" s="58"/>
-      <c r="H131" s="58"/>
-      <c r="I131" s="58"/>
-      <c r="J131" s="59">
-        <f t="array" ref="J131:L133">MMULT(MMULT(N38:P40,N43:P45),N48:P50)</f>
-        <v>0.99853667032621174</v>
-      </c>
-      <c r="K131" s="59">
-        <v>-5.4078812984775293E-2</v>
-      </c>
-      <c r="L131" s="59">
-        <v>0</v>
-      </c>
-      <c r="M131" s="74">
-        <f>COS(C18)*COS(C19)*COS(C20)-SIN(C18)*SIN(C20)</f>
-        <v>0.99853667032621174</v>
-      </c>
-      <c r="N131" s="74">
-        <f>-COS(C18)*COS(C19)*SIN(C20)-SIN(C18)*COS(C20)</f>
-        <v>-5.4078812984775293E-2</v>
-      </c>
-      <c r="O131" s="74">
-        <f>-COS(C18)*SIN(C19)</f>
-        <v>0</v>
-      </c>
+      <c r="M131" s="41"/>
+      <c r="N131" s="38"/>
+      <c r="O131" s="38"/>
+      <c r="P131" s="38"/>
+      <c r="Q131" s="38"/>
+      <c r="R131" s="38"/>
+      <c r="S131" s="40"/>
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="E132" s="58"/>
-      <c r="F132" s="58"/>
-      <c r="G132" s="58"/>
-      <c r="H132" s="58"/>
-      <c r="I132" s="58"/>
-      <c r="J132" s="59">
-        <v>5.4078812984775293E-2</v>
-      </c>
-      <c r="K132" s="59">
-        <v>0.99853667032621174</v>
-      </c>
-      <c r="L132" s="59">
+      <c r="E132" t="s">
+        <v>47</v>
+      </c>
+      <c r="M132" s="42">
+        <f>PI()/2-(M122-M116)</f>
+        <v>1.1760052070951348</v>
+      </c>
+      <c r="N132" s="43">
+        <f>DEGREES(M132)</f>
+        <v>67.380135051959556</v>
+      </c>
+      <c r="O132" s="44" t="str">
+        <f>IF(ABS(N132-B16)&lt; 0.001,"OK","NOT OK!")</f>
+        <v>NOT OK!</v>
+      </c>
+      <c r="P132" s="38"/>
+      <c r="Q132" s="45">
+        <f>PI()/2-(Q122-M116)</f>
         <v>0</v>
       </c>
-      <c r="M132" s="74">
-        <f>SIN(C18)*COS(C19)*COS(C20)+COS(C18)*SIN(C20)</f>
-        <v>5.4078812984775293E-2</v>
-      </c>
-      <c r="N132" s="74">
-        <f>-SIN(C18)*COS(C19)*SIN(C20)+COS(C18)*COS(C20)</f>
-        <v>0.99853667032621174</v>
-      </c>
-      <c r="O132" s="74">
-        <f>-SIN(C18)*SIN(C19)</f>
+      <c r="R132" s="43">
+        <f>DEGREES(Q132)</f>
         <v>0</v>
       </c>
+      <c r="S132" s="46" t="str">
+        <f>IF(ABS(R132-H16)&lt; 0.001,"OK","NOT OK!")</f>
+        <v>NOT OK!</v>
+      </c>
     </row>
-    <row r="133" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="J133" s="59">
-        <v>0</v>
-      </c>
-      <c r="K133" s="59">
-        <v>0</v>
-      </c>
-      <c r="L133" s="59">
-        <v>1</v>
-      </c>
-      <c r="M133" s="74">
-        <f>SIN(C19)*COS(C20)</f>
-        <v>0</v>
-      </c>
-      <c r="N133" s="74">
-        <f>-SIN(C19)*SIN(C20)</f>
-        <v>0</v>
-      </c>
-      <c r="O133" s="74">
-        <f>COS(C19)</f>
-        <v>1</v>
+    <row r="133" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A133" s="15"/>
+      <c r="M133" s="49">
+        <f>(M118- PI()*3/2)</f>
+        <v>-3.1415926535897931</v>
+      </c>
+      <c r="N133" s="50">
+        <f>DEGREES(M133)</f>
+        <v>-180</v>
+      </c>
+      <c r="O133" s="51" t="str">
+        <f>IF(ABS(N133-B17)&lt; 0.001,"OK","NOT OK!")</f>
+        <v>NOT OK!</v>
+      </c>
+      <c r="P133" s="52"/>
+      <c r="Q133" s="53">
+        <f>(M118- PI()*3/2)</f>
+        <v>-3.1415926535897931</v>
+      </c>
+      <c r="R133" s="50">
+        <f>DEGREES(Q133)</f>
+        <v>-180</v>
+      </c>
+      <c r="S133" s="54" t="str">
+        <f>IF(ABS(R133-H17)&lt; 0.001,"OK","NOT OK!")</f>
+        <v>NOT OK!</v>
       </c>
     </row>
-    <row r="135" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="135" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A135" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B136" s="65">
-        <f t="array" ref="B136:D138">MMULT(MMULT(N23:P25,N28:P30),N33:P35)</f>
-        <v>6.1257422745431001E-17</v>
-      </c>
-      <c r="C136" s="66">
-        <v>6.1257422745431001E-17</v>
-      </c>
-      <c r="D136" s="67">
-        <v>1</v>
-      </c>
-      <c r="H136" s="65">
-        <f t="array" ref="H136:J138">TRANSPOSE(B136:D138)</f>
-        <v>6.1257422745431001E-17</v>
-      </c>
-      <c r="I136" s="66">
-        <v>-6.1257422745431001E-17</v>
-      </c>
-      <c r="J136" s="67">
-        <v>1</v>
-      </c>
-      <c r="M136" s="65">
-        <f t="array" ref="M136:O138">B62:D64</f>
-        <v>6.3352272028674918E-17</v>
-      </c>
-      <c r="N136" s="66">
-        <v>1.2080058338996191E-16</v>
-      </c>
-      <c r="O136" s="67">
-        <v>1</v>
-      </c>
-      <c r="S136" s="99">
-        <f t="array" ref="S136:U138">MMULT(H136:J138,M136:O138)</f>
-        <v>0.99853667032621174</v>
-      </c>
-      <c r="T136" s="100">
-        <v>-5.4078812984775251E-2</v>
-      </c>
-      <c r="U136" s="101">
-        <v>4.5306081339150385E-18</v>
+      <c r="E136" s="58"/>
+      <c r="F136" s="58"/>
+      <c r="G136" s="58"/>
+      <c r="J136" t="s">
+        <v>51</v>
+      </c>
+      <c r="M136" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B137" s="68">
+      <c r="E137" s="58"/>
+      <c r="F137" s="58"/>
+      <c r="G137" s="58"/>
+      <c r="H137" s="58"/>
+      <c r="I137" s="58"/>
+      <c r="J137" s="59">
+        <f t="array" ref="J137:L139">MMULT(MMULT(N38:P40,N43:P45),N48:P50)</f>
+        <v>-5.2335956242943772E-2</v>
+      </c>
+      <c r="K137" s="59">
+        <v>-0.99862953475457383</v>
+      </c>
+      <c r="L137" s="59">
+        <v>-2.1005368562915366E-18</v>
+      </c>
+      <c r="M137" s="74">
+        <f>COS(C18)*COS(C19)*COS(C20)-SIN(C18)*SIN(C20)</f>
+        <v>-5.2335956242943772E-2</v>
+      </c>
+      <c r="N137" s="74">
+        <f>-COS(C18)*COS(C19)*SIN(C20)-SIN(C18)*COS(C20)</f>
+        <v>-0.99862953475457383</v>
+      </c>
+      <c r="O137" s="74">
+        <f>-COS(C18)*SIN(C19)</f>
+        <v>-2.1378532231078771E-18</v>
+      </c>
+    </row>
+    <row r="138" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="E138" s="58"/>
+      <c r="F138" s="58"/>
+      <c r="G138" s="58"/>
+      <c r="H138" s="58"/>
+      <c r="I138" s="58"/>
+      <c r="J138" s="59">
+        <v>0.99802119662406841</v>
+      </c>
+      <c r="K138" s="59">
+        <v>-5.2304074592470787E-2</v>
+      </c>
+      <c r="L138" s="59">
+        <v>-3.4899496702500969E-2</v>
+      </c>
+      <c r="M138" s="74">
+        <f>SIN(C18)*COS(C19)*COS(C20)+COS(C18)*SIN(C20)</f>
+        <v>0.99802119662406841</v>
+      </c>
+      <c r="N138" s="74">
+        <f>-SIN(C18)*COS(C19)*SIN(C20)+COS(C18)*COS(C20)</f>
+        <v>-5.2304074592470787E-2</v>
+      </c>
+      <c r="O138" s="74">
+        <f>-SIN(C18)*SIN(C19)</f>
+        <v>-3.4899496702500969E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J139" s="59">
+        <v>3.4851668155187324E-2</v>
+      </c>
+      <c r="K139" s="59">
+        <v>-1.8264985323228533E-3</v>
+      </c>
+      <c r="L139" s="59">
+        <v>0.99939082701909576</v>
+      </c>
+      <c r="M139" s="74">
+        <f>SIN(C19)*COS(C20)</f>
+        <v>3.4851668155187324E-2</v>
+      </c>
+      <c r="N139" s="74">
+        <f>-SIN(C19)*SIN(C20)</f>
+        <v>-1.8264985323228533E-3</v>
+      </c>
+      <c r="O139" s="74">
+        <f>COS(C19)</f>
+        <v>0.99939082701909576</v>
+      </c>
+    </row>
+    <row r="141" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="142" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B142" s="65">
+        <f t="array" ref="B142:D144">MMULT(MMULT(N23:P25,N28:P30),N33:P35)</f>
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="C142" s="66">
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="D142" s="67">
+        <v>1</v>
+      </c>
+      <c r="H142" s="65">
+        <f t="array" ref="H142:J144">TRANSPOSE(B142:D144)</f>
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="I142" s="66">
         <v>-6.1257422745431001E-17</v>
       </c>
-      <c r="C137" s="69">
-        <v>-1</v>
-      </c>
-      <c r="D137" s="70">
-        <v>6.1257422745431001E-17</v>
-      </c>
-      <c r="H137" s="68">
-        <v>6.1257422745431001E-17</v>
-      </c>
-      <c r="I137" s="69">
-        <v>-1</v>
-      </c>
-      <c r="J137" s="70">
-        <v>-6.1257422745431001E-17</v>
-      </c>
-      <c r="M137" s="68">
-        <v>-5.4078812984775314E-2</v>
-      </c>
-      <c r="N137" s="69">
-        <v>-0.99853667032621174</v>
-      </c>
-      <c r="O137" s="70">
-        <v>1.2404982798287571E-16</v>
-      </c>
-      <c r="S137" s="102">
-        <v>5.4078812984775251E-2</v>
-      </c>
-      <c r="T137" s="103">
-        <v>0.99853667032621174</v>
-      </c>
-      <c r="U137" s="104">
-        <v>-6.2792405237444708E-17</v>
-      </c>
-    </row>
-    <row r="138" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B138" s="71">
+      <c r="J142" s="67">
         <v>1</v>
       </c>
-      <c r="C138" s="72">
-        <v>-6.1257422745431001E-17</v>
-      </c>
-      <c r="D138" s="73">
-        <v>-6.1257422745431001E-17</v>
-      </c>
-      <c r="H138" s="71">
-        <v>1</v>
-      </c>
-      <c r="I138" s="72">
-        <v>6.1257422745431001E-17</v>
-      </c>
-      <c r="J138" s="73">
-        <v>-6.1257422745431001E-17</v>
-      </c>
-      <c r="M138" s="71">
-        <v>0.99853667032621174</v>
-      </c>
-      <c r="N138" s="72">
-        <v>-5.4078812984775314E-2</v>
-      </c>
-      <c r="O138" s="73">
-        <v>-5.672681461151595E-17</v>
-      </c>
-      <c r="S138" s="105">
-        <v>-1.1282396208923959E-18</v>
-      </c>
-      <c r="T138" s="106">
-        <v>6.2945529157553581E-17</v>
-      </c>
-      <c r="U138" s="107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="D142" s="76">
-        <f>U138</f>
-        <v>1</v>
-      </c>
-      <c r="E142" s="5"/>
-      <c r="G142" s="80">
-        <f>IF(ABS(D142)=1,0,ACOS(D142))</f>
-        <v>0</v>
-      </c>
-      <c r="H142" s="81">
-        <f>DEGREES(G142)</f>
-        <v>0</v>
-      </c>
-      <c r="J142" s="80">
-        <f>IF(SIN(G142)=0,ATAN2(D146,-D144),ATAN2(D146/SIN(G142),-D144/SIN(G142)))</f>
-        <v>-1.5887184705171242</v>
-      </c>
-      <c r="K142" s="81">
-        <f>DEGREES(J142)</f>
-        <v>-91.026863195110522</v>
-      </c>
-      <c r="N142" s="2">
-        <f>IF(SIN(G142)=0,-ATAN2(-D150,D148),-ATAN2(-D150/SIN(G142),D148/SIN(G142)))</f>
-        <v>1.6428236773289482</v>
-      </c>
-      <c r="O142" s="81">
-        <f>DEGREES(N142)</f>
-        <v>94.126863195110516</v>
+      <c r="M142" s="65">
+        <f t="array" ref="M142:O144">B68:D70</f>
+        <v>3.4851668155187435E-2</v>
+      </c>
+      <c r="N142" s="66">
+        <v>-1.8264985323227982E-3</v>
+      </c>
+      <c r="O142" s="67">
+        <v>0.99939082701909576</v>
+      </c>
+      <c r="S142" s="99">
+        <f t="array" ref="S142:U144">MMULT(H142:J144,M142:O144)</f>
+        <v>-5.2335956242943779E-2</v>
+      </c>
+      <c r="T142" s="100">
+        <v>-0.99862953475457383</v>
+      </c>
+      <c r="U142" s="101">
+        <v>1.202557247320408E-16</v>
       </c>
     </row>
     <row r="143" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="G143" s="80">
-        <f>IF(ABS(D142)=1,0,-ACOS(D142))</f>
-        <v>0</v>
-      </c>
-      <c r="H143" s="81">
-        <f>DEGREES(G143)</f>
-        <v>0</v>
-      </c>
-      <c r="J143" s="80">
-        <f>IF(SIN(G143)=0,ATAN2(D146,-D144),ATAN2(D146/SIN(G143),-D144/SIN(G143)))</f>
-        <v>-1.5887184705171242</v>
-      </c>
-      <c r="K143" s="81">
-        <f>DEGREES(J143)</f>
-        <v>-91.026863195110522</v>
-      </c>
-      <c r="N143" s="2">
-        <f>IF(SIN(G143)=0,-ATAN2(-D150,D148),-ATAN2(-D150/SIN(G143),D148/SIN(G143)))</f>
-        <v>1.6428236773289482</v>
-      </c>
-      <c r="O143" s="81">
-        <f>DEGREES(N143)</f>
-        <v>94.126863195110516</v>
+      <c r="B143" s="68">
+        <v>-6.1257422745431001E-17</v>
+      </c>
+      <c r="C143" s="69">
+        <v>-1</v>
+      </c>
+      <c r="D143" s="70">
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="H143" s="68">
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="I143" s="69">
+        <v>-1</v>
+      </c>
+      <c r="J143" s="70">
+        <v>-6.1257422745431001E-17</v>
+      </c>
+      <c r="M143" s="68">
+        <v>-0.99802119662406841</v>
+      </c>
+      <c r="N143" s="69">
+        <v>5.2304074592470856E-2</v>
+      </c>
+      <c r="O143" s="70">
+        <v>3.489949670250108E-2</v>
+      </c>
+      <c r="S143" s="102">
+        <v>0.99802119662406841</v>
+      </c>
+      <c r="T143" s="103">
+        <v>-5.2304074592470794E-2</v>
+      </c>
+      <c r="U143" s="104">
+        <v>-3.4899496702501018E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="D144" s="75">
-        <f>T138</f>
-        <v>6.2945529157553581E-17</v>
-      </c>
-      <c r="G144" s="2"/>
-      <c r="H144" s="2"/>
-      <c r="I144" s="2"/>
-      <c r="J144" s="94"/>
-      <c r="K144" s="81"/>
-      <c r="L144" s="2"/>
-      <c r="M144" s="2"/>
-      <c r="N144" s="92"/>
-      <c r="O144" s="81"/>
-    </row>
-    <row r="145" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="G145" s="2"/>
-      <c r="H145" s="2"/>
-      <c r="I145" s="2"/>
-      <c r="J145" s="80"/>
-      <c r="K145" s="81"/>
-      <c r="L145" s="2"/>
-      <c r="M145" s="2"/>
-      <c r="N145" s="92"/>
-      <c r="O145" s="81"/>
-    </row>
-    <row r="146" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D146" s="58">
-        <f>S138</f>
-        <v>-1.1282396208923959E-18</v>
-      </c>
-      <c r="I146" s="2"/>
-      <c r="J146" s="2"/>
-      <c r="K146" s="81"/>
-      <c r="L146" s="2"/>
-      <c r="M146" s="2"/>
-      <c r="N146" s="82"/>
-      <c r="O146" s="81"/>
-    </row>
-    <row r="147" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="I147" s="2"/>
-      <c r="J147" s="2"/>
-      <c r="K147" s="81"/>
-      <c r="L147" s="2"/>
-      <c r="M147" s="2"/>
-      <c r="N147" s="2"/>
-      <c r="O147" s="2"/>
+    <row r="144" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B144" s="71">
+        <v>1</v>
+      </c>
+      <c r="C144" s="72">
+        <v>-6.1257422745431001E-17</v>
+      </c>
+      <c r="D144" s="73">
+        <v>-6.1257422745431001E-17</v>
+      </c>
+      <c r="H144" s="71">
+        <v>1</v>
+      </c>
+      <c r="I144" s="72">
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="J144" s="73">
+        <v>-6.1257422745431001E-17</v>
+      </c>
+      <c r="M144" s="71">
+        <v>-5.2335956242943842E-2</v>
+      </c>
+      <c r="N144" s="72">
+        <v>-0.99862953475457383</v>
+      </c>
+      <c r="O144" s="73">
+        <v>6.1173471576534015E-17</v>
+      </c>
+      <c r="S144" s="105">
+        <v>3.4851668155187372E-2</v>
+      </c>
+      <c r="T144" s="106">
+        <v>-1.8264985323227338E-3</v>
+      </c>
+      <c r="U144" s="107">
+        <v>0.99939082701909576</v>
+      </c>
     </row>
     <row r="148" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D148" s="58">
-        <f>U137</f>
-        <v>-6.2792405237444708E-17</v>
-      </c>
-      <c r="G148" s="2"/>
-      <c r="H148" s="2"/>
-      <c r="I148" s="2"/>
-      <c r="J148" s="2"/>
-      <c r="K148" s="2"/>
-      <c r="L148" s="2"/>
-      <c r="M148" s="2"/>
-      <c r="N148" s="2"/>
-      <c r="O148" s="2"/>
+      <c r="D148" s="76">
+        <f>U144</f>
+        <v>0.99939082701909576</v>
+      </c>
+      <c r="E148" s="5"/>
+      <c r="G148" s="80">
+        <f>IF(ABS(D148)=1,0,ACOS(D148))</f>
+        <v>3.4906585039885529E-2</v>
+      </c>
+      <c r="H148" s="81">
+        <f>DEGREES(G148)</f>
+        <v>1.9999999999999392</v>
+      </c>
+      <c r="J148" s="80">
+        <f>IF(SIN(G148)=0,ATAN2(D152,-D150),ATAN2(D152/SIN(G148),-D150/SIN(G148)))</f>
+        <v>5.2359877559826407E-2</v>
+      </c>
+      <c r="K148" s="81">
+        <f>DEGREES(J148)</f>
+        <v>2.9999999999998006</v>
+      </c>
+      <c r="N148" s="2">
+        <f>IF(SIN(G148)=0,-ATAN2(-D156,D154),-ATAN2(-D156/SIN(G148),D154/SIN(G148)))</f>
+        <v>1.5707963267948999</v>
+      </c>
+      <c r="O148" s="81">
+        <f>DEGREES(N148)</f>
+        <v>90.000000000000185</v>
+      </c>
     </row>
     <row r="149" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="G149" s="2"/>
-      <c r="H149" s="2"/>
-      <c r="I149" s="2"/>
-      <c r="J149" s="2"/>
-      <c r="K149" s="2"/>
-      <c r="L149" s="2"/>
-      <c r="M149" s="2"/>
-      <c r="N149" s="2"/>
-      <c r="O149" s="2"/>
+      <c r="G149" s="80">
+        <f>IF(ABS(D148)=1,0,-ACOS(D148))</f>
+        <v>-3.4906585039885529E-2</v>
+      </c>
+      <c r="H149" s="81">
+        <f>DEGREES(G149)</f>
+        <v>-1.9999999999999392</v>
+      </c>
+      <c r="J149" s="80">
+        <f>IF(SIN(G149)=0,ATAN2(D152,-D150),ATAN2(D152/SIN(G149),-D150/SIN(G149)))</f>
+        <v>-3.0892327760299665</v>
+      </c>
+      <c r="K149" s="81">
+        <f>DEGREES(J149)</f>
+        <v>-177.0000000000002</v>
+      </c>
+      <c r="N149" s="2">
+        <f>IF(SIN(G149)=0,-ATAN2(-D156,D154),-ATAN2(-D156/SIN(G149),D154/SIN(G149)))</f>
+        <v>-1.5707963267948932</v>
+      </c>
+      <c r="O149" s="81">
+        <f>DEGREES(N149)</f>
+        <v>-89.999999999999815</v>
+      </c>
     </row>
     <row r="150" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D150" s="76">
-        <f>U136</f>
-        <v>4.5306081339150385E-18</v>
-      </c>
+      <c r="D150" s="75">
+        <f>T144</f>
+        <v>-1.8264985323227338E-3</v>
+      </c>
+      <c r="G150" s="2"/>
+      <c r="H150" s="2"/>
       <c r="I150" s="2"/>
-      <c r="J150" s="2"/>
+      <c r="J150" s="94"/>
       <c r="K150" s="81"/>
       <c r="L150" s="2"/>
       <c r="M150" s="2"/>
-      <c r="N150" s="82"/>
+      <c r="N150" s="92"/>
       <c r="O150" s="81"/>
     </row>
     <row r="151" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="G151" s="2"/>
+      <c r="H151" s="2"/>
       <c r="I151" s="2"/>
-      <c r="J151" s="2"/>
+      <c r="J151" s="80"/>
       <c r="K151" s="81"/>
       <c r="L151" s="2"/>
       <c r="M151" s="2"/>
-      <c r="N151" s="2"/>
-      <c r="O151" s="2"/>
+      <c r="N151" s="92"/>
+      <c r="O151" s="81"/>
     </row>
     <row r="152" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D152" t="s">
+      <c r="D152" s="58">
+        <f>S144</f>
+        <v>3.4851668155187372E-2</v>
+      </c>
+      <c r="I152" s="2"/>
+      <c r="J152" s="2"/>
+      <c r="K152" s="81"/>
+      <c r="L152" s="2"/>
+      <c r="M152" s="2"/>
+      <c r="N152" s="82"/>
+      <c r="O152" s="81"/>
+    </row>
+    <row r="153" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="I153" s="2"/>
+      <c r="J153" s="2"/>
+      <c r="K153" s="81"/>
+      <c r="L153" s="2"/>
+      <c r="M153" s="2"/>
+      <c r="N153" s="2"/>
+      <c r="O153" s="2"/>
+    </row>
+    <row r="154" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D154" s="58">
+        <f>U143</f>
+        <v>-3.4899496702501018E-2</v>
+      </c>
+      <c r="G154" s="2"/>
+      <c r="H154" s="2"/>
+      <c r="I154" s="2"/>
+      <c r="J154" s="2"/>
+      <c r="K154" s="2"/>
+      <c r="L154" s="2"/>
+      <c r="M154" s="2"/>
+      <c r="N154" s="2"/>
+      <c r="O154" s="2"/>
+    </row>
+    <row r="155" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="G155" s="2"/>
+      <c r="H155" s="2"/>
+      <c r="I155" s="2"/>
+      <c r="J155" s="2"/>
+      <c r="K155" s="2"/>
+      <c r="L155" s="2"/>
+      <c r="M155" s="2"/>
+      <c r="N155" s="2"/>
+      <c r="O155" s="2"/>
+    </row>
+    <row r="156" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D156" s="76">
+        <f>U142</f>
+        <v>1.202557247320408E-16</v>
+      </c>
+      <c r="I156" s="2"/>
+      <c r="J156" s="2"/>
+      <c r="K156" s="81"/>
+      <c r="L156" s="2"/>
+      <c r="M156" s="2"/>
+      <c r="N156" s="82"/>
+      <c r="O156" s="81"/>
+    </row>
+    <row r="157" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="I157" s="2"/>
+      <c r="J157" s="2"/>
+      <c r="K157" s="81"/>
+      <c r="L157" s="2"/>
+      <c r="M157" s="2"/>
+      <c r="N157" s="2"/>
+      <c r="O157" s="2"/>
+    </row>
+    <row r="158" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D158" t="s">
         <v>59</v>
       </c>
     </row>
@@ -26746,8 +27819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O111" sqref="O111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
fix: end node of trajectory now at endtime and not above
</commit_message>
<xml_diff>
--- a/theory/Kinematik.xlsx
+++ b/theory/Kinematik.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Trajectory Speed profile" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1752,11 +1753,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69088056"/>
-        <c:axId val="69089624"/>
+        <c:axId val="330255024"/>
+        <c:axId val="330252672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69088056"/>
+        <c:axId val="330255024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1794,13 +1795,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69089624"/>
+        <c:crossAx val="330252672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69089624"/>
+        <c:axId val="330252672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1839,7 +1840,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69088056"/>
+        <c:crossAx val="330255024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
@@ -1935,11 +1936,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69090408"/>
-        <c:axId val="69087272"/>
+        <c:axId val="330248360"/>
+        <c:axId val="330251496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69090408"/>
+        <c:axId val="330248360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -1951,13 +1952,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69087272"/>
+        <c:crossAx val="330251496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69087272"/>
+        <c:axId val="330251496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -1970,7 +1971,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69090408"/>
+        <c:crossAx val="330248360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
@@ -2111,10 +2112,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>400</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>600</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
                   <c:v>1000</c:v>
@@ -2129,13 +2130,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>4</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
                   <c:v>0</c:v>
@@ -2153,11 +2154,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="338365832"/>
-        <c:axId val="338365048"/>
+        <c:axId val="330247968"/>
+        <c:axId val="330253064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="338365832"/>
+        <c:axId val="330247968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2200,12 +2201,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338365048"/>
+        <c:crossAx val="330253064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="338365048"/>
+        <c:axId val="330253064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2256,7 +2257,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338365832"/>
+        <c:crossAx val="330247968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2624,154 +2625,154 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.9</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8</c:v>
+                  <c:v>0.18000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.7</c:v>
+                  <c:v>0.17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.6</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.5</c:v>
+                  <c:v>0.15000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.4</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.3</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.2</c:v>
+                  <c:v>0.12000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.1</c:v>
+                  <c:v>0.11000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.9</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.8</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.7</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.5999999999999996</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.5</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.4</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.2000000000000002</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.0999999999999996</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.9</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.8</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.7</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.6</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.5</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.4</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.2999999999999998</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.89999999999999991</c:v>
+                  <c:v>9.0000000000000011E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.8</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.7</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.59999999999999987</c:v>
+                  <c:v>6.0000000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.5</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.39999999999999991</c:v>
+                  <c:v>4.0000000000000008E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.19999999999999996</c:v>
+                  <c:v>2.0000000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>9.9999999999999867E-2</c:v>
+                  <c:v>1.0000000000000009E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>0</c:v>
@@ -2789,11 +2790,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="432761976"/>
-        <c:axId val="432760408"/>
+        <c:axId val="330254632"/>
+        <c:axId val="330248752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="432761976"/>
+        <c:axId val="330254632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2844,12 +2845,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="432760408"/>
+        <c:crossAx val="330248752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="432760408"/>
+        <c:axId val="330248752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2900,7 +2901,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="432761976"/>
+        <c:crossAx val="330254632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3294,154 +3295,154 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>79</c:v>
+                  <c:v>3.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>156</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>231</c:v>
+                  <c:v>11.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>304</c:v>
+                  <c:v>14.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>375</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>444</c:v>
+                  <c:v>20.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>511</c:v>
+                  <c:v>23.1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>576</c:v>
+                  <c:v>25.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>639</c:v>
+                  <c:v>27.9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>700</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>759</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>816</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>871</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>924</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>975</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1024</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1071</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1116</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1159</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1200</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1240</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1280</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1320</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1360</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1400</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1440</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1480</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1520</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1560</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1600</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1639</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1676</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1711</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1744</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1775</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1804</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1831</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1856</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1879</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1900</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1919</c:v>
+                  <c:v>91.9</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1936</c:v>
+                  <c:v>93.6</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1951</c:v>
+                  <c:v>95.1</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1964</c:v>
+                  <c:v>96.4</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1975</c:v>
+                  <c:v>97.5</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1984</c:v>
+                  <c:v>98.4</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1991</c:v>
+                  <c:v>99.1</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1996</c:v>
+                  <c:v>99.6</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1999</c:v>
+                  <c:v>99.9</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2000</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3456,11 +3457,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="432756488"/>
-        <c:axId val="432757272"/>
+        <c:axId val="316250016"/>
+        <c:axId val="316253936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="432756488"/>
+        <c:axId val="316250016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3516,12 +3517,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="432757272"/>
+        <c:crossAx val="316253936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="432757272"/>
+        <c:axId val="316253936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3577,7 +3578,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="432756488"/>
+        <c:crossAx val="316250016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -33215,8 +33216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33234,7 +33235,7 @@
         <v>85</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>0.2</v>
       </c>
       <c r="C3" t="s">
         <v>87</v>
@@ -33256,7 +33257,7 @@
         <v>88</v>
       </c>
       <c r="B5">
-        <v>2000</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
         <v>91</v>
@@ -33278,7 +33279,7 @@
         <v>71</v>
       </c>
       <c r="B7">
-        <v>5.0000000000000001E-3</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="C7" t="s">
         <v>95</v>
@@ -33288,9 +33289,9 @@
       <c r="A10" t="s">
         <v>99</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="60">
         <f>B5/B6</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="C10" t="s">
         <v>87</v>
@@ -33305,11 +33306,11 @@
       </c>
       <c r="I11" s="4">
         <f>ABS(B12)</f>
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="J11" s="3">
         <f>B6-ABS(B13)</f>
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="K11">
         <f>B6</f>
@@ -33320,27 +33321,31 @@
       <c r="A12" t="s">
         <v>93</v>
       </c>
-      <c r="B12" s="4">
-        <f>(B5- (B3*B6 + 0.5*(B4-B3)*B4/B7-0.5*(B4-B3)*B3/B7)) / ( B7*B6 + 0.5*B3 - 0.5 *(B4-B3) - 0.5*B4)</f>
-        <v>-400</v>
+      <c r="B12" s="127">
+        <f>(B5- B3*B6 - 0.5*(B4-B3)*(B4-B3)/B7) / ( B7*B6 + B3 - B4)</f>
+        <v>-200</v>
       </c>
       <c r="C12" t="s">
         <v>92</v>
       </c>
+      <c r="D12">
+        <f>(B5 - B3*B6 - 0.5*(B4-B3)*(B4-B3)/B7) / ( B7*B6 - B3 - B4)</f>
+        <v>-466.66666666666669</v>
+      </c>
       <c r="G12" t="s">
         <v>84</v>
       </c>
       <c r="H12">
         <f>B3</f>
-        <v>4</v>
+        <v>0.2</v>
       </c>
       <c r="I12" s="3">
         <f>B14</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="J12" s="3">
         <f>I12</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="K12">
         <f>B4</f>
@@ -33353,11 +33358,12 @@
       </c>
       <c r="B13" s="3">
         <f>(B4-B3)/B7-B12</f>
-        <v>-400</v>
+        <v>-200</v>
       </c>
       <c r="C13" t="s">
         <v>92</v>
       </c>
+      <c r="D13" s="75"/>
     </row>
     <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -33365,10 +33371,14 @@
       </c>
       <c r="B14" s="3">
         <f>B3+B7*B12</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="C14" t="s">
         <v>87</v>
+      </c>
+      <c r="D14">
+        <f>$B$3*$B$18+SIGN($B$12)*0.5*$B$7*$B$18*$B$18+($B$19-$B$18)*$B$14 + $B$14*(B6-$B$19) + SIGN($B$13)*0.5*$B$7*(B6-$B$19)*(B6-$B$19)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -33377,7 +33387,7 @@
       </c>
       <c r="B15" s="127">
         <f>(B3+B14)/2*B12+B14*(B6-B12-B13)+(B14+B4)/2*B13</f>
-        <v>2000</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
         <v>91</v>
@@ -33401,7 +33411,7 @@
       </c>
       <c r="B18" s="127">
         <f>ABS(B12)</f>
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="C18" t="s">
         <v>92</v>
@@ -33413,7 +33423,7 @@
       </c>
       <c r="B19" s="127">
         <f>B6-ABS(B13)</f>
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="C19" t="s">
         <v>92</v>
@@ -33437,7 +33447,7 @@
         <v>20</v>
       </c>
       <c r="J20">
-        <f t="shared" ref="J20:BR20" si="0">(I20+$B$6/50)</f>
+        <f t="shared" ref="J20:BF20" si="0">(I20+$B$6/50)</f>
         <v>40</v>
       </c>
       <c r="K20">
@@ -33645,203 +33655,203 @@
       </c>
       <c r="H21" s="127">
         <f>IF(H20&lt;ABS($B$12),$B$3+SIGN($B$12)*H$20*$B$7,IF(H20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(H20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>4</v>
+        <v>0.2</v>
       </c>
       <c r="I21" s="127">
-        <f t="shared" ref="I21:AB21" si="1">IF(I20&lt;ABS($B$12),$B$3+SIGN($B$12)*I$20*$B$7,IF(I20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(I20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>3.9</v>
+        <f t="shared" ref="I21" si="1">IF(I20&lt;ABS($B$12),$B$3+SIGN($B$12)*I$20*$B$7,IF(I20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(I20-($B$6-ABS($B$13)))*$B$7))</f>
+        <v>0.19</v>
       </c>
       <c r="J21" s="127">
         <f t="shared" ref="J21" si="2">IF(J20&lt;ABS($B$12),$B$3+SIGN($B$12)*J$20*$B$7,IF(J20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(J20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>3.8</v>
+        <v>0.18000000000000002</v>
       </c>
       <c r="K21" s="127">
         <f t="shared" ref="K21" si="3">IF(K20&lt;ABS($B$12),$B$3+SIGN($B$12)*K$20*$B$7,IF(K20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(K20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>3.7</v>
+        <v>0.17</v>
       </c>
       <c r="L21" s="127">
         <f t="shared" ref="L21" si="4">IF(L20&lt;ABS($B$12),$B$3+SIGN($B$12)*L$20*$B$7,IF(L20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(L20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>3.6</v>
+        <v>0.16</v>
       </c>
       <c r="M21" s="127">
         <f t="shared" ref="M21" si="5">IF(M20&lt;ABS($B$12),$B$3+SIGN($B$12)*M$20*$B$7,IF(M20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(M20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>3.5</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="N21" s="127">
         <f t="shared" ref="N21" si="6">IF(N20&lt;ABS($B$12),$B$3+SIGN($B$12)*N$20*$B$7,IF(N20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(N20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>3.4</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="O21" s="127">
         <f t="shared" ref="O21" si="7">IF(O20&lt;ABS($B$12),$B$3+SIGN($B$12)*O$20*$B$7,IF(O20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(O20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>3.3</v>
+        <v>0.13</v>
       </c>
       <c r="P21" s="127">
         <f t="shared" ref="P21" si="8">IF(P20&lt;ABS($B$12),$B$3+SIGN($B$12)*P$20*$B$7,IF(P20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(P20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>3.2</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="Q21" s="127">
         <f t="shared" ref="Q21" si="9">IF(Q20&lt;ABS($B$12),$B$3+SIGN($B$12)*Q$20*$B$7,IF(Q20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(Q20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>3.1</v>
+        <v>0.11000000000000001</v>
       </c>
       <c r="R21" s="127">
         <f t="shared" ref="R21" si="10">IF(R20&lt;ABS($B$12),$B$3+SIGN($B$12)*R$20*$B$7,IF(R20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(R20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="S21" s="127">
         <f t="shared" ref="S21" si="11">IF(S20&lt;ABS($B$12),$B$3+SIGN($B$12)*S$20*$B$7,IF(S20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(S20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2.9</v>
+        <v>0.1</v>
       </c>
       <c r="T21" s="127">
         <f t="shared" ref="T21" si="12">IF(T20&lt;ABS($B$12),$B$3+SIGN($B$12)*T$20*$B$7,IF(T20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(T20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2.8</v>
+        <v>0.1</v>
       </c>
       <c r="U21" s="127">
         <f t="shared" ref="U21" si="13">IF(U20&lt;ABS($B$12),$B$3+SIGN($B$12)*U$20*$B$7,IF(U20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(U20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2.7</v>
+        <v>0.1</v>
       </c>
       <c r="V21" s="127">
         <f t="shared" ref="V21" si="14">IF(V20&lt;ABS($B$12),$B$3+SIGN($B$12)*V$20*$B$7,IF(V20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(V20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2.5999999999999996</v>
+        <v>0.1</v>
       </c>
       <c r="W21" s="127">
         <f t="shared" ref="W21" si="15">IF(W20&lt;ABS($B$12),$B$3+SIGN($B$12)*W$20*$B$7,IF(W20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(W20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="X21" s="127">
         <f t="shared" ref="X21" si="16">IF(X20&lt;ABS($B$12),$B$3+SIGN($B$12)*X$20*$B$7,IF(X20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(X20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2.4</v>
+        <v>0.1</v>
       </c>
       <c r="Y21" s="127">
         <f t="shared" ref="Y21" si="17">IF(Y20&lt;ABS($B$12),$B$3+SIGN($B$12)*Y$20*$B$7,IF(Y20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(Y20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2.2999999999999998</v>
+        <v>0.1</v>
       </c>
       <c r="Z21" s="127">
         <f t="shared" ref="Z21" si="18">IF(Z20&lt;ABS($B$12),$B$3+SIGN($B$12)*Z$20*$B$7,IF(Z20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(Z20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2.2000000000000002</v>
+        <v>0.1</v>
       </c>
       <c r="AA21" s="127">
         <f t="shared" ref="AA21" si="19">IF(AA20&lt;ABS($B$12),$B$3+SIGN($B$12)*AA$20*$B$7,IF(AA20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AA20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2.0999999999999996</v>
+        <v>0.1</v>
       </c>
       <c r="AB21" s="127">
         <f t="shared" ref="AB21" si="20">IF(AB20&lt;ABS($B$12),$B$3+SIGN($B$12)*AB$20*$B$7,IF(AB20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AB20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="AC21" s="127">
         <f t="shared" ref="AC21" si="21">IF(AC20&lt;ABS($B$12),$B$3+SIGN($B$12)*AC$20*$B$7,IF(AC20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AC20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="AD21" s="127">
         <f t="shared" ref="AD21" si="22">IF(AD20&lt;ABS($B$12),$B$3+SIGN($B$12)*AD$20*$B$7,IF(AD20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AD20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="AE21" s="127">
         <f t="shared" ref="AE21" si="23">IF(AE20&lt;ABS($B$12),$B$3+SIGN($B$12)*AE$20*$B$7,IF(AE20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AE20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="AF21" s="127">
         <f t="shared" ref="AF21" si="24">IF(AF20&lt;ABS($B$12),$B$3+SIGN($B$12)*AF$20*$B$7,IF(AF20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AF20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="AG21" s="127">
         <f t="shared" ref="AG21" si="25">IF(AG20&lt;ABS($B$12),$B$3+SIGN($B$12)*AG$20*$B$7,IF(AG20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AG20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="AH21" s="127">
         <f t="shared" ref="AH21" si="26">IF(AH20&lt;ABS($B$12),$B$3+SIGN($B$12)*AH$20*$B$7,IF(AH20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AH20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="AI21" s="127">
         <f t="shared" ref="AI21" si="27">IF(AI20&lt;ABS($B$12),$B$3+SIGN($B$12)*AI$20*$B$7,IF(AI20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AI20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="AJ21" s="127">
         <f t="shared" ref="AJ21" si="28">IF(AJ20&lt;ABS($B$12),$B$3+SIGN($B$12)*AJ$20*$B$7,IF(AJ20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AJ20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="AK21" s="127">
         <f t="shared" ref="AK21" si="29">IF(AK20&lt;ABS($B$12),$B$3+SIGN($B$12)*AK$20*$B$7,IF(AK20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AK20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="AL21" s="127">
         <f t="shared" ref="AL21" si="30">IF(AL20&lt;ABS($B$12),$B$3+SIGN($B$12)*AL$20*$B$7,IF(AL20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AL20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="AM21" s="127">
         <f t="shared" ref="AM21" si="31">IF(AM20&lt;ABS($B$12),$B$3+SIGN($B$12)*AM$20*$B$7,IF(AM20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AM20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>1.9</v>
+        <v>0.1</v>
       </c>
       <c r="AN21" s="127">
         <f t="shared" ref="AN21" si="32">IF(AN20&lt;ABS($B$12),$B$3+SIGN($B$12)*AN$20*$B$7,IF(AN20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AN20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>1.8</v>
+        <v>0.1</v>
       </c>
       <c r="AO21" s="127">
         <f t="shared" ref="AO21" si="33">IF(AO20&lt;ABS($B$12),$B$3+SIGN($B$12)*AO$20*$B$7,IF(AO20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AO20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>1.7</v>
+        <v>0.1</v>
       </c>
       <c r="AP21" s="127">
         <f t="shared" ref="AP21" si="34">IF(AP20&lt;ABS($B$12),$B$3+SIGN($B$12)*AP$20*$B$7,IF(AP20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AP20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>1.6</v>
+        <v>0.1</v>
       </c>
       <c r="AQ21" s="127">
         <f t="shared" ref="AQ21" si="35">IF(AQ20&lt;ABS($B$12),$B$3+SIGN($B$12)*AQ$20*$B$7,IF(AQ20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AQ20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>1.5</v>
+        <v>0.1</v>
       </c>
       <c r="AR21" s="127">
         <f t="shared" ref="AR21" si="36">IF(AR20&lt;ABS($B$12),$B$3+SIGN($B$12)*AR$20*$B$7,IF(AR20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AR20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>1.4</v>
+        <v>0.1</v>
       </c>
       <c r="AS21" s="127">
         <f t="shared" ref="AS21" si="37">IF(AS20&lt;ABS($B$12),$B$3+SIGN($B$12)*AS$20*$B$7,IF(AS20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AS20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>1.2999999999999998</v>
+        <v>0.1</v>
       </c>
       <c r="AT21" s="127">
         <f t="shared" ref="AT21" si="38">IF(AT20&lt;ABS($B$12),$B$3+SIGN($B$12)*AT$20*$B$7,IF(AT20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AT20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>1.2</v>
+        <v>0.1</v>
       </c>
       <c r="AU21" s="127">
         <f t="shared" ref="AU21" si="39">IF(AU20&lt;ABS($B$12),$B$3+SIGN($B$12)*AU$20*$B$7,IF(AU20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AU20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>1.1000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="AV21" s="127">
         <f t="shared" ref="AV21" si="40">IF(AV20&lt;ABS($B$12),$B$3+SIGN($B$12)*AV$20*$B$7,IF(AV20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AV20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="AW21" s="127">
         <f t="shared" ref="AW21" si="41">IF(AW20&lt;ABS($B$12),$B$3+SIGN($B$12)*AW$20*$B$7,IF(AW20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AW20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.89999999999999991</v>
+        <v>9.0000000000000011E-2</v>
       </c>
       <c r="AX21" s="127">
         <f t="shared" ref="AX21" si="42">IF(AX20&lt;ABS($B$12),$B$3+SIGN($B$12)*AX$20*$B$7,IF(AX20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AX20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.8</v>
+        <v>0.08</v>
       </c>
       <c r="AY21" s="127">
         <f t="shared" ref="AY21" si="43">IF(AY20&lt;ABS($B$12),$B$3+SIGN($B$12)*AY$20*$B$7,IF(AY20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AY20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.7</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="AZ21" s="127">
         <f t="shared" ref="AZ21" si="44">IF(AZ20&lt;ABS($B$12),$B$3+SIGN($B$12)*AZ$20*$B$7,IF(AZ20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AZ20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.59999999999999987</v>
+        <v>6.0000000000000005E-2</v>
       </c>
       <c r="BA21" s="127">
         <f t="shared" ref="BA21" si="45">IF(BA20&lt;ABS($B$12),$B$3+SIGN($B$12)*BA$20*$B$7,IF(BA20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(BA20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="BB21" s="127">
         <f t="shared" ref="BB21" si="46">IF(BB20&lt;ABS($B$12),$B$3+SIGN($B$12)*BB$20*$B$7,IF(BB20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(BB20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.39999999999999991</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="BC21" s="127">
         <f t="shared" ref="BC21" si="47">IF(BC20&lt;ABS($B$12),$B$3+SIGN($B$12)*BC$20*$B$7,IF(BC20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(BC20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.30000000000000004</v>
+        <v>0.03</v>
       </c>
       <c r="BD21" s="127">
         <f t="shared" ref="BD21" si="48">IF(BD20&lt;ABS($B$12),$B$3+SIGN($B$12)*BD$20*$B$7,IF(BD20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(BD20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.19999999999999996</v>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="BE21" s="127">
         <f t="shared" ref="BE21" si="49">IF(BE20&lt;ABS($B$12),$B$3+SIGN($B$12)*BE$20*$B$7,IF(BE20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(BE20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>9.9999999999999867E-2</v>
+        <v>1.0000000000000009E-2</v>
       </c>
       <c r="BF21" s="127">
         <f t="shared" ref="BF21" si="50">IF(BF20&lt;ABS($B$12),$B$3+SIGN($B$12)*BF$20*$B$7,IF(BF20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(BF20-($B$6-ABS($B$13)))*$B$7))</f>
@@ -33884,410 +33894,410 @@
 IF(I20&lt;$B$19,
 $B$3*$B$18+SIGN($B$12)*0.5*$B$7*$B$18*$B$18+(I20-$B$18)*$B$14,
 $B$3*$B$18+SIGN($B$12)*0.5*$B$7*$B$18*$B$18+($B$19-$B$18)*$B$14 + $B$14*(I20-$B$19) + SIGN($B$13)*0.5*$B$7*(I20-$B$19)*(I20-$B$19)))</f>
-        <v>79</v>
+        <v>3.9</v>
       </c>
       <c r="J22">
         <f t="shared" si="51"/>
-        <v>156</v>
+        <v>7.6</v>
       </c>
       <c r="K22">
         <f t="shared" si="51"/>
-        <v>231</v>
+        <v>11.1</v>
       </c>
       <c r="L22">
         <f t="shared" si="51"/>
-        <v>304</v>
+        <v>14.4</v>
       </c>
       <c r="M22">
         <f t="shared" si="51"/>
-        <v>375</v>
+        <v>17.5</v>
       </c>
       <c r="N22">
         <f t="shared" si="51"/>
-        <v>444</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="O22">
         <f t="shared" si="51"/>
-        <v>511</v>
+        <v>23.1</v>
       </c>
       <c r="P22">
         <f t="shared" si="51"/>
-        <v>576</v>
+        <v>25.6</v>
       </c>
       <c r="Q22">
         <f t="shared" si="51"/>
-        <v>639</v>
+        <v>27.9</v>
       </c>
       <c r="R22">
         <f t="shared" si="51"/>
-        <v>700</v>
+        <v>30</v>
       </c>
       <c r="S22">
         <f t="shared" si="51"/>
-        <v>759</v>
+        <v>32</v>
       </c>
       <c r="T22">
         <f t="shared" si="51"/>
-        <v>816</v>
+        <v>34</v>
       </c>
       <c r="U22">
         <f t="shared" si="51"/>
-        <v>871</v>
+        <v>36</v>
       </c>
       <c r="V22">
         <f t="shared" si="51"/>
-        <v>924</v>
+        <v>38</v>
       </c>
       <c r="W22">
         <f t="shared" si="51"/>
-        <v>975</v>
+        <v>40</v>
       </c>
       <c r="X22">
         <f t="shared" si="51"/>
-        <v>1024</v>
+        <v>42</v>
       </c>
       <c r="Y22">
         <f t="shared" si="51"/>
-        <v>1071</v>
+        <v>44</v>
       </c>
       <c r="Z22">
         <f t="shared" si="51"/>
-        <v>1116</v>
+        <v>46</v>
       </c>
       <c r="AA22">
         <f t="shared" si="51"/>
-        <v>1159</v>
+        <v>48</v>
       </c>
       <c r="AB22">
         <f t="shared" si="51"/>
-        <v>1200</v>
+        <v>50</v>
       </c>
       <c r="AC22">
         <f t="shared" si="51"/>
-        <v>1240</v>
+        <v>52</v>
       </c>
       <c r="AD22">
         <f t="shared" si="51"/>
-        <v>1280</v>
+        <v>54</v>
       </c>
       <c r="AE22">
         <f t="shared" si="51"/>
-        <v>1320</v>
+        <v>56</v>
       </c>
       <c r="AF22">
         <f t="shared" si="51"/>
-        <v>1360</v>
+        <v>58</v>
       </c>
       <c r="AG22">
         <f t="shared" si="51"/>
-        <v>1400</v>
+        <v>60</v>
       </c>
       <c r="AH22">
         <f t="shared" si="51"/>
-        <v>1440</v>
+        <v>62</v>
       </c>
       <c r="AI22">
         <f t="shared" si="51"/>
-        <v>1480</v>
+        <v>64</v>
       </c>
       <c r="AJ22">
         <f t="shared" si="51"/>
-        <v>1520</v>
+        <v>66</v>
       </c>
       <c r="AK22">
         <f t="shared" si="51"/>
-        <v>1560</v>
+        <v>68</v>
       </c>
       <c r="AL22">
         <f t="shared" si="51"/>
-        <v>1600</v>
+        <v>70</v>
       </c>
       <c r="AM22">
         <f t="shared" si="51"/>
-        <v>1639</v>
+        <v>72</v>
       </c>
       <c r="AN22">
         <f t="shared" si="51"/>
-        <v>1676</v>
+        <v>74</v>
       </c>
       <c r="AO22">
         <f t="shared" si="51"/>
-        <v>1711</v>
+        <v>76</v>
       </c>
       <c r="AP22">
         <f t="shared" si="51"/>
-        <v>1744</v>
+        <v>78</v>
       </c>
       <c r="AQ22">
         <f t="shared" si="51"/>
-        <v>1775</v>
+        <v>80</v>
       </c>
       <c r="AR22">
         <f t="shared" si="51"/>
-        <v>1804</v>
+        <v>82</v>
       </c>
       <c r="AS22">
         <f t="shared" si="51"/>
-        <v>1831</v>
+        <v>84</v>
       </c>
       <c r="AT22">
         <f t="shared" si="51"/>
-        <v>1856</v>
+        <v>86</v>
       </c>
       <c r="AU22">
         <f t="shared" si="51"/>
-        <v>1879</v>
+        <v>88</v>
       </c>
       <c r="AV22">
         <f t="shared" si="51"/>
-        <v>1900</v>
+        <v>90</v>
       </c>
       <c r="AW22">
         <f t="shared" si="51"/>
-        <v>1919</v>
+        <v>91.9</v>
       </c>
       <c r="AX22">
         <f t="shared" si="51"/>
-        <v>1936</v>
+        <v>93.6</v>
       </c>
       <c r="AY22">
         <f t="shared" si="51"/>
-        <v>1951</v>
+        <v>95.1</v>
       </c>
       <c r="AZ22">
         <f t="shared" si="51"/>
-        <v>1964</v>
+        <v>96.4</v>
       </c>
       <c r="BA22">
         <f t="shared" si="51"/>
-        <v>1975</v>
+        <v>97.5</v>
       </c>
       <c r="BB22">
         <f t="shared" si="51"/>
-        <v>1984</v>
+        <v>98.4</v>
       </c>
       <c r="BC22">
         <f t="shared" si="51"/>
-        <v>1991</v>
+        <v>99.1</v>
       </c>
       <c r="BD22">
         <f t="shared" si="51"/>
-        <v>1996</v>
+        <v>99.6</v>
       </c>
       <c r="BE22">
         <f t="shared" si="51"/>
-        <v>1999</v>
+        <v>99.9</v>
       </c>
       <c r="BF22">
         <f t="shared" si="51"/>
-        <v>2000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:70" x14ac:dyDescent="0.3">
       <c r="B23" s="58"/>
       <c r="H23">
         <f>$B$3*$B$18+0.5*$B$7*$B$18*$B$18+(H20-ABS($B$12))*$B$14</f>
-        <v>1200</v>
+        <v>30</v>
       </c>
       <c r="I23">
         <f t="shared" ref="I23:BF23" si="52">$B$3*ABS($B$12)+0.5*$B$7*ABS($B$12)*ABS($B$12)+(I20-ABS($B$12))*$B$14</f>
-        <v>1240</v>
+        <v>32</v>
       </c>
       <c r="J23">
         <f t="shared" si="52"/>
-        <v>1280</v>
+        <v>34</v>
       </c>
       <c r="K23">
         <f t="shared" si="52"/>
-        <v>1320</v>
+        <v>36</v>
       </c>
       <c r="L23">
         <f t="shared" si="52"/>
-        <v>1360</v>
+        <v>38</v>
       </c>
       <c r="M23">
         <f t="shared" si="52"/>
-        <v>1400</v>
+        <v>40</v>
       </c>
       <c r="N23">
         <f t="shared" si="52"/>
-        <v>1440</v>
+        <v>42</v>
       </c>
       <c r="O23">
         <f t="shared" si="52"/>
-        <v>1480</v>
+        <v>44</v>
       </c>
       <c r="P23">
         <f t="shared" si="52"/>
-        <v>1520</v>
+        <v>46</v>
       </c>
       <c r="Q23">
         <f t="shared" si="52"/>
-        <v>1560</v>
+        <v>48</v>
       </c>
       <c r="R23">
         <f t="shared" si="52"/>
-        <v>1600</v>
+        <v>50</v>
       </c>
       <c r="S23">
         <f t="shared" si="52"/>
-        <v>1640</v>
+        <v>52</v>
       </c>
       <c r="T23">
         <f t="shared" si="52"/>
-        <v>1680</v>
+        <v>54</v>
       </c>
       <c r="U23">
         <f t="shared" si="52"/>
-        <v>1720</v>
+        <v>56</v>
       </c>
       <c r="V23">
         <f t="shared" si="52"/>
-        <v>1760</v>
+        <v>58</v>
       </c>
       <c r="W23">
         <f t="shared" si="52"/>
-        <v>1800</v>
+        <v>60</v>
       </c>
       <c r="X23">
         <f t="shared" si="52"/>
-        <v>1840</v>
+        <v>62</v>
       </c>
       <c r="Y23">
         <f t="shared" si="52"/>
-        <v>1880</v>
+        <v>64</v>
       </c>
       <c r="Z23">
         <f t="shared" si="52"/>
-        <v>1920</v>
+        <v>66</v>
       </c>
       <c r="AA23">
         <f t="shared" si="52"/>
-        <v>1960</v>
+        <v>68</v>
       </c>
       <c r="AB23">
         <f t="shared" si="52"/>
-        <v>2000</v>
+        <v>70</v>
       </c>
       <c r="AC23">
         <f t="shared" si="52"/>
-        <v>2040</v>
+        <v>72</v>
       </c>
       <c r="AD23">
         <f t="shared" si="52"/>
-        <v>2080</v>
+        <v>74</v>
       </c>
       <c r="AE23">
         <f t="shared" si="52"/>
-        <v>2120</v>
+        <v>76</v>
       </c>
       <c r="AF23">
         <f t="shared" si="52"/>
-        <v>2160</v>
+        <v>78</v>
       </c>
       <c r="AG23">
         <f t="shared" si="52"/>
-        <v>2200</v>
+        <v>80</v>
       </c>
       <c r="AH23">
         <f t="shared" si="52"/>
-        <v>2240</v>
+        <v>82</v>
       </c>
       <c r="AI23">
         <f t="shared" si="52"/>
-        <v>2280</v>
+        <v>84</v>
       </c>
       <c r="AJ23">
         <f t="shared" si="52"/>
-        <v>2320</v>
+        <v>86</v>
       </c>
       <c r="AK23">
         <f t="shared" si="52"/>
-        <v>2360</v>
+        <v>88</v>
       </c>
       <c r="AL23">
         <f t="shared" si="52"/>
-        <v>2400</v>
+        <v>90</v>
       </c>
       <c r="AM23">
         <f t="shared" si="52"/>
-        <v>2440</v>
+        <v>92</v>
       </c>
       <c r="AN23">
         <f t="shared" si="52"/>
-        <v>2480</v>
+        <v>94</v>
       </c>
       <c r="AO23">
         <f t="shared" si="52"/>
-        <v>2520</v>
+        <v>96</v>
       </c>
       <c r="AP23">
         <f t="shared" si="52"/>
-        <v>2560</v>
+        <v>98</v>
       </c>
       <c r="AQ23">
         <f t="shared" si="52"/>
-        <v>2600</v>
+        <v>100</v>
       </c>
       <c r="AR23">
         <f t="shared" si="52"/>
-        <v>2640</v>
+        <v>102</v>
       </c>
       <c r="AS23">
         <f t="shared" si="52"/>
-        <v>2680</v>
+        <v>104</v>
       </c>
       <c r="AT23">
         <f t="shared" si="52"/>
-        <v>2720</v>
+        <v>106</v>
       </c>
       <c r="AU23">
         <f t="shared" si="52"/>
-        <v>2760</v>
+        <v>108</v>
       </c>
       <c r="AV23">
         <f t="shared" si="52"/>
-        <v>2800</v>
+        <v>110</v>
       </c>
       <c r="AW23">
         <f t="shared" si="52"/>
-        <v>2840</v>
+        <v>112</v>
       </c>
       <c r="AX23">
         <f t="shared" si="52"/>
-        <v>2880</v>
+        <v>114</v>
       </c>
       <c r="AY23">
         <f t="shared" si="52"/>
-        <v>2920</v>
+        <v>116</v>
       </c>
       <c r="AZ23">
         <f t="shared" si="52"/>
-        <v>2960</v>
+        <v>118</v>
       </c>
       <c r="BA23">
         <f t="shared" si="52"/>
-        <v>3000</v>
+        <v>120</v>
       </c>
       <c r="BB23">
         <f t="shared" si="52"/>
-        <v>3040</v>
+        <v>122</v>
       </c>
       <c r="BC23">
         <f t="shared" si="52"/>
-        <v>3080</v>
+        <v>124</v>
       </c>
       <c r="BD23">
         <f t="shared" si="52"/>
-        <v>3120</v>
+        <v>126</v>
       </c>
       <c r="BE23">
         <f t="shared" si="52"/>
-        <v>3160</v>
+        <v>128</v>
       </c>
       <c r="BF23">
         <f t="shared" si="52"/>
-        <v>3200</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:70" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix in speed profile
</commit_message>
<xml_diff>
--- a/theory/Kinematik.xlsx
+++ b/theory/Kinematik.xlsx
@@ -1753,11 +1753,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="330255024"/>
-        <c:axId val="330252672"/>
+        <c:axId val="339422008"/>
+        <c:axId val="339425536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="330255024"/>
+        <c:axId val="339422008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1795,13 +1795,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="330252672"/>
+        <c:crossAx val="339425536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="330252672"/>
+        <c:axId val="339425536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1840,7 +1840,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="330255024"/>
+        <c:crossAx val="339422008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
@@ -1936,11 +1936,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="330248360"/>
-        <c:axId val="330251496"/>
+        <c:axId val="339420048"/>
+        <c:axId val="339425928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="330248360"/>
+        <c:axId val="339420048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -1952,13 +1952,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="330251496"/>
+        <c:crossAx val="339425928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="330251496"/>
+        <c:axId val="339425928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -1971,7 +1971,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="330248360"/>
+        <c:crossAx val="339420048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
@@ -2112,10 +2112,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>183.33333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>800</c:v>
+                  <c:v>983.33333333333337</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
                   <c:v>1000</c:v>
@@ -2130,16 +2130,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0.2</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2154,11 +2154,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="330247968"/>
-        <c:axId val="330253064"/>
+        <c:axId val="339422400"/>
+        <c:axId val="339419656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="330247968"/>
+        <c:axId val="339422400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2201,12 +2201,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330253064"/>
+        <c:crossAx val="339419656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="330253064"/>
+        <c:axId val="339419656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2257,7 +2257,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330247968"/>
+        <c:crossAx val="339422400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2625,157 +2625,157 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>0.2</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19</c:v>
+                  <c:v>0.27999999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.18000000000000002</c:v>
+                  <c:v>0.26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.16</c:v>
+                  <c:v>0.21999999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.15000000000000002</c:v>
+                  <c:v>0.19999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.13</c:v>
+                  <c:v>0.15999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.12000000000000001</c:v>
+                  <c:v>0.13999999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.11000000000000001</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.1</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>9.0000000000000011E-2</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.08</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>6.0000000000000005E-2</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.05</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4.0000000000000008E-2</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.03</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.0000000000000004E-2</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.0000000000000009E-2</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2790,11 +2790,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="330254632"/>
-        <c:axId val="330248752"/>
+        <c:axId val="339427104"/>
+        <c:axId val="339423968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="330254632"/>
+        <c:axId val="339427104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2845,12 +2845,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330248752"/>
+        <c:crossAx val="339423968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="330248752"/>
+        <c:axId val="339423968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2901,7 +2901,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330254632"/>
+        <c:crossAx val="339427104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3295,154 +3295,154 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.9</c:v>
+                  <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.6</c:v>
+                  <c:v>11.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.1</c:v>
+                  <c:v>16.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.4</c:v>
+                  <c:v>20.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.5</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.399999999999999</c:v>
+                  <c:v>28.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.1</c:v>
+                  <c:v>32.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25.6</c:v>
+                  <c:v>35.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27.9</c:v>
+                  <c:v>37.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>30</c:v>
+                  <c:v>40.138888888888886</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32</c:v>
+                  <c:v>42.472222222222221</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34</c:v>
+                  <c:v>44.80555555555555</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36</c:v>
+                  <c:v>47.138888888888886</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>38</c:v>
+                  <c:v>49.472222222222214</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>40</c:v>
+                  <c:v>51.80555555555555</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>42</c:v>
+                  <c:v>54.138888888888886</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44</c:v>
+                  <c:v>56.472222222222214</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>46</c:v>
+                  <c:v>58.80555555555555</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>48</c:v>
+                  <c:v>61.138888888888886</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>50</c:v>
+                  <c:v>63.472222222222214</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>52</c:v>
+                  <c:v>65.805555555555543</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>54</c:v>
+                  <c:v>68.138888888888872</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>56</c:v>
+                  <c:v>70.4722222222222</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>58</c:v>
+                  <c:v>72.805555555555543</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>60</c:v>
+                  <c:v>75.138888888888872</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>62</c:v>
+                  <c:v>77.4722222222222</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>64</c:v>
+                  <c:v>79.805555555555543</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>66</c:v>
+                  <c:v>82.138888888888872</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>68</c:v>
+                  <c:v>84.4722222222222</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>70</c:v>
+                  <c:v>86.805555555555543</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>72</c:v>
+                  <c:v>89.138888888888872</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>74</c:v>
+                  <c:v>91.4722222222222</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>76</c:v>
+                  <c:v>93.805555555555543</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>78</c:v>
+                  <c:v>96.138888888888872</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>80</c:v>
+                  <c:v>98.4722222222222</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>82</c:v>
+                  <c:v>100.80555555555554</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>84</c:v>
+                  <c:v>103.13888888888887</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>86</c:v>
+                  <c:v>105.4722222222222</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>88</c:v>
+                  <c:v>107.80555555555553</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>90</c:v>
+                  <c:v>110.13888888888887</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>91.9</c:v>
+                  <c:v>112.4722222222222</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>93.6</c:v>
+                  <c:v>114.80555555555553</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>95.1</c:v>
+                  <c:v>117.13888888888887</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>96.4</c:v>
+                  <c:v>119.4722222222222</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>97.5</c:v>
+                  <c:v>121.80555555555553</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>98.4</c:v>
+                  <c:v>124.13888888888886</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>99.1</c:v>
+                  <c:v>126.4722222222222</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>99.6</c:v>
+                  <c:v>128.80555555555554</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>99.9</c:v>
+                  <c:v>131.13888888888886</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>100</c:v>
+                  <c:v>133.33333333333331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3457,11 +3457,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="316250016"/>
-        <c:axId val="316253936"/>
+        <c:axId val="339424752"/>
+        <c:axId val="339425144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="316250016"/>
+        <c:axId val="339424752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3517,12 +3517,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316253936"/>
+        <c:crossAx val="339425144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="316253936"/>
+        <c:axId val="339425144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3578,7 +3578,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316250016"/>
+        <c:crossAx val="339424752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -30177,7 +30177,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="21">
-        <f>RADIANS(B15)</f>
+        <f t="shared" ref="C15:C20" si="0">RADIANS(B15)</f>
         <v>5.235987755982989E-2</v>
       </c>
       <c r="E15" s="20">
@@ -30200,7 +30200,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="21">
-        <f t="shared" ref="C16:C20" si="0">RADIANS(B16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D16" s="106">
@@ -30554,7 +30554,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="3">
-        <f t="shared" ref="D28" si="1">RADIANS(C28)</f>
+        <f>RADIANS(C28)</f>
         <v>0</v>
       </c>
       <c r="E28">
@@ -33217,7 +33217,7 @@
   <dimension ref="A1:BR24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33235,7 +33235,7 @@
         <v>85</v>
       </c>
       <c r="B3">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="C3" t="s">
         <v>87</v>
@@ -33246,7 +33246,7 @@
         <v>86</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C4" t="s">
         <v>87</v>
@@ -33262,6 +33262,10 @@
       <c r="C5" t="s">
         <v>91</v>
       </c>
+      <c r="D5">
+        <f>$B$3*$B$18+SIGN($B$12)*0.5*$B$7*$B$18*$B$18+($B$19-$B$18)*$B$14 + $B$14*(B6-$B$19) + SIGN($B$13)*0.5*$B$7*(B6-$B$19)*(B6-$B$19)</f>
+        <v>133.33333333333331</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -33279,7 +33283,7 @@
         <v>71</v>
       </c>
       <c r="B7">
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="C7" t="s">
         <v>95</v>
@@ -33306,11 +33310,11 @@
       </c>
       <c r="I11" s="4">
         <f>ABS(B12)</f>
-        <v>200</v>
+        <v>183.33333333333334</v>
       </c>
       <c r="J11" s="3">
         <f>B6-ABS(B13)</f>
-        <v>800</v>
+        <v>983.33333333333337</v>
       </c>
       <c r="K11">
         <f>B6</f>
@@ -33323,33 +33327,33 @@
       </c>
       <c r="B12" s="127">
         <f>(B5- B3*B6 - 0.5*(B4-B3)*(B4-B3)/B7) / ( B7*B6 + B3 - B4)</f>
-        <v>-200</v>
+        <v>-183.33333333333334</v>
       </c>
       <c r="C12" t="s">
         <v>92</v>
       </c>
       <c r="D12">
         <f>(B5 - B3*B6 - 0.5*(B4-B3)*(B4-B3)/B7) / ( B7*B6 - B3 - B4)</f>
-        <v>-466.66666666666669</v>
+        <v>-366.66666666666669</v>
       </c>
       <c r="G12" t="s">
         <v>84</v>
       </c>
       <c r="H12">
         <f>B3</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="I12" s="3">
         <f>B14</f>
-        <v>0.1</v>
+        <v>0.11666666666666664</v>
       </c>
       <c r="J12" s="3">
         <f>I12</f>
-        <v>0.1</v>
+        <v>0.11666666666666664</v>
       </c>
       <c r="K12">
         <f>B4</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
@@ -33358,7 +33362,7 @@
       </c>
       <c r="B13" s="3">
         <f>(B4-B3)/B7-B12</f>
-        <v>-200</v>
+        <v>-16.666666666666629</v>
       </c>
       <c r="C13" t="s">
         <v>92</v>
@@ -33371,14 +33375,10 @@
       </c>
       <c r="B14" s="3">
         <f>B3+B7*B12</f>
-        <v>0.1</v>
+        <v>0.11666666666666664</v>
       </c>
       <c r="C14" t="s">
         <v>87</v>
-      </c>
-      <c r="D14">
-        <f>$B$3*$B$18+SIGN($B$12)*0.5*$B$7*$B$18*$B$18+($B$19-$B$18)*$B$14 + $B$14*(B6-$B$19) + SIGN($B$13)*0.5*$B$7*(B6-$B$19)*(B6-$B$19)</f>
-        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -33387,7 +33387,7 @@
       </c>
       <c r="B15" s="127">
         <f>(B3+B14)/2*B12+B14*(B6-B12-B13)+(B14+B4)/2*B13</f>
-        <v>100</v>
+        <v>99.999999999999972</v>
       </c>
       <c r="C15" t="s">
         <v>91</v>
@@ -33399,7 +33399,7 @@
       </c>
       <c r="B16">
         <f>B14+B13*B7</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C16" t="s">
         <v>87</v>
@@ -33411,7 +33411,7 @@
       </c>
       <c r="B18" s="127">
         <f>ABS(B12)</f>
-        <v>200</v>
+        <v>183.33333333333334</v>
       </c>
       <c r="C18" t="s">
         <v>92</v>
@@ -33423,7 +33423,7 @@
       </c>
       <c r="B19" s="127">
         <f>B6-ABS(B13)</f>
-        <v>800</v>
+        <v>983.33333333333337</v>
       </c>
       <c r="C19" t="s">
         <v>92</v>
@@ -33654,208 +33654,208 @@
         <v>107</v>
       </c>
       <c r="H21" s="127">
-        <f>IF(H20&lt;ABS($B$12),$B$3+SIGN($B$12)*H$20*$B$7,IF(H20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(H20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.2</v>
+        <f t="shared" ref="H21:AM21" si="1">IF(H20&lt;ABS($B$12),$B$3+SIGN($B$12)*H$20*$B$7,IF(H20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(H20-($B$6-ABS($B$13)))*$B$7))</f>
+        <v>0.3</v>
       </c>
       <c r="I21" s="127">
-        <f t="shared" ref="I21" si="1">IF(I20&lt;ABS($B$12),$B$3+SIGN($B$12)*I$20*$B$7,IF(I20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(I20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.19</v>
+        <f t="shared" si="1"/>
+        <v>0.27999999999999997</v>
       </c>
       <c r="J21" s="127">
-        <f t="shared" ref="J21" si="2">IF(J20&lt;ABS($B$12),$B$3+SIGN($B$12)*J$20*$B$7,IF(J20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(J20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.18000000000000002</v>
+        <f t="shared" si="1"/>
+        <v>0.26</v>
       </c>
       <c r="K21" s="127">
-        <f t="shared" ref="K21" si="3">IF(K20&lt;ABS($B$12),$B$3+SIGN($B$12)*K$20*$B$7,IF(K20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(K20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.17</v>
+        <f t="shared" si="1"/>
+        <v>0.24</v>
       </c>
       <c r="L21" s="127">
-        <f t="shared" ref="L21" si="4">IF(L20&lt;ABS($B$12),$B$3+SIGN($B$12)*L$20*$B$7,IF(L20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(L20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.16</v>
+        <f t="shared" si="1"/>
+        <v>0.21999999999999997</v>
       </c>
       <c r="M21" s="127">
-        <f t="shared" ref="M21" si="5">IF(M20&lt;ABS($B$12),$B$3+SIGN($B$12)*M$20*$B$7,IF(M20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(M20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.15000000000000002</v>
+        <f t="shared" si="1"/>
+        <v>0.19999999999999998</v>
       </c>
       <c r="N21" s="127">
-        <f t="shared" ref="N21" si="6">IF(N20&lt;ABS($B$12),$B$3+SIGN($B$12)*N$20*$B$7,IF(N20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(N20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.14000000000000001</v>
+        <f t="shared" si="1"/>
+        <v>0.18</v>
       </c>
       <c r="O21" s="127">
-        <f t="shared" ref="O21" si="7">IF(O20&lt;ABS($B$12),$B$3+SIGN($B$12)*O$20*$B$7,IF(O20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(O20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.13</v>
+        <f t="shared" si="1"/>
+        <v>0.15999999999999998</v>
       </c>
       <c r="P21" s="127">
-        <f t="shared" ref="P21" si="8">IF(P20&lt;ABS($B$12),$B$3+SIGN($B$12)*P$20*$B$7,IF(P20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(P20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.12000000000000001</v>
+        <f t="shared" si="1"/>
+        <v>0.13999999999999999</v>
       </c>
       <c r="Q21" s="127">
-        <f t="shared" ref="Q21" si="9">IF(Q20&lt;ABS($B$12),$B$3+SIGN($B$12)*Q$20*$B$7,IF(Q20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(Q20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.11000000000000001</v>
+        <f t="shared" si="1"/>
+        <v>0.12</v>
       </c>
       <c r="R21" s="127">
-        <f t="shared" ref="R21" si="10">IF(R20&lt;ABS($B$12),$B$3+SIGN($B$12)*R$20*$B$7,IF(R20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(R20-($B$6-ABS($B$13)))*$B$7))</f>
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="S21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="T21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="U21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="V21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="W21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="X21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="Y21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="Z21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AA21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AB21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AC21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AD21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AE21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AF21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AG21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AH21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AI21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AJ21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AK21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AL21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AM21" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AN21" s="127">
+        <f t="shared" ref="AN21:BS21" si="2">IF(AN20&lt;ABS($B$12),$B$3+SIGN($B$12)*AN$20*$B$7,IF(AN20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AN20-($B$6-ABS($B$13)))*$B$7))</f>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AO21" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AP21" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AQ21" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AR21" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AS21" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AT21" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AU21" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AV21" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AW21" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AX21" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AY21" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="AZ21" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="BA21" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="BB21" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="BC21" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="BD21" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="BE21" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11666666666666664</v>
+      </c>
+      <c r="BF21" s="127">
+        <f t="shared" si="2"/>
         <v>0.1</v>
-      </c>
-      <c r="S21" s="127">
-        <f t="shared" ref="S21" si="11">IF(S20&lt;ABS($B$12),$B$3+SIGN($B$12)*S$20*$B$7,IF(S20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(S20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="T21" s="127">
-        <f t="shared" ref="T21" si="12">IF(T20&lt;ABS($B$12),$B$3+SIGN($B$12)*T$20*$B$7,IF(T20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(T20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="U21" s="127">
-        <f t="shared" ref="U21" si="13">IF(U20&lt;ABS($B$12),$B$3+SIGN($B$12)*U$20*$B$7,IF(U20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(U20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="V21" s="127">
-        <f t="shared" ref="V21" si="14">IF(V20&lt;ABS($B$12),$B$3+SIGN($B$12)*V$20*$B$7,IF(V20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(V20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="W21" s="127">
-        <f t="shared" ref="W21" si="15">IF(W20&lt;ABS($B$12),$B$3+SIGN($B$12)*W$20*$B$7,IF(W20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(W20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="X21" s="127">
-        <f t="shared" ref="X21" si="16">IF(X20&lt;ABS($B$12),$B$3+SIGN($B$12)*X$20*$B$7,IF(X20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(X20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="Y21" s="127">
-        <f t="shared" ref="Y21" si="17">IF(Y20&lt;ABS($B$12),$B$3+SIGN($B$12)*Y$20*$B$7,IF(Y20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(Y20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="Z21" s="127">
-        <f t="shared" ref="Z21" si="18">IF(Z20&lt;ABS($B$12),$B$3+SIGN($B$12)*Z$20*$B$7,IF(Z20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(Z20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AA21" s="127">
-        <f t="shared" ref="AA21" si="19">IF(AA20&lt;ABS($B$12),$B$3+SIGN($B$12)*AA$20*$B$7,IF(AA20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AA20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AB21" s="127">
-        <f t="shared" ref="AB21" si="20">IF(AB20&lt;ABS($B$12),$B$3+SIGN($B$12)*AB$20*$B$7,IF(AB20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AB20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AC21" s="127">
-        <f t="shared" ref="AC21" si="21">IF(AC20&lt;ABS($B$12),$B$3+SIGN($B$12)*AC$20*$B$7,IF(AC20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AC20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AD21" s="127">
-        <f t="shared" ref="AD21" si="22">IF(AD20&lt;ABS($B$12),$B$3+SIGN($B$12)*AD$20*$B$7,IF(AD20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AD20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AE21" s="127">
-        <f t="shared" ref="AE21" si="23">IF(AE20&lt;ABS($B$12),$B$3+SIGN($B$12)*AE$20*$B$7,IF(AE20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AE20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AF21" s="127">
-        <f t="shared" ref="AF21" si="24">IF(AF20&lt;ABS($B$12),$B$3+SIGN($B$12)*AF$20*$B$7,IF(AF20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AF20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AG21" s="127">
-        <f t="shared" ref="AG21" si="25">IF(AG20&lt;ABS($B$12),$B$3+SIGN($B$12)*AG$20*$B$7,IF(AG20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AG20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AH21" s="127">
-        <f t="shared" ref="AH21" si="26">IF(AH20&lt;ABS($B$12),$B$3+SIGN($B$12)*AH$20*$B$7,IF(AH20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AH20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AI21" s="127">
-        <f t="shared" ref="AI21" si="27">IF(AI20&lt;ABS($B$12),$B$3+SIGN($B$12)*AI$20*$B$7,IF(AI20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AI20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AJ21" s="127">
-        <f t="shared" ref="AJ21" si="28">IF(AJ20&lt;ABS($B$12),$B$3+SIGN($B$12)*AJ$20*$B$7,IF(AJ20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AJ20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AK21" s="127">
-        <f t="shared" ref="AK21" si="29">IF(AK20&lt;ABS($B$12),$B$3+SIGN($B$12)*AK$20*$B$7,IF(AK20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AK20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AL21" s="127">
-        <f t="shared" ref="AL21" si="30">IF(AL20&lt;ABS($B$12),$B$3+SIGN($B$12)*AL$20*$B$7,IF(AL20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AL20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AM21" s="127">
-        <f t="shared" ref="AM21" si="31">IF(AM20&lt;ABS($B$12),$B$3+SIGN($B$12)*AM$20*$B$7,IF(AM20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AM20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AN21" s="127">
-        <f t="shared" ref="AN21" si="32">IF(AN20&lt;ABS($B$12),$B$3+SIGN($B$12)*AN$20*$B$7,IF(AN20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AN20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AO21" s="127">
-        <f t="shared" ref="AO21" si="33">IF(AO20&lt;ABS($B$12),$B$3+SIGN($B$12)*AO$20*$B$7,IF(AO20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AO20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AP21" s="127">
-        <f t="shared" ref="AP21" si="34">IF(AP20&lt;ABS($B$12),$B$3+SIGN($B$12)*AP$20*$B$7,IF(AP20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AP20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AQ21" s="127">
-        <f t="shared" ref="AQ21" si="35">IF(AQ20&lt;ABS($B$12),$B$3+SIGN($B$12)*AQ$20*$B$7,IF(AQ20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AQ20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AR21" s="127">
-        <f t="shared" ref="AR21" si="36">IF(AR20&lt;ABS($B$12),$B$3+SIGN($B$12)*AR$20*$B$7,IF(AR20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AR20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AS21" s="127">
-        <f t="shared" ref="AS21" si="37">IF(AS20&lt;ABS($B$12),$B$3+SIGN($B$12)*AS$20*$B$7,IF(AS20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AS20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AT21" s="127">
-        <f t="shared" ref="AT21" si="38">IF(AT20&lt;ABS($B$12),$B$3+SIGN($B$12)*AT$20*$B$7,IF(AT20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AT20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AU21" s="127">
-        <f t="shared" ref="AU21" si="39">IF(AU20&lt;ABS($B$12),$B$3+SIGN($B$12)*AU$20*$B$7,IF(AU20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AU20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AV21" s="127">
-        <f t="shared" ref="AV21" si="40">IF(AV20&lt;ABS($B$12),$B$3+SIGN($B$12)*AV$20*$B$7,IF(AV20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AV20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.1</v>
-      </c>
-      <c r="AW21" s="127">
-        <f t="shared" ref="AW21" si="41">IF(AW20&lt;ABS($B$12),$B$3+SIGN($B$12)*AW$20*$B$7,IF(AW20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AW20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>9.0000000000000011E-2</v>
-      </c>
-      <c r="AX21" s="127">
-        <f t="shared" ref="AX21" si="42">IF(AX20&lt;ABS($B$12),$B$3+SIGN($B$12)*AX$20*$B$7,IF(AX20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AX20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.08</v>
-      </c>
-      <c r="AY21" s="127">
-        <f t="shared" ref="AY21" si="43">IF(AY20&lt;ABS($B$12),$B$3+SIGN($B$12)*AY$20*$B$7,IF(AY20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AY20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AZ21" s="127">
-        <f t="shared" ref="AZ21" si="44">IF(AZ20&lt;ABS($B$12),$B$3+SIGN($B$12)*AZ$20*$B$7,IF(AZ20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AZ20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>6.0000000000000005E-2</v>
-      </c>
-      <c r="BA21" s="127">
-        <f t="shared" ref="BA21" si="45">IF(BA20&lt;ABS($B$12),$B$3+SIGN($B$12)*BA$20*$B$7,IF(BA20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(BA20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.05</v>
-      </c>
-      <c r="BB21" s="127">
-        <f t="shared" ref="BB21" si="46">IF(BB20&lt;ABS($B$12),$B$3+SIGN($B$12)*BB$20*$B$7,IF(BB20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(BB20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>4.0000000000000008E-2</v>
-      </c>
-      <c r="BC21" s="127">
-        <f t="shared" ref="BC21" si="47">IF(BC20&lt;ABS($B$12),$B$3+SIGN($B$12)*BC$20*$B$7,IF(BC20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(BC20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.03</v>
-      </c>
-      <c r="BD21" s="127">
-        <f t="shared" ref="BD21" si="48">IF(BD20&lt;ABS($B$12),$B$3+SIGN($B$12)*BD$20*$B$7,IF(BD20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(BD20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>2.0000000000000004E-2</v>
-      </c>
-      <c r="BE21" s="127">
-        <f t="shared" ref="BE21" si="49">IF(BE20&lt;ABS($B$12),$B$3+SIGN($B$12)*BE$20*$B$7,IF(BE20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(BE20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>1.0000000000000009E-2</v>
-      </c>
-      <c r="BF21" s="127">
-        <f t="shared" ref="BF21" si="50">IF(BF20&lt;ABS($B$12),$B$3+SIGN($B$12)*BF$20*$B$7,IF(BF20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(BF20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0</v>
       </c>
       <c r="BG21" s="127"/>
       <c r="BH21" s="127"/>
@@ -33889,415 +33889,415 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <f t="shared" ref="I22:BF22" si="51">IF(I20&lt;$B$18,
+        <f t="shared" ref="I22:BF22" si="3">IF(I20&lt;$B$18,
 $B$3*I20+SIGN($B$12)*0.5*$B$7*I20*I20,
 IF(I20&lt;$B$19,
 $B$3*$B$18+SIGN($B$12)*0.5*$B$7*$B$18*$B$18+(I20-$B$18)*$B$14,
 $B$3*$B$18+SIGN($B$12)*0.5*$B$7*$B$18*$B$18+($B$19-$B$18)*$B$14 + $B$14*(I20-$B$19) + SIGN($B$13)*0.5*$B$7*(I20-$B$19)*(I20-$B$19)))</f>
-        <v>3.9</v>
+        <v>5.8</v>
       </c>
       <c r="J22">
-        <f t="shared" si="51"/>
-        <v>7.6</v>
+        <f t="shared" si="3"/>
+        <v>11.2</v>
       </c>
       <c r="K22">
-        <f t="shared" si="51"/>
-        <v>11.1</v>
+        <f t="shared" si="3"/>
+        <v>16.2</v>
       </c>
       <c r="L22">
-        <f t="shared" si="51"/>
-        <v>14.4</v>
+        <f t="shared" si="3"/>
+        <v>20.8</v>
       </c>
       <c r="M22">
-        <f t="shared" si="51"/>
-        <v>17.5</v>
+        <f t="shared" si="3"/>
+        <v>25</v>
       </c>
       <c r="N22">
-        <f t="shared" si="51"/>
-        <v>20.399999999999999</v>
+        <f t="shared" si="3"/>
+        <v>28.8</v>
       </c>
       <c r="O22">
-        <f t="shared" si="51"/>
-        <v>23.1</v>
+        <f t="shared" si="3"/>
+        <v>32.200000000000003</v>
       </c>
       <c r="P22">
-        <f t="shared" si="51"/>
-        <v>25.6</v>
+        <f t="shared" si="3"/>
+        <v>35.200000000000003</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="51"/>
-        <v>27.9</v>
+        <f t="shared" si="3"/>
+        <v>37.799999999999997</v>
       </c>
       <c r="R22">
-        <f t="shared" si="51"/>
-        <v>30</v>
+        <f t="shared" si="3"/>
+        <v>40.138888888888886</v>
       </c>
       <c r="S22">
-        <f t="shared" si="51"/>
-        <v>32</v>
+        <f t="shared" si="3"/>
+        <v>42.472222222222221</v>
       </c>
       <c r="T22">
-        <f t="shared" si="51"/>
-        <v>34</v>
+        <f t="shared" si="3"/>
+        <v>44.80555555555555</v>
       </c>
       <c r="U22">
-        <f t="shared" si="51"/>
-        <v>36</v>
+        <f t="shared" si="3"/>
+        <v>47.138888888888886</v>
       </c>
       <c r="V22">
-        <f t="shared" si="51"/>
-        <v>38</v>
+        <f t="shared" si="3"/>
+        <v>49.472222222222214</v>
       </c>
       <c r="W22">
-        <f t="shared" si="51"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>51.80555555555555</v>
       </c>
       <c r="X22">
-        <f t="shared" si="51"/>
-        <v>42</v>
+        <f t="shared" si="3"/>
+        <v>54.138888888888886</v>
       </c>
       <c r="Y22">
-        <f t="shared" si="51"/>
-        <v>44</v>
+        <f t="shared" si="3"/>
+        <v>56.472222222222214</v>
       </c>
       <c r="Z22">
-        <f t="shared" si="51"/>
-        <v>46</v>
+        <f t="shared" si="3"/>
+        <v>58.80555555555555</v>
       </c>
       <c r="AA22">
-        <f t="shared" si="51"/>
-        <v>48</v>
+        <f t="shared" si="3"/>
+        <v>61.138888888888886</v>
       </c>
       <c r="AB22">
-        <f t="shared" si="51"/>
-        <v>50</v>
+        <f t="shared" si="3"/>
+        <v>63.472222222222214</v>
       </c>
       <c r="AC22">
-        <f t="shared" si="51"/>
-        <v>52</v>
+        <f t="shared" si="3"/>
+        <v>65.805555555555543</v>
       </c>
       <c r="AD22">
-        <f t="shared" si="51"/>
-        <v>54</v>
+        <f t="shared" si="3"/>
+        <v>68.138888888888872</v>
       </c>
       <c r="AE22">
-        <f t="shared" si="51"/>
-        <v>56</v>
+        <f t="shared" si="3"/>
+        <v>70.4722222222222</v>
       </c>
       <c r="AF22">
-        <f t="shared" si="51"/>
-        <v>58</v>
+        <f t="shared" si="3"/>
+        <v>72.805555555555543</v>
       </c>
       <c r="AG22">
-        <f t="shared" si="51"/>
-        <v>60</v>
+        <f t="shared" si="3"/>
+        <v>75.138888888888872</v>
       </c>
       <c r="AH22">
-        <f t="shared" si="51"/>
-        <v>62</v>
+        <f t="shared" si="3"/>
+        <v>77.4722222222222</v>
       </c>
       <c r="AI22">
-        <f t="shared" si="51"/>
-        <v>64</v>
+        <f t="shared" si="3"/>
+        <v>79.805555555555543</v>
       </c>
       <c r="AJ22">
-        <f t="shared" si="51"/>
-        <v>66</v>
+        <f t="shared" si="3"/>
+        <v>82.138888888888872</v>
       </c>
       <c r="AK22">
-        <f t="shared" si="51"/>
-        <v>68</v>
+        <f t="shared" si="3"/>
+        <v>84.4722222222222</v>
       </c>
       <c r="AL22">
-        <f t="shared" si="51"/>
-        <v>70</v>
+        <f t="shared" si="3"/>
+        <v>86.805555555555543</v>
       </c>
       <c r="AM22">
-        <f t="shared" si="51"/>
-        <v>72</v>
+        <f t="shared" si="3"/>
+        <v>89.138888888888872</v>
       </c>
       <c r="AN22">
-        <f t="shared" si="51"/>
-        <v>74</v>
+        <f t="shared" si="3"/>
+        <v>91.4722222222222</v>
       </c>
       <c r="AO22">
-        <f t="shared" si="51"/>
-        <v>76</v>
+        <f t="shared" si="3"/>
+        <v>93.805555555555543</v>
       </c>
       <c r="AP22">
-        <f t="shared" si="51"/>
-        <v>78</v>
+        <f t="shared" si="3"/>
+        <v>96.138888888888872</v>
       </c>
       <c r="AQ22">
-        <f t="shared" si="51"/>
-        <v>80</v>
+        <f t="shared" si="3"/>
+        <v>98.4722222222222</v>
       </c>
       <c r="AR22">
-        <f t="shared" si="51"/>
-        <v>82</v>
+        <f t="shared" si="3"/>
+        <v>100.80555555555554</v>
       </c>
       <c r="AS22">
-        <f t="shared" si="51"/>
-        <v>84</v>
+        <f t="shared" si="3"/>
+        <v>103.13888888888887</v>
       </c>
       <c r="AT22">
-        <f t="shared" si="51"/>
-        <v>86</v>
+        <f t="shared" si="3"/>
+        <v>105.4722222222222</v>
       </c>
       <c r="AU22">
-        <f t="shared" si="51"/>
-        <v>88</v>
+        <f t="shared" si="3"/>
+        <v>107.80555555555553</v>
       </c>
       <c r="AV22">
-        <f t="shared" si="51"/>
-        <v>90</v>
+        <f t="shared" si="3"/>
+        <v>110.13888888888887</v>
       </c>
       <c r="AW22">
-        <f t="shared" si="51"/>
-        <v>91.9</v>
+        <f t="shared" si="3"/>
+        <v>112.4722222222222</v>
       </c>
       <c r="AX22">
-        <f t="shared" si="51"/>
-        <v>93.6</v>
+        <f t="shared" si="3"/>
+        <v>114.80555555555553</v>
       </c>
       <c r="AY22">
-        <f t="shared" si="51"/>
-        <v>95.1</v>
+        <f t="shared" si="3"/>
+        <v>117.13888888888887</v>
       </c>
       <c r="AZ22">
-        <f t="shared" si="51"/>
-        <v>96.4</v>
+        <f t="shared" si="3"/>
+        <v>119.4722222222222</v>
       </c>
       <c r="BA22">
-        <f t="shared" si="51"/>
-        <v>97.5</v>
+        <f t="shared" si="3"/>
+        <v>121.80555555555553</v>
       </c>
       <c r="BB22">
-        <f t="shared" si="51"/>
-        <v>98.4</v>
+        <f t="shared" si="3"/>
+        <v>124.13888888888886</v>
       </c>
       <c r="BC22">
-        <f t="shared" si="51"/>
-        <v>99.1</v>
+        <f t="shared" si="3"/>
+        <v>126.4722222222222</v>
       </c>
       <c r="BD22">
-        <f t="shared" si="51"/>
-        <v>99.6</v>
+        <f t="shared" si="3"/>
+        <v>128.80555555555554</v>
       </c>
       <c r="BE22">
-        <f t="shared" si="51"/>
-        <v>99.9</v>
+        <f t="shared" si="3"/>
+        <v>131.13888888888886</v>
       </c>
       <c r="BF22">
-        <f t="shared" si="51"/>
-        <v>100</v>
+        <f t="shared" si="3"/>
+        <v>133.33333333333331</v>
       </c>
     </row>
     <row r="23" spans="1:70" x14ac:dyDescent="0.3">
       <c r="B23" s="58"/>
       <c r="H23">
         <f>$B$3*$B$18+0.5*$B$7*$B$18*$B$18+(H20-ABS($B$12))*$B$14</f>
-        <v>30</v>
+        <v>50.416666666666671</v>
       </c>
       <c r="I23">
-        <f t="shared" ref="I23:BF23" si="52">$B$3*ABS($B$12)+0.5*$B$7*ABS($B$12)*ABS($B$12)+(I20-ABS($B$12))*$B$14</f>
-        <v>32</v>
+        <f t="shared" ref="I23:BF23" si="4">$B$3*ABS($B$12)+0.5*$B$7*ABS($B$12)*ABS($B$12)+(I20-ABS($B$12))*$B$14</f>
+        <v>52.75</v>
       </c>
       <c r="J23">
-        <f t="shared" si="52"/>
-        <v>34</v>
+        <f t="shared" si="4"/>
+        <v>55.083333333333343</v>
       </c>
       <c r="K23">
-        <f t="shared" si="52"/>
-        <v>36</v>
+        <f t="shared" si="4"/>
+        <v>57.416666666666671</v>
       </c>
       <c r="L23">
-        <f t="shared" si="52"/>
-        <v>38</v>
+        <f t="shared" si="4"/>
+        <v>59.75</v>
       </c>
       <c r="M23">
-        <f t="shared" si="52"/>
-        <v>40</v>
+        <f t="shared" si="4"/>
+        <v>62.083333333333336</v>
       </c>
       <c r="N23">
-        <f t="shared" si="52"/>
-        <v>42</v>
+        <f t="shared" si="4"/>
+        <v>64.416666666666671</v>
       </c>
       <c r="O23">
-        <f t="shared" si="52"/>
-        <v>44</v>
+        <f t="shared" si="4"/>
+        <v>66.75</v>
       </c>
       <c r="P23">
-        <f t="shared" si="52"/>
-        <v>46</v>
+        <f t="shared" si="4"/>
+        <v>69.083333333333329</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="52"/>
-        <v>48</v>
+        <f t="shared" si="4"/>
+        <v>71.416666666666671</v>
       </c>
       <c r="R23">
-        <f t="shared" si="52"/>
-        <v>50</v>
+        <f t="shared" si="4"/>
+        <v>73.75</v>
       </c>
       <c r="S23">
-        <f t="shared" si="52"/>
-        <v>52</v>
+        <f t="shared" si="4"/>
+        <v>76.083333333333329</v>
       </c>
       <c r="T23">
-        <f t="shared" si="52"/>
-        <v>54</v>
+        <f t="shared" si="4"/>
+        <v>78.416666666666671</v>
       </c>
       <c r="U23">
-        <f t="shared" si="52"/>
-        <v>56</v>
+        <f t="shared" si="4"/>
+        <v>80.75</v>
       </c>
       <c r="V23">
-        <f t="shared" si="52"/>
-        <v>58</v>
+        <f t="shared" si="4"/>
+        <v>83.083333333333329</v>
       </c>
       <c r="W23">
-        <f t="shared" si="52"/>
-        <v>60</v>
+        <f t="shared" si="4"/>
+        <v>85.416666666666657</v>
       </c>
       <c r="X23">
-        <f t="shared" si="52"/>
-        <v>62</v>
+        <f t="shared" si="4"/>
+        <v>87.75</v>
       </c>
       <c r="Y23">
-        <f t="shared" si="52"/>
-        <v>64</v>
+        <f t="shared" si="4"/>
+        <v>90.083333333333329</v>
       </c>
       <c r="Z23">
-        <f t="shared" si="52"/>
-        <v>66</v>
+        <f t="shared" si="4"/>
+        <v>92.416666666666657</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="52"/>
-        <v>68</v>
+        <f t="shared" si="4"/>
+        <v>94.75</v>
       </c>
       <c r="AB23">
-        <f t="shared" si="52"/>
-        <v>70</v>
+        <f t="shared" si="4"/>
+        <v>97.083333333333329</v>
       </c>
       <c r="AC23">
-        <f t="shared" si="52"/>
-        <v>72</v>
+        <f t="shared" si="4"/>
+        <v>99.416666666666657</v>
       </c>
       <c r="AD23">
-        <f t="shared" si="52"/>
-        <v>74</v>
+        <f t="shared" si="4"/>
+        <v>101.74999999999999</v>
       </c>
       <c r="AE23">
-        <f t="shared" si="52"/>
-        <v>76</v>
+        <f t="shared" si="4"/>
+        <v>104.08333333333331</v>
       </c>
       <c r="AF23">
-        <f t="shared" si="52"/>
-        <v>78</v>
+        <f t="shared" si="4"/>
+        <v>106.41666666666666</v>
       </c>
       <c r="AG23">
-        <f t="shared" si="52"/>
-        <v>80</v>
+        <f t="shared" si="4"/>
+        <v>108.74999999999999</v>
       </c>
       <c r="AH23">
-        <f t="shared" si="52"/>
-        <v>82</v>
+        <f t="shared" si="4"/>
+        <v>111.08333333333331</v>
       </c>
       <c r="AI23">
-        <f t="shared" si="52"/>
-        <v>84</v>
+        <f t="shared" si="4"/>
+        <v>113.41666666666666</v>
       </c>
       <c r="AJ23">
-        <f t="shared" si="52"/>
-        <v>86</v>
+        <f t="shared" si="4"/>
+        <v>115.74999999999999</v>
       </c>
       <c r="AK23">
-        <f t="shared" si="52"/>
-        <v>88</v>
+        <f t="shared" si="4"/>
+        <v>118.08333333333331</v>
       </c>
       <c r="AL23">
-        <f t="shared" si="52"/>
-        <v>90</v>
+        <f t="shared" si="4"/>
+        <v>120.41666666666666</v>
       </c>
       <c r="AM23">
-        <f t="shared" si="52"/>
-        <v>92</v>
+        <f t="shared" si="4"/>
+        <v>122.74999999999999</v>
       </c>
       <c r="AN23">
-        <f t="shared" si="52"/>
-        <v>94</v>
+        <f t="shared" si="4"/>
+        <v>125.08333333333331</v>
       </c>
       <c r="AO23">
-        <f t="shared" si="52"/>
-        <v>96</v>
+        <f t="shared" si="4"/>
+        <v>127.41666666666666</v>
       </c>
       <c r="AP23">
-        <f t="shared" si="52"/>
-        <v>98</v>
+        <f t="shared" si="4"/>
+        <v>129.75</v>
       </c>
       <c r="AQ23">
-        <f t="shared" si="52"/>
-        <v>100</v>
+        <f t="shared" si="4"/>
+        <v>132.08333333333331</v>
       </c>
       <c r="AR23">
-        <f t="shared" si="52"/>
-        <v>102</v>
+        <f t="shared" si="4"/>
+        <v>134.41666666666666</v>
       </c>
       <c r="AS23">
-        <f t="shared" si="52"/>
-        <v>104</v>
+        <f t="shared" si="4"/>
+        <v>136.75</v>
       </c>
       <c r="AT23">
-        <f t="shared" si="52"/>
-        <v>106</v>
+        <f t="shared" si="4"/>
+        <v>139.08333333333331</v>
       </c>
       <c r="AU23">
-        <f t="shared" si="52"/>
-        <v>108</v>
+        <f t="shared" si="4"/>
+        <v>141.41666666666663</v>
       </c>
       <c r="AV23">
-        <f t="shared" si="52"/>
-        <v>110</v>
+        <f t="shared" si="4"/>
+        <v>143.75</v>
       </c>
       <c r="AW23">
-        <f t="shared" si="52"/>
-        <v>112</v>
+        <f t="shared" si="4"/>
+        <v>146.08333333333331</v>
       </c>
       <c r="AX23">
-        <f t="shared" si="52"/>
-        <v>114</v>
+        <f t="shared" si="4"/>
+        <v>148.41666666666663</v>
       </c>
       <c r="AY23">
-        <f t="shared" si="52"/>
-        <v>116</v>
+        <f t="shared" si="4"/>
+        <v>150.75</v>
       </c>
       <c r="AZ23">
-        <f t="shared" si="52"/>
-        <v>118</v>
+        <f t="shared" si="4"/>
+        <v>153.08333333333331</v>
       </c>
       <c r="BA23">
-        <f t="shared" si="52"/>
-        <v>120</v>
+        <f t="shared" si="4"/>
+        <v>155.41666666666663</v>
       </c>
       <c r="BB23">
-        <f t="shared" si="52"/>
-        <v>122</v>
+        <f t="shared" si="4"/>
+        <v>157.74999999999997</v>
       </c>
       <c r="BC23">
-        <f t="shared" si="52"/>
-        <v>124</v>
+        <f t="shared" si="4"/>
+        <v>160.08333333333331</v>
       </c>
       <c r="BD23">
-        <f t="shared" si="52"/>
-        <v>126</v>
+        <f t="shared" si="4"/>
+        <v>162.41666666666663</v>
       </c>
       <c r="BE23">
-        <f t="shared" si="52"/>
-        <v>128</v>
+        <f t="shared" si="4"/>
+        <v>164.74999999999997</v>
       </c>
       <c r="BF23">
-        <f t="shared" si="52"/>
-        <v>130</v>
+        <f t="shared" si="4"/>
+        <v>167.08333333333331</v>
       </c>
     </row>
     <row r="24" spans="1:70" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixed Beziercurve::curvelength of  angle interpolation
</commit_message>
<xml_diff>
--- a/theory/Kinematik.xlsx
+++ b/theory/Kinematik.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="114">
   <si>
     <r>
       <t>Hüfte (T</t>
@@ -1009,22 +1009,6 @@
   </si>
   <si>
     <r>
-      <t>v</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>average</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
@@ -1171,6 +1155,18 @@
       </rPr>
       <t>abs,1</t>
     </r>
+  </si>
+  <si>
+    <t>Steigend:</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>trapez</t>
   </si>
 </sst>
 </file>
@@ -1753,11 +1749,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="339422008"/>
-        <c:axId val="339425536"/>
+        <c:axId val="317526856"/>
+        <c:axId val="317519800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="339422008"/>
+        <c:axId val="317526856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1795,13 +1791,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="339425536"/>
+        <c:crossAx val="317519800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="339425536"/>
+        <c:axId val="317519800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1840,7 +1836,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="339422008"/>
+        <c:crossAx val="317526856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
@@ -1936,11 +1932,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="339420048"/>
-        <c:axId val="339425928"/>
+        <c:axId val="317522936"/>
+        <c:axId val="317520192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="339420048"/>
+        <c:axId val="317522936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -1952,13 +1948,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="339425928"/>
+        <c:crossAx val="317520192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="339425928"/>
+        <c:axId val="317520192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -1971,7 +1967,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="339420048"/>
+        <c:crossAx val="317522936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
@@ -2104,7 +2100,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Trajectory Speed profile'!$H$11:$K$11</c:f>
+              <c:f>'Trajectory Speed profile'!$H$14:$K$14</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2112,34 +2108,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>183.33333333333334</c:v>
+                  <c:v>244</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>983.33333333333337</c:v>
+                  <c:v>446</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>1000</c:v>
+                  <c:v>690</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Trajectory Speed profile'!$H$12:$K$12</c:f>
+              <c:f>'Trajectory Speed profile'!$H$15:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0.3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>0.1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2154,11 +2150,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="339422400"/>
-        <c:axId val="339419656"/>
+        <c:axId val="339615528"/>
+        <c:axId val="339615136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="339422400"/>
+        <c:axId val="339615528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2201,12 +2197,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="339419656"/>
+        <c:crossAx val="339615136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="339419656"/>
+        <c:axId val="339615136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2257,7 +2253,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="339422400"/>
+        <c:crossAx val="339615528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2378,7 +2374,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2458,7 +2453,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Trajectory Speed profile'!$H$20:$BF$20</c:f>
+              <c:f>'Trajectory Speed profile'!$H$23:$BF$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -2466,316 +2461,316 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>13.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>27.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>41.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80</c:v>
+                  <c:v>55.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>120</c:v>
+                  <c:v>82.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>140</c:v>
+                  <c:v>96.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>160</c:v>
+                  <c:v>110.39999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>180</c:v>
+                  <c:v>124.19999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>200</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>220</c:v>
+                  <c:v>151.80000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>240</c:v>
+                  <c:v>165.60000000000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>260</c:v>
+                  <c:v>179.40000000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>280</c:v>
+                  <c:v>193.20000000000005</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>300</c:v>
+                  <c:v>207.00000000000006</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>320</c:v>
+                  <c:v>220.80000000000007</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>340</c:v>
+                  <c:v>234.60000000000008</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>360</c:v>
+                  <c:v>248.40000000000009</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>380</c:v>
+                  <c:v>262.2000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>400</c:v>
+                  <c:v>276.00000000000011</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>420</c:v>
+                  <c:v>289.80000000000013</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>440</c:v>
+                  <c:v>303.60000000000014</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>460</c:v>
+                  <c:v>317.40000000000015</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>480</c:v>
+                  <c:v>331.20000000000016</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>500</c:v>
+                  <c:v>345.00000000000017</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>520</c:v>
+                  <c:v>358.80000000000018</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>540</c:v>
+                  <c:v>372.60000000000019</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>560</c:v>
+                  <c:v>386.4000000000002</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>580</c:v>
+                  <c:v>400.20000000000022</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>600</c:v>
+                  <c:v>414.00000000000023</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>620</c:v>
+                  <c:v>427.80000000000024</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>640</c:v>
+                  <c:v>441.60000000000025</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>660</c:v>
+                  <c:v>455.40000000000026</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>680</c:v>
+                  <c:v>469.20000000000027</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>700</c:v>
+                  <c:v>483.00000000000028</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>720</c:v>
+                  <c:v>496.8000000000003</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>740</c:v>
+                  <c:v>510.60000000000031</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>760</c:v>
+                  <c:v>524.40000000000032</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>780</c:v>
+                  <c:v>538.20000000000027</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>800</c:v>
+                  <c:v>552.00000000000023</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>820</c:v>
+                  <c:v>565.80000000000018</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>840</c:v>
+                  <c:v>579.60000000000014</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>860</c:v>
+                  <c:v>593.40000000000009</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>880</c:v>
+                  <c:v>607.20000000000005</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>900</c:v>
+                  <c:v>621</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>920</c:v>
+                  <c:v>634.79999999999995</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>940</c:v>
+                  <c:v>648.59999999999991</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>960</c:v>
+                  <c:v>662.39999999999986</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>980</c:v>
+                  <c:v>676.19999999999982</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1000</c:v>
+                  <c:v>689.99999999999977</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Trajectory Speed profile'!$H$21:$BF$21</c:f>
+              <c:f>'Trajectory Speed profile'!$H$24:$BF$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>0.3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.27999999999999997</c:v>
+                  <c:v>6.9000000000000008E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.26</c:v>
+                  <c:v>1.3800000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.24</c:v>
+                  <c:v>2.0700000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.21999999999999997</c:v>
+                  <c:v>2.7600000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.19999999999999998</c:v>
+                  <c:v>3.4500000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.18</c:v>
+                  <c:v>4.1399999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.15999999999999998</c:v>
+                  <c:v>4.8299999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.13999999999999999</c:v>
+                  <c:v>5.5199999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.12</c:v>
+                  <c:v>6.2099999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>6.9000000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>7.5900000000000009E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>8.2800000000000012E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>8.9700000000000016E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>9.6600000000000019E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.10350000000000004</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.11040000000000004</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.11730000000000004</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.11729999999999986</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.11039999999999986</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>0.10349999999999986</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>9.6599999999999853E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>8.9699999999999835E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>8.2799999999999846E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>7.5899999999999856E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>6.8999999999999881E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>6.2099999999999905E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>5.519999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>4.8299999999999954E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>4.1399999999999978E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>3.4499999999999989E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>2.7600000000000013E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>2.0700000000000038E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>1.3800000000000062E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.11666666666666664</c:v>
+                  <c:v>6.9000000000000866E-3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.1</c:v>
+                  <c:v>1.1102230246251565E-16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2790,11 +2785,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="339427104"/>
-        <c:axId val="339423968"/>
+        <c:axId val="339617096"/>
+        <c:axId val="339618664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="339427104"/>
+        <c:axId val="339617096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2845,12 +2840,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="339423968"/>
+        <c:crossAx val="339618664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="339423968"/>
+        <c:axId val="339618664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2901,7 +2896,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="339427104"/>
+        <c:crossAx val="339617096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2915,7 +2910,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3034,7 +3028,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3125,7 +3118,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Trajectory Speed profile'!$H$20:$BF$20</c:f>
+              <c:f>'Trajectory Speed profile'!$H$23:$BF$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -3133,161 +3126,161 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>13.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>27.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>41.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80</c:v>
+                  <c:v>55.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>120</c:v>
+                  <c:v>82.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>140</c:v>
+                  <c:v>96.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>160</c:v>
+                  <c:v>110.39999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>180</c:v>
+                  <c:v>124.19999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>200</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>220</c:v>
+                  <c:v>151.80000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>240</c:v>
+                  <c:v>165.60000000000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>260</c:v>
+                  <c:v>179.40000000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>280</c:v>
+                  <c:v>193.20000000000005</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>300</c:v>
+                  <c:v>207.00000000000006</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>320</c:v>
+                  <c:v>220.80000000000007</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>340</c:v>
+                  <c:v>234.60000000000008</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>360</c:v>
+                  <c:v>248.40000000000009</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>380</c:v>
+                  <c:v>262.2000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>400</c:v>
+                  <c:v>276.00000000000011</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>420</c:v>
+                  <c:v>289.80000000000013</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>440</c:v>
+                  <c:v>303.60000000000014</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>460</c:v>
+                  <c:v>317.40000000000015</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>480</c:v>
+                  <c:v>331.20000000000016</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>500</c:v>
+                  <c:v>345.00000000000017</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>520</c:v>
+                  <c:v>358.80000000000018</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>540</c:v>
+                  <c:v>372.60000000000019</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>560</c:v>
+                  <c:v>386.4000000000002</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>580</c:v>
+                  <c:v>400.20000000000022</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>600</c:v>
+                  <c:v>414.00000000000023</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>620</c:v>
+                  <c:v>427.80000000000024</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>640</c:v>
+                  <c:v>441.60000000000025</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>660</c:v>
+                  <c:v>455.40000000000026</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>680</c:v>
+                  <c:v>469.20000000000027</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>700</c:v>
+                  <c:v>483.00000000000028</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>720</c:v>
+                  <c:v>496.8000000000003</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>740</c:v>
+                  <c:v>510.60000000000031</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>760</c:v>
+                  <c:v>524.40000000000032</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>780</c:v>
+                  <c:v>538.20000000000027</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>800</c:v>
+                  <c:v>552.00000000000023</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>820</c:v>
+                  <c:v>565.80000000000018</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>840</c:v>
+                  <c:v>579.60000000000014</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>860</c:v>
+                  <c:v>593.40000000000009</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>880</c:v>
+                  <c:v>607.20000000000005</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>900</c:v>
+                  <c:v>621</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>920</c:v>
+                  <c:v>634.79999999999995</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>940</c:v>
+                  <c:v>648.59999999999991</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>960</c:v>
+                  <c:v>662.39999999999986</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>980</c:v>
+                  <c:v>676.19999999999982</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1000</c:v>
+                  <c:v>689.99999999999977</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Trajectory Speed profile'!$H$22:$BF$22</c:f>
+              <c:f>'Trajectory Speed profile'!$H$25:$BF$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -3295,154 +3288,154 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.8</c:v>
+                  <c:v>4.7610000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.2</c:v>
+                  <c:v>0.19044000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.2</c:v>
+                  <c:v>0.42849000000000015</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.8</c:v>
+                  <c:v>0.7617600000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25</c:v>
+                  <c:v>1.19025</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.8</c:v>
+                  <c:v>1.7139599999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32.200000000000003</c:v>
+                  <c:v>2.3328899999999995</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35.200000000000003</c:v>
+                  <c:v>3.0470399999999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37.799999999999997</c:v>
+                  <c:v>3.8564099999999994</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40.138888888888886</c:v>
+                  <c:v>4.7610000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42.472222222222221</c:v>
+                  <c:v>5.7608100000000011</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44.80555555555555</c:v>
+                  <c:v>6.8558400000000024</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>47.138888888888886</c:v>
+                  <c:v>8.0460900000000031</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>49.472222222222214</c:v>
+                  <c:v>9.3315600000000032</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>51.80555555555555</c:v>
+                  <c:v>10.712250000000006</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>54.138888888888886</c:v>
+                  <c:v>12.188160000000009</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>56.472222222222214</c:v>
+                  <c:v>13.759290000000009</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>58.80555555555555</c:v>
+                  <c:v>15.42080000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>61.138888888888886</c:v>
+                  <c:v>17.104400000000012</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>63.472222222222214</c:v>
+                  <c:v>18.788000000000014</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>65.805555555555543</c:v>
+                  <c:v>20.471600000000016</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>68.138888888888872</c:v>
+                  <c:v>22.155200000000015</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>70.4722222222222</c:v>
+                  <c:v>23.83880000000002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>72.805555555555543</c:v>
+                  <c:v>25.522400000000019</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>75.138888888888872</c:v>
+                  <c:v>27.206000000000021</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>77.4722222222222</c:v>
+                  <c:v>28.889600000000023</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>79.805555555555543</c:v>
+                  <c:v>30.573200000000021</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>82.138888888888872</c:v>
+                  <c:v>32.256800000000027</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>84.4722222222222</c:v>
+                  <c:v>33.940400000000025</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>86.805555555555543</c:v>
+                  <c:v>35.624000000000024</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>89.138888888888872</c:v>
+                  <c:v>37.307600000000029</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>91.4722222222222</c:v>
+                  <c:v>38.991200000000035</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>93.805555555555543</c:v>
+                  <c:v>40.652710000000035</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>96.138888888888872</c:v>
+                  <c:v>42.223840000000031</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>98.4722222222222</c:v>
+                  <c:v>43.699750000000023</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>100.80555555555554</c:v>
+                  <c:v>45.080440000000031</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>103.13888888888887</c:v>
+                  <c:v>46.365910000000021</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>105.4722222222222</c:v>
+                  <c:v>47.556160000000027</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>107.80555555555553</c:v>
+                  <c:v>48.651190000000021</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>110.13888888888887</c:v>
+                  <c:v>49.65100000000001</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>112.4722222222222</c:v>
+                  <c:v>50.555590000000009</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>114.80555555555553</c:v>
+                  <c:v>51.364960000000011</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>117.13888888888887</c:v>
+                  <c:v>52.07911</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>119.4722222222222</c:v>
+                  <c:v>52.698039999999999</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>121.80555555555553</c:v>
+                  <c:v>53.22175</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>124.13888888888886</c:v>
+                  <c:v>53.650239999999997</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>126.4722222222222</c:v>
+                  <c:v>53.983509999999995</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>128.80555555555554</c:v>
+                  <c:v>54.221559999999997</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>131.13888888888886</c:v>
+                  <c:v>54.36439</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>133.33333333333331</c:v>
+                  <c:v>54.411999999999992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3457,11 +3450,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="339424752"/>
-        <c:axId val="339425144"/>
+        <c:axId val="339615920"/>
+        <c:axId val="339620624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="339424752"/>
+        <c:axId val="339615920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3517,12 +3510,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="339425144"/>
+        <c:crossAx val="339620624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="339425144"/>
+        <c:axId val="339620624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3578,7 +3571,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="339424752"/>
+        <c:crossAx val="339615920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3592,7 +3585,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -29669,7 +29661,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>605790</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -29693,13 +29685,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>784860</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -29725,13 +29717,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>708660</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -33214,10 +33206,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BR24"/>
+  <dimension ref="A1:BR27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33235,7 +33227,7 @@
         <v>85</v>
       </c>
       <c r="B3">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>87</v>
@@ -33246,7 +33238,7 @@
         <v>86</v>
       </c>
       <c r="B4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>87</v>
@@ -33257,14 +33249,18 @@
         <v>88</v>
       </c>
       <c r="B5">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
         <v>91</v>
       </c>
       <c r="D5">
-        <f>$B$3*$B$18+SIGN($B$12)*0.5*$B$7*$B$18*$B$18+($B$19-$B$18)*$B$14 + $B$14*(B6-$B$19) + SIGN($B$13)*0.5*$B$7*(B6-$B$19)*(B6-$B$19)</f>
-        <v>133.33333333333331</v>
+        <f>$B$3*$B$21+SIGN($B$15)*0.5*$B$7*$B$21*$B$21+($B$22-$B$21)*$B$17 + $B$17*(B6-$B$22) + SIGN($B$16)*0.5*$B$7*(B6-$B$22)*(B6-$B$22)</f>
+        <v>54.411999999999992</v>
+      </c>
+      <c r="E5">
+        <f>B3*B15+0.5*B7*B15*B15+(B3+B7*B15)*(B6-B9-2*B15) + (B3+B7*B15)*(B9+B15)-0.5*B7*(B9+B15)*(B9+B15)</f>
+        <v>54.411999999999992</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
@@ -33272,10 +33268,14 @@
         <v>90</v>
       </c>
       <c r="B6">
-        <v>1000</v>
+        <v>690</v>
       </c>
       <c r="C6" t="s">
         <v>92</v>
+      </c>
+      <c r="E6">
+        <f>B3*B6-B3*B9+B3*B9-0.5*B7*B9*B9 + B15*(B3+B7*B6-B7*B9-2*B3+B7*B9+B3-B7*B9) + B15*B15*(0.5*B7-2*B7+B7-0.5*B7)</f>
+        <v>54.412000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
@@ -33283,1025 +33283,1074 @@
         <v>71</v>
       </c>
       <c r="B7">
-        <v>1E-3</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="C7" t="s">
         <v>95</v>
       </c>
+      <c r="E7">
+        <f>B3*B6-0.5*B7*B9*B9 + B15*(B7*B6-B7*B9) + B15*B15*(-B7)</f>
+        <v>54.412000000000006</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9">
+        <f>(B3-B4)/B7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B10" s="60">
-        <f>B5/B6</f>
-        <v>0.1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>87</v>
+        <v>112</v>
+      </c>
+      <c r="B10">
+        <f>B3*B6-0.5*B7*B9*B9 - B5</f>
+        <v>-69</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G11" t="s">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11">
+        <f>B7*B6-B7*B9</f>
+        <v>0.34500000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12">
+        <f>-B7</f>
+        <v>-5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="60" t="e">
+        <f>(-B11+SQRT(B11*B11-4*B12*B10))/(2*B12)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C13" s="60" t="e">
+        <f>(-B11-SQRT(B11*B11-4*B12*B10))/(2*B12)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
         <v>89</v>
       </c>
-      <c r="H11">
+      <c r="H14">
         <v>0</v>
       </c>
-      <c r="I11" s="4">
-        <f>ABS(B12)</f>
-        <v>183.33333333333334</v>
-      </c>
-      <c r="J11" s="3">
-        <f>B6-ABS(B13)</f>
-        <v>983.33333333333337</v>
-      </c>
-      <c r="K11">
+      <c r="I14" s="4">
+        <f>ABS(B15)</f>
+        <v>244</v>
+      </c>
+      <c r="J14" s="3">
+        <f>B6-ABS(B16)</f>
+        <v>446</v>
+      </c>
+      <c r="K14">
         <f>B6</f>
-        <v>1000</v>
+        <v>690</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>93</v>
       </c>
-      <c r="B12" s="127">
-        <f>(B5- B3*B6 - 0.5*(B4-B3)*(B4-B3)/B7) / ( B7*B6 + B3 - B4)</f>
-        <v>-183.33333333333334</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B15" s="127">
+        <v>244</v>
+      </c>
+      <c r="C15" t="s">
         <v>92</v>
       </c>
-      <c r="D12">
-        <f>(B5 - B3*B6 - 0.5*(B4-B3)*(B4-B3)/B7) / ( B7*B6 - B3 - B4)</f>
-        <v>-366.66666666666669</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="D15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15">
+        <f>(B5-B3*B6-0.5*(B4-B3)*(B4-B3)/B7)/(B6*B7+(B3-B4))</f>
+        <v>199.99999999999997</v>
+      </c>
+      <c r="G15" t="s">
         <v>84</v>
       </c>
-      <c r="H12">
+      <c r="H15">
         <f>B3</f>
-        <v>0.3</v>
-      </c>
-      <c r="I12" s="3">
-        <f>B14</f>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="J12" s="3">
-        <f>I12</f>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <f>B17</f>
+        <v>0.122</v>
+      </c>
+      <c r="J15" s="3">
+        <f>I15</f>
+        <v>0.122</v>
+      </c>
+      <c r="K15">
         <f>B4</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>94</v>
-      </c>
-      <c r="B13" s="3">
-        <f>(B4-B3)/B7-B12</f>
-        <v>-16.666666666666629</v>
-      </c>
-      <c r="C13" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="75"/>
-    </row>
-    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>97</v>
-      </c>
-      <c r="B14" s="3">
-        <f>B3+B7*B12</f>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="C14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="127">
-        <f>(B3+B14)/2*B12+B14*(B6-B12-B13)+(B14+B4)/2*B13</f>
-        <v>99.999999999999972</v>
-      </c>
-      <c r="C15" t="s">
-        <v>91</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16">
-        <f>B14+B13*B7</f>
-        <v>0.1</v>
+        <v>94</v>
+      </c>
+      <c r="B16" s="3">
+        <f>(B4-B3)/B7-B15</f>
+        <v>-244</v>
       </c>
       <c r="C16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="75" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" t="e">
+        <f>(-B11+SQRT(B11*B11-4*B12*B10))/(2*B12)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:70" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="3">
+        <f>B3+B7*B15</f>
+        <v>0.122</v>
+      </c>
+      <c r="C17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:70" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="B18" s="127">
-        <f>ABS(B12)</f>
-        <v>183.33333333333334</v>
+        <f>(B3+B17)/2*B15+B17*(B6-B15-B16)+(B17+B4)/2*B16</f>
+        <v>84.179999999999993</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:70" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>110</v>
-      </c>
-      <c r="B19" s="127">
-        <f>B6-ABS(B13)</f>
-        <v>983.33333333333337</v>
+        <v>86</v>
+      </c>
+      <c r="B19">
+        <f>B17+B16*B7</f>
+        <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:70" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A20" s="128" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" t="s">
-        <v>101</v>
-      </c>
-      <c r="G20" t="s">
-        <v>106</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <f>(H20+$B$6/50)</f>
-        <v>20</v>
-      </c>
-      <c r="J20">
-        <f t="shared" ref="J20:BF20" si="0">(I20+$B$6/50)</f>
-        <v>40</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="O20">
-        <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-      <c r="P20">
-        <f t="shared" si="0"/>
-        <v>160</v>
-      </c>
-      <c r="Q20">
-        <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-      <c r="R20">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="S20">
-        <f t="shared" si="0"/>
-        <v>220</v>
-      </c>
-      <c r="T20">
-        <f t="shared" si="0"/>
-        <v>240</v>
-      </c>
-      <c r="U20">
-        <f t="shared" si="0"/>
-        <v>260</v>
-      </c>
-      <c r="V20">
-        <f t="shared" si="0"/>
-        <v>280</v>
-      </c>
-      <c r="W20">
-        <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-      <c r="X20">
-        <f t="shared" si="0"/>
-        <v>320</v>
-      </c>
-      <c r="Y20">
-        <f t="shared" si="0"/>
-        <v>340</v>
-      </c>
-      <c r="Z20">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="AA20">
-        <f t="shared" si="0"/>
-        <v>380</v>
-      </c>
-      <c r="AB20">
-        <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="AC20">
-        <f t="shared" si="0"/>
-        <v>420</v>
-      </c>
-      <c r="AD20">
-        <f t="shared" si="0"/>
-        <v>440</v>
-      </c>
-      <c r="AE20">
-        <f t="shared" si="0"/>
-        <v>460</v>
-      </c>
-      <c r="AF20">
-        <f t="shared" si="0"/>
-        <v>480</v>
-      </c>
-      <c r="AG20">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="AH20">
-        <f t="shared" si="0"/>
-        <v>520</v>
-      </c>
-      <c r="AI20">
-        <f t="shared" si="0"/>
-        <v>540</v>
-      </c>
-      <c r="AJ20">
-        <f t="shared" si="0"/>
-        <v>560</v>
-      </c>
-      <c r="AK20">
-        <f t="shared" si="0"/>
-        <v>580</v>
-      </c>
-      <c r="AL20">
-        <f t="shared" si="0"/>
-        <v>600</v>
-      </c>
-      <c r="AM20">
-        <f t="shared" si="0"/>
-        <v>620</v>
-      </c>
-      <c r="AN20">
-        <f t="shared" si="0"/>
-        <v>640</v>
-      </c>
-      <c r="AO20">
-        <f t="shared" si="0"/>
-        <v>660</v>
-      </c>
-      <c r="AP20">
-        <f t="shared" si="0"/>
-        <v>680</v>
-      </c>
-      <c r="AQ20">
-        <f t="shared" si="0"/>
-        <v>700</v>
-      </c>
-      <c r="AR20">
-        <f t="shared" si="0"/>
-        <v>720</v>
-      </c>
-      <c r="AS20">
-        <f t="shared" si="0"/>
-        <v>740</v>
-      </c>
-      <c r="AT20">
-        <f t="shared" si="0"/>
-        <v>760</v>
-      </c>
-      <c r="AU20">
-        <f t="shared" si="0"/>
-        <v>780</v>
-      </c>
-      <c r="AV20">
-        <f t="shared" si="0"/>
-        <v>800</v>
-      </c>
-      <c r="AW20">
-        <f t="shared" si="0"/>
-        <v>820</v>
-      </c>
-      <c r="AX20">
-        <f t="shared" si="0"/>
-        <v>840</v>
-      </c>
-      <c r="AY20">
-        <f t="shared" si="0"/>
-        <v>860</v>
-      </c>
-      <c r="AZ20">
-        <f t="shared" si="0"/>
-        <v>880</v>
-      </c>
-      <c r="BA20">
-        <f t="shared" si="0"/>
-        <v>900</v>
-      </c>
-      <c r="BB20">
-        <f t="shared" si="0"/>
-        <v>920</v>
-      </c>
-      <c r="BC20">
-        <f t="shared" si="0"/>
-        <v>940</v>
-      </c>
-      <c r="BD20">
-        <f t="shared" si="0"/>
-        <v>960</v>
-      </c>
-      <c r="BE20">
-        <f t="shared" si="0"/>
-        <v>980</v>
-      </c>
-      <c r="BF20">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:70" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A21" s="128" t="s">
-        <v>102</v>
-      </c>
-      <c r="B21" s="129" t="s">
-        <v>103</v>
-      </c>
-      <c r="G21" t="s">
-        <v>107</v>
-      </c>
-      <c r="H21" s="127">
-        <f t="shared" ref="H21:AM21" si="1">IF(H20&lt;ABS($B$12),$B$3+SIGN($B$12)*H$20*$B$7,IF(H20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(H20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.3</v>
-      </c>
-      <c r="I21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.27999999999999997</v>
-      </c>
-      <c r="J21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.26</v>
-      </c>
-      <c r="K21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.24</v>
-      </c>
-      <c r="L21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.21999999999999997</v>
-      </c>
-      <c r="M21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="N21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.18</v>
-      </c>
-      <c r="O21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.15999999999999998</v>
-      </c>
-      <c r="P21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.13999999999999999</v>
-      </c>
-      <c r="Q21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.12</v>
-      </c>
-      <c r="R21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="S21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="T21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="U21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="V21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="W21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="X21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="Y21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="Z21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AA21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AB21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AC21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AD21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AE21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AF21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AG21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AH21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AI21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AJ21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AK21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AL21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AM21" s="127">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AN21" s="127">
-        <f t="shared" ref="AN21:BS21" si="2">IF(AN20&lt;ABS($B$12),$B$3+SIGN($B$12)*AN$20*$B$7,IF(AN20&lt;$B$6-ABS($B$13),$B$14,$B$14+SIGN($B$13)*(AN20-($B$6-ABS($B$13)))*$B$7))</f>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AO21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AP21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AQ21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AR21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AS21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AT21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AU21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AV21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AW21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AX21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AY21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="AZ21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="BA21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="BB21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="BC21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="BD21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="BE21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.11666666666666664</v>
-      </c>
-      <c r="BF21" s="127">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="BG21" s="127"/>
-      <c r="BH21" s="127"/>
-      <c r="BI21" s="127"/>
-      <c r="BJ21" s="127"/>
-      <c r="BK21" s="127"/>
-      <c r="BL21" s="127"/>
-      <c r="BM21" s="127"/>
-      <c r="BN21" s="127"/>
-      <c r="BO21" s="127"/>
-      <c r="BP21" s="127"/>
-      <c r="BQ21" s="127"/>
-      <c r="BR21" s="127"/>
+      <c r="A21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="127">
+        <f>ABS(B15)</f>
+        <v>244</v>
+      </c>
+      <c r="C21" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="22" spans="1:70" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A22" s="128" t="s">
+      <c r="A22" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="127">
+        <f>B6-ABS(B16)</f>
+        <v>446</v>
+      </c>
+      <c r="C22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:70" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A23" s="128" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23" t="s">
+        <v>105</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f>(H23+$B$6/50)</f>
+        <v>13.8</v>
+      </c>
+      <c r="J23">
+        <f t="shared" ref="J23:BF23" si="0">(I23+$B$6/50)</f>
+        <v>27.6</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>41.400000000000006</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>55.2</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>82.8</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="0"/>
+        <v>96.6</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="0"/>
+        <v>110.39999999999999</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="0"/>
+        <v>124.19999999999999</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="0"/>
+        <v>151.80000000000001</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="0"/>
+        <v>165.60000000000002</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="0"/>
+        <v>179.40000000000003</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="0"/>
+        <v>193.20000000000005</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="0"/>
+        <v>207.00000000000006</v>
+      </c>
+      <c r="X23">
+        <f t="shared" si="0"/>
+        <v>220.80000000000007</v>
+      </c>
+      <c r="Y23">
+        <f t="shared" si="0"/>
+        <v>234.60000000000008</v>
+      </c>
+      <c r="Z23">
+        <f t="shared" si="0"/>
+        <v>248.40000000000009</v>
+      </c>
+      <c r="AA23">
+        <f t="shared" si="0"/>
+        <v>262.2000000000001</v>
+      </c>
+      <c r="AB23">
+        <f t="shared" si="0"/>
+        <v>276.00000000000011</v>
+      </c>
+      <c r="AC23">
+        <f t="shared" si="0"/>
+        <v>289.80000000000013</v>
+      </c>
+      <c r="AD23">
+        <f t="shared" si="0"/>
+        <v>303.60000000000014</v>
+      </c>
+      <c r="AE23">
+        <f t="shared" si="0"/>
+        <v>317.40000000000015</v>
+      </c>
+      <c r="AF23">
+        <f t="shared" si="0"/>
+        <v>331.20000000000016</v>
+      </c>
+      <c r="AG23">
+        <f t="shared" si="0"/>
+        <v>345.00000000000017</v>
+      </c>
+      <c r="AH23">
+        <f t="shared" si="0"/>
+        <v>358.80000000000018</v>
+      </c>
+      <c r="AI23">
+        <f t="shared" si="0"/>
+        <v>372.60000000000019</v>
+      </c>
+      <c r="AJ23">
+        <f t="shared" si="0"/>
+        <v>386.4000000000002</v>
+      </c>
+      <c r="AK23">
+        <f t="shared" si="0"/>
+        <v>400.20000000000022</v>
+      </c>
+      <c r="AL23">
+        <f t="shared" si="0"/>
+        <v>414.00000000000023</v>
+      </c>
+      <c r="AM23">
+        <f t="shared" si="0"/>
+        <v>427.80000000000024</v>
+      </c>
+      <c r="AN23">
+        <f t="shared" si="0"/>
+        <v>441.60000000000025</v>
+      </c>
+      <c r="AO23">
+        <f t="shared" si="0"/>
+        <v>455.40000000000026</v>
+      </c>
+      <c r="AP23">
+        <f t="shared" si="0"/>
+        <v>469.20000000000027</v>
+      </c>
+      <c r="AQ23">
+        <f t="shared" si="0"/>
+        <v>483.00000000000028</v>
+      </c>
+      <c r="AR23">
+        <f t="shared" si="0"/>
+        <v>496.8000000000003</v>
+      </c>
+      <c r="AS23">
+        <f t="shared" si="0"/>
+        <v>510.60000000000031</v>
+      </c>
+      <c r="AT23">
+        <f t="shared" si="0"/>
+        <v>524.40000000000032</v>
+      </c>
+      <c r="AU23">
+        <f t="shared" si="0"/>
+        <v>538.20000000000027</v>
+      </c>
+      <c r="AV23">
+        <f t="shared" si="0"/>
+        <v>552.00000000000023</v>
+      </c>
+      <c r="AW23">
+        <f t="shared" si="0"/>
+        <v>565.80000000000018</v>
+      </c>
+      <c r="AX23">
+        <f t="shared" si="0"/>
+        <v>579.60000000000014</v>
+      </c>
+      <c r="AY23">
+        <f t="shared" si="0"/>
+        <v>593.40000000000009</v>
+      </c>
+      <c r="AZ23">
+        <f t="shared" si="0"/>
+        <v>607.20000000000005</v>
+      </c>
+      <c r="BA23">
+        <f t="shared" si="0"/>
+        <v>621</v>
+      </c>
+      <c r="BB23">
+        <f t="shared" si="0"/>
+        <v>634.79999999999995</v>
+      </c>
+      <c r="BC23">
+        <f t="shared" si="0"/>
+        <v>648.59999999999991</v>
+      </c>
+      <c r="BD23">
+        <f t="shared" si="0"/>
+        <v>662.39999999999986</v>
+      </c>
+      <c r="BE23">
+        <f t="shared" si="0"/>
+        <v>676.19999999999982</v>
+      </c>
+      <c r="BF23">
+        <f t="shared" si="0"/>
+        <v>689.99999999999977</v>
+      </c>
+    </row>
+    <row r="24" spans="1:70" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A24" s="128" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="129" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" t="s">
+        <v>106</v>
+      </c>
+      <c r="H24" s="127">
+        <f t="shared" ref="H24:AM24" si="1">IF(H23&lt;ABS($B$15),$B$3+SIGN($B$15)*H$23*$B$7,IF(H23&lt;$B$6-ABS($B$16),$B$17,$B$17+SIGN($B$16)*(H23-($B$6-ABS($B$16)))*$B$7))</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="127">
+        <f t="shared" si="1"/>
+        <v>6.9000000000000008E-3</v>
+      </c>
+      <c r="J24" s="127">
+        <f t="shared" si="1"/>
+        <v>1.3800000000000002E-2</v>
+      </c>
+      <c r="K24" s="127">
+        <f t="shared" si="1"/>
+        <v>2.0700000000000003E-2</v>
+      </c>
+      <c r="L24" s="127">
+        <f t="shared" si="1"/>
+        <v>2.7600000000000003E-2</v>
+      </c>
+      <c r="M24" s="127">
+        <f t="shared" si="1"/>
+        <v>3.4500000000000003E-2</v>
+      </c>
+      <c r="N24" s="127">
+        <f t="shared" si="1"/>
+        <v>4.1399999999999999E-2</v>
+      </c>
+      <c r="O24" s="127">
+        <f t="shared" si="1"/>
+        <v>4.8299999999999996E-2</v>
+      </c>
+      <c r="P24" s="127">
+        <f t="shared" si="1"/>
+        <v>5.5199999999999999E-2</v>
+      </c>
+      <c r="Q24" s="127">
+        <f t="shared" si="1"/>
+        <v>6.2099999999999995E-2</v>
+      </c>
+      <c r="R24" s="127">
+        <f t="shared" si="1"/>
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="S24" s="127">
+        <f t="shared" si="1"/>
+        <v>7.5900000000000009E-2</v>
+      </c>
+      <c r="T24" s="127">
+        <f t="shared" si="1"/>
+        <v>8.2800000000000012E-2</v>
+      </c>
+      <c r="U24" s="127">
+        <f t="shared" si="1"/>
+        <v>8.9700000000000016E-2</v>
+      </c>
+      <c r="V24" s="127">
+        <f t="shared" si="1"/>
+        <v>9.6600000000000019E-2</v>
+      </c>
+      <c r="W24" s="127">
+        <f t="shared" si="1"/>
+        <v>0.10350000000000004</v>
+      </c>
+      <c r="X24" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11040000000000004</v>
+      </c>
+      <c r="Y24" s="127">
+        <f t="shared" si="1"/>
+        <v>0.11730000000000004</v>
+      </c>
+      <c r="Z24" s="127">
+        <f t="shared" si="1"/>
+        <v>0.122</v>
+      </c>
+      <c r="AA24" s="127">
+        <f t="shared" si="1"/>
+        <v>0.122</v>
+      </c>
+      <c r="AB24" s="127">
+        <f t="shared" si="1"/>
+        <v>0.122</v>
+      </c>
+      <c r="AC24" s="127">
+        <f t="shared" si="1"/>
+        <v>0.122</v>
+      </c>
+      <c r="AD24" s="127">
+        <f t="shared" si="1"/>
+        <v>0.122</v>
+      </c>
+      <c r="AE24" s="127">
+        <f t="shared" si="1"/>
+        <v>0.122</v>
+      </c>
+      <c r="AF24" s="127">
+        <f t="shared" si="1"/>
+        <v>0.122</v>
+      </c>
+      <c r="AG24" s="127">
+        <f t="shared" si="1"/>
+        <v>0.122</v>
+      </c>
+      <c r="AH24" s="127">
+        <f t="shared" si="1"/>
+        <v>0.122</v>
+      </c>
+      <c r="AI24" s="127">
+        <f t="shared" si="1"/>
+        <v>0.122</v>
+      </c>
+      <c r="AJ24" s="127">
+        <f t="shared" si="1"/>
+        <v>0.122</v>
+      </c>
+      <c r="AK24" s="127">
+        <f t="shared" si="1"/>
+        <v>0.122</v>
+      </c>
+      <c r="AL24" s="127">
+        <f t="shared" si="1"/>
+        <v>0.122</v>
+      </c>
+      <c r="AM24" s="127">
+        <f t="shared" si="1"/>
+        <v>0.122</v>
+      </c>
+      <c r="AN24" s="127">
+        <f t="shared" ref="AN24:BS24" si="2">IF(AN23&lt;ABS($B$15),$B$3+SIGN($B$15)*AN$23*$B$7,IF(AN23&lt;$B$6-ABS($B$16),$B$17,$B$17+SIGN($B$16)*(AN23-($B$6-ABS($B$16)))*$B$7))</f>
+        <v>0.122</v>
+      </c>
+      <c r="AO24" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11729999999999986</v>
+      </c>
+      <c r="AP24" s="127">
+        <f t="shared" si="2"/>
+        <v>0.11039999999999986</v>
+      </c>
+      <c r="AQ24" s="127">
+        <f t="shared" si="2"/>
+        <v>0.10349999999999986</v>
+      </c>
+      <c r="AR24" s="127">
+        <f t="shared" si="2"/>
+        <v>9.6599999999999853E-2</v>
+      </c>
+      <c r="AS24" s="127">
+        <f t="shared" si="2"/>
+        <v>8.9699999999999835E-2</v>
+      </c>
+      <c r="AT24" s="127">
+        <f t="shared" si="2"/>
+        <v>8.2799999999999846E-2</v>
+      </c>
+      <c r="AU24" s="127">
+        <f t="shared" si="2"/>
+        <v>7.5899999999999856E-2</v>
+      </c>
+      <c r="AV24" s="127">
+        <f t="shared" si="2"/>
+        <v>6.8999999999999881E-2</v>
+      </c>
+      <c r="AW24" s="127">
+        <f t="shared" si="2"/>
+        <v>6.2099999999999905E-2</v>
+      </c>
+      <c r="AX24" s="127">
+        <f t="shared" si="2"/>
+        <v>5.519999999999993E-2</v>
+      </c>
+      <c r="AY24" s="127">
+        <f t="shared" si="2"/>
+        <v>4.8299999999999954E-2</v>
+      </c>
+      <c r="AZ24" s="127">
+        <f t="shared" si="2"/>
+        <v>4.1399999999999978E-2</v>
+      </c>
+      <c r="BA24" s="127">
+        <f t="shared" si="2"/>
+        <v>3.4499999999999989E-2</v>
+      </c>
+      <c r="BB24" s="127">
+        <f t="shared" si="2"/>
+        <v>2.7600000000000013E-2</v>
+      </c>
+      <c r="BC24" s="127">
+        <f t="shared" si="2"/>
+        <v>2.0700000000000038E-2</v>
+      </c>
+      <c r="BD24" s="127">
+        <f t="shared" si="2"/>
+        <v>1.3800000000000062E-2</v>
+      </c>
+      <c r="BE24" s="127">
+        <f t="shared" si="2"/>
+        <v>6.9000000000000866E-3</v>
+      </c>
+      <c r="BF24" s="127">
+        <f t="shared" si="2"/>
+        <v>1.1102230246251565E-16</v>
+      </c>
+      <c r="BG24" s="127"/>
+      <c r="BH24" s="127"/>
+      <c r="BI24" s="127"/>
+      <c r="BJ24" s="127"/>
+      <c r="BK24" s="127"/>
+      <c r="BL24" s="127"/>
+      <c r="BM24" s="127"/>
+      <c r="BN24" s="127"/>
+      <c r="BO24" s="127"/>
+      <c r="BP24" s="127"/>
+      <c r="BQ24" s="127"/>
+      <c r="BR24" s="127"/>
+    </row>
+    <row r="25" spans="1:70" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A25" s="128" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="129" t="s">
         <v>104</v>
       </c>
-      <c r="B22" s="129" t="s">
-        <v>105</v>
-      </c>
-      <c r="G22" t="s">
-        <v>108</v>
-      </c>
-      <c r="H22">
-        <f>IF(H20&lt;$B$18,
-$B$3*H20+SIGN($B$12)*0.5*$B$7*H20*H20,
-IF(H20&lt;$B$19,
-$B$3*$B$18+SIGN($B$12)*0.5*$B$7*$B$18*$B$18+(H20-$B$18)*$B$14,
-$B$3*$B$18+SIGN($B$12)*0.5*$B$7*$B$18*$B$18+($B$19-$B$18)*$B$14 + $B$14*(H20-$B$19) + SIGN($B$13)*0.5*$B$7*(H20-$B$19)*(H20-$B$19)))</f>
+      <c r="G25" t="s">
+        <v>107</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ref="H25:AM25" si="3">IF(H23&lt;$B$21,
+$B$3*H23+SIGN($B$15)*0.5*$B$7*H23*H23,
+IF(H23&lt;$B$22,
+$B$3*$B$21+SIGN($B$15)*0.5*$B$7*$B$21*$B$21+(H23-$B$21)*$B$17,
+$B$3*$B$21+SIGN($B$15)*0.5*$B$7*$B$21*$B$21+($B$22-$B$21)*$B$17 + $B$17*(H23-$B$22) + SIGN($B$16)*0.5*$B$7*(H23-$B$22)*(H23-$B$22)))</f>
         <v>0</v>
       </c>
-      <c r="I22">
-        <f t="shared" ref="I22:BF22" si="3">IF(I20&lt;$B$18,
-$B$3*I20+SIGN($B$12)*0.5*$B$7*I20*I20,
-IF(I20&lt;$B$19,
-$B$3*$B$18+SIGN($B$12)*0.5*$B$7*$B$18*$B$18+(I20-$B$18)*$B$14,
-$B$3*$B$18+SIGN($B$12)*0.5*$B$7*$B$18*$B$18+($B$19-$B$18)*$B$14 + $B$14*(I20-$B$19) + SIGN($B$13)*0.5*$B$7*(I20-$B$19)*(I20-$B$19)))</f>
-        <v>5.8</v>
-      </c>
-      <c r="J22">
+      <c r="I25">
         <f t="shared" si="3"/>
-        <v>11.2</v>
-      </c>
-      <c r="K22">
+        <v>4.7610000000000006E-2</v>
+      </c>
+      <c r="J25">
         <f t="shared" si="3"/>
-        <v>16.2</v>
-      </c>
-      <c r="L22">
+        <v>0.19044000000000003</v>
+      </c>
+      <c r="K25">
         <f t="shared" si="3"/>
-        <v>20.8</v>
-      </c>
-      <c r="M22">
+        <v>0.42849000000000015</v>
+      </c>
+      <c r="L25">
         <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="N22">
+        <v>0.7617600000000001</v>
+      </c>
+      <c r="M25">
         <f t="shared" si="3"/>
-        <v>28.8</v>
-      </c>
-      <c r="O22">
+        <v>1.19025</v>
+      </c>
+      <c r="N25">
         <f t="shared" si="3"/>
-        <v>32.200000000000003</v>
-      </c>
-      <c r="P22">
+        <v>1.7139599999999999</v>
+      </c>
+      <c r="O25">
         <f t="shared" si="3"/>
-        <v>35.200000000000003</v>
-      </c>
-      <c r="Q22">
+        <v>2.3328899999999995</v>
+      </c>
+      <c r="P25">
         <f t="shared" si="3"/>
-        <v>37.799999999999997</v>
-      </c>
-      <c r="R22">
+        <v>3.0470399999999995</v>
+      </c>
+      <c r="Q25">
         <f t="shared" si="3"/>
-        <v>40.138888888888886</v>
-      </c>
-      <c r="S22">
+        <v>3.8564099999999994</v>
+      </c>
+      <c r="R25">
         <f t="shared" si="3"/>
-        <v>42.472222222222221</v>
-      </c>
-      <c r="T22">
+        <v>4.7610000000000001</v>
+      </c>
+      <c r="S25">
         <f t="shared" si="3"/>
-        <v>44.80555555555555</v>
-      </c>
-      <c r="U22">
+        <v>5.7608100000000011</v>
+      </c>
+      <c r="T25">
         <f t="shared" si="3"/>
-        <v>47.138888888888886</v>
-      </c>
-      <c r="V22">
+        <v>6.8558400000000024</v>
+      </c>
+      <c r="U25">
         <f t="shared" si="3"/>
-        <v>49.472222222222214</v>
-      </c>
-      <c r="W22">
+        <v>8.0460900000000031</v>
+      </c>
+      <c r="V25">
         <f t="shared" si="3"/>
-        <v>51.80555555555555</v>
-      </c>
-      <c r="X22">
+        <v>9.3315600000000032</v>
+      </c>
+      <c r="W25">
         <f t="shared" si="3"/>
-        <v>54.138888888888886</v>
-      </c>
-      <c r="Y22">
+        <v>10.712250000000006</v>
+      </c>
+      <c r="X25">
         <f t="shared" si="3"/>
-        <v>56.472222222222214</v>
-      </c>
-      <c r="Z22">
+        <v>12.188160000000009</v>
+      </c>
+      <c r="Y25">
         <f t="shared" si="3"/>
-        <v>58.80555555555555</v>
-      </c>
-      <c r="AA22">
+        <v>13.759290000000009</v>
+      </c>
+      <c r="Z25">
         <f t="shared" si="3"/>
-        <v>61.138888888888886</v>
-      </c>
-      <c r="AB22">
+        <v>15.42080000000001</v>
+      </c>
+      <c r="AA25">
         <f t="shared" si="3"/>
-        <v>63.472222222222214</v>
-      </c>
-      <c r="AC22">
+        <v>17.104400000000012</v>
+      </c>
+      <c r="AB25">
         <f t="shared" si="3"/>
-        <v>65.805555555555543</v>
-      </c>
-      <c r="AD22">
+        <v>18.788000000000014</v>
+      </c>
+      <c r="AC25">
         <f t="shared" si="3"/>
-        <v>68.138888888888872</v>
-      </c>
-      <c r="AE22">
+        <v>20.471600000000016</v>
+      </c>
+      <c r="AD25">
         <f t="shared" si="3"/>
-        <v>70.4722222222222</v>
-      </c>
-      <c r="AF22">
+        <v>22.155200000000015</v>
+      </c>
+      <c r="AE25">
         <f t="shared" si="3"/>
-        <v>72.805555555555543</v>
-      </c>
-      <c r="AG22">
+        <v>23.83880000000002</v>
+      </c>
+      <c r="AF25">
         <f t="shared" si="3"/>
-        <v>75.138888888888872</v>
-      </c>
-      <c r="AH22">
+        <v>25.522400000000019</v>
+      </c>
+      <c r="AG25">
         <f t="shared" si="3"/>
-        <v>77.4722222222222</v>
-      </c>
-      <c r="AI22">
+        <v>27.206000000000021</v>
+      </c>
+      <c r="AH25">
         <f t="shared" si="3"/>
-        <v>79.805555555555543</v>
-      </c>
-      <c r="AJ22">
+        <v>28.889600000000023</v>
+      </c>
+      <c r="AI25">
         <f t="shared" si="3"/>
-        <v>82.138888888888872</v>
-      </c>
-      <c r="AK22">
+        <v>30.573200000000021</v>
+      </c>
+      <c r="AJ25">
         <f t="shared" si="3"/>
-        <v>84.4722222222222</v>
-      </c>
-      <c r="AL22">
+        <v>32.256800000000027</v>
+      </c>
+      <c r="AK25">
         <f t="shared" si="3"/>
-        <v>86.805555555555543</v>
-      </c>
-      <c r="AM22">
+        <v>33.940400000000025</v>
+      </c>
+      <c r="AL25">
         <f t="shared" si="3"/>
-        <v>89.138888888888872</v>
-      </c>
-      <c r="AN22">
+        <v>35.624000000000024</v>
+      </c>
+      <c r="AM25">
         <f t="shared" si="3"/>
-        <v>91.4722222222222</v>
-      </c>
-      <c r="AO22">
-        <f t="shared" si="3"/>
-        <v>93.805555555555543</v>
-      </c>
-      <c r="AP22">
-        <f t="shared" si="3"/>
-        <v>96.138888888888872</v>
-      </c>
-      <c r="AQ22">
-        <f t="shared" si="3"/>
-        <v>98.4722222222222</v>
-      </c>
-      <c r="AR22">
-        <f t="shared" si="3"/>
-        <v>100.80555555555554</v>
-      </c>
-      <c r="AS22">
-        <f t="shared" si="3"/>
-        <v>103.13888888888887</v>
-      </c>
-      <c r="AT22">
-        <f t="shared" si="3"/>
-        <v>105.4722222222222</v>
-      </c>
-      <c r="AU22">
-        <f t="shared" si="3"/>
-        <v>107.80555555555553</v>
-      </c>
-      <c r="AV22">
-        <f t="shared" si="3"/>
-        <v>110.13888888888887</v>
-      </c>
-      <c r="AW22">
-        <f t="shared" si="3"/>
-        <v>112.4722222222222</v>
-      </c>
-      <c r="AX22">
-        <f t="shared" si="3"/>
-        <v>114.80555555555553</v>
-      </c>
-      <c r="AY22">
-        <f t="shared" si="3"/>
-        <v>117.13888888888887</v>
-      </c>
-      <c r="AZ22">
-        <f t="shared" si="3"/>
-        <v>119.4722222222222</v>
-      </c>
-      <c r="BA22">
-        <f t="shared" si="3"/>
-        <v>121.80555555555553</v>
-      </c>
-      <c r="BB22">
-        <f t="shared" si="3"/>
-        <v>124.13888888888886</v>
-      </c>
-      <c r="BC22">
-        <f t="shared" si="3"/>
-        <v>126.4722222222222</v>
-      </c>
-      <c r="BD22">
-        <f t="shared" si="3"/>
-        <v>128.80555555555554</v>
-      </c>
-      <c r="BE22">
-        <f t="shared" si="3"/>
-        <v>131.13888888888886</v>
-      </c>
-      <c r="BF22">
-        <f t="shared" si="3"/>
-        <v>133.33333333333331</v>
+        <v>37.307600000000029</v>
+      </c>
+      <c r="AN25">
+        <f t="shared" ref="AN25:BF25" si="4">IF(AN23&lt;$B$21,
+$B$3*AN23+SIGN($B$15)*0.5*$B$7*AN23*AN23,
+IF(AN23&lt;$B$22,
+$B$3*$B$21+SIGN($B$15)*0.5*$B$7*$B$21*$B$21+(AN23-$B$21)*$B$17,
+$B$3*$B$21+SIGN($B$15)*0.5*$B$7*$B$21*$B$21+($B$22-$B$21)*$B$17 + $B$17*(AN23-$B$22) + SIGN($B$16)*0.5*$B$7*(AN23-$B$22)*(AN23-$B$22)))</f>
+        <v>38.991200000000035</v>
+      </c>
+      <c r="AO25">
+        <f t="shared" si="4"/>
+        <v>40.652710000000035</v>
+      </c>
+      <c r="AP25">
+        <f t="shared" si="4"/>
+        <v>42.223840000000031</v>
+      </c>
+      <c r="AQ25">
+        <f t="shared" si="4"/>
+        <v>43.699750000000023</v>
+      </c>
+      <c r="AR25">
+        <f t="shared" si="4"/>
+        <v>45.080440000000031</v>
+      </c>
+      <c r="AS25">
+        <f t="shared" si="4"/>
+        <v>46.365910000000021</v>
+      </c>
+      <c r="AT25">
+        <f t="shared" si="4"/>
+        <v>47.556160000000027</v>
+      </c>
+      <c r="AU25">
+        <f t="shared" si="4"/>
+        <v>48.651190000000021</v>
+      </c>
+      <c r="AV25">
+        <f t="shared" si="4"/>
+        <v>49.65100000000001</v>
+      </c>
+      <c r="AW25">
+        <f t="shared" si="4"/>
+        <v>50.555590000000009</v>
+      </c>
+      <c r="AX25">
+        <f t="shared" si="4"/>
+        <v>51.364960000000011</v>
+      </c>
+      <c r="AY25">
+        <f t="shared" si="4"/>
+        <v>52.07911</v>
+      </c>
+      <c r="AZ25">
+        <f t="shared" si="4"/>
+        <v>52.698039999999999</v>
+      </c>
+      <c r="BA25">
+        <f t="shared" si="4"/>
+        <v>53.22175</v>
+      </c>
+      <c r="BB25">
+        <f t="shared" si="4"/>
+        <v>53.650239999999997</v>
+      </c>
+      <c r="BC25">
+        <f t="shared" si="4"/>
+        <v>53.983509999999995</v>
+      </c>
+      <c r="BD25">
+        <f t="shared" si="4"/>
+        <v>54.221559999999997</v>
+      </c>
+      <c r="BE25">
+        <f t="shared" si="4"/>
+        <v>54.36439</v>
+      </c>
+      <c r="BF25">
+        <f t="shared" si="4"/>
+        <v>54.411999999999992</v>
       </c>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="B23" s="58"/>
-      <c r="H23">
-        <f>$B$3*$B$18+0.5*$B$7*$B$18*$B$18+(H20-ABS($B$12))*$B$14</f>
-        <v>50.416666666666671</v>
-      </c>
-      <c r="I23">
-        <f t="shared" ref="I23:BF23" si="4">$B$3*ABS($B$12)+0.5*$B$7*ABS($B$12)*ABS($B$12)+(I20-ABS($B$12))*$B$14</f>
-        <v>52.75</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="4"/>
-        <v>55.083333333333343</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="4"/>
-        <v>57.416666666666671</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="4"/>
-        <v>59.75</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="4"/>
-        <v>62.083333333333336</v>
-      </c>
-      <c r="N23">
-        <f t="shared" si="4"/>
-        <v>64.416666666666671</v>
-      </c>
-      <c r="O23">
-        <f t="shared" si="4"/>
-        <v>66.75</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="4"/>
-        <v>69.083333333333329</v>
-      </c>
-      <c r="Q23">
-        <f t="shared" si="4"/>
-        <v>71.416666666666671</v>
-      </c>
-      <c r="R23">
-        <f t="shared" si="4"/>
-        <v>73.75</v>
-      </c>
-      <c r="S23">
-        <f t="shared" si="4"/>
-        <v>76.083333333333329</v>
-      </c>
-      <c r="T23">
-        <f t="shared" si="4"/>
-        <v>78.416666666666671</v>
-      </c>
-      <c r="U23">
-        <f t="shared" si="4"/>
-        <v>80.75</v>
-      </c>
-      <c r="V23">
-        <f t="shared" si="4"/>
-        <v>83.083333333333329</v>
-      </c>
-      <c r="W23">
-        <f t="shared" si="4"/>
-        <v>85.416666666666657</v>
-      </c>
-      <c r="X23">
-        <f t="shared" si="4"/>
-        <v>87.75</v>
-      </c>
-      <c r="Y23">
-        <f t="shared" si="4"/>
-        <v>90.083333333333329</v>
-      </c>
-      <c r="Z23">
-        <f t="shared" si="4"/>
-        <v>92.416666666666657</v>
-      </c>
-      <c r="AA23">
-        <f t="shared" si="4"/>
-        <v>94.75</v>
-      </c>
-      <c r="AB23">
-        <f t="shared" si="4"/>
-        <v>97.083333333333329</v>
-      </c>
-      <c r="AC23">
-        <f t="shared" si="4"/>
-        <v>99.416666666666657</v>
-      </c>
-      <c r="AD23">
-        <f t="shared" si="4"/>
-        <v>101.74999999999999</v>
-      </c>
-      <c r="AE23">
-        <f t="shared" si="4"/>
-        <v>104.08333333333331</v>
-      </c>
-      <c r="AF23">
-        <f t="shared" si="4"/>
-        <v>106.41666666666666</v>
-      </c>
-      <c r="AG23">
-        <f t="shared" si="4"/>
-        <v>108.74999999999999</v>
-      </c>
-      <c r="AH23">
-        <f t="shared" si="4"/>
-        <v>111.08333333333331</v>
-      </c>
-      <c r="AI23">
-        <f t="shared" si="4"/>
-        <v>113.41666666666666</v>
-      </c>
-      <c r="AJ23">
-        <f t="shared" si="4"/>
-        <v>115.74999999999999</v>
-      </c>
-      <c r="AK23">
-        <f t="shared" si="4"/>
-        <v>118.08333333333331</v>
-      </c>
-      <c r="AL23">
-        <f t="shared" si="4"/>
-        <v>120.41666666666666</v>
-      </c>
-      <c r="AM23">
-        <f t="shared" si="4"/>
-        <v>122.74999999999999</v>
-      </c>
-      <c r="AN23">
-        <f t="shared" si="4"/>
-        <v>125.08333333333331</v>
-      </c>
-      <c r="AO23">
-        <f t="shared" si="4"/>
-        <v>127.41666666666666</v>
-      </c>
-      <c r="AP23">
-        <f t="shared" si="4"/>
-        <v>129.75</v>
-      </c>
-      <c r="AQ23">
-        <f t="shared" si="4"/>
-        <v>132.08333333333331</v>
-      </c>
-      <c r="AR23">
-        <f t="shared" si="4"/>
-        <v>134.41666666666666</v>
-      </c>
-      <c r="AS23">
-        <f t="shared" si="4"/>
-        <v>136.75</v>
-      </c>
-      <c r="AT23">
-        <f t="shared" si="4"/>
-        <v>139.08333333333331</v>
-      </c>
-      <c r="AU23">
-        <f t="shared" si="4"/>
-        <v>141.41666666666663</v>
-      </c>
-      <c r="AV23">
-        <f t="shared" si="4"/>
-        <v>143.75</v>
-      </c>
-      <c r="AW23">
-        <f t="shared" si="4"/>
-        <v>146.08333333333331</v>
-      </c>
-      <c r="AX23">
-        <f t="shared" si="4"/>
-        <v>148.41666666666663</v>
-      </c>
-      <c r="AY23">
-        <f t="shared" si="4"/>
-        <v>150.75</v>
-      </c>
-      <c r="AZ23">
-        <f t="shared" si="4"/>
-        <v>153.08333333333331</v>
-      </c>
-      <c r="BA23">
-        <f t="shared" si="4"/>
-        <v>155.41666666666663</v>
-      </c>
-      <c r="BB23">
-        <f t="shared" si="4"/>
-        <v>157.74999999999997</v>
-      </c>
-      <c r="BC23">
-        <f t="shared" si="4"/>
-        <v>160.08333333333331</v>
-      </c>
-      <c r="BD23">
-        <f t="shared" si="4"/>
-        <v>162.41666666666663</v>
-      </c>
-      <c r="BE23">
-        <f t="shared" si="4"/>
-        <v>164.74999999999997</v>
-      </c>
-      <c r="BF23">
-        <f t="shared" si="4"/>
-        <v>167.08333333333331</v>
+    <row r="26" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="B26" s="58"/>
+      <c r="H26">
+        <f>$B$3*$B$21+0.5*$B$7*$B$21*$B$21+(H23-ABS($B$15))*$B$17</f>
+        <v>-14.884</v>
+      </c>
+      <c r="I26">
+        <f t="shared" ref="I26:AN26" si="5">$B$3*ABS($B$15)+0.5*$B$7*ABS($B$15)*ABS($B$15)+(I23-ABS($B$15))*$B$17</f>
+        <v>-13.200399999999998</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="5"/>
+        <v>-11.5168</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="5"/>
+        <v>-9.8331999999999979</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="5"/>
+        <v>-8.1495999999999995</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="5"/>
+        <v>-6.4659999999999975</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="5"/>
+        <v>-4.7823999999999991</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="5"/>
+        <v>-3.0988000000000007</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="5"/>
+        <v>-1.4152000000000022</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="5"/>
+        <v>0.26839999999999975</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="5"/>
+        <v>1.952</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="5"/>
+        <v>3.6356000000000019</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="5"/>
+        <v>5.3192000000000039</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="5"/>
+        <v>7.002800000000005</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="5"/>
+        <v>8.6864000000000061</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="5"/>
+        <v>10.370000000000008</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="5"/>
+        <v>12.053600000000008</v>
+      </c>
+      <c r="Y26">
+        <f t="shared" si="5"/>
+        <v>13.73720000000001</v>
+      </c>
+      <c r="Z26">
+        <f t="shared" si="5"/>
+        <v>15.42080000000001</v>
+      </c>
+      <c r="AA26">
+        <f t="shared" si="5"/>
+        <v>17.104400000000012</v>
+      </c>
+      <c r="AB26">
+        <f t="shared" si="5"/>
+        <v>18.788000000000014</v>
+      </c>
+      <c r="AC26">
+        <f t="shared" si="5"/>
+        <v>20.471600000000016</v>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="5"/>
+        <v>22.155200000000015</v>
+      </c>
+      <c r="AE26">
+        <f t="shared" si="5"/>
+        <v>23.83880000000002</v>
+      </c>
+      <c r="AF26">
+        <f t="shared" si="5"/>
+        <v>25.522400000000019</v>
+      </c>
+      <c r="AG26">
+        <f t="shared" si="5"/>
+        <v>27.206000000000021</v>
+      </c>
+      <c r="AH26">
+        <f t="shared" si="5"/>
+        <v>28.889600000000023</v>
+      </c>
+      <c r="AI26">
+        <f t="shared" si="5"/>
+        <v>30.573200000000021</v>
+      </c>
+      <c r="AJ26">
+        <f t="shared" si="5"/>
+        <v>32.256800000000027</v>
+      </c>
+      <c r="AK26">
+        <f t="shared" si="5"/>
+        <v>33.940400000000025</v>
+      </c>
+      <c r="AL26">
+        <f t="shared" si="5"/>
+        <v>35.624000000000024</v>
+      </c>
+      <c r="AM26">
+        <f t="shared" si="5"/>
+        <v>37.307600000000029</v>
+      </c>
+      <c r="AN26">
+        <f t="shared" si="5"/>
+        <v>38.991200000000035</v>
+      </c>
+      <c r="AO26">
+        <f t="shared" ref="AO26:BF26" si="6">$B$3*ABS($B$15)+0.5*$B$7*ABS($B$15)*ABS($B$15)+(AO23-ABS($B$15))*$B$17</f>
+        <v>40.674800000000033</v>
+      </c>
+      <c r="AP26">
+        <f t="shared" si="6"/>
+        <v>42.358400000000032</v>
+      </c>
+      <c r="AQ26">
+        <f t="shared" si="6"/>
+        <v>44.04200000000003</v>
+      </c>
+      <c r="AR26">
+        <f t="shared" si="6"/>
+        <v>45.725600000000036</v>
+      </c>
+      <c r="AS26">
+        <f t="shared" si="6"/>
+        <v>47.409200000000034</v>
+      </c>
+      <c r="AT26">
+        <f t="shared" si="6"/>
+        <v>49.09280000000004</v>
+      </c>
+      <c r="AU26">
+        <f t="shared" si="6"/>
+        <v>50.776400000000031</v>
+      </c>
+      <c r="AV26">
+        <f t="shared" si="6"/>
+        <v>52.460000000000029</v>
+      </c>
+      <c r="AW26">
+        <f t="shared" si="6"/>
+        <v>54.143600000000021</v>
+      </c>
+      <c r="AX26">
+        <f t="shared" si="6"/>
+        <v>55.827200000000019</v>
+      </c>
+      <c r="AY26">
+        <f t="shared" si="6"/>
+        <v>57.51080000000001</v>
+      </c>
+      <c r="AZ26">
+        <f t="shared" si="6"/>
+        <v>59.194400000000002</v>
+      </c>
+      <c r="BA26">
+        <f t="shared" si="6"/>
+        <v>60.878</v>
+      </c>
+      <c r="BB26">
+        <f t="shared" si="6"/>
+        <v>62.561599999999991</v>
+      </c>
+      <c r="BC26">
+        <f t="shared" si="6"/>
+        <v>64.245199999999983</v>
+      </c>
+      <c r="BD26">
+        <f t="shared" si="6"/>
+        <v>65.928799999999981</v>
+      </c>
+      <c r="BE26">
+        <f t="shared" si="6"/>
+        <v>67.61239999999998</v>
+      </c>
+      <c r="BF26">
+        <f t="shared" si="6"/>
+        <v>69.295999999999964</v>
       </c>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="B24" s="58"/>
+    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="B27" s="58"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Speed profile completely reworked
</commit_message>
<xml_diff>
--- a/theory/Kinematik.xlsx
+++ b/theory/Kinematik.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="127">
   <si>
     <r>
       <t>Hüfte (T</t>
@@ -840,9 +840,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>v</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1178,10 +1175,62 @@
     </r>
   </si>
   <si>
-    <t>Monotron</t>
+    <t>v monotron</t>
   </si>
   <si>
-    <t>Trapez</t>
+    <t>v Trapez</t>
+  </si>
+  <si>
+    <t>Monoton</t>
+  </si>
+  <si>
+    <t>vTrapez(t)</t>
+  </si>
+  <si>
+    <t>xMonoton(t)</t>
+  </si>
+  <si>
+    <t>Ramp-Up</t>
+  </si>
+  <si>
+    <t>v ramp up</t>
+  </si>
+  <si>
+    <t>rampup tges</t>
+  </si>
+  <si>
+    <t>max v  rampup</t>
+  </si>
+  <si>
+    <t>pos Trapez</t>
+  </si>
+  <si>
+    <t>min v ramp up</t>
+  </si>
+  <si>
+    <t>neg Trapez</t>
+  </si>
+  <si>
+    <r>
+      <t>min t</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>g</t>
+    </r>
+  </si>
+  <si>
+    <t>peak</t>
+  </si>
+  <si>
+    <t>peakdown</t>
   </si>
 </sst>
 </file>
@@ -1489,7 +1538,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1630,6 +1679,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -1764,11 +1814,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="428522608"/>
-        <c:axId val="428525352"/>
+        <c:axId val="326751456"/>
+        <c:axId val="326751064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="428522608"/>
+        <c:axId val="326751456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1806,13 +1856,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="428525352"/>
+        <c:crossAx val="326751064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="428525352"/>
+        <c:axId val="326751064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1851,7 +1901,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="428522608"/>
+        <c:crossAx val="326751456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
@@ -1947,11 +1997,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="428519864"/>
-        <c:axId val="337497864"/>
+        <c:axId val="326752240"/>
+        <c:axId val="326752632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="428519864"/>
+        <c:axId val="326752240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -1963,13 +2013,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="337497864"/>
+        <c:crossAx val="326752632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="337497864"/>
+        <c:axId val="326752632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -1982,7 +2032,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="428519864"/>
+        <c:crossAx val="326752240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
@@ -2049,26 +2099,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2077,8 +2107,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.0344925634295714E-2"/>
-          <c:y val="0.16245364030583134"/>
+          <c:x val="8.670603674540682E-2"/>
+          <c:y val="1.90111225850867E-2"/>
           <c:w val="0.86987729658792656"/>
           <c:h val="0.6714577865266842"/>
         </c:manualLayout>
@@ -2089,6 +2119,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Monoton</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -2115,7 +2148,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Trajectory Speed profile'!$H$15:$K$15</c:f>
+              <c:f>'Trajectory Speed profile'!$M$16:$P$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2123,34 +2156,134 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>900</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>1100</c:v>
+                  <c:v>4125</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>4000</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Trajectory Speed profile'!$H$16:$K$16</c:f>
+              <c:f>'Trajectory Speed profile'!$M$17:$P$17</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Trapez</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Trajectory Speed profile'!$M$18:$P$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.45</c:v>
+                  <c:v>261.38721247416942</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000">
+                  <c:v>4261.3872124741692</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Trajectory Speed profile'!$M$19:$P$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23069360623708471</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.45</c:v>
+                  <c:v>0.23069360623708471</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>1</c:v>
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Ramp Up</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Trajectory Speed profile'!$M$21:$P$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Trajectory Speed profile'!$M$22:$P$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2165,11 +2298,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="320599176"/>
-        <c:axId val="320599960"/>
+        <c:axId val="326750280"/>
+        <c:axId val="326750672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="320599176"/>
+        <c:axId val="326750280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2212,12 +2345,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="320599960"/>
+        <c:crossAx val="326750672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="320599960"/>
+        <c:axId val="326750672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2268,7 +2401,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="320599176"/>
+        <c:crossAx val="326750280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2469,324 +2602,321 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Trajectory Speed profile'!$H$24:$BF$24</c:f>
+              <c:f>'Trajectory Speed profile'!$K$28:$BH$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="51"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>160</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>240</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>320</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>400</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>480</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>560</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>640</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>720</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>800</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>880</c:v>
+                  <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>960</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1040</c:v>
+                  <c:v>1300</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1120</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1200</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1280</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1360</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1440</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1520</c:v>
+                  <c:v>1900</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1600</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1680</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1760</c:v>
+                  <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1840</c:v>
+                  <c:v>2300</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1920</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2000</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2080</c:v>
+                  <c:v>2600</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2160</c:v>
+                  <c:v>2700</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2240</c:v>
+                  <c:v>2800</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2320</c:v>
+                  <c:v>2900</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2400</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2480</c:v>
+                  <c:v>3100</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2560</c:v>
+                  <c:v>3200</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2640</c:v>
+                  <c:v>3300</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2720</c:v>
+                  <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2800</c:v>
+                  <c:v>3500</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2880</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2960</c:v>
+                  <c:v>3700</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3040</c:v>
+                  <c:v>3800</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3120</c:v>
+                  <c:v>3900</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3200</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3280</c:v>
+                  <c:v>4100</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3360</c:v>
+                  <c:v>4200</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3440</c:v>
+                  <c:v>4300</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3520</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3600</c:v>
+                  <c:v>4500</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3680</c:v>
+                  <c:v>4600</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3760</c:v>
+                  <c:v>4700</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3840</c:v>
+                  <c:v>4800</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3920</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>4000</c:v>
+                  <c:v>4900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Trajectory Speed profile'!$H$25:$BF$25</c:f>
+              <c:f>'Trajectory Speed profile'!$J$29:$BH$29</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.04</c:v>
+                  <c:v>0.15000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.08</c:v>
+                  <c:v>0.15000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.12</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.16</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.2</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.24</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.28000000000000003</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.32</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.36</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.4</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.44</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.45</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.45</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.44</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.4</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.36</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.32</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.28000000000000003</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.24000000000000002</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.2</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.16000000000000003</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.12</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-8.0000000000000016E-2</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-3.999999999999998E-2</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.999999999999998E-2</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8.0000000000000016E-2</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.12000000000000005</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.15999999999999998</c:v>
+                  <c:v>0.16250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v>0.2</c:v>
                 </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.24000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.27999999999999997</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.32</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.36000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.39999999999999997</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.44</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.48000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.52</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.56000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.60000000000000009</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.64000000000000012</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.68000000000000016</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.72</c:v>
-                </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.76</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.8</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.84000000000000008</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.88000000000000012</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.92000000000000015</c:v>
+                  <c:v>0.45000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.96</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2801,11 +2931,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="430887976"/>
-        <c:axId val="430888760"/>
+        <c:axId val="326912360"/>
+        <c:axId val="326912752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="430887976"/>
+        <c:axId val="326912360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2856,12 +2986,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430888760"/>
+        <c:crossAx val="326912752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="430888760"/>
+        <c:axId val="326912752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2912,7 +3042,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430887976"/>
+        <c:crossAx val="326912360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3136,7 +3266,166 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Trajectory Speed profile'!$H$24:$BF$24</c:f>
+              <c:f>'Trajectory Speed profile'!$K$28:$BH$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3100</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3800</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3900</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4400</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4700</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4800</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Trajectory Speed profile'!$J$30:$BH$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -3144,316 +3433,154 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>160</c:v>
+                  <c:v>28.59375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>240</c:v>
+                  <c:v>28.59375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>320</c:v>
+                  <c:v>44.84375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>400</c:v>
+                  <c:v>61.09375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>480</c:v>
+                  <c:v>77.34375</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>560</c:v>
+                  <c:v>93.59375</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>640</c:v>
+                  <c:v>109.84375</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>720</c:v>
+                  <c:v>126.09375</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>142.34375</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>158.59375</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>174.84375</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>191.09375</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>207.34375</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>223.59375</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>239.84375</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>256.09375</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>272.34375</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>288.59375</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>304.84375</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>321.09375</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>337.34375</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>353.59375</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>369.84375</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>386.09375</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>402.34375</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>418.59375</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>434.84375</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>451.09375</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>467.34375</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>483.59375</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>499.84375</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>516.09375</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>532.34375</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>548.59375</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>564.84375</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>581.09375</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>597.34375</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>613.59375</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>629.84375</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>646.09375</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>662.34375</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>702.5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>762.5</c:v>
+                </c:pt>
+                <c:pt idx="47">
                   <c:v>800</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>880</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>960</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1040</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1120</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1280</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1360</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1440</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1520</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1600</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1680</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1760</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1840</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1920</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2080</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2160</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2240</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2320</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2400</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2480</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2560</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2640</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2720</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2800</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2880</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2960</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>3040</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>3120</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>3200</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>3280</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>3360</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>3440</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>3520</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>3600</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>3680</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>3760</c:v>
-                </c:pt>
                 <c:pt idx="48">
-                  <c:v>3840</c:v>
+                  <c:v>842.5</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3920</c:v>
+                  <c:v>890</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Trajectory Speed profile'!$H$26:$BF$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="51"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-1.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-6.4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-14.399999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-25.6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-40</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-57.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-78.400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-102.4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-129.6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-160</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-193.6</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-229.5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-265.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-301.39999999999998</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-335</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-365.4</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-392.6</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-416.6</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-437.4</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-455</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-469.4</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-480.6</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-488.6</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-493.4</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-495</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>-493.4</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-488.59999999999997</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-480.59999999999997</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>-469.40000000000003</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>-455</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>-437.4</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>-416.6</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>-392.6</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>-365.4</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>-335</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>-301.39999999999998</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>-264.59999999999991</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>-224.60000000000002</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>-181.39999999999998</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>-135</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>-85.399999999999864</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>-32.599999999999909</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>23.399999999999864</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>82.599999999999909</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>210.60000000000014</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>279.40000000000009</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>351.40000000000009</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>426.59999999999991</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>505</c:v>
+                  <c:v>942.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3468,11 +3595,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="430888368"/>
-        <c:axId val="430889152"/>
+        <c:axId val="326913928"/>
+        <c:axId val="326915104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="430888368"/>
+        <c:axId val="326913928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3528,12 +3655,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430889152"/>
+        <c:crossAx val="326915104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="430889152"/>
+        <c:axId val="326915104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3589,7 +3716,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430888368"/>
+        <c:crossAx val="326913928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3752,563 +3879,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="244">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4828,7 +4399,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -29672,16 +29243,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>34290</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>643890</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -29702,15 +29273,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>784860</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -29734,15 +29305,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>708660</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -33225,10 +32796,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BR28"/>
+  <dimension ref="A1:BT32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33236,60 +32807,56 @@
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3">
+        <v>0.1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>85</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4">
+        <v>0.6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>87</v>
       </c>
+      <c r="B5">
+        <v>1000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>87</v>
+    <row r="6" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6">
+        <v>5000</v>
+      </c>
+      <c r="C6" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5">
-        <v>100</v>
-      </c>
-      <c r="C5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5">
-        <f>$B$3*$B$22+SIGN($B$16)*0.5*$B$7*$B$22*$B$22+($B$23-$B$22)*$B$18 + $B$18*(B6-$B$23) + SIGN($B$17)*0.5*$B$7*(B6-$B$23)*(B6-$B$23)</f>
-        <v>505</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6">
-        <v>4000</v>
-      </c>
-      <c r="C6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -33297,1084 +32864,1346 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B9">
         <f>B5/B6</f>
-        <v>2.5000000000000001E-2</v>
+        <v>0.2</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10">
+        <f>(B3-B4)/B7</f>
+        <v>-1000</v>
+      </c>
+      <c r="F10">
+        <f>(B3-B4)/B7</f>
+        <v>-1000</v>
+      </c>
+      <c r="G10">
+        <f>(B3-B4)/B7</f>
+        <v>-1000</v>
+      </c>
+      <c r="H10">
+        <f>(B3-B4)/B7</f>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>110</v>
       </c>
-      <c r="B10">
-        <f>(B3-B4)/B7</f>
-        <v>-2000</v>
+      <c r="E11" s="127">
+        <f>B3*B6-0.5*B7*E10*E10 - B5</f>
+        <v>-750</v>
+      </c>
+      <c r="F11">
+        <f>B3*B6+0.5*B7*F10*F10 - B5</f>
+        <v>-250</v>
+      </c>
+      <c r="G11">
+        <f>B4*G10+0.5*B7*G10*G10- B5</f>
+        <v>-1350</v>
+      </c>
+      <c r="H11">
+        <f>-B4*G10-0.5*B7*G10*G10- B5</f>
+        <v>-650</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11">
+        <f>-B5*B7-0.5*B3*B3</f>
+        <v>-0.505</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11">
-        <f>B3*B6-0.5*B7*B10*B10 - B5</f>
-        <v>-1100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>73</v>
       </c>
-      <c r="B12">
-        <f>B7*B6-B7*B10</f>
+      <c r="E12">
+        <f>B7*(B6-E10)</f>
         <v>3</v>
       </c>
+      <c r="F12">
+        <f>B7*(B6+F10)</f>
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <f>B3+B4+B7*G10</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="H12">
+        <f>B3+B4+B7*G10</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="L12">
+        <f>B3</f>
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>71</v>
       </c>
-      <c r="B13">
+      <c r="E13">
         <f>-B7</f>
         <v>-5.0000000000000001E-4</v>
       </c>
-      <c r="C13">
-        <f>B12*B12-4*B13*B11</f>
-        <v>6.8</v>
+      <c r="F13">
+        <f>B7</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G13">
+        <f>B7</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H13">
+        <f>-B7</f>
+        <v>-5.0000000000000001E-4</v>
+      </c>
+      <c r="L13">
+        <f>0.5</f>
+        <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>105</v>
-      </c>
-      <c r="B14" s="60">
-        <f>(-B12+SQRT(B12*B12-4*B13*B11))/(2*B13)</f>
-        <v>392.31903791894052</v>
-      </c>
-      <c r="C14" s="60">
-        <f>(-B12-SQRT(B12*B12-4*B13*B11))/(2*B13)</f>
-        <v>5607.6809620810591</v>
-      </c>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
+      <c r="L16" t="s">
+        <v>88</v>
+      </c>
+      <c r="M16">
         <v>0</v>
       </c>
-      <c r="I15" s="4">
-        <f>ABS(B16)</f>
-        <v>900</v>
-      </c>
-      <c r="J15" s="3">
-        <f>B6-ABS(B17)</f>
-        <v>1100</v>
-      </c>
-      <c r="K15">
+      <c r="N16" s="4">
+        <f>B26</f>
+        <v>125</v>
+      </c>
+      <c r="O16" s="3">
+        <f>B27</f>
+        <v>4125</v>
+      </c>
+      <c r="P16">
         <f>B6</f>
-        <v>4000</v>
+        <v>5000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="17" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" t="s">
+        <v>123</v>
+      </c>
+      <c r="G17" t="s">
+        <v>125</v>
+      </c>
+      <c r="H17" t="s">
+        <v>126</v>
+      </c>
+      <c r="I17" t="s">
+        <v>117</v>
+      </c>
+      <c r="L17" t="s">
+        <v>112</v>
+      </c>
+      <c r="M17">
+        <f>B3</f>
+        <v>0.1</v>
+      </c>
+      <c r="N17" s="3">
+        <f>B21</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="O17" s="3">
+        <f>N17</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="P17">
+        <f>B4</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="127">
+        <f>(B5-B3*B6-0.5*(B4-B3)*(B4-B3)/B7)/(B6*B7+(B3-B4))</f>
+        <v>125</v>
+      </c>
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="3">
+        <f>(-E12+SQRT(E12*E12-4*E13*E11))/(2*E13)</f>
+        <v>261.38721247416942</v>
+      </c>
+      <c r="F18" s="130">
+        <f>(-F12+SQRT(F12*F12-4*F13*F11))/(2*F13)</f>
+        <v>121.32034355964238</v>
+      </c>
+      <c r="G18" s="3">
+        <f>(-G12+SQRT(G12*G12-4*G13*G11))/(2*G13)</f>
+        <v>1455.2945357246849</v>
+      </c>
+      <c r="H18" s="3" t="e">
+        <f>-(-H12+SQRT(H12*H12-4*H13*H11))/(2*H13)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="I18" s="127">
+        <f>(B4-B3)/B7</f>
+        <v>1000</v>
+      </c>
+      <c r="L18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4">
+        <f>E26</f>
+        <v>261.38721247416942</v>
+      </c>
+      <c r="O18" s="3">
+        <f>E27</f>
+        <v>4261.3872124741692</v>
+      </c>
+      <c r="P18">
+        <f>B6</f>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="127">
-        <f>IF(OR(AND(B3&lt;B9,B9&lt;B4), AND(B3&gt;=B9,B9&gt;=B4)),E16,E17)</f>
-        <v>-900</v>
-      </c>
-      <c r="C16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" s="127">
-        <f>(B5-B3*B6-0.5*(B4-B3)*(B4-B3)/B7)/(B6*B7+(B3-B4))</f>
-        <v>-900</v>
-      </c>
-      <c r="G16" t="s">
-        <v>84</v>
-      </c>
-      <c r="H16">
-        <f>B3</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="3">
-        <f>B18</f>
-        <v>-0.45</v>
-      </c>
-      <c r="J16" s="3">
-        <f>I16</f>
-        <v>-0.45</v>
-      </c>
-      <c r="K16">
-        <f>B4</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:70" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B17" s="3">
-        <f>(B4-B3)/B7-B16</f>
-        <v>2900</v>
-      </c>
-      <c r="C17" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="75" t="s">
-        <v>114</v>
-      </c>
-      <c r="E17" s="127">
-        <f>(-B12+SQRT(B12*B12-4*B13*B11))/(2*B13)</f>
-        <v>392.31903791894052</v>
-      </c>
-    </row>
-    <row r="18" spans="1:70" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>97</v>
-      </c>
-      <c r="B18" s="3">
-        <f>B3+B7*B16</f>
-        <v>-0.45</v>
-      </c>
-      <c r="C18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" s="127">
-        <f>(B3+B18)/2*B16+B18*(B6-B16-B17)+(B18+B4)/2*B17</f>
-        <v>100.00000000000011</v>
+      <c r="B19" s="3">
+        <f>(B4-B3)/B7-B18</f>
+        <v>875</v>
       </c>
       <c r="C19" t="s">
         <v>91</v>
       </c>
+      <c r="D19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="3">
+        <f>(B4-B3)/B7-E18</f>
+        <v>738.61278752583053</v>
+      </c>
+      <c r="F19" s="3">
+        <f>(B4-B3)/B7-F18</f>
+        <v>878.67965644035758</v>
+      </c>
+      <c r="G19" s="127">
+        <f>-(G10+G18)</f>
+        <v>-455.29453572468492</v>
+      </c>
+      <c r="H19" s="127" t="e">
+        <f>-(H10+H18)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="I19" s="127">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>113</v>
+      </c>
+      <c r="M19">
+        <f>B3</f>
+        <v>0.1</v>
+      </c>
+      <c r="N19" s="3">
+        <f>E21</f>
+        <v>0.23069360623708471</v>
+      </c>
+      <c r="O19" s="3">
+        <f>N19</f>
+        <v>0.23069360623708471</v>
+      </c>
+      <c r="P19">
+        <f>B4</f>
+        <v>0.6</v>
+      </c>
     </row>
-    <row r="20" spans="1:70" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="127">
+        <f>ABS(G18)+ABS(G19)</f>
+        <v>1910.5890714493698</v>
+      </c>
+      <c r="H20" s="127" t="e">
+        <f>ABS(H18)+ABS(H19)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="I20" s="127"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+    </row>
+    <row r="21" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="3">
+        <f>B3+B7*B18</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="C21" t="s">
         <v>86</v>
       </c>
-      <c r="B20">
-        <f>B18+B17*B7</f>
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>87</v>
+      <c r="D21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="3">
+        <f>B3+B7*E18</f>
+        <v>0.23069360623708471</v>
+      </c>
+      <c r="F21" s="3">
+        <f>B3+B7*F18</f>
+        <v>0.1606601717798212</v>
+      </c>
+      <c r="G21">
+        <f>B3+B7*G18</f>
+        <v>0.82764726786234244</v>
+      </c>
+      <c r="H21" t="e">
+        <f>B3+B7*H18</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="I21" s="3">
+        <f>B3+B7*I18</f>
+        <v>0.6</v>
+      </c>
+      <c r="L21" t="s">
+        <v>88</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21" s="4">
+        <f>I26</f>
+        <v>1000</v>
+      </c>
+      <c r="O21" s="3">
+        <f>I27</f>
+        <v>5000</v>
+      </c>
+      <c r="P21">
+        <f>B6</f>
+        <v>5000</v>
       </c>
     </row>
-    <row r="22" spans="1:70" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="127">
+        <f>$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(B6-$B$27) + SIGN($B$19)*0.5*$B$7*(B6-$B$27)*(B6-$B$27)</f>
+        <v>1000</v>
+      </c>
+      <c r="C22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="127">
+        <f>$B$3*$E$26+SIGN($E$18)*0.5*$B$7*$E$26*$E$26+($E$27-$E$26)*$E$21 + $E$21*(B6-$E$27) + SIGN($E$19)*0.5*$B$7*(B6-$E$27)*(B6-$E$27)</f>
+        <v>1272.7744249483389</v>
+      </c>
+      <c r="F22" s="127">
+        <f>$B$3*$F$26+SIGN($F$18)*0.5*$B$7*$F$26*$F$26+($F$27-$F$26)*$F$21 + $F$21*(B6-$F$27) + SIGN($F$19)*0.5*$B$7*(B6-$F$27)*(B6-$F$27)</f>
+        <v>992.64068711928485</v>
+      </c>
+      <c r="G22" s="127">
+        <f>$B$3*$G$26+SIGN($G$18)*0.5*$B$7*$G$26*$G$26+($G$27-$G$26)*$G$21 + $G$21*(G20-$G$27) + SIGN($G$19)*0.5*$B$7*(G20-$G$27)*(G20-$G$27)</f>
+        <v>1000.0000000000001</v>
+      </c>
+      <c r="H22" s="127" t="e">
+        <f>$B$3*$H$26+SIGN($H$18)*0.5*$B$7*$H$26*$H$26+($H$27-$H$26)*$H$21 + $H$21*(H20-$H$27) + SIGN($H$19)*0.5*$B$7*(H20-$H$27)*(H20-$H$27)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="I22">
+        <f>$B$3*$I$26+SIGN($I$18)*0.5*$B$7*$I$26*$I$26+($I$27-$I$26)*$I$21 + $I$21*(B6-$I$27) + SIGN($I$19)*0.5*$B$7*(B6-$I$27)*(B6-$I$27)</f>
+        <v>2750</v>
+      </c>
+      <c r="J22" t="s">
+        <v>119</v>
+      </c>
+      <c r="K22">
+        <f>(B5-B3*I18-0.5*B7*I18*I18)/B4+I18</f>
+        <v>2083.3333333333335</v>
+      </c>
+      <c r="L22" t="s">
+        <v>118</v>
+      </c>
+      <c r="M22">
+        <f>B3</f>
+        <v>0.1</v>
+      </c>
+      <c r="N22" s="3">
+        <f>I21</f>
+        <v>0.6</v>
+      </c>
+      <c r="O22" s="3">
+        <f>I21</f>
+        <v>0.6</v>
+      </c>
+      <c r="P22" s="3">
+        <f>I21</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23">
+        <f>B21+B19*B7</f>
+        <v>0.6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="3">
+        <f>E21+E19*B7</f>
+        <v>0.6</v>
+      </c>
+      <c r="F23" s="3">
+        <f>F21+F19*B7</f>
+        <v>0.6</v>
+      </c>
+      <c r="G23" s="3">
+        <f>G21+G19*B7</f>
+        <v>0.6</v>
+      </c>
+      <c r="H23" s="3" t="e">
+        <f>H21+H19*B7</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="I23" s="3">
+        <f>I21+I19*B7</f>
+        <v>0.6</v>
+      </c>
+      <c r="J23" t="s">
+        <v>120</v>
+      </c>
+      <c r="K23" s="3">
+        <f>SQRT(B3*B3 +2*B5*B7)</f>
+        <v>1.004987562112089</v>
+      </c>
+    </row>
+    <row r="24" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24">
+        <f>(B5+0.5*B7*E10*E10)/B3</f>
+        <v>12500</v>
+      </c>
+      <c r="J24" t="s">
+        <v>122</v>
+      </c>
+      <c r="K24" s="3" t="e">
+        <f>SQRT(B3*B3 -2*B5*B7)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26" s="127">
+        <f>ABS(B18)</f>
+        <v>125</v>
+      </c>
+      <c r="C26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="127">
+        <f>ABS(E18)</f>
+        <v>261.38721247416942</v>
+      </c>
+      <c r="F26" s="127">
+        <f>ABS(F18)</f>
+        <v>121.32034355964238</v>
+      </c>
+      <c r="G26" s="127">
+        <f>ABS(G18)</f>
+        <v>1455.2945357246849</v>
+      </c>
+      <c r="H26" s="127" t="e">
+        <f>ABS(H18)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="I26" s="127">
+        <f>ABS(I18)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="127">
-        <f>ABS(B16)</f>
-        <v>900</v>
-      </c>
-      <c r="C22" t="s">
-        <v>92</v>
+      <c r="B27" s="127">
+        <f>B6-ABS(B19)</f>
+        <v>4125</v>
+      </c>
+      <c r="C27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="127">
+        <f>B6-ABS(E19)</f>
+        <v>4261.3872124741692</v>
+      </c>
+      <c r="F27" s="127">
+        <f>B6-ABS(F19)</f>
+        <v>4121.3203435596424</v>
+      </c>
+      <c r="G27" s="127">
+        <f>G26</f>
+        <v>1455.2945357246849</v>
+      </c>
+      <c r="H27" s="127" t="e">
+        <f>H26</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="I27" s="127">
+        <f>B6-ABS(I19)</f>
+        <v>5000</v>
       </c>
     </row>
-    <row r="23" spans="1:70" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>109</v>
-      </c>
-      <c r="B23" s="127">
-        <f>B6-ABS(B17)</f>
-        <v>1100</v>
-      </c>
-      <c r="C23" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:70" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A24" s="128" t="s">
+    <row r="28" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A28" s="128" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" t="s">
         <v>99</v>
       </c>
-      <c r="B24" t="s">
+      <c r="J28" t="s">
+        <v>104</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f>(K28+$B$6/50)</f>
         <v>100</v>
       </c>
-      <c r="G24" t="s">
-        <v>105</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <f>(H24+$B$6/50)</f>
-        <v>80</v>
-      </c>
-      <c r="J24">
-        <f t="shared" ref="J24:BF24" si="0">(I24+$B$6/50)</f>
-        <v>160</v>
-      </c>
-      <c r="K24">
+      <c r="M28">
+        <f t="shared" ref="M28:BH28" si="0">(L28+$B$6/50)</f>
+        <v>200</v>
+      </c>
+      <c r="N28">
         <f t="shared" si="0"/>
-        <v>240</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="0"/>
-        <v>320</v>
-      </c>
-      <c r="M24">
+        <v>300</v>
+      </c>
+      <c r="O28">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="N24">
+      <c r="P28">
         <f t="shared" si="0"/>
-        <v>480</v>
-      </c>
-      <c r="O24">
+        <v>500</v>
+      </c>
+      <c r="Q28">
         <f t="shared" si="0"/>
-        <v>560</v>
-      </c>
-      <c r="P24">
+        <v>600</v>
+      </c>
+      <c r="R28">
         <f t="shared" si="0"/>
-        <v>640</v>
-      </c>
-      <c r="Q24">
-        <f t="shared" si="0"/>
-        <v>720</v>
-      </c>
-      <c r="R24">
+        <v>700</v>
+      </c>
+      <c r="S28">
         <f t="shared" si="0"/>
         <v>800</v>
       </c>
-      <c r="S24">
+      <c r="T28">
         <f t="shared" si="0"/>
-        <v>880</v>
-      </c>
-      <c r="T24">
+        <v>900</v>
+      </c>
+      <c r="U28">
         <f t="shared" si="0"/>
-        <v>960</v>
-      </c>
-      <c r="U24">
+        <v>1000</v>
+      </c>
+      <c r="V28">
         <f t="shared" si="0"/>
-        <v>1040</v>
-      </c>
-      <c r="V24">
-        <f t="shared" si="0"/>
-        <v>1120</v>
-      </c>
-      <c r="W24">
+        <v>1100</v>
+      </c>
+      <c r="W28">
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
-      <c r="X24">
+      <c r="X28">
         <f t="shared" si="0"/>
-        <v>1280</v>
-      </c>
-      <c r="Y24">
+        <v>1300</v>
+      </c>
+      <c r="Y28">
         <f t="shared" si="0"/>
-        <v>1360</v>
-      </c>
-      <c r="Z24">
+        <v>1400</v>
+      </c>
+      <c r="Z28">
         <f t="shared" si="0"/>
-        <v>1440</v>
-      </c>
-      <c r="AA24">
-        <f t="shared" si="0"/>
-        <v>1520</v>
-      </c>
-      <c r="AB24">
+        <v>1500</v>
+      </c>
+      <c r="AA28">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-      <c r="AC24">
+      <c r="AB28">
         <f t="shared" si="0"/>
-        <v>1680</v>
-      </c>
-      <c r="AD24">
+        <v>1700</v>
+      </c>
+      <c r="AC28">
         <f t="shared" si="0"/>
-        <v>1760</v>
-      </c>
-      <c r="AE24">
+        <v>1800</v>
+      </c>
+      <c r="AD28">
         <f t="shared" si="0"/>
-        <v>1840</v>
-      </c>
-      <c r="AF24">
-        <f t="shared" si="0"/>
-        <v>1920</v>
-      </c>
-      <c r="AG24">
+        <v>1900</v>
+      </c>
+      <c r="AE28">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="AH24">
+      <c r="AF28">
         <f t="shared" si="0"/>
-        <v>2080</v>
-      </c>
-      <c r="AI24">
+        <v>2100</v>
+      </c>
+      <c r="AG28">
         <f t="shared" si="0"/>
-        <v>2160</v>
-      </c>
-      <c r="AJ24">
+        <v>2200</v>
+      </c>
+      <c r="AH28">
         <f t="shared" si="0"/>
-        <v>2240</v>
-      </c>
-      <c r="AK24">
-        <f t="shared" si="0"/>
-        <v>2320</v>
-      </c>
-      <c r="AL24">
+        <v>2300</v>
+      </c>
+      <c r="AI28">
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
-      <c r="AM24">
+      <c r="AJ28">
         <f t="shared" si="0"/>
-        <v>2480</v>
-      </c>
-      <c r="AN24">
+        <v>2500</v>
+      </c>
+      <c r="AK28">
         <f t="shared" si="0"/>
-        <v>2560</v>
-      </c>
-      <c r="AO24">
+        <v>2600</v>
+      </c>
+      <c r="AL28">
         <f t="shared" si="0"/>
-        <v>2640</v>
-      </c>
-      <c r="AP24">
-        <f t="shared" si="0"/>
-        <v>2720</v>
-      </c>
-      <c r="AQ24">
+        <v>2700</v>
+      </c>
+      <c r="AM28">
         <f t="shared" si="0"/>
         <v>2800</v>
       </c>
-      <c r="AR24">
+      <c r="AN28">
         <f t="shared" si="0"/>
-        <v>2880</v>
-      </c>
-      <c r="AS24">
+        <v>2900</v>
+      </c>
+      <c r="AO28">
         <f t="shared" si="0"/>
-        <v>2960</v>
-      </c>
-      <c r="AT24">
+        <v>3000</v>
+      </c>
+      <c r="AP28">
         <f t="shared" si="0"/>
-        <v>3040</v>
-      </c>
-      <c r="AU24">
-        <f t="shared" si="0"/>
-        <v>3120</v>
-      </c>
-      <c r="AV24">
+        <v>3100</v>
+      </c>
+      <c r="AQ28">
         <f t="shared" si="0"/>
         <v>3200</v>
       </c>
-      <c r="AW24">
+      <c r="AR28">
         <f t="shared" si="0"/>
-        <v>3280</v>
-      </c>
-      <c r="AX24">
+        <v>3300</v>
+      </c>
+      <c r="AS28">
         <f t="shared" si="0"/>
-        <v>3360</v>
-      </c>
-      <c r="AY24">
+        <v>3400</v>
+      </c>
+      <c r="AT28">
         <f t="shared" si="0"/>
-        <v>3440</v>
-      </c>
-      <c r="AZ24">
-        <f t="shared" si="0"/>
-        <v>3520</v>
-      </c>
-      <c r="BA24">
+        <v>3500</v>
+      </c>
+      <c r="AU28">
         <f t="shared" si="0"/>
         <v>3600</v>
       </c>
-      <c r="BB24">
+      <c r="AV28">
         <f t="shared" si="0"/>
-        <v>3680</v>
-      </c>
-      <c r="BC24">
+        <v>3700</v>
+      </c>
+      <c r="AW28">
         <f t="shared" si="0"/>
-        <v>3760</v>
-      </c>
-      <c r="BD24">
+        <v>3800</v>
+      </c>
+      <c r="AX28">
         <f t="shared" si="0"/>
-        <v>3840</v>
-      </c>
-      <c r="BE24">
-        <f t="shared" si="0"/>
-        <v>3920</v>
-      </c>
-      <c r="BF24">
+        <v>3900</v>
+      </c>
+      <c r="AY28">
         <f t="shared" si="0"/>
         <v>4000</v>
       </c>
+      <c r="AZ28">
+        <f t="shared" si="0"/>
+        <v>4100</v>
+      </c>
+      <c r="BA28">
+        <f t="shared" si="0"/>
+        <v>4200</v>
+      </c>
+      <c r="BB28">
+        <f t="shared" si="0"/>
+        <v>4300</v>
+      </c>
+      <c r="BC28">
+        <f t="shared" si="0"/>
+        <v>4400</v>
+      </c>
+      <c r="BD28">
+        <f t="shared" si="0"/>
+        <v>4500</v>
+      </c>
+      <c r="BE28">
+        <f t="shared" si="0"/>
+        <v>4600</v>
+      </c>
+      <c r="BF28">
+        <f t="shared" si="0"/>
+        <v>4700</v>
+      </c>
+      <c r="BG28">
+        <f t="shared" si="0"/>
+        <v>4800</v>
+      </c>
+      <c r="BH28">
+        <f t="shared" si="0"/>
+        <v>4900</v>
+      </c>
     </row>
-    <row r="25" spans="1:70" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A25" s="128" t="s">
+    <row r="29" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A29" s="128" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="129" t="s">
         <v>101</v>
       </c>
-      <c r="B25" s="129" t="s">
-        <v>102</v>
-      </c>
-      <c r="G25" t="s">
-        <v>106</v>
-      </c>
-      <c r="H25" s="127">
-        <f t="shared" ref="H25:AM25" si="1">IF(H24&lt;ABS($B$16),$B$3+SIGN($B$16)*H$24*$B$7,IF(H24&lt;$B$6-ABS($B$17),$B$18,$B$18+SIGN($B$17)*(H24-($B$6-ABS($B$17)))*$B$7))</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="127">
+      <c r="I29" t="s">
+        <v>105</v>
+      </c>
+      <c r="J29" s="127">
+        <f>IF(K28&lt;ABS($B$18),$B$3+SIGN($B$18)*K$28*$B$7,IF(K28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(K28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.1</v>
+      </c>
+      <c r="K29" s="127">
+        <f>IF(L28&lt;ABS($B$18),$B$3+SIGN($B$18)*L$28*$B$7,IF(L28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(L28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="L29" s="127">
+        <f>IF(L28&lt;ABS($B$18),$B$3+SIGN($B$18)*L$28*$B$7,IF(L28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(L28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="M29" s="127">
+        <f>IF(M28&lt;ABS($B$18),$B$3+SIGN($B$18)*M$28*$B$7,IF(M28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(M28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="N29" s="127">
+        <f>IF(N28&lt;ABS($B$18),$B$3+SIGN($B$18)*N$28*$B$7,IF(N28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(N28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="O29" s="127">
+        <f>IF(O28&lt;ABS($B$18),$B$3+SIGN($B$18)*O$28*$B$7,IF(O28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(O28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="P29" s="127">
+        <f>IF(P28&lt;ABS($B$18),$B$3+SIGN($B$18)*P$28*$B$7,IF(P28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(P28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="Q29" s="127">
+        <f>IF(Q28&lt;ABS($B$18),$B$3+SIGN($B$18)*Q$28*$B$7,IF(Q28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(Q28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="R29" s="127">
+        <f>IF(R28&lt;ABS($B$18),$B$3+SIGN($B$18)*R$28*$B$7,IF(R28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(R28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="S29" s="127">
+        <f>IF(S28&lt;ABS($B$18),$B$3+SIGN($B$18)*S$28*$B$7,IF(S28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(S28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="T29" s="127">
+        <f>IF(T28&lt;ABS($B$18),$B$3+SIGN($B$18)*T$28*$B$7,IF(T28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(T28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="U29" s="127">
+        <f>IF(U28&lt;ABS($B$18),$B$3+SIGN($B$18)*U$28*$B$7,IF(U28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(U28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="V29" s="127">
+        <f>IF(V28&lt;ABS($B$18),$B$3+SIGN($B$18)*V$28*$B$7,IF(V28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(V28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="W29" s="127">
+        <f>IF(W28&lt;ABS($B$18),$B$3+SIGN($B$18)*W$28*$B$7,IF(W28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(W28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="X29" s="127">
+        <f>IF(X28&lt;ABS($B$18),$B$3+SIGN($B$18)*X$28*$B$7,IF(X28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(X28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="Y29" s="127">
+        <f>IF(Y28&lt;ABS($B$18),$B$3+SIGN($B$18)*Y$28*$B$7,IF(Y28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(Y28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="Z29" s="127">
+        <f>IF(Z28&lt;ABS($B$18),$B$3+SIGN($B$18)*Z$28*$B$7,IF(Z28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(Z28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AA29" s="127">
+        <f>IF(AA28&lt;ABS($B$18),$B$3+SIGN($B$18)*AA$28*$B$7,IF(AA28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AA28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AB29" s="127">
+        <f>IF(AB28&lt;ABS($B$18),$B$3+SIGN($B$18)*AB$28*$B$7,IF(AB28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AB28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AC29" s="127">
+        <f>IF(AC28&lt;ABS($B$18),$B$3+SIGN($B$18)*AC$28*$B$7,IF(AC28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AC28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AD29" s="127">
+        <f>IF(AD28&lt;ABS($B$18),$B$3+SIGN($B$18)*AD$28*$B$7,IF(AD28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AD28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AE29" s="127">
+        <f>IF(AE28&lt;ABS($B$18),$B$3+SIGN($B$18)*AE$28*$B$7,IF(AE28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AE28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AF29" s="127">
+        <f>IF(AF28&lt;ABS($B$18),$B$3+SIGN($B$18)*AF$28*$B$7,IF(AF28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AF28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AG29" s="127">
+        <f>IF(AG28&lt;ABS($B$18),$B$3+SIGN($B$18)*AG$28*$B$7,IF(AG28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AG28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AH29" s="127">
+        <f>IF(AH28&lt;ABS($B$18),$B$3+SIGN($B$18)*AH$28*$B$7,IF(AH28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AH28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AI29" s="127">
+        <f>IF(AI28&lt;ABS($B$18),$B$3+SIGN($B$18)*AI$28*$B$7,IF(AI28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AI28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AJ29" s="127">
+        <f>IF(AJ28&lt;ABS($B$18),$B$3+SIGN($B$18)*AJ$28*$B$7,IF(AJ28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AJ28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AK29" s="127">
+        <f>IF(AK28&lt;ABS($B$18),$B$3+SIGN($B$18)*AK$28*$B$7,IF(AK28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AK28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AL29" s="127">
+        <f>IF(AL28&lt;ABS($B$18),$B$3+SIGN($B$18)*AL$28*$B$7,IF(AL28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AL28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AM29" s="127">
+        <f>IF(AM28&lt;ABS($B$18),$B$3+SIGN($B$18)*AM$28*$B$7,IF(AM28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AM28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AN29" s="127">
+        <f>IF(AN28&lt;ABS($B$18),$B$3+SIGN($B$18)*AN$28*$B$7,IF(AN28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AN28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AO29" s="127">
+        <f>IF(AO28&lt;ABS($B$18),$B$3+SIGN($B$18)*AO$28*$B$7,IF(AO28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AO28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AP29" s="127">
+        <f t="shared" ref="AP29:BH29" si="1">IF(AP28&lt;ABS($B$18),$B$3+SIGN($B$18)*AP$28*$B$7,IF(AP28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AP28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AQ29" s="127">
         <f t="shared" si="1"/>
-        <v>-0.04</v>
-      </c>
-      <c r="J25" s="127">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AR29" s="127">
         <f t="shared" si="1"/>
-        <v>-0.08</v>
-      </c>
-      <c r="K25" s="127">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AS29" s="127">
         <f t="shared" si="1"/>
-        <v>-0.12</v>
-      </c>
-      <c r="L25" s="127">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AT29" s="127">
         <f t="shared" si="1"/>
-        <v>-0.16</v>
-      </c>
-      <c r="M25" s="127">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AU29" s="127">
         <f t="shared" si="1"/>
-        <v>-0.2</v>
-      </c>
-      <c r="N25" s="127">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AV29" s="127">
         <f t="shared" si="1"/>
-        <v>-0.24</v>
-      </c>
-      <c r="O25" s="127">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AW29" s="127">
         <f t="shared" si="1"/>
-        <v>-0.28000000000000003</v>
-      </c>
-      <c r="P25" s="127">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AX29" s="127">
         <f t="shared" si="1"/>
-        <v>-0.32</v>
-      </c>
-      <c r="Q25" s="127">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AY29" s="127">
         <f t="shared" si="1"/>
-        <v>-0.36</v>
-      </c>
-      <c r="R25" s="127">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="AZ29" s="127">
         <f t="shared" si="1"/>
-        <v>-0.4</v>
-      </c>
-      <c r="S25" s="127">
-        <f t="shared" si="1"/>
-        <v>-0.44</v>
-      </c>
-      <c r="T25" s="127">
-        <f t="shared" si="1"/>
-        <v>-0.45</v>
-      </c>
-      <c r="U25" s="127">
-        <f t="shared" si="1"/>
-        <v>-0.45</v>
-      </c>
-      <c r="V25" s="127">
-        <f t="shared" si="1"/>
-        <v>-0.44</v>
-      </c>
-      <c r="W25" s="127">
-        <f t="shared" si="1"/>
-        <v>-0.4</v>
-      </c>
-      <c r="X25" s="127">
-        <f t="shared" si="1"/>
-        <v>-0.36</v>
-      </c>
-      <c r="Y25" s="127">
-        <f t="shared" si="1"/>
-        <v>-0.32</v>
-      </c>
-      <c r="Z25" s="127">
-        <f t="shared" si="1"/>
-        <v>-0.28000000000000003</v>
-      </c>
-      <c r="AA25" s="127">
-        <f t="shared" si="1"/>
-        <v>-0.24000000000000002</v>
-      </c>
-      <c r="AB25" s="127">
-        <f t="shared" si="1"/>
-        <v>-0.2</v>
-      </c>
-      <c r="AC25" s="127">
-        <f t="shared" si="1"/>
-        <v>-0.16000000000000003</v>
-      </c>
-      <c r="AD25" s="127">
-        <f t="shared" si="1"/>
-        <v>-0.12</v>
-      </c>
-      <c r="AE25" s="127">
-        <f t="shared" si="1"/>
-        <v>-8.0000000000000016E-2</v>
-      </c>
-      <c r="AF25" s="127">
-        <f t="shared" si="1"/>
-        <v>-3.999999999999998E-2</v>
-      </c>
-      <c r="AG25" s="127">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AH25" s="127">
-        <f t="shared" si="1"/>
-        <v>3.999999999999998E-2</v>
-      </c>
-      <c r="AI25" s="127">
-        <f t="shared" si="1"/>
-        <v>8.0000000000000016E-2</v>
-      </c>
-      <c r="AJ25" s="127">
-        <f t="shared" si="1"/>
-        <v>0.12000000000000005</v>
-      </c>
-      <c r="AK25" s="127">
-        <f t="shared" si="1"/>
-        <v>0.15999999999999998</v>
-      </c>
-      <c r="AL25" s="127">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="BA29" s="127">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="AM25" s="127">
+      <c r="BB29" s="127">
         <f t="shared" si="1"/>
-        <v>0.24000000000000005</v>
-      </c>
-      <c r="AN25" s="127">
-        <f t="shared" ref="AN25:BF25" si="2">IF(AN24&lt;ABS($B$16),$B$3+SIGN($B$16)*AN$24*$B$7,IF(AN24&lt;$B$6-ABS($B$17),$B$18,$B$18+SIGN($B$17)*(AN24-($B$6-ABS($B$17)))*$B$7))</f>
-        <v>0.27999999999999997</v>
-      </c>
-      <c r="AO25" s="127">
+        <v>0.25</v>
+      </c>
+      <c r="BC29" s="127">
+        <f t="shared" si="1"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="BD29" s="127">
+        <f t="shared" si="1"/>
+        <v>0.35</v>
+      </c>
+      <c r="BE29" s="127">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="BF29" s="127">
+        <f t="shared" si="1"/>
+        <v>0.45000000000000007</v>
+      </c>
+      <c r="BG29" s="127">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="BH29" s="127">
+        <f t="shared" si="1"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="BI29" s="127"/>
+      <c r="BJ29" s="127"/>
+      <c r="BK29" s="127"/>
+      <c r="BL29" s="127"/>
+      <c r="BM29" s="127"/>
+      <c r="BN29" s="127"/>
+      <c r="BO29" s="127"/>
+      <c r="BP29" s="127"/>
+      <c r="BQ29" s="127"/>
+      <c r="BR29" s="127"/>
+      <c r="BS29" s="127"/>
+      <c r="BT29" s="127"/>
+    </row>
+    <row r="30" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A30" s="128" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="129" t="s">
+        <v>103</v>
+      </c>
+      <c r="I30" t="s">
+        <v>106</v>
+      </c>
+      <c r="J30">
+        <f>IF(K28&lt;$B$26,
+$B$3*K28+SIGN($B$18)*0.5*$B$7*K28*K28,
+IF(K28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(K28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(K28-$B$27) + SIGN($B$19)*0.5*$B$7*(K28-$B$27)*(K28-$B$27)))</f>
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <f>IF(L28&lt;$B$26,
+$B$3*L28+SIGN($B$18)*0.5*$B$7*L28*L28,
+IF(L28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(L28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(L28-$B$27) + SIGN($B$19)*0.5*$B$7*(L28-$B$27)*(L28-$B$27)))</f>
+        <v>12.5</v>
+      </c>
+      <c r="L30">
+        <f>IF(M28&lt;$B$26,
+$B$3*M28+SIGN($B$18)*0.5*$B$7*M28*M28,
+IF(M28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(M28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(M28-$B$27) + SIGN($B$19)*0.5*$B$7*(M28-$B$27)*(M28-$B$27)))</f>
+        <v>28.59375</v>
+      </c>
+      <c r="M30">
+        <f>IF(M28&lt;$B$26,
+$B$3*M28+SIGN($B$18)*0.5*$B$7*M28*M28,
+IF(M28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(M28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(M28-$B$27) + SIGN($B$19)*0.5*$B$7*(M28-$B$27)*(M28-$B$27)))</f>
+        <v>28.59375</v>
+      </c>
+      <c r="N30">
+        <f>IF(N28&lt;$B$26,
+$B$3*N28+SIGN($B$18)*0.5*$B$7*N28*N28,
+IF(N28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(N28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(N28-$B$27) + SIGN($B$19)*0.5*$B$7*(N28-$B$27)*(N28-$B$27)))</f>
+        <v>44.84375</v>
+      </c>
+      <c r="O30">
+        <f>IF(O28&lt;$B$26,
+$B$3*O28+SIGN($B$18)*0.5*$B$7*O28*O28,
+IF(O28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(O28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(O28-$B$27) + SIGN($B$19)*0.5*$B$7*(O28-$B$27)*(O28-$B$27)))</f>
+        <v>61.09375</v>
+      </c>
+      <c r="P30">
+        <f>IF(P28&lt;$B$26,
+$B$3*P28+SIGN($B$18)*0.5*$B$7*P28*P28,
+IF(P28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(P28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(P28-$B$27) + SIGN($B$19)*0.5*$B$7*(P28-$B$27)*(P28-$B$27)))</f>
+        <v>77.34375</v>
+      </c>
+      <c r="Q30">
+        <f>IF(Q28&lt;$B$26,
+$B$3*Q28+SIGN($B$18)*0.5*$B$7*Q28*Q28,
+IF(Q28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(Q28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(Q28-$B$27) + SIGN($B$19)*0.5*$B$7*(Q28-$B$27)*(Q28-$B$27)))</f>
+        <v>93.59375</v>
+      </c>
+      <c r="R30">
+        <f>IF(R28&lt;$B$26,
+$B$3*R28+SIGN($B$18)*0.5*$B$7*R28*R28,
+IF(R28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(R28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(R28-$B$27) + SIGN($B$19)*0.5*$B$7*(R28-$B$27)*(R28-$B$27)))</f>
+        <v>109.84375</v>
+      </c>
+      <c r="S30">
+        <f>IF(S28&lt;$B$26,
+$B$3*S28+SIGN($B$18)*0.5*$B$7*S28*S28,
+IF(S28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(S28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(S28-$B$27) + SIGN($B$19)*0.5*$B$7*(S28-$B$27)*(S28-$B$27)))</f>
+        <v>126.09375</v>
+      </c>
+      <c r="T30">
+        <f>IF(T28&lt;$B$26,
+$B$3*T28+SIGN($B$18)*0.5*$B$7*T28*T28,
+IF(T28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(T28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(T28-$B$27) + SIGN($B$19)*0.5*$B$7*(T28-$B$27)*(T28-$B$27)))</f>
+        <v>142.34375</v>
+      </c>
+      <c r="U30">
+        <f>IF(U28&lt;$B$26,
+$B$3*U28+SIGN($B$18)*0.5*$B$7*U28*U28,
+IF(U28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(U28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(U28-$B$27) + SIGN($B$19)*0.5*$B$7*(U28-$B$27)*(U28-$B$27)))</f>
+        <v>158.59375</v>
+      </c>
+      <c r="V30">
+        <f>IF(V28&lt;$B$26,
+$B$3*V28+SIGN($B$18)*0.5*$B$7*V28*V28,
+IF(V28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(V28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(V28-$B$27) + SIGN($B$19)*0.5*$B$7*(V28-$B$27)*(V28-$B$27)))</f>
+        <v>174.84375</v>
+      </c>
+      <c r="W30">
+        <f>IF(W28&lt;$B$26,
+$B$3*W28+SIGN($B$18)*0.5*$B$7*W28*W28,
+IF(W28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(W28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(W28-$B$27) + SIGN($B$19)*0.5*$B$7*(W28-$B$27)*(W28-$B$27)))</f>
+        <v>191.09375</v>
+      </c>
+      <c r="X30">
+        <f>IF(X28&lt;$B$26,
+$B$3*X28+SIGN($B$18)*0.5*$B$7*X28*X28,
+IF(X28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(X28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(X28-$B$27) + SIGN($B$19)*0.5*$B$7*(X28-$B$27)*(X28-$B$27)))</f>
+        <v>207.34375</v>
+      </c>
+      <c r="Y30">
+        <f>IF(Y28&lt;$B$26,
+$B$3*Y28+SIGN($B$18)*0.5*$B$7*Y28*Y28,
+IF(Y28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(Y28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(Y28-$B$27) + SIGN($B$19)*0.5*$B$7*(Y28-$B$27)*(Y28-$B$27)))</f>
+        <v>223.59375</v>
+      </c>
+      <c r="Z30">
+        <f>IF(Z28&lt;$B$26,
+$B$3*Z28+SIGN($B$18)*0.5*$B$7*Z28*Z28,
+IF(Z28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(Z28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(Z28-$B$27) + SIGN($B$19)*0.5*$B$7*(Z28-$B$27)*(Z28-$B$27)))</f>
+        <v>239.84375</v>
+      </c>
+      <c r="AA30">
+        <f>IF(AA28&lt;$B$26,
+$B$3*AA28+SIGN($B$18)*0.5*$B$7*AA28*AA28,
+IF(AA28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AA28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AA28-$B$27) + SIGN($B$19)*0.5*$B$7*(AA28-$B$27)*(AA28-$B$27)))</f>
+        <v>256.09375</v>
+      </c>
+      <c r="AB30">
+        <f>IF(AB28&lt;$B$26,
+$B$3*AB28+SIGN($B$18)*0.5*$B$7*AB28*AB28,
+IF(AB28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AB28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AB28-$B$27) + SIGN($B$19)*0.5*$B$7*(AB28-$B$27)*(AB28-$B$27)))</f>
+        <v>272.34375</v>
+      </c>
+      <c r="AC30">
+        <f>IF(AC28&lt;$B$26,
+$B$3*AC28+SIGN($B$18)*0.5*$B$7*AC28*AC28,
+IF(AC28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AC28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AC28-$B$27) + SIGN($B$19)*0.5*$B$7*(AC28-$B$27)*(AC28-$B$27)))</f>
+        <v>288.59375</v>
+      </c>
+      <c r="AD30">
+        <f>IF(AD28&lt;$B$26,
+$B$3*AD28+SIGN($B$18)*0.5*$B$7*AD28*AD28,
+IF(AD28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AD28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AD28-$B$27) + SIGN($B$19)*0.5*$B$7*(AD28-$B$27)*(AD28-$B$27)))</f>
+        <v>304.84375</v>
+      </c>
+      <c r="AE30">
+        <f>IF(AE28&lt;$B$26,
+$B$3*AE28+SIGN($B$18)*0.5*$B$7*AE28*AE28,
+IF(AE28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AE28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AE28-$B$27) + SIGN($B$19)*0.5*$B$7*(AE28-$B$27)*(AE28-$B$27)))</f>
+        <v>321.09375</v>
+      </c>
+      <c r="AF30">
+        <f>IF(AF28&lt;$B$26,
+$B$3*AF28+SIGN($B$18)*0.5*$B$7*AF28*AF28,
+IF(AF28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AF28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AF28-$B$27) + SIGN($B$19)*0.5*$B$7*(AF28-$B$27)*(AF28-$B$27)))</f>
+        <v>337.34375</v>
+      </c>
+      <c r="AG30">
+        <f>IF(AG28&lt;$B$26,
+$B$3*AG28+SIGN($B$18)*0.5*$B$7*AG28*AG28,
+IF(AG28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AG28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AG28-$B$27) + SIGN($B$19)*0.5*$B$7*(AG28-$B$27)*(AG28-$B$27)))</f>
+        <v>353.59375</v>
+      </c>
+      <c r="AH30">
+        <f>IF(AH28&lt;$B$26,
+$B$3*AH28+SIGN($B$18)*0.5*$B$7*AH28*AH28,
+IF(AH28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AH28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AH28-$B$27) + SIGN($B$19)*0.5*$B$7*(AH28-$B$27)*(AH28-$B$27)))</f>
+        <v>369.84375</v>
+      </c>
+      <c r="AI30">
+        <f>IF(AI28&lt;$B$26,
+$B$3*AI28+SIGN($B$18)*0.5*$B$7*AI28*AI28,
+IF(AI28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AI28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AI28-$B$27) + SIGN($B$19)*0.5*$B$7*(AI28-$B$27)*(AI28-$B$27)))</f>
+        <v>386.09375</v>
+      </c>
+      <c r="AJ30">
+        <f>IF(AJ28&lt;$B$26,
+$B$3*AJ28+SIGN($B$18)*0.5*$B$7*AJ28*AJ28,
+IF(AJ28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AJ28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AJ28-$B$27) + SIGN($B$19)*0.5*$B$7*(AJ28-$B$27)*(AJ28-$B$27)))</f>
+        <v>402.34375</v>
+      </c>
+      <c r="AK30">
+        <f>IF(AK28&lt;$B$26,
+$B$3*AK28+SIGN($B$18)*0.5*$B$7*AK28*AK28,
+IF(AK28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AK28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AK28-$B$27) + SIGN($B$19)*0.5*$B$7*(AK28-$B$27)*(AK28-$B$27)))</f>
+        <v>418.59375</v>
+      </c>
+      <c r="AL30">
+        <f>IF(AL28&lt;$B$26,
+$B$3*AL28+SIGN($B$18)*0.5*$B$7*AL28*AL28,
+IF(AL28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AL28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AL28-$B$27) + SIGN($B$19)*0.5*$B$7*(AL28-$B$27)*(AL28-$B$27)))</f>
+        <v>434.84375</v>
+      </c>
+      <c r="AM30">
+        <f>IF(AM28&lt;$B$26,
+$B$3*AM28+SIGN($B$18)*0.5*$B$7*AM28*AM28,
+IF(AM28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AM28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AM28-$B$27) + SIGN($B$19)*0.5*$B$7*(AM28-$B$27)*(AM28-$B$27)))</f>
+        <v>451.09375</v>
+      </c>
+      <c r="AN30">
+        <f>IF(AN28&lt;$B$26,
+$B$3*AN28+SIGN($B$18)*0.5*$B$7*AN28*AN28,
+IF(AN28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AN28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AN28-$B$27) + SIGN($B$19)*0.5*$B$7*(AN28-$B$27)*(AN28-$B$27)))</f>
+        <v>467.34375</v>
+      </c>
+      <c r="AO30">
+        <f>IF(AO28&lt;$B$26,
+$B$3*AO28+SIGN($B$18)*0.5*$B$7*AO28*AO28,
+IF(AO28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AO28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AO28-$B$27) + SIGN($B$19)*0.5*$B$7*(AO28-$B$27)*(AO28-$B$27)))</f>
+        <v>483.59375</v>
+      </c>
+      <c r="AP30">
+        <f t="shared" ref="AP30:BH30" si="2">IF(AP28&lt;$B$26,
+$B$3*AP28+SIGN($B$18)*0.5*$B$7*AP28*AP28,
+IF(AP28&lt;$B$27,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AP28-$B$26)*$B$21,
+$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AP28-$B$27) + SIGN($B$19)*0.5*$B$7*(AP28-$B$27)*(AP28-$B$27)))</f>
+        <v>499.84375</v>
+      </c>
+      <c r="AQ30">
         <f t="shared" si="2"/>
-        <v>0.32</v>
-      </c>
-      <c r="AP25" s="127">
+        <v>516.09375</v>
+      </c>
+      <c r="AR30">
         <f t="shared" si="2"/>
-        <v>0.36000000000000004</v>
-      </c>
-      <c r="AQ25" s="127">
+        <v>532.34375</v>
+      </c>
+      <c r="AS30">
         <f t="shared" si="2"/>
-        <v>0.39999999999999997</v>
-      </c>
-      <c r="AR25" s="127">
+        <v>548.59375</v>
+      </c>
+      <c r="AT30">
         <f t="shared" si="2"/>
-        <v>0.44</v>
-      </c>
-      <c r="AS25" s="127">
+        <v>564.84375</v>
+      </c>
+      <c r="AU30">
         <f t="shared" si="2"/>
-        <v>0.48000000000000004</v>
-      </c>
-      <c r="AT25" s="127">
+        <v>581.09375</v>
+      </c>
+      <c r="AV30">
         <f t="shared" si="2"/>
-        <v>0.52</v>
-      </c>
-      <c r="AU25" s="127">
+        <v>597.34375</v>
+      </c>
+      <c r="AW30">
         <f t="shared" si="2"/>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="AV25" s="127">
+        <v>613.59375</v>
+      </c>
+      <c r="AX30">
         <f t="shared" si="2"/>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="AW25" s="127">
+        <v>629.84375</v>
+      </c>
+      <c r="AY30">
         <f t="shared" si="2"/>
-        <v>0.64000000000000012</v>
-      </c>
-      <c r="AX25" s="127">
+        <v>646.09375</v>
+      </c>
+      <c r="AZ30">
         <f t="shared" si="2"/>
-        <v>0.68000000000000016</v>
-      </c>
-      <c r="AY25" s="127">
+        <v>662.34375</v>
+      </c>
+      <c r="BA30">
         <f t="shared" si="2"/>
-        <v>0.72</v>
-      </c>
-      <c r="AZ25" s="127">
+        <v>680</v>
+      </c>
+      <c r="BB30">
         <f t="shared" si="2"/>
-        <v>0.76</v>
-      </c>
-      <c r="BA25" s="127">
+        <v>702.5</v>
+      </c>
+      <c r="BC30">
         <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
-      <c r="BB25" s="127">
+        <v>730</v>
+      </c>
+      <c r="BD30">
         <f t="shared" si="2"/>
-        <v>0.84000000000000008</v>
-      </c>
-      <c r="BC25" s="127">
+        <v>762.5</v>
+      </c>
+      <c r="BE30">
         <f t="shared" si="2"/>
-        <v>0.88000000000000012</v>
-      </c>
-      <c r="BD25" s="127">
+        <v>800</v>
+      </c>
+      <c r="BF30">
         <f t="shared" si="2"/>
-        <v>0.92000000000000015</v>
-      </c>
-      <c r="BE25" s="127">
+        <v>842.5</v>
+      </c>
+      <c r="BG30">
         <f t="shared" si="2"/>
-        <v>0.96</v>
-      </c>
-      <c r="BF25" s="127">
+        <v>890</v>
+      </c>
+      <c r="BH30">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="BG25" s="127"/>
-      <c r="BH25" s="127"/>
-      <c r="BI25" s="127"/>
-      <c r="BJ25" s="127"/>
-      <c r="BK25" s="127"/>
-      <c r="BL25" s="127"/>
-      <c r="BM25" s="127"/>
-      <c r="BN25" s="127"/>
-      <c r="BO25" s="127"/>
-      <c r="BP25" s="127"/>
-      <c r="BQ25" s="127"/>
-      <c r="BR25" s="127"/>
+        <v>942.5</v>
+      </c>
     </row>
-    <row r="26" spans="1:70" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A26" s="128" t="s">
-        <v>103</v>
-      </c>
-      <c r="B26" s="129" t="s">
-        <v>104</v>
-      </c>
-      <c r="G26" t="s">
-        <v>107</v>
-      </c>
-      <c r="H26">
-        <f t="shared" ref="H26:AM26" si="3">IF(H24&lt;$B$22,
-$B$3*H24+SIGN($B$16)*0.5*$B$7*H24*H24,
-IF(H24&lt;$B$23,
-$B$3*$B$22+SIGN($B$16)*0.5*$B$7*$B$22*$B$22+(H24-$B$22)*$B$18,
-$B$3*$B$22+SIGN($B$16)*0.5*$B$7*$B$22*$B$22+($B$23-$B$22)*$B$18 + $B$18*(H24-$B$23) + SIGN($B$17)*0.5*$B$7*(H24-$B$23)*(H24-$B$23)))</f>
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <f t="shared" si="3"/>
-        <v>-1.6</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="3"/>
-        <v>-6.4</v>
-      </c>
-      <c r="K26">
-        <f t="shared" si="3"/>
-        <v>-14.399999999999999</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="3"/>
-        <v>-25.6</v>
-      </c>
-      <c r="M26">
-        <f t="shared" si="3"/>
-        <v>-40</v>
-      </c>
-      <c r="N26">
-        <f t="shared" si="3"/>
-        <v>-57.599999999999994</v>
-      </c>
-      <c r="O26">
-        <f t="shared" si="3"/>
-        <v>-78.400000000000006</v>
-      </c>
-      <c r="P26">
-        <f t="shared" si="3"/>
-        <v>-102.4</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" si="3"/>
-        <v>-129.6</v>
-      </c>
-      <c r="R26">
-        <f t="shared" si="3"/>
-        <v>-160</v>
-      </c>
-      <c r="S26">
-        <f t="shared" si="3"/>
-        <v>-193.6</v>
-      </c>
-      <c r="T26">
-        <f t="shared" si="3"/>
-        <v>-229.5</v>
-      </c>
-      <c r="U26">
-        <f t="shared" si="3"/>
-        <v>-265.5</v>
-      </c>
-      <c r="V26">
-        <f t="shared" si="3"/>
-        <v>-301.39999999999998</v>
-      </c>
-      <c r="W26">
-        <f t="shared" si="3"/>
-        <v>-335</v>
-      </c>
-      <c r="X26">
-        <f t="shared" si="3"/>
-        <v>-365.4</v>
-      </c>
-      <c r="Y26">
-        <f t="shared" si="3"/>
-        <v>-392.6</v>
-      </c>
-      <c r="Z26">
-        <f t="shared" si="3"/>
-        <v>-416.6</v>
-      </c>
-      <c r="AA26">
-        <f t="shared" si="3"/>
-        <v>-437.4</v>
-      </c>
-      <c r="AB26">
-        <f t="shared" si="3"/>
-        <v>-455</v>
-      </c>
-      <c r="AC26">
-        <f t="shared" si="3"/>
-        <v>-469.4</v>
-      </c>
-      <c r="AD26">
-        <f t="shared" si="3"/>
-        <v>-480.6</v>
-      </c>
-      <c r="AE26">
-        <f t="shared" si="3"/>
-        <v>-488.6</v>
-      </c>
-      <c r="AF26">
-        <f t="shared" si="3"/>
-        <v>-493.4</v>
-      </c>
-      <c r="AG26">
-        <f t="shared" si="3"/>
-        <v>-495</v>
-      </c>
-      <c r="AH26">
-        <f t="shared" si="3"/>
-        <v>-493.4</v>
-      </c>
-      <c r="AI26">
-        <f t="shared" si="3"/>
-        <v>-488.59999999999997</v>
-      </c>
-      <c r="AJ26">
-        <f t="shared" si="3"/>
-        <v>-480.59999999999997</v>
-      </c>
-      <c r="AK26">
-        <f t="shared" si="3"/>
-        <v>-469.40000000000003</v>
-      </c>
-      <c r="AL26">
-        <f t="shared" si="3"/>
-        <v>-455</v>
-      </c>
-      <c r="AM26">
-        <f t="shared" si="3"/>
-        <v>-437.4</v>
-      </c>
-      <c r="AN26">
-        <f t="shared" ref="AN26:BF26" si="4">IF(AN24&lt;$B$22,
-$B$3*AN24+SIGN($B$16)*0.5*$B$7*AN24*AN24,
-IF(AN24&lt;$B$23,
-$B$3*$B$22+SIGN($B$16)*0.5*$B$7*$B$22*$B$22+(AN24-$B$22)*$B$18,
-$B$3*$B$22+SIGN($B$16)*0.5*$B$7*$B$22*$B$22+($B$23-$B$22)*$B$18 + $B$18*(AN24-$B$23) + SIGN($B$17)*0.5*$B$7*(AN24-$B$23)*(AN24-$B$23)))</f>
-        <v>-416.6</v>
-      </c>
-      <c r="AO26">
-        <f t="shared" si="4"/>
-        <v>-392.6</v>
-      </c>
-      <c r="AP26">
-        <f t="shared" si="4"/>
-        <v>-365.4</v>
-      </c>
-      <c r="AQ26">
-        <f t="shared" si="4"/>
-        <v>-335</v>
-      </c>
-      <c r="AR26">
-        <f t="shared" si="4"/>
-        <v>-301.39999999999998</v>
-      </c>
-      <c r="AS26">
-        <f t="shared" si="4"/>
-        <v>-264.59999999999991</v>
-      </c>
-      <c r="AT26">
-        <f t="shared" si="4"/>
-        <v>-224.60000000000002</v>
-      </c>
-      <c r="AU26">
-        <f t="shared" si="4"/>
-        <v>-181.39999999999998</v>
-      </c>
-      <c r="AV26">
-        <f t="shared" si="4"/>
-        <v>-135</v>
-      </c>
-      <c r="AW26">
-        <f t="shared" si="4"/>
-        <v>-85.399999999999864</v>
-      </c>
-      <c r="AX26">
-        <f t="shared" si="4"/>
-        <v>-32.599999999999909</v>
-      </c>
-      <c r="AY26">
-        <f t="shared" si="4"/>
-        <v>23.399999999999864</v>
-      </c>
-      <c r="AZ26">
-        <f t="shared" si="4"/>
-        <v>82.599999999999909</v>
-      </c>
-      <c r="BA26">
-        <f t="shared" si="4"/>
-        <v>145</v>
-      </c>
-      <c r="BB26">
-        <f t="shared" si="4"/>
-        <v>210.60000000000014</v>
-      </c>
-      <c r="BC26">
-        <f t="shared" si="4"/>
-        <v>279.40000000000009</v>
-      </c>
-      <c r="BD26">
-        <f t="shared" si="4"/>
-        <v>351.40000000000009</v>
-      </c>
-      <c r="BE26">
-        <f t="shared" si="4"/>
-        <v>426.59999999999991</v>
-      </c>
-      <c r="BF26">
-        <f t="shared" si="4"/>
-        <v>505</v>
+    <row r="31" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="B31" s="58"/>
+      <c r="I31" t="s">
+        <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="B27" s="58"/>
-      <c r="H27">
-        <f>$B$3*$B$22+0.5*$B$7*$B$22*$B$22+(H24-ABS($B$16))*$B$18</f>
-        <v>607.5</v>
-      </c>
-      <c r="I27">
-        <f t="shared" ref="I27:AN27" si="5">$B$3*ABS($B$16)+0.5*$B$7*ABS($B$16)*ABS($B$16)+(I24-ABS($B$16))*$B$18</f>
-        <v>571.5</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="5"/>
-        <v>535.5</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="5"/>
-        <v>499.5</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="5"/>
-        <v>463.5</v>
-      </c>
-      <c r="M27">
-        <f t="shared" si="5"/>
-        <v>427.5</v>
-      </c>
-      <c r="N27">
-        <f t="shared" si="5"/>
-        <v>391.5</v>
-      </c>
-      <c r="O27">
-        <f t="shared" si="5"/>
-        <v>355.5</v>
-      </c>
-      <c r="P27">
-        <f t="shared" si="5"/>
-        <v>319.5</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="5"/>
-        <v>283.5</v>
-      </c>
-      <c r="R27">
-        <f t="shared" si="5"/>
-        <v>247.5</v>
-      </c>
-      <c r="S27">
-        <f t="shared" si="5"/>
-        <v>211.5</v>
-      </c>
-      <c r="T27">
-        <f t="shared" si="5"/>
-        <v>175.5</v>
-      </c>
-      <c r="U27">
-        <f t="shared" si="5"/>
-        <v>139.5</v>
-      </c>
-      <c r="V27">
-        <f t="shared" si="5"/>
-        <v>103.5</v>
-      </c>
-      <c r="W27">
-        <f t="shared" si="5"/>
-        <v>67.5</v>
-      </c>
-      <c r="X27">
-        <f t="shared" si="5"/>
-        <v>31.5</v>
-      </c>
-      <c r="Y27">
-        <f t="shared" si="5"/>
-        <v>-4.5</v>
-      </c>
-      <c r="Z27">
-        <f t="shared" si="5"/>
-        <v>-40.5</v>
-      </c>
-      <c r="AA27">
-        <f t="shared" si="5"/>
-        <v>-76.5</v>
-      </c>
-      <c r="AB27">
-        <f t="shared" si="5"/>
-        <v>-112.5</v>
-      </c>
-      <c r="AC27">
-        <f t="shared" si="5"/>
-        <v>-148.5</v>
-      </c>
-      <c r="AD27">
-        <f t="shared" si="5"/>
-        <v>-184.5</v>
-      </c>
-      <c r="AE27">
-        <f t="shared" si="5"/>
-        <v>-220.5</v>
-      </c>
-      <c r="AF27">
-        <f t="shared" si="5"/>
-        <v>-256.5</v>
-      </c>
-      <c r="AG27">
-        <f t="shared" si="5"/>
-        <v>-292.5</v>
-      </c>
-      <c r="AH27">
-        <f t="shared" si="5"/>
-        <v>-328.5</v>
-      </c>
-      <c r="AI27">
-        <f t="shared" si="5"/>
-        <v>-364.5</v>
-      </c>
-      <c r="AJ27">
-        <f t="shared" si="5"/>
-        <v>-400.5</v>
-      </c>
-      <c r="AK27">
-        <f t="shared" si="5"/>
-        <v>-436.5</v>
-      </c>
-      <c r="AL27">
-        <f t="shared" si="5"/>
-        <v>-472.5</v>
-      </c>
-      <c r="AM27">
-        <f t="shared" si="5"/>
-        <v>-508.5</v>
-      </c>
-      <c r="AN27">
-        <f t="shared" si="5"/>
-        <v>-544.5</v>
-      </c>
-      <c r="AO27">
-        <f t="shared" ref="AO27:BF27" si="6">$B$3*ABS($B$16)+0.5*$B$7*ABS($B$16)*ABS($B$16)+(AO24-ABS($B$16))*$B$18</f>
-        <v>-580.5</v>
-      </c>
-      <c r="AP27">
-        <f t="shared" si="6"/>
-        <v>-616.5</v>
-      </c>
-      <c r="AQ27">
-        <f t="shared" si="6"/>
-        <v>-652.5</v>
-      </c>
-      <c r="AR27">
-        <f t="shared" si="6"/>
-        <v>-688.5</v>
-      </c>
-      <c r="AS27">
-        <f t="shared" si="6"/>
-        <v>-724.5</v>
-      </c>
-      <c r="AT27">
-        <f t="shared" si="6"/>
-        <v>-760.5</v>
-      </c>
-      <c r="AU27">
-        <f t="shared" si="6"/>
-        <v>-796.5</v>
-      </c>
-      <c r="AV27">
-        <f t="shared" si="6"/>
-        <v>-832.5</v>
-      </c>
-      <c r="AW27">
-        <f t="shared" si="6"/>
-        <v>-868.5</v>
-      </c>
-      <c r="AX27">
-        <f t="shared" si="6"/>
-        <v>-904.5</v>
-      </c>
-      <c r="AY27">
-        <f t="shared" si="6"/>
-        <v>-940.5</v>
-      </c>
-      <c r="AZ27">
-        <f t="shared" si="6"/>
-        <v>-976.5</v>
-      </c>
-      <c r="BA27">
-        <f t="shared" si="6"/>
-        <v>-1012.5</v>
-      </c>
-      <c r="BB27">
-        <f t="shared" si="6"/>
-        <v>-1048.5</v>
-      </c>
-      <c r="BC27">
-        <f t="shared" si="6"/>
-        <v>-1084.5</v>
-      </c>
-      <c r="BD27">
-        <f t="shared" si="6"/>
-        <v>-1120.5</v>
-      </c>
-      <c r="BE27">
-        <f t="shared" si="6"/>
-        <v>-1156.5</v>
-      </c>
-      <c r="BF27">
-        <f t="shared" si="6"/>
-        <v>-1192.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="B28" s="58"/>
+    <row r="32" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="B32" s="58"/>
+      <c r="I32" t="s">
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bugfxi in negative trapez profile
</commit_message>
<xml_diff>
--- a/theory/Kinematik.xlsx
+++ b/theory/Kinematik.xlsx
@@ -1814,11 +1814,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="326751456"/>
-        <c:axId val="326751064"/>
+        <c:axId val="319337224"/>
+        <c:axId val="319337608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="326751456"/>
+        <c:axId val="319337224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1856,13 +1856,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="326751064"/>
+        <c:crossAx val="319337608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="326751064"/>
+        <c:axId val="319337608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1901,7 +1901,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="326751456"/>
+        <c:crossAx val="319337224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
@@ -1997,11 +1997,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="326752240"/>
-        <c:axId val="326752632"/>
+        <c:axId val="319327904"/>
+        <c:axId val="319328288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="326752240"/>
+        <c:axId val="319327904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -2013,13 +2013,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="326752632"/>
+        <c:crossAx val="319328288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="326752632"/>
+        <c:axId val="319328288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -2032,7 +2032,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="326752240"/>
+        <c:crossAx val="319327904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
@@ -2156,13 +2156,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>125</c:v>
+                  <c:v>8.9010989010989032</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>4125</c:v>
+                  <c:v>1811.098901098901</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>5000</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2174,16 +2174,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0.1</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>0.6</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2206,13 +2206,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>261.38721247416942</c:v>
+                  <c:v>7.456698325651212</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>4261.3872124741692</c:v>
+                  <c:v>1827.4566983256511</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>5000</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2224,16 +2224,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0.1</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.23069360623708471</c:v>
+                  <c:v>5.3728349162825609E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.23069360623708471</c:v>
+                  <c:v>5.3728349162825609E-2</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>0.6</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2256,13 +2256,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000</c:v>
+                  <c:v>180.00000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>5000</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>5000</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2274,16 +2274,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0.1</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2298,11 +2298,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="326750280"/>
-        <c:axId val="326750672"/>
+        <c:axId val="318220688"/>
+        <c:axId val="318221072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="326750280"/>
+        <c:axId val="318220688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2345,12 +2345,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326750672"/>
+        <c:crossAx val="318221072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="326750672"/>
+        <c:axId val="318221072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2401,7 +2401,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326750280"/>
+        <c:crossAx val="318220688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2522,7 +2522,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2610,151 +2609,151 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>300</c:v>
+                <c:pt idx="6">
+                  <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>400</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>500</c:v>
+                <c:pt idx="11">
+                  <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="12">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>600</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>700</c:v>
+                <c:pt idx="16">
+                  <c:v>640</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="17">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>800</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>900</c:v>
+                <c:pt idx="21">
+                  <c:v>840</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="22">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>1100</c:v>
+                <c:pt idx="26">
+                  <c:v>1040</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="27">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1120</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1160</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>1200</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>1300</c:v>
+                <c:pt idx="31">
+                  <c:v>1240</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="32">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1320</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>1400</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>1500</c:v>
+                <c:pt idx="36">
+                  <c:v>1440</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="37">
+                  <c:v>1480</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1520</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1560</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>1600</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>1700</c:v>
+                <c:pt idx="41">
+                  <c:v>1640</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="42">
+                  <c:v>1680</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1720</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1760</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>1800</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>1900</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2100</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2200</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2300</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2400</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2600</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2700</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2800</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2900</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>3100</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3200</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3300</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>3400</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3600</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>3700</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>3800</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>3900</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>4100</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>4200</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>4300</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>4400</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>4500</c:v>
-                </c:pt>
                 <c:pt idx="46">
-                  <c:v>4600</c:v>
+                  <c:v>1840</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4700</c:v>
+                  <c:v>1880</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4800</c:v>
+                  <c:v>1920</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4900</c:v>
+                  <c:v>1960</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2766,157 +2765,157 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15000000000000002</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15000000000000002</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.2</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.25</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.35</c:v>
+                  <c:v>4.5549450549450553E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.4</c:v>
+                  <c:v>6.0000000000000039E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.45000000000000007</c:v>
+                  <c:v>8.0000000000000043E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.5</c:v>
+                  <c:v>0.10000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.12000000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2931,11 +2930,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="326912360"/>
-        <c:axId val="326912752"/>
+        <c:axId val="337301520"/>
+        <c:axId val="337301904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="326912360"/>
+        <c:axId val="337301520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2986,12 +2985,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326912752"/>
+        <c:crossAx val="337301904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="326912752"/>
+        <c:axId val="337301904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3042,7 +3041,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326912360"/>
+        <c:crossAx val="337301520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3056,7 +3055,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3175,7 +3173,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3274,151 +3271,151 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>300</c:v>
+                <c:pt idx="6">
+                  <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>400</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>500</c:v>
+                <c:pt idx="11">
+                  <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="12">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>600</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>700</c:v>
+                <c:pt idx="16">
+                  <c:v>640</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="17">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>800</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>900</c:v>
+                <c:pt idx="21">
+                  <c:v>840</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="22">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>1100</c:v>
+                <c:pt idx="26">
+                  <c:v>1040</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="27">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1120</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1160</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>1200</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>1300</c:v>
+                <c:pt idx="31">
+                  <c:v>1240</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="32">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1320</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>1400</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>1500</c:v>
+                <c:pt idx="36">
+                  <c:v>1440</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="37">
+                  <c:v>1480</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1520</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1560</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>1600</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>1700</c:v>
+                <c:pt idx="41">
+                  <c:v>1640</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="42">
+                  <c:v>1680</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1720</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1760</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>1800</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>1900</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2100</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2200</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2300</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2400</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2600</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2700</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2800</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2900</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>3100</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3200</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3300</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>3400</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3600</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>3700</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>3800</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>3900</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>4100</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>4200</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>4300</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>4400</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>4500</c:v>
-                </c:pt>
                 <c:pt idx="46">
-                  <c:v>4600</c:v>
+                  <c:v>1840</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4700</c:v>
+                  <c:v>1880</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4800</c:v>
+                  <c:v>1920</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4900</c:v>
+                  <c:v>1960</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3433,154 +3430,154 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.5</c:v>
+                  <c:v>1.8417854123898081</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.59375</c:v>
+                  <c:v>3.66376343436783</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.59375</c:v>
+                  <c:v>3.66376343436783</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44.84375</c:v>
+                  <c:v>5.4857414563458526</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>61.09375</c:v>
+                  <c:v>7.3077194783238753</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>77.34375</c:v>
+                  <c:v>9.1296975003018961</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>93.59375</c:v>
+                  <c:v>10.951675522279919</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>109.84375</c:v>
+                  <c:v>12.77365354425794</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>126.09375</c:v>
+                  <c:v>14.595631566235962</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>142.34375</c:v>
+                  <c:v>16.417609588213985</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>158.59375</c:v>
+                  <c:v>18.239587610192007</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>174.84375</c:v>
+                  <c:v>20.06156563217003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>191.09375</c:v>
+                  <c:v>21.883543654148053</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>207.34375</c:v>
+                  <c:v>23.705521676126075</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>223.59375</c:v>
+                  <c:v>25.527499698104098</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>239.84375</c:v>
+                  <c:v>27.34947772008212</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>256.09375</c:v>
+                  <c:v>29.171455742060143</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>272.34375</c:v>
+                  <c:v>30.993433764038166</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>288.59375</c:v>
+                  <c:v>32.815411786016185</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>304.84375</c:v>
+                  <c:v>34.637389807994204</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>321.09375</c:v>
+                  <c:v>36.45936782997223</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>337.34375</c:v>
+                  <c:v>38.281345851950249</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>353.59375</c:v>
+                  <c:v>40.103323873928275</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>369.84375</c:v>
+                  <c:v>41.925301895906294</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>386.09375</c:v>
+                  <c:v>43.747279917884313</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>402.34375</c:v>
+                  <c:v>45.569257939862339</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>418.59375</c:v>
+                  <c:v>47.391235961840358</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>434.84375</c:v>
+                  <c:v>49.213213983818378</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>451.09375</c:v>
+                  <c:v>51.035192005796397</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>467.34375</c:v>
+                  <c:v>52.857170027774423</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>483.59375</c:v>
+                  <c:v>54.679148049752442</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>499.84375</c:v>
+                  <c:v>56.501126071730468</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>516.09375</c:v>
+                  <c:v>58.323104093708487</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>532.34375</c:v>
+                  <c:v>60.145082115686513</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>548.59375</c:v>
+                  <c:v>61.967060137664532</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>564.84375</c:v>
+                  <c:v>63.789038159642551</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>581.09375</c:v>
+                  <c:v>65.611016181620585</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>597.34375</c:v>
+                  <c:v>67.432994203598611</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>613.59375</c:v>
+                  <c:v>69.254972225576623</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>629.84375</c:v>
+                  <c:v>71.076950247554649</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>646.09375</c:v>
+                  <c:v>72.898928269532675</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>662.34375</c:v>
+                  <c:v>74.720906291510687</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>680</c:v>
+                  <c:v>76.542884313488713</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>702.5</c:v>
+                  <c:v>78.364862335466739</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>730</c:v>
+                  <c:v>80.186840357444765</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>762.5</c:v>
+                  <c:v>82.008818379422777</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>800</c:v>
+                  <c:v>84.039614780823584</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>842.5</c:v>
+                  <c:v>86.839614780823567</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>890</c:v>
+                  <c:v>90.439614780823575</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>942.5</c:v>
+                  <c:v>94.839614780823581</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3595,11 +3592,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="326913928"/>
-        <c:axId val="326915104"/>
+        <c:axId val="336758456"/>
+        <c:axId val="336707800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="326913928"/>
+        <c:axId val="336758456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3655,12 +3652,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326915104"/>
+        <c:crossAx val="336707800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="326915104"/>
+        <c:axId val="336707800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3716,7 +3713,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326913928"/>
+        <c:crossAx val="336758456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3730,7 +3727,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -32799,7 +32795,7 @@
   <dimension ref="A1:BT32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32817,7 +32813,7 @@
         <v>84</v>
       </c>
       <c r="B3">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C3" t="s">
         <v>86</v>
@@ -32828,7 +32824,7 @@
         <v>85</v>
       </c>
       <c r="B4">
-        <v>0.6</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="C4" t="s">
         <v>86</v>
@@ -32839,7 +32835,7 @@
         <v>87</v>
       </c>
       <c r="B5">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
         <v>90</v>
@@ -32850,7 +32846,7 @@
         <v>89</v>
       </c>
       <c r="B6">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="C6" t="s">
         <v>91</v>
@@ -32873,7 +32869,7 @@
       </c>
       <c r="B9">
         <f>B5/B6</f>
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="C9" t="s">
         <v>86</v>
@@ -32885,19 +32881,19 @@
       </c>
       <c r="E10">
         <f>(B3-B4)/B7</f>
-        <v>-1000</v>
+        <v>-180.00000000000003</v>
       </c>
       <c r="F10">
         <f>(B3-B4)/B7</f>
-        <v>-1000</v>
+        <v>-180.00000000000003</v>
       </c>
       <c r="G10">
         <f>(B3-B4)/B7</f>
-        <v>-1000</v>
+        <v>-180.00000000000003</v>
       </c>
       <c r="H10">
         <f>(B3-B4)/B7</f>
-        <v>-1000</v>
+        <v>-180.00000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -32906,24 +32902,24 @@
       </c>
       <c r="E11" s="127">
         <f>B3*B6-0.5*B7*E10*E10 - B5</f>
-        <v>-750</v>
+        <v>-8.0999999999999943</v>
       </c>
       <c r="F11">
         <f>B3*B6+0.5*B7*F10*F10 - B5</f>
-        <v>-250</v>
+        <v>8.0999999999999943</v>
       </c>
       <c r="G11">
         <f>B4*G10+0.5*B7*G10*G10- B5</f>
-        <v>-1350</v>
+        <v>-117.10000000000001</v>
       </c>
       <c r="H11">
         <f>-B4*G10-0.5*B7*G10*G10- B5</f>
-        <v>-650</v>
+        <v>-82.899999999999991</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11">
         <f>-B5*B7-0.5*B3*B3</f>
-        <v>-0.505</v>
+        <v>-5.1250000000000004E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -32932,23 +32928,23 @@
       </c>
       <c r="E12">
         <f>B7*(B6-E10)</f>
-        <v>3</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="F12">
         <f>B7*(B6+F10)</f>
-        <v>2</v>
+        <v>0.91</v>
       </c>
       <c r="G12">
         <f>B3+B4+B7*G10</f>
-        <v>0.19999999999999996</v>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="H12">
         <f>B3+B4+B7*G10</f>
-        <v>0.19999999999999996</v>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="L12">
         <f>B3</f>
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -32995,15 +32991,15 @@
       </c>
       <c r="N16" s="4">
         <f>B26</f>
-        <v>125</v>
+        <v>8.9010989010989032</v>
       </c>
       <c r="O16" s="3">
         <f>B27</f>
-        <v>4125</v>
+        <v>1811.098901098901</v>
       </c>
       <c r="P16">
         <f>B6</f>
-        <v>5000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="17" spans="1:72" x14ac:dyDescent="0.3">
@@ -33030,19 +33026,19 @@
       </c>
       <c r="M17">
         <f>B3</f>
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="N17" s="3">
         <f>B21</f>
-        <v>0.16250000000000001</v>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="O17" s="3">
         <f>N17</f>
-        <v>0.16250000000000001</v>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="P17">
         <f>B4</f>
-        <v>0.6</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
@@ -33051,7 +33047,7 @@
       </c>
       <c r="B18" s="127">
         <f>(B5-B3*B6-0.5*(B4-B3)*(B4-B3)/B7)/(B6*B7+(B3-B4))</f>
-        <v>125</v>
+        <v>-8.9010989010989032</v>
       </c>
       <c r="C18" t="s">
         <v>91</v>
@@ -33061,15 +33057,15 @@
       </c>
       <c r="E18" s="3">
         <f>(-E12+SQRT(E12*E12-4*E13*E11))/(2*E13)</f>
-        <v>261.38721247416942</v>
+        <v>7.456698325651212</v>
       </c>
       <c r="F18" s="130">
         <f>(-F12+SQRT(F12*F12-4*F13*F11))/(2*F13)</f>
-        <v>121.32034355964238</v>
+        <v>-8.9450627181492095</v>
       </c>
       <c r="G18" s="3">
         <f>(-G12+SQRT(G12*G12-4*G13*G11))/(2*G13)</f>
-        <v>1455.2945357246849</v>
+        <v>394.16596402423352</v>
       </c>
       <c r="H18" s="3" t="e">
         <f>-(-H12+SQRT(H12*H12-4*H13*H11))/(2*H13)</f>
@@ -33077,7 +33073,7 @@
       </c>
       <c r="I18" s="127">
         <f>(B4-B3)/B7</f>
-        <v>1000</v>
+        <v>180.00000000000003</v>
       </c>
       <c r="L18" t="s">
         <v>88</v>
@@ -33087,15 +33083,15 @@
       </c>
       <c r="N18" s="4">
         <f>E26</f>
-        <v>261.38721247416942</v>
+        <v>7.456698325651212</v>
       </c>
       <c r="O18" s="3">
         <f>E27</f>
-        <v>4261.3872124741692</v>
+        <v>1827.4566983256511</v>
       </c>
       <c r="P18">
         <f>B6</f>
-        <v>5000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="19" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
@@ -33104,7 +33100,7 @@
       </c>
       <c r="B19" s="3">
         <f>(B4-B3)/B7-B18</f>
-        <v>875</v>
+        <v>188.90109890109892</v>
       </c>
       <c r="C19" t="s">
         <v>91</v>
@@ -33114,15 +33110,15 @@
       </c>
       <c r="E19" s="3">
         <f>(B4-B3)/B7-E18</f>
-        <v>738.61278752583053</v>
+        <v>172.54330167434881</v>
       </c>
       <c r="F19" s="3">
         <f>(B4-B3)/B7-F18</f>
-        <v>878.67965644035758</v>
+        <v>188.94506271814925</v>
       </c>
       <c r="G19" s="127">
         <f>-(G10+G18)</f>
-        <v>-455.29453572468492</v>
+        <v>-214.16596402423349</v>
       </c>
       <c r="H19" s="127" t="e">
         <f>-(H10+H18)</f>
@@ -33136,19 +33132,19 @@
       </c>
       <c r="M19">
         <f>B3</f>
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="N19" s="3">
         <f>E21</f>
-        <v>0.23069360623708471</v>
+        <v>5.3728349162825609E-2</v>
       </c>
       <c r="O19" s="3">
         <f>N19</f>
-        <v>0.23069360623708471</v>
+        <v>5.3728349162825609E-2</v>
       </c>
       <c r="P19">
         <f>B4</f>
-        <v>0.6</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
@@ -33160,7 +33156,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="127">
         <f>ABS(G18)+ABS(G19)</f>
-        <v>1910.5890714493698</v>
+        <v>608.33192804846703</v>
       </c>
       <c r="H20" s="127" t="e">
         <f>ABS(H18)+ABS(H19)</f>
@@ -33176,7 +33172,7 @@
       </c>
       <c r="B21" s="3">
         <f>B3+B7*B18</f>
-        <v>0.16250000000000001</v>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="C21" t="s">
         <v>86</v>
@@ -33186,15 +33182,15 @@
       </c>
       <c r="E21" s="3">
         <f>B3+B7*E18</f>
-        <v>0.23069360623708471</v>
+        <v>5.3728349162825609E-2</v>
       </c>
       <c r="F21" s="3">
         <f>B3+B7*F18</f>
-        <v>0.1606601717798212</v>
+        <v>4.5527468640925398E-2</v>
       </c>
       <c r="G21">
         <f>B3+B7*G18</f>
-        <v>0.82764726786234244</v>
+        <v>0.24708298201211676</v>
       </c>
       <c r="H21" t="e">
         <f>B3+B7*H18</f>
@@ -33202,7 +33198,7 @@
       </c>
       <c r="I21" s="3">
         <f>B3+B7*I18</f>
-        <v>0.6</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="L21" t="s">
         <v>88</v>
@@ -33212,15 +33208,15 @@
       </c>
       <c r="N21" s="4">
         <f>I26</f>
-        <v>1000</v>
+        <v>180.00000000000003</v>
       </c>
       <c r="O21" s="3">
         <f>I27</f>
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="P21">
         <f>B6</f>
-        <v>5000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="22" spans="1:72" x14ac:dyDescent="0.3">
@@ -33229,7 +33225,7 @@
       </c>
       <c r="B22" s="127">
         <f>$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(B6-$B$27) + SIGN($B$19)*0.5*$B$7*(B6-$B$27)*(B6-$B$27)</f>
-        <v>1000</v>
+        <v>100.03961478082358</v>
       </c>
       <c r="C22" t="s">
         <v>90</v>
@@ -33239,15 +33235,15 @@
       </c>
       <c r="E22" s="127">
         <f>$B$3*$E$26+SIGN($E$18)*0.5*$B$7*$E$26*$E$26+($E$27-$E$26)*$E$21 + $E$21*(B6-$E$27) + SIGN($E$19)*0.5*$B$7*(B6-$E$27)*(B6-$E$27)</f>
-        <v>1272.7744249483389</v>
+        <v>114.88559547634262</v>
       </c>
       <c r="F22" s="127">
         <f>$B$3*$F$26+SIGN($F$18)*0.5*$B$7*$F$26*$F$26+($F$27-$F$26)*$F$21 + $F$21*(B6-$F$27) + SIGN($F$19)*0.5*$B$7*(B6-$F$27)*(B6-$F$27)</f>
-        <v>992.64068711928485</v>
+        <v>100.00000000000004</v>
       </c>
       <c r="G22" s="127">
         <f>$B$3*$G$26+SIGN($G$18)*0.5*$B$7*$G$26*$G$26+($G$27-$G$26)*$G$21 + $G$21*(G20-$G$27) + SIGN($G$19)*0.5*$B$7*(G20-$G$27)*(G20-$G$27)</f>
-        <v>1000.0000000000001</v>
+        <v>100.00000000000003</v>
       </c>
       <c r="H22" s="127" t="e">
         <f>$B$3*$H$26+SIGN($H$18)*0.5*$B$7*$H$26*$H$26+($H$27-$H$26)*$H$21 + $H$21*(H20-$H$27) + SIGN($H$19)*0.5*$B$7*(H20-$H$27)*(H20-$H$27)</f>
@@ -33255,33 +33251,33 @@
       </c>
       <c r="I22">
         <f>$B$3*$I$26+SIGN($I$18)*0.5*$B$7*$I$26*$I$26+($I$27-$I$26)*$I$21 + $I$21*(B6-$I$27) + SIGN($I$19)*0.5*$B$7*(B6-$I$27)*(B6-$I$27)</f>
-        <v>2750</v>
+        <v>271.90000000000003</v>
       </c>
       <c r="J22" t="s">
         <v>119</v>
       </c>
       <c r="K22">
         <f>(B5-B3*I18-0.5*B7*I18*I18)/B4+I18</f>
-        <v>2083.3333333333335</v>
+        <v>772.14285714285711</v>
       </c>
       <c r="L22" t="s">
         <v>118</v>
       </c>
       <c r="M22">
         <f>B3</f>
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="N22" s="3">
         <f>I21</f>
-        <v>0.6</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="O22" s="3">
         <f>I21</f>
-        <v>0.6</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="P22" s="3">
         <f>I21</f>
-        <v>0.6</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
@@ -33290,7 +33286,7 @@
       </c>
       <c r="B23">
         <f>B21+B19*B7</f>
-        <v>0.6</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="C23" t="s">
         <v>86</v>
@@ -33300,15 +33296,15 @@
       </c>
       <c r="E23" s="3">
         <f>E21+E19*B7</f>
-        <v>0.6</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F23" s="3">
         <f>F21+F19*B7</f>
-        <v>0.6</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G23" s="3">
         <f>G21+G19*B7</f>
-        <v>0.6</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H23" s="3" t="e">
         <f>H21+H19*B7</f>
@@ -33316,14 +33312,14 @@
       </c>
       <c r="I23" s="3">
         <f>I21+I19*B7</f>
-        <v>0.6</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J23" t="s">
         <v>120</v>
       </c>
       <c r="K23" s="3">
         <f>SQRT(B3*B3 +2*B5*B7)</f>
-        <v>1.004987562112089</v>
+        <v>0.32015621187164245</v>
       </c>
     </row>
     <row r="24" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
@@ -33332,7 +33328,7 @@
       </c>
       <c r="E24">
         <f>(B5+0.5*B7*E10*E10)/B3</f>
-        <v>12500</v>
+        <v>2161.9999999999995</v>
       </c>
       <c r="J24" t="s">
         <v>122</v>
@@ -33351,22 +33347,22 @@
       </c>
       <c r="B26" s="127">
         <f>ABS(B18)</f>
-        <v>125</v>
+        <v>8.9010989010989032</v>
       </c>
       <c r="C26" t="s">
         <v>91</v>
       </c>
       <c r="E26" s="127">
         <f>ABS(E18)</f>
-        <v>261.38721247416942</v>
+        <v>7.456698325651212</v>
       </c>
       <c r="F26" s="127">
         <f>ABS(F18)</f>
-        <v>121.32034355964238</v>
+        <v>8.9450627181492095</v>
       </c>
       <c r="G26" s="127">
         <f>ABS(G18)</f>
-        <v>1455.2945357246849</v>
+        <v>394.16596402423352</v>
       </c>
       <c r="H26" s="127" t="e">
         <f>ABS(H18)</f>
@@ -33374,7 +33370,7 @@
       </c>
       <c r="I26" s="127">
         <f>ABS(I18)</f>
-        <v>1000</v>
+        <v>180.00000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
@@ -33383,22 +33379,22 @@
       </c>
       <c r="B27" s="127">
         <f>B6-ABS(B19)</f>
-        <v>4125</v>
+        <v>1811.098901098901</v>
       </c>
       <c r="C27" t="s">
         <v>91</v>
       </c>
       <c r="E27" s="127">
         <f>B6-ABS(E19)</f>
-        <v>4261.3872124741692</v>
+        <v>1827.4566983256511</v>
       </c>
       <c r="F27" s="127">
         <f>B6-ABS(F19)</f>
-        <v>4121.3203435596424</v>
+        <v>1811.0549372818507</v>
       </c>
       <c r="G27" s="127">
         <f>G26</f>
-        <v>1455.2945357246849</v>
+        <v>394.16596402423352</v>
       </c>
       <c r="H27" s="127" t="e">
         <f>H26</f>
@@ -33406,7 +33402,7 @@
       </c>
       <c r="I27" s="127">
         <f>B6-ABS(I19)</f>
-        <v>5000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="28" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
@@ -33424,199 +33420,199 @@
       </c>
       <c r="L28">
         <f>(K28+$B$6/50)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M28">
         <f t="shared" ref="M28:BH28" si="0">(L28+$B$6/50)</f>
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="N28">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>120</v>
       </c>
       <c r="O28">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>160</v>
       </c>
       <c r="P28">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="Q28">
         <f t="shared" si="0"/>
-        <v>600</v>
+        <v>240</v>
       </c>
       <c r="R28">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>280</v>
       </c>
       <c r="S28">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>320</v>
       </c>
       <c r="T28">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>360</v>
       </c>
       <c r="U28">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>400</v>
       </c>
       <c r="V28">
         <f t="shared" si="0"/>
-        <v>1100</v>
+        <v>440</v>
       </c>
       <c r="W28">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>480</v>
       </c>
       <c r="X28">
         <f t="shared" si="0"/>
-        <v>1300</v>
+        <v>520</v>
       </c>
       <c r="Y28">
         <f t="shared" si="0"/>
-        <v>1400</v>
+        <v>560</v>
       </c>
       <c r="Z28">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="AA28">
         <f t="shared" si="0"/>
-        <v>1600</v>
+        <v>640</v>
       </c>
       <c r="AB28">
         <f t="shared" si="0"/>
-        <v>1700</v>
+        <v>680</v>
       </c>
       <c r="AC28">
         <f t="shared" si="0"/>
-        <v>1800</v>
+        <v>720</v>
       </c>
       <c r="AD28">
         <f t="shared" si="0"/>
-        <v>1900</v>
+        <v>760</v>
       </c>
       <c r="AE28">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>800</v>
       </c>
       <c r="AF28">
         <f t="shared" si="0"/>
-        <v>2100</v>
+        <v>840</v>
       </c>
       <c r="AG28">
         <f t="shared" si="0"/>
-        <v>2200</v>
+        <v>880</v>
       </c>
       <c r="AH28">
         <f t="shared" si="0"/>
-        <v>2300</v>
+        <v>920</v>
       </c>
       <c r="AI28">
         <f t="shared" si="0"/>
-        <v>2400</v>
+        <v>960</v>
       </c>
       <c r="AJ28">
         <f t="shared" si="0"/>
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="AK28">
         <f t="shared" si="0"/>
-        <v>2600</v>
+        <v>1040</v>
       </c>
       <c r="AL28">
         <f t="shared" si="0"/>
-        <v>2700</v>
+        <v>1080</v>
       </c>
       <c r="AM28">
         <f t="shared" si="0"/>
-        <v>2800</v>
+        <v>1120</v>
       </c>
       <c r="AN28">
         <f t="shared" si="0"/>
-        <v>2900</v>
+        <v>1160</v>
       </c>
       <c r="AO28">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>1200</v>
       </c>
       <c r="AP28">
         <f t="shared" si="0"/>
-        <v>3100</v>
+        <v>1240</v>
       </c>
       <c r="AQ28">
         <f t="shared" si="0"/>
-        <v>3200</v>
+        <v>1280</v>
       </c>
       <c r="AR28">
         <f t="shared" si="0"/>
-        <v>3300</v>
+        <v>1320</v>
       </c>
       <c r="AS28">
         <f t="shared" si="0"/>
-        <v>3400</v>
+        <v>1360</v>
       </c>
       <c r="AT28">
         <f t="shared" si="0"/>
-        <v>3500</v>
+        <v>1400</v>
       </c>
       <c r="AU28">
         <f t="shared" si="0"/>
-        <v>3600</v>
+        <v>1440</v>
       </c>
       <c r="AV28">
         <f t="shared" si="0"/>
-        <v>3700</v>
+        <v>1480</v>
       </c>
       <c r="AW28">
         <f t="shared" si="0"/>
-        <v>3800</v>
+        <v>1520</v>
       </c>
       <c r="AX28">
         <f t="shared" si="0"/>
-        <v>3900</v>
+        <v>1560</v>
       </c>
       <c r="AY28">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>1600</v>
       </c>
       <c r="AZ28">
         <f t="shared" si="0"/>
-        <v>4100</v>
+        <v>1640</v>
       </c>
       <c r="BA28">
         <f t="shared" si="0"/>
-        <v>4200</v>
+        <v>1680</v>
       </c>
       <c r="BB28">
         <f t="shared" si="0"/>
-        <v>4300</v>
+        <v>1720</v>
       </c>
       <c r="BC28">
         <f t="shared" si="0"/>
-        <v>4400</v>
+        <v>1760</v>
       </c>
       <c r="BD28">
         <f t="shared" si="0"/>
-        <v>4500</v>
+        <v>1800</v>
       </c>
       <c r="BE28">
         <f t="shared" si="0"/>
-        <v>4600</v>
+        <v>1840</v>
       </c>
       <c r="BF28">
         <f t="shared" si="0"/>
-        <v>4700</v>
+        <v>1880</v>
       </c>
       <c r="BG28">
         <f t="shared" si="0"/>
-        <v>4800</v>
+        <v>1920</v>
       </c>
       <c r="BH28">
         <f t="shared" si="0"/>
-        <v>4900</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="29" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
@@ -33631,207 +33627,207 @@
       </c>
       <c r="J29" s="127">
         <f>IF(K28&lt;ABS($B$18),$B$3+SIGN($B$18)*K$28*$B$7,IF(K28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(K28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="K29" s="127">
         <f>IF(L28&lt;ABS($B$18),$B$3+SIGN($B$18)*L$28*$B$7,IF(L28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(L28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.15000000000000002</v>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="L29" s="127">
-        <f>IF(L28&lt;ABS($B$18),$B$3+SIGN($B$18)*L$28*$B$7,IF(L28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(L28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.15000000000000002</v>
+        <f t="shared" ref="L29:AO29" si="1">IF(L28&lt;ABS($B$18),$B$3+SIGN($B$18)*L$28*$B$7,IF(L28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(L28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="M29" s="127">
-        <f>IF(M28&lt;ABS($B$18),$B$3+SIGN($B$18)*M$28*$B$7,IF(M28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(M28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="N29" s="127">
-        <f>IF(N28&lt;ABS($B$18),$B$3+SIGN($B$18)*N$28*$B$7,IF(N28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(N28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="O29" s="127">
-        <f>IF(O28&lt;ABS($B$18),$B$3+SIGN($B$18)*O$28*$B$7,IF(O28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(O28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="P29" s="127">
-        <f>IF(P28&lt;ABS($B$18),$B$3+SIGN($B$18)*P$28*$B$7,IF(P28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(P28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="Q29" s="127">
-        <f>IF(Q28&lt;ABS($B$18),$B$3+SIGN($B$18)*Q$28*$B$7,IF(Q28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(Q28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="R29" s="127">
-        <f>IF(R28&lt;ABS($B$18),$B$3+SIGN($B$18)*R$28*$B$7,IF(R28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(R28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="S29" s="127">
-        <f>IF(S28&lt;ABS($B$18),$B$3+SIGN($B$18)*S$28*$B$7,IF(S28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(S28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="T29" s="127">
-        <f>IF(T28&lt;ABS($B$18),$B$3+SIGN($B$18)*T$28*$B$7,IF(T28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(T28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="U29" s="127">
-        <f>IF(U28&lt;ABS($B$18),$B$3+SIGN($B$18)*U$28*$B$7,IF(U28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(U28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="V29" s="127">
-        <f>IF(V28&lt;ABS($B$18),$B$3+SIGN($B$18)*V$28*$B$7,IF(V28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(V28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="W29" s="127">
-        <f>IF(W28&lt;ABS($B$18),$B$3+SIGN($B$18)*W$28*$B$7,IF(W28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(W28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="X29" s="127">
-        <f>IF(X28&lt;ABS($B$18),$B$3+SIGN($B$18)*X$28*$B$7,IF(X28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(X28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="Y29" s="127">
-        <f>IF(Y28&lt;ABS($B$18),$B$3+SIGN($B$18)*Y$28*$B$7,IF(Y28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(Y28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="Z29" s="127">
-        <f>IF(Z28&lt;ABS($B$18),$B$3+SIGN($B$18)*Z$28*$B$7,IF(Z28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(Z28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AA29" s="127">
-        <f>IF(AA28&lt;ABS($B$18),$B$3+SIGN($B$18)*AA$28*$B$7,IF(AA28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AA28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AB29" s="127">
-        <f>IF(AB28&lt;ABS($B$18),$B$3+SIGN($B$18)*AB$28*$B$7,IF(AB28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AB28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AC29" s="127">
-        <f>IF(AC28&lt;ABS($B$18),$B$3+SIGN($B$18)*AC$28*$B$7,IF(AC28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AC28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AD29" s="127">
-        <f>IF(AD28&lt;ABS($B$18),$B$3+SIGN($B$18)*AD$28*$B$7,IF(AD28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AD28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AE29" s="127">
-        <f>IF(AE28&lt;ABS($B$18),$B$3+SIGN($B$18)*AE$28*$B$7,IF(AE28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AE28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AF29" s="127">
-        <f>IF(AF28&lt;ABS($B$18),$B$3+SIGN($B$18)*AF$28*$B$7,IF(AF28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AF28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AG29" s="127">
-        <f>IF(AG28&lt;ABS($B$18),$B$3+SIGN($B$18)*AG$28*$B$7,IF(AG28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AG28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AH29" s="127">
-        <f>IF(AH28&lt;ABS($B$18),$B$3+SIGN($B$18)*AH$28*$B$7,IF(AH28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AH28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AI29" s="127">
-        <f>IF(AI28&lt;ABS($B$18),$B$3+SIGN($B$18)*AI$28*$B$7,IF(AI28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AI28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AJ29" s="127">
-        <f>IF(AJ28&lt;ABS($B$18),$B$3+SIGN($B$18)*AJ$28*$B$7,IF(AJ28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AJ28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AK29" s="127">
-        <f>IF(AK28&lt;ABS($B$18),$B$3+SIGN($B$18)*AK$28*$B$7,IF(AK28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AK28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AL29" s="127">
-        <f>IF(AL28&lt;ABS($B$18),$B$3+SIGN($B$18)*AL$28*$B$7,IF(AL28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AL28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AM29" s="127">
-        <f>IF(AM28&lt;ABS($B$18),$B$3+SIGN($B$18)*AM$28*$B$7,IF(AM28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AM28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AN29" s="127">
-        <f>IF(AN28&lt;ABS($B$18),$B$3+SIGN($B$18)*AN$28*$B$7,IF(AN28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AN28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AO29" s="127">
-        <f>IF(AO28&lt;ABS($B$18),$B$3+SIGN($B$18)*AO$28*$B$7,IF(AO28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AO28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="1"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AP29" s="127">
-        <f t="shared" ref="AP29:BH29" si="1">IF(AP28&lt;ABS($B$18),$B$3+SIGN($B$18)*AP$28*$B$7,IF(AP28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AP28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0.16250000000000001</v>
+        <f t="shared" ref="AP29:BH29" si="2">IF(AP28&lt;ABS($B$18),$B$3+SIGN($B$18)*AP$28*$B$7,IF(AP28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(AP28-($B$6-ABS($B$19)))*$B$7))</f>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AQ29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="2"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AR29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="2"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AS29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="2"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AT29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="2"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AU29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="2"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AV29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="2"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AW29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="2"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AX29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="2"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AY29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="2"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="AZ29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.16250000000000001</v>
+        <f t="shared" si="2"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="BA29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
+        <f t="shared" si="2"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="BB29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
+        <f t="shared" si="2"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="BC29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.30000000000000004</v>
+        <f t="shared" si="2"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="BD29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.35</v>
+        <f t="shared" si="2"/>
+        <v>4.5549450549450553E-2</v>
       </c>
       <c r="BE29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
+        <f t="shared" si="2"/>
+        <v>6.0000000000000039E-2</v>
       </c>
       <c r="BF29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.45000000000000007</v>
+        <f t="shared" si="2"/>
+        <v>8.0000000000000043E-2</v>
       </c>
       <c r="BG29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
+        <f t="shared" si="2"/>
+        <v>0.10000000000000003</v>
       </c>
       <c r="BH29" s="127">
-        <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
+        <f t="shared" si="2"/>
+        <v>0.12000000000000005</v>
       </c>
       <c r="BI29" s="127"/>
       <c r="BJ29" s="127"/>
@@ -33870,7 +33866,7 @@
 IF(L28&lt;$B$27,
 $B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(L28-$B$26)*$B$21,
 $B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(L28-$B$27) + SIGN($B$19)*0.5*$B$7*(L28-$B$27)*(L28-$B$27)))</f>
-        <v>12.5</v>
+        <v>1.8417854123898081</v>
       </c>
       <c r="L30">
         <f>IF(M28&lt;$B$26,
@@ -33878,319 +33874,207 @@
 IF(M28&lt;$B$27,
 $B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(M28-$B$26)*$B$21,
 $B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(M28-$B$27) + SIGN($B$19)*0.5*$B$7*(M28-$B$27)*(M28-$B$27)))</f>
-        <v>28.59375</v>
+        <v>3.66376343436783</v>
       </c>
       <c r="M30">
-        <f>IF(M28&lt;$B$26,
+        <f t="shared" ref="M30:AO30" si="3">IF(M28&lt;$B$26,
 $B$3*M28+SIGN($B$18)*0.5*$B$7*M28*M28,
 IF(M28&lt;$B$27,
 $B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(M28-$B$26)*$B$21,
 $B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(M28-$B$27) + SIGN($B$19)*0.5*$B$7*(M28-$B$27)*(M28-$B$27)))</f>
-        <v>28.59375</v>
+        <v>3.66376343436783</v>
       </c>
       <c r="N30">
-        <f>IF(N28&lt;$B$26,
-$B$3*N28+SIGN($B$18)*0.5*$B$7*N28*N28,
-IF(N28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(N28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(N28-$B$27) + SIGN($B$19)*0.5*$B$7*(N28-$B$27)*(N28-$B$27)))</f>
-        <v>44.84375</v>
+        <f t="shared" si="3"/>
+        <v>5.4857414563458526</v>
       </c>
       <c r="O30">
-        <f>IF(O28&lt;$B$26,
-$B$3*O28+SIGN($B$18)*0.5*$B$7*O28*O28,
-IF(O28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(O28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(O28-$B$27) + SIGN($B$19)*0.5*$B$7*(O28-$B$27)*(O28-$B$27)))</f>
-        <v>61.09375</v>
+        <f t="shared" si="3"/>
+        <v>7.3077194783238753</v>
       </c>
       <c r="P30">
-        <f>IF(P28&lt;$B$26,
-$B$3*P28+SIGN($B$18)*0.5*$B$7*P28*P28,
-IF(P28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(P28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(P28-$B$27) + SIGN($B$19)*0.5*$B$7*(P28-$B$27)*(P28-$B$27)))</f>
-        <v>77.34375</v>
+        <f t="shared" si="3"/>
+        <v>9.1296975003018961</v>
       </c>
       <c r="Q30">
-        <f>IF(Q28&lt;$B$26,
-$B$3*Q28+SIGN($B$18)*0.5*$B$7*Q28*Q28,
-IF(Q28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(Q28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(Q28-$B$27) + SIGN($B$19)*0.5*$B$7*(Q28-$B$27)*(Q28-$B$27)))</f>
-        <v>93.59375</v>
+        <f t="shared" si="3"/>
+        <v>10.951675522279919</v>
       </c>
       <c r="R30">
-        <f>IF(R28&lt;$B$26,
-$B$3*R28+SIGN($B$18)*0.5*$B$7*R28*R28,
-IF(R28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(R28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(R28-$B$27) + SIGN($B$19)*0.5*$B$7*(R28-$B$27)*(R28-$B$27)))</f>
-        <v>109.84375</v>
+        <f t="shared" si="3"/>
+        <v>12.77365354425794</v>
       </c>
       <c r="S30">
-        <f>IF(S28&lt;$B$26,
-$B$3*S28+SIGN($B$18)*0.5*$B$7*S28*S28,
-IF(S28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(S28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(S28-$B$27) + SIGN($B$19)*0.5*$B$7*(S28-$B$27)*(S28-$B$27)))</f>
-        <v>126.09375</v>
+        <f t="shared" si="3"/>
+        <v>14.595631566235962</v>
       </c>
       <c r="T30">
-        <f>IF(T28&lt;$B$26,
-$B$3*T28+SIGN($B$18)*0.5*$B$7*T28*T28,
-IF(T28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(T28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(T28-$B$27) + SIGN($B$19)*0.5*$B$7*(T28-$B$27)*(T28-$B$27)))</f>
-        <v>142.34375</v>
+        <f t="shared" si="3"/>
+        <v>16.417609588213985</v>
       </c>
       <c r="U30">
-        <f>IF(U28&lt;$B$26,
-$B$3*U28+SIGN($B$18)*0.5*$B$7*U28*U28,
-IF(U28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(U28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(U28-$B$27) + SIGN($B$19)*0.5*$B$7*(U28-$B$27)*(U28-$B$27)))</f>
-        <v>158.59375</v>
+        <f t="shared" si="3"/>
+        <v>18.239587610192007</v>
       </c>
       <c r="V30">
-        <f>IF(V28&lt;$B$26,
-$B$3*V28+SIGN($B$18)*0.5*$B$7*V28*V28,
-IF(V28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(V28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(V28-$B$27) + SIGN($B$19)*0.5*$B$7*(V28-$B$27)*(V28-$B$27)))</f>
-        <v>174.84375</v>
+        <f t="shared" si="3"/>
+        <v>20.06156563217003</v>
       </c>
       <c r="W30">
-        <f>IF(W28&lt;$B$26,
-$B$3*W28+SIGN($B$18)*0.5*$B$7*W28*W28,
-IF(W28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(W28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(W28-$B$27) + SIGN($B$19)*0.5*$B$7*(W28-$B$27)*(W28-$B$27)))</f>
-        <v>191.09375</v>
+        <f t="shared" si="3"/>
+        <v>21.883543654148053</v>
       </c>
       <c r="X30">
-        <f>IF(X28&lt;$B$26,
-$B$3*X28+SIGN($B$18)*0.5*$B$7*X28*X28,
-IF(X28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(X28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(X28-$B$27) + SIGN($B$19)*0.5*$B$7*(X28-$B$27)*(X28-$B$27)))</f>
-        <v>207.34375</v>
+        <f t="shared" si="3"/>
+        <v>23.705521676126075</v>
       </c>
       <c r="Y30">
-        <f>IF(Y28&lt;$B$26,
-$B$3*Y28+SIGN($B$18)*0.5*$B$7*Y28*Y28,
-IF(Y28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(Y28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(Y28-$B$27) + SIGN($B$19)*0.5*$B$7*(Y28-$B$27)*(Y28-$B$27)))</f>
-        <v>223.59375</v>
+        <f t="shared" si="3"/>
+        <v>25.527499698104098</v>
       </c>
       <c r="Z30">
-        <f>IF(Z28&lt;$B$26,
-$B$3*Z28+SIGN($B$18)*0.5*$B$7*Z28*Z28,
-IF(Z28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(Z28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(Z28-$B$27) + SIGN($B$19)*0.5*$B$7*(Z28-$B$27)*(Z28-$B$27)))</f>
-        <v>239.84375</v>
+        <f t="shared" si="3"/>
+        <v>27.34947772008212</v>
       </c>
       <c r="AA30">
-        <f>IF(AA28&lt;$B$26,
-$B$3*AA28+SIGN($B$18)*0.5*$B$7*AA28*AA28,
-IF(AA28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AA28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AA28-$B$27) + SIGN($B$19)*0.5*$B$7*(AA28-$B$27)*(AA28-$B$27)))</f>
-        <v>256.09375</v>
+        <f t="shared" si="3"/>
+        <v>29.171455742060143</v>
       </c>
       <c r="AB30">
-        <f>IF(AB28&lt;$B$26,
-$B$3*AB28+SIGN($B$18)*0.5*$B$7*AB28*AB28,
-IF(AB28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AB28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AB28-$B$27) + SIGN($B$19)*0.5*$B$7*(AB28-$B$27)*(AB28-$B$27)))</f>
-        <v>272.34375</v>
+        <f t="shared" si="3"/>
+        <v>30.993433764038166</v>
       </c>
       <c r="AC30">
-        <f>IF(AC28&lt;$B$26,
-$B$3*AC28+SIGN($B$18)*0.5*$B$7*AC28*AC28,
-IF(AC28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AC28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AC28-$B$27) + SIGN($B$19)*0.5*$B$7*(AC28-$B$27)*(AC28-$B$27)))</f>
-        <v>288.59375</v>
+        <f t="shared" si="3"/>
+        <v>32.815411786016185</v>
       </c>
       <c r="AD30">
-        <f>IF(AD28&lt;$B$26,
-$B$3*AD28+SIGN($B$18)*0.5*$B$7*AD28*AD28,
-IF(AD28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AD28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AD28-$B$27) + SIGN($B$19)*0.5*$B$7*(AD28-$B$27)*(AD28-$B$27)))</f>
-        <v>304.84375</v>
+        <f t="shared" si="3"/>
+        <v>34.637389807994204</v>
       </c>
       <c r="AE30">
-        <f>IF(AE28&lt;$B$26,
-$B$3*AE28+SIGN($B$18)*0.5*$B$7*AE28*AE28,
-IF(AE28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AE28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AE28-$B$27) + SIGN($B$19)*0.5*$B$7*(AE28-$B$27)*(AE28-$B$27)))</f>
-        <v>321.09375</v>
+        <f t="shared" si="3"/>
+        <v>36.45936782997223</v>
       </c>
       <c r="AF30">
-        <f>IF(AF28&lt;$B$26,
-$B$3*AF28+SIGN($B$18)*0.5*$B$7*AF28*AF28,
-IF(AF28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AF28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AF28-$B$27) + SIGN($B$19)*0.5*$B$7*(AF28-$B$27)*(AF28-$B$27)))</f>
-        <v>337.34375</v>
+        <f t="shared" si="3"/>
+        <v>38.281345851950249</v>
       </c>
       <c r="AG30">
-        <f>IF(AG28&lt;$B$26,
-$B$3*AG28+SIGN($B$18)*0.5*$B$7*AG28*AG28,
-IF(AG28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AG28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AG28-$B$27) + SIGN($B$19)*0.5*$B$7*(AG28-$B$27)*(AG28-$B$27)))</f>
-        <v>353.59375</v>
+        <f t="shared" si="3"/>
+        <v>40.103323873928275</v>
       </c>
       <c r="AH30">
-        <f>IF(AH28&lt;$B$26,
-$B$3*AH28+SIGN($B$18)*0.5*$B$7*AH28*AH28,
-IF(AH28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AH28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AH28-$B$27) + SIGN($B$19)*0.5*$B$7*(AH28-$B$27)*(AH28-$B$27)))</f>
-        <v>369.84375</v>
+        <f t="shared" si="3"/>
+        <v>41.925301895906294</v>
       </c>
       <c r="AI30">
-        <f>IF(AI28&lt;$B$26,
-$B$3*AI28+SIGN($B$18)*0.5*$B$7*AI28*AI28,
-IF(AI28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AI28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AI28-$B$27) + SIGN($B$19)*0.5*$B$7*(AI28-$B$27)*(AI28-$B$27)))</f>
-        <v>386.09375</v>
+        <f t="shared" si="3"/>
+        <v>43.747279917884313</v>
       </c>
       <c r="AJ30">
-        <f>IF(AJ28&lt;$B$26,
-$B$3*AJ28+SIGN($B$18)*0.5*$B$7*AJ28*AJ28,
-IF(AJ28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AJ28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AJ28-$B$27) + SIGN($B$19)*0.5*$B$7*(AJ28-$B$27)*(AJ28-$B$27)))</f>
-        <v>402.34375</v>
+        <f t="shared" si="3"/>
+        <v>45.569257939862339</v>
       </c>
       <c r="AK30">
-        <f>IF(AK28&lt;$B$26,
-$B$3*AK28+SIGN($B$18)*0.5*$B$7*AK28*AK28,
-IF(AK28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AK28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AK28-$B$27) + SIGN($B$19)*0.5*$B$7*(AK28-$B$27)*(AK28-$B$27)))</f>
-        <v>418.59375</v>
+        <f t="shared" si="3"/>
+        <v>47.391235961840358</v>
       </c>
       <c r="AL30">
-        <f>IF(AL28&lt;$B$26,
-$B$3*AL28+SIGN($B$18)*0.5*$B$7*AL28*AL28,
-IF(AL28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AL28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AL28-$B$27) + SIGN($B$19)*0.5*$B$7*(AL28-$B$27)*(AL28-$B$27)))</f>
-        <v>434.84375</v>
+        <f t="shared" si="3"/>
+        <v>49.213213983818378</v>
       </c>
       <c r="AM30">
-        <f>IF(AM28&lt;$B$26,
-$B$3*AM28+SIGN($B$18)*0.5*$B$7*AM28*AM28,
-IF(AM28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AM28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AM28-$B$27) + SIGN($B$19)*0.5*$B$7*(AM28-$B$27)*(AM28-$B$27)))</f>
-        <v>451.09375</v>
+        <f t="shared" si="3"/>
+        <v>51.035192005796397</v>
       </c>
       <c r="AN30">
-        <f>IF(AN28&lt;$B$26,
-$B$3*AN28+SIGN($B$18)*0.5*$B$7*AN28*AN28,
-IF(AN28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AN28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AN28-$B$27) + SIGN($B$19)*0.5*$B$7*(AN28-$B$27)*(AN28-$B$27)))</f>
-        <v>467.34375</v>
+        <f t="shared" si="3"/>
+        <v>52.857170027774423</v>
       </c>
       <c r="AO30">
-        <f>IF(AO28&lt;$B$26,
-$B$3*AO28+SIGN($B$18)*0.5*$B$7*AO28*AO28,
-IF(AO28&lt;$B$27,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AO28-$B$26)*$B$21,
-$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AO28-$B$27) + SIGN($B$19)*0.5*$B$7*(AO28-$B$27)*(AO28-$B$27)))</f>
-        <v>483.59375</v>
+        <f t="shared" si="3"/>
+        <v>54.679148049752442</v>
       </c>
       <c r="AP30">
-        <f t="shared" ref="AP30:BH30" si="2">IF(AP28&lt;$B$26,
+        <f t="shared" ref="AP30:BH30" si="4">IF(AP28&lt;$B$26,
 $B$3*AP28+SIGN($B$18)*0.5*$B$7*AP28*AP28,
 IF(AP28&lt;$B$27,
 $B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(AP28-$B$26)*$B$21,
 $B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(AP28-$B$27) + SIGN($B$19)*0.5*$B$7*(AP28-$B$27)*(AP28-$B$27)))</f>
-        <v>499.84375</v>
+        <v>56.501126071730468</v>
       </c>
       <c r="AQ30">
-        <f t="shared" si="2"/>
-        <v>516.09375</v>
+        <f t="shared" si="4"/>
+        <v>58.323104093708487</v>
       </c>
       <c r="AR30">
-        <f t="shared" si="2"/>
-        <v>532.34375</v>
+        <f t="shared" si="4"/>
+        <v>60.145082115686513</v>
       </c>
       <c r="AS30">
-        <f t="shared" si="2"/>
-        <v>548.59375</v>
+        <f t="shared" si="4"/>
+        <v>61.967060137664532</v>
       </c>
       <c r="AT30">
-        <f t="shared" si="2"/>
-        <v>564.84375</v>
+        <f t="shared" si="4"/>
+        <v>63.789038159642551</v>
       </c>
       <c r="AU30">
-        <f t="shared" si="2"/>
-        <v>581.09375</v>
+        <f t="shared" si="4"/>
+        <v>65.611016181620585</v>
       </c>
       <c r="AV30">
-        <f t="shared" si="2"/>
-        <v>597.34375</v>
+        <f t="shared" si="4"/>
+        <v>67.432994203598611</v>
       </c>
       <c r="AW30">
-        <f t="shared" si="2"/>
-        <v>613.59375</v>
+        <f t="shared" si="4"/>
+        <v>69.254972225576623</v>
       </c>
       <c r="AX30">
-        <f t="shared" si="2"/>
-        <v>629.84375</v>
+        <f t="shared" si="4"/>
+        <v>71.076950247554649</v>
       </c>
       <c r="AY30">
-        <f t="shared" si="2"/>
-        <v>646.09375</v>
+        <f t="shared" si="4"/>
+        <v>72.898928269532675</v>
       </c>
       <c r="AZ30">
-        <f t="shared" si="2"/>
-        <v>662.34375</v>
+        <f t="shared" si="4"/>
+        <v>74.720906291510687</v>
       </c>
       <c r="BA30">
-        <f t="shared" si="2"/>
-        <v>680</v>
+        <f t="shared" si="4"/>
+        <v>76.542884313488713</v>
       </c>
       <c r="BB30">
-        <f t="shared" si="2"/>
-        <v>702.5</v>
+        <f t="shared" si="4"/>
+        <v>78.364862335466739</v>
       </c>
       <c r="BC30">
-        <f t="shared" si="2"/>
-        <v>730</v>
+        <f t="shared" si="4"/>
+        <v>80.186840357444765</v>
       </c>
       <c r="BD30">
-        <f t="shared" si="2"/>
-        <v>762.5</v>
+        <f t="shared" si="4"/>
+        <v>82.008818379422777</v>
       </c>
       <c r="BE30">
-        <f t="shared" si="2"/>
-        <v>800</v>
+        <f t="shared" si="4"/>
+        <v>84.039614780823584</v>
       </c>
       <c r="BF30">
-        <f t="shared" si="2"/>
-        <v>842.5</v>
+        <f t="shared" si="4"/>
+        <v>86.839614780823567</v>
       </c>
       <c r="BG30">
-        <f t="shared" si="2"/>
-        <v>890</v>
+        <f t="shared" si="4"/>
+        <v>90.439614780823575</v>
       </c>
       <c r="BH30">
-        <f t="shared" si="2"/>
-        <v>942.5</v>
+        <f t="shared" si="4"/>
+        <v>94.839614780823581</v>
       </c>
     </row>
     <row r="31" spans="1:72" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
BugFix in SpeedProfile removed Mixed view in UI added handview panel in UI
</commit_message>
<xml_diff>
--- a/theory/Kinematik.xlsx
+++ b/theory/Kinematik.xlsx
@@ -1814,11 +1814,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="153173560"/>
-        <c:axId val="153170816"/>
+        <c:axId val="39860040"/>
+        <c:axId val="39861608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="153173560"/>
+        <c:axId val="39860040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1856,13 +1856,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153170816"/>
+        <c:crossAx val="39861608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="153170816"/>
+        <c:axId val="39861608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1901,7 +1901,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153173560"/>
+        <c:crossAx val="39860040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
@@ -1997,11 +1997,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="153171208"/>
-        <c:axId val="153173952"/>
+        <c:axId val="39861216"/>
+        <c:axId val="39862000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="153171208"/>
+        <c:axId val="39861216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -2013,13 +2013,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153173952"/>
+        <c:crossAx val="39862000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="153173952"/>
+        <c:axId val="39862000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -2032,7 +2032,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153171208"/>
+        <c:crossAx val="39861216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
@@ -2156,10 +2156,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>125</c:v>
+                  <c:v>22.395075557352065</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>1475</c:v>
+                  <c:v>1585.6549244426478</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
                   <c:v>1600</c:v>
@@ -2174,16 +2174,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>0.21609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2206,10 +2206,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>136.67504192892</c:v>
+                  <c:v>22.269339653504748</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>1463.3249580710799</c:v>
+                  <c:v>1585.7806603464953</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
                   <c:v>1600</c:v>
@@ -2224,16 +2224,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>0.21609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.8337520964459997E-2</c:v>
+                  <c:v>0.17156132069299049</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.8337520964459997E-2</c:v>
+                  <c:v>0.17156132069299049</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2256,7 +2256,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>8.0499999999999883</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
                   <c:v>1600</c:v>
@@ -2274,16 +2274,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>0.21609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2298,11 +2298,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="204112896"/>
-        <c:axId val="204110544"/>
+        <c:axId val="39863568"/>
+        <c:axId val="226834616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="204112896"/>
+        <c:axId val="39863568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2345,12 +2345,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="204110544"/>
+        <c:crossAx val="226834616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="204110544"/>
+        <c:axId val="226834616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2401,7 +2401,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="204112896"/>
+        <c:crossAx val="39863568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2769,157 +2769,157 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.21609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2000000000000001E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8000000000000001E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4.8000000000000001E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.2000000000000001E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.6E-2</c:v>
+                  <c:v>0.17130984888529585</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0</c:v>
+                  <c:v>0.20000000000000021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2934,11 +2934,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="204113288"/>
-        <c:axId val="204115248"/>
+        <c:axId val="226830696"/>
+        <c:axId val="226834224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="204113288"/>
+        <c:axId val="226830696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2989,12 +2989,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="204115248"/>
+        <c:crossAx val="226834224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="204115248"/>
+        <c:axId val="226834224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3045,7 +3045,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="204113288"/>
+        <c:crossAx val="226830696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3439,154 +3439,154 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25600000000000001</c:v>
+                  <c:v>5.9834545735489755</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.024</c:v>
+                  <c:v>11.465369737878442</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3040000000000003</c:v>
+                  <c:v>16.947284902207908</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.09375</c:v>
+                  <c:v>22.429200066537376</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.09375</c:v>
+                  <c:v>27.911115230866841</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.09375</c:v>
+                  <c:v>33.393030395196313</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.09375</c:v>
+                  <c:v>38.874945559525777</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.09375</c:v>
+                  <c:v>44.356860723855242</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14.09375</c:v>
+                  <c:v>49.838775888184713</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16.09375</c:v>
+                  <c:v>55.320691052514178</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18.09375</c:v>
+                  <c:v>60.802606216843643</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>20.09375</c:v>
+                  <c:v>66.284521381173121</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>22.09375</c:v>
+                  <c:v>71.766436545502586</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>24.09375</c:v>
+                  <c:v>77.24835170983205</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26.09375</c:v>
+                  <c:v>82.730266874161515</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28.09375</c:v>
+                  <c:v>88.21218203849098</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>30.09375</c:v>
+                  <c:v>93.694097202820458</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>32.09375</c:v>
+                  <c:v>99.176012367149923</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>34.09375</c:v>
+                  <c:v>104.65792753147939</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>36.09375</c:v>
+                  <c:v>110.13984269580887</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>38.09375</c:v>
+                  <c:v>115.62175786013833</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>40.09375</c:v>
+                  <c:v>121.1036730244678</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>42.09375</c:v>
+                  <c:v>126.58558818879726</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>44.09375</c:v>
+                  <c:v>132.06750335312674</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>46.09375</c:v>
+                  <c:v>137.54941851745619</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>48.09375</c:v>
+                  <c:v>143.03133368178567</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>50.09375</c:v>
+                  <c:v>148.51324884611512</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>52.09375</c:v>
+                  <c:v>153.9951640104446</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>54.09375</c:v>
+                  <c:v>159.47707917477408</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>56.09375</c:v>
+                  <c:v>164.95899433910353</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>58.09375</c:v>
+                  <c:v>170.44090950343301</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>60.09375</c:v>
+                  <c:v>175.92282466776246</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>62.09375</c:v>
+                  <c:v>181.40473983209191</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>64.09375</c:v>
+                  <c:v>186.88665499642138</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>66.09375</c:v>
+                  <c:v>192.36857016075086</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>68.09375</c:v>
+                  <c:v>197.85048532508031</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>70.09375</c:v>
+                  <c:v>203.33240048940979</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>72.09375</c:v>
+                  <c:v>208.81431565373924</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>74.09375</c:v>
+                  <c:v>214.29623081806872</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>76.09375</c:v>
+                  <c:v>219.77814598239817</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>78.09375</c:v>
+                  <c:v>225.26006114672765</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>80.09375</c:v>
+                  <c:v>230.74197631105713</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>82.09375</c:v>
+                  <c:v>236.22389147538658</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>84.09375</c:v>
+                  <c:v>241.70580663971606</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>86.09375</c:v>
+                  <c:v>247.18772180404551</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>88.09375</c:v>
+                  <c:v>252.66963696837499</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>89.883499999999998</c:v>
+                  <c:v>258.15155213270447</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>91.163499999999999</c:v>
+                  <c:v>263.63346729703397</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>91.9315</c:v>
+                  <c:v>269.11538246136342</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>92.1875</c:v>
+                  <c:v>274.80307881843902</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3601,11 +3601,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="204110936"/>
-        <c:axId val="204108976"/>
+        <c:axId val="226831872"/>
+        <c:axId val="226831088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="204110936"/>
+        <c:axId val="226831872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3661,12 +3661,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="204108976"/>
+        <c:crossAx val="226831088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="204108976"/>
+        <c:axId val="226831088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3722,7 +3722,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="204110936"/>
+        <c:crossAx val="226831872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -32804,8 +32804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BT32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="P51" sqref="P51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32823,7 +32823,7 @@
         <v>84</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.21609999999999999</v>
       </c>
       <c r="C3" t="s">
         <v>86</v>
@@ -32834,7 +32834,7 @@
         <v>85</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C4" t="s">
         <v>86</v>
@@ -32845,7 +32845,7 @@
         <v>87</v>
       </c>
       <c r="B5">
-        <v>100</v>
+        <v>273.8</v>
       </c>
       <c r="C5" t="s">
         <v>90</v>
@@ -32867,7 +32867,7 @@
         <v>71</v>
       </c>
       <c r="B7">
-        <v>5.0000000000000001E-4</v>
+        <v>2E-3</v>
       </c>
       <c r="C7" t="s">
         <v>94</v>
@@ -32879,7 +32879,7 @@
       </c>
       <c r="B9">
         <f>B5/B6</f>
-        <v>6.25E-2</v>
+        <v>0.171125</v>
       </c>
       <c r="C9" t="s">
         <v>86</v>
@@ -32891,19 +32891,19 @@
       </c>
       <c r="E10">
         <f>(B3-B4)/B7</f>
-        <v>0</v>
+        <v>8.0499999999999883</v>
       </c>
       <c r="F10">
         <f>(B3-B4)/B7</f>
-        <v>0</v>
+        <v>8.0499999999999883</v>
       </c>
       <c r="G10">
         <f>(B3-B4)/B7</f>
-        <v>0</v>
+        <v>8.0499999999999883</v>
       </c>
       <c r="H10">
         <f>(B3-B4)/B7</f>
-        <v>0</v>
+        <v>8.0499999999999883</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -32912,24 +32912,24 @@
       </c>
       <c r="E11" s="127">
         <f>B3*B6-0.5*B7*E10*E10 - B5</f>
-        <v>-100</v>
+        <v>71.895197499999995</v>
       </c>
       <c r="F11">
         <f>B3*B6+0.5*B7*F10*F10 - B5</f>
-        <v>-100</v>
+        <v>72.024802499999964</v>
       </c>
       <c r="G11">
         <f>B4*G10+0.5*B7*G10*G10- B5</f>
-        <v>-100</v>
+        <v>-272.12519750000001</v>
       </c>
       <c r="H11">
         <f>-B4*G10-0.5*B7*G10*G10- B5</f>
-        <v>-100</v>
+        <v>-275.47480250000001</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11">
         <f>-B5*B7-0.5*B3*B3</f>
-        <v>-0.05</v>
+        <v>-0.57094960500000003</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -32938,23 +32938,23 @@
       </c>
       <c r="E12">
         <f>B7*(B6-E10)</f>
-        <v>0.8</v>
+        <v>3.1839</v>
       </c>
       <c r="F12">
         <f>B7*(B6+F10)</f>
-        <v>0.8</v>
+        <v>3.2161</v>
       </c>
       <c r="G12">
         <f>B3+B4+B7*G10</f>
-        <v>0</v>
+        <v>0.43220000000000003</v>
       </c>
       <c r="H12">
         <f>B3+B4+B7*G10</f>
-        <v>0</v>
+        <v>0.43220000000000003</v>
       </c>
       <c r="L12">
         <f>B3</f>
-        <v>0</v>
+        <v>0.21609999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -32963,19 +32963,19 @@
       </c>
       <c r="E13">
         <f>-B7</f>
-        <v>-5.0000000000000001E-4</v>
+        <v>-2E-3</v>
       </c>
       <c r="F13">
         <f>B7</f>
-        <v>5.0000000000000001E-4</v>
+        <v>2E-3</v>
       </c>
       <c r="G13">
         <f>B7</f>
-        <v>5.0000000000000001E-4</v>
+        <v>2E-3</v>
       </c>
       <c r="H13">
         <f>-B7</f>
-        <v>-5.0000000000000001E-4</v>
+        <v>-2E-3</v>
       </c>
       <c r="L13">
         <f>0.5</f>
@@ -33001,11 +33001,11 @@
       </c>
       <c r="N16" s="4">
         <f>B26</f>
-        <v>125</v>
+        <v>22.395075557352065</v>
       </c>
       <c r="O16" s="3">
         <f>B27</f>
-        <v>1475</v>
+        <v>1585.6549244426478</v>
       </c>
       <c r="P16">
         <f>B6</f>
@@ -33036,19 +33036,19 @@
       </c>
       <c r="M17">
         <f>B3</f>
-        <v>0</v>
+        <v>0.21609999999999999</v>
       </c>
       <c r="N17" s="3">
         <f>B21</f>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="O17" s="3">
         <f>N17</f>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="P17">
         <f>B4</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
@@ -33057,7 +33057,7 @@
       </c>
       <c r="B18" s="127">
         <f>(B5-B3*B6-0.5*(B4-B3)*(B4-B3)/B7)/(B6*B7+(B3-B4))</f>
-        <v>125</v>
+        <v>-22.395075557352065</v>
       </c>
       <c r="C18" t="s">
         <v>91</v>
@@ -33067,15 +33067,15 @@
       </c>
       <c r="E18" s="3">
         <f>(-E12+SQRT(E12*E12-4*E13*E11))/(2*E13)</f>
-        <v>136.67504192892</v>
+        <v>-22.269339653504748</v>
       </c>
       <c r="F18" s="130">
         <f>(-F12+SQRT(F12*F12-4*F13*F11))/(2*F13)</f>
-        <v>116.51513899116806</v>
+        <v>-22.715970630058479</v>
       </c>
       <c r="G18" s="3">
         <f>(-G12+SQRT(G12*G12-4*G13*G11))/(2*G13)</f>
-        <v>447.21359549995793</v>
+        <v>276.31623323335776</v>
       </c>
       <c r="H18" s="3" t="e">
         <f>-(-H12+SQRT(H12*H12-4*H13*H11))/(2*H13)</f>
@@ -33083,7 +33083,7 @@
       </c>
       <c r="I18" s="127">
         <f>(B4-B3)/B7</f>
-        <v>0</v>
+        <v>-8.0499999999999883</v>
       </c>
       <c r="L18" t="s">
         <v>126</v>
@@ -33093,11 +33093,11 @@
       </c>
       <c r="N18" s="4">
         <f>E26</f>
-        <v>136.67504192892</v>
+        <v>22.269339653504748</v>
       </c>
       <c r="O18" s="3">
         <f>E27</f>
-        <v>1463.3249580710799</v>
+        <v>1585.7806603464953</v>
       </c>
       <c r="P18">
         <f>B6</f>
@@ -33110,7 +33110,7 @@
       </c>
       <c r="B19" s="3">
         <f>(B4-B3)/B7-B18</f>
-        <v>-125</v>
+        <v>14.345075557352077</v>
       </c>
       <c r="C19" t="s">
         <v>91</v>
@@ -33120,15 +33120,15 @@
       </c>
       <c r="E19" s="3">
         <f>(B4-B3)/B7-E18</f>
-        <v>-136.67504192892</v>
+        <v>14.219339653504759</v>
       </c>
       <c r="F19" s="3">
         <f>(B4-B3)/B7-F18</f>
-        <v>-116.51513899116806</v>
+        <v>14.66597063005849</v>
       </c>
       <c r="G19" s="127">
         <f>-(G10+G18)</f>
-        <v>-447.21359549995793</v>
+        <v>-284.36623323335778</v>
       </c>
       <c r="H19" s="127" t="e">
         <f>-(H10+H18)</f>
@@ -33142,19 +33142,19 @@
       </c>
       <c r="M19">
         <f>B3</f>
-        <v>0</v>
+        <v>0.21609999999999999</v>
       </c>
       <c r="N19" s="3">
         <f>E21</f>
-        <v>6.8337520964459997E-2</v>
+        <v>0.17156132069299049</v>
       </c>
       <c r="O19" s="3">
         <f>N19</f>
-        <v>6.8337520964459997E-2</v>
+        <v>0.17156132069299049</v>
       </c>
       <c r="P19">
         <f>B4</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="20" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
@@ -33166,7 +33166,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="127">
         <f>ABS(G18)+ABS(G19)</f>
-        <v>894.42719099991587</v>
+        <v>560.6824664667156</v>
       </c>
       <c r="H20" s="127" t="e">
         <f>ABS(H18)+ABS(H19)</f>
@@ -33182,7 +33182,7 @@
       </c>
       <c r="B21" s="3">
         <f>B3+B7*B18</f>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="C21" t="s">
         <v>86</v>
@@ -33192,15 +33192,15 @@
       </c>
       <c r="E21" s="3">
         <f>B3+B7*E18</f>
-        <v>6.8337520964459997E-2</v>
+        <v>0.17156132069299049</v>
       </c>
       <c r="F21" s="3">
         <f>B3+B7*F18</f>
-        <v>5.8257569495584027E-2</v>
+        <v>0.17066805873988303</v>
       </c>
       <c r="G21">
         <f>B3+B7*G18</f>
-        <v>0.22360679774997896</v>
+        <v>0.76873246646671545</v>
       </c>
       <c r="H21" t="e">
         <f>B3+B7*H18</f>
@@ -33208,7 +33208,7 @@
       </c>
       <c r="I21" s="3">
         <f>B3+B7*I18</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="L21" t="s">
         <v>88</v>
@@ -33218,7 +33218,7 @@
       </c>
       <c r="N21" s="4">
         <f>I26</f>
-        <v>0</v>
+        <v>8.0499999999999883</v>
       </c>
       <c r="O21" s="3">
         <f>I27</f>
@@ -33235,7 +33235,7 @@
       </c>
       <c r="B22" s="127">
         <f>$B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(B6-$B$27) + SIGN($B$19)*0.5*$B$7*(B6-$B$27)*(B6-$B$27)</f>
-        <v>92.1875</v>
+        <v>274.80307881843902</v>
       </c>
       <c r="C22" t="s">
         <v>90</v>
@@ -33245,15 +33245,15 @@
       </c>
       <c r="E22" s="127">
         <f>$B$3*$E$26+SIGN($E$18)*0.5*$B$7*$E$26*$E$26+($E$27-$E$26)*$E$21 + $E$21*(B6-$E$27) + SIGN($E$19)*0.5*$B$7*(B6-$E$27)*(B6-$E$27)</f>
-        <v>99.999999999999972</v>
+        <v>275.19622621756969</v>
       </c>
       <c r="F22" s="127">
         <f>$B$3*$F$26+SIGN($F$18)*0.5*$B$7*$F$26*$F$26+($F$27-$F$26)*$F$21 + $F$21*(B6-$F$27) + SIGN($F$19)*0.5*$B$7*(B6-$F$27)*(B6-$F$27)</f>
-        <v>86.424222385868845</v>
+        <v>273.8000000000003</v>
       </c>
       <c r="G22" s="127">
         <f>$B$3*$G$26+SIGN($G$18)*0.5*$B$7*$G$26*$G$26+($G$27-$G$26)*$G$21 + $G$21*(G20-$G$27) + SIGN($G$19)*0.5*$B$7*(G20-$G$27)*(G20-$G$27)</f>
-        <v>100</v>
+        <v>273.7999999999999</v>
       </c>
       <c r="H22" s="127" t="e">
         <f>$B$3*$H$26+SIGN($H$18)*0.5*$B$7*$H$26*$H$26+($H$27-$H$26)*$H$21 + $H$21*(H20-$H$27) + SIGN($H$19)*0.5*$B$7*(H20-$H$27)*(H20-$H$27)</f>
@@ -33261,33 +33261,33 @@
       </c>
       <c r="I22">
         <f>$B$3*$I$26+SIGN($I$18)*0.5*$B$7*$I$26*$I$26+($I$27-$I$26)*$I$21 + $I$21*(B6-$I$27) + SIGN($I$19)*0.5*$B$7*(B6-$I$27)*(B6-$I$27)</f>
-        <v>0</v>
+        <v>320.06480250000004</v>
       </c>
       <c r="J22" t="s">
         <v>117</v>
       </c>
-      <c r="K22" t="e">
+      <c r="K22">
         <f>(B5-B3*I18-0.5*B7*I18*I18)/B4+I18</f>
-        <v>#DIV/0!</v>
+        <v>1369.3240125</v>
       </c>
       <c r="L22" t="s">
         <v>125</v>
       </c>
       <c r="M22">
         <f>B3</f>
-        <v>0</v>
+        <v>0.21609999999999999</v>
       </c>
       <c r="N22" s="3">
         <f>I21</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="O22" s="3">
         <f>I21</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="P22" s="3">
         <f>I21</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="23" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
@@ -33296,7 +33296,7 @@
       </c>
       <c r="B23">
         <f>B21+B19*B7</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C23" t="s">
         <v>86</v>
@@ -33306,15 +33306,15 @@
       </c>
       <c r="E23" s="3">
         <f>E21+E19*B7</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F23" s="3">
         <f>F21+F19*B7</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G23" s="3">
         <f>G21+G19*B7</f>
-        <v>0</v>
+        <v>0.19999999999999984</v>
       </c>
       <c r="H23" s="3" t="e">
         <f>H21+H19*B7</f>
@@ -33322,27 +33322,27 @@
       </c>
       <c r="I23" s="3">
         <f>I21+I19*B7</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="J23" t="s">
         <v>118</v>
       </c>
       <c r="K23" s="3">
         <f>SQRT(B3*B3 +2*B5*B7)</f>
-        <v>0.31622776601683794</v>
+        <v>1.0685968416573204</v>
       </c>
     </row>
     <row r="24" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>122</v>
       </c>
-      <c r="B24" t="e">
+      <c r="B24">
         <f>(B5-0.5*(B4-B3)*(B4-B3)/B7)/B3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E24" t="e">
+        <v>1266.706142989357</v>
+      </c>
+      <c r="E24">
         <f>(B5+0.5*B7*E10*E10)/B3</f>
-        <v>#DIV/0!</v>
+        <v>1267.3058884775567</v>
       </c>
       <c r="J24" t="s">
         <v>120</v>
@@ -33361,22 +33361,22 @@
       </c>
       <c r="B26" s="127">
         <f>ABS(B18)</f>
-        <v>125</v>
+        <v>22.395075557352065</v>
       </c>
       <c r="C26" t="s">
         <v>91</v>
       </c>
       <c r="E26" s="127">
         <f>ABS(E18)</f>
-        <v>136.67504192892</v>
+        <v>22.269339653504748</v>
       </c>
       <c r="F26" s="127">
         <f>ABS(F18)</f>
-        <v>116.51513899116806</v>
+        <v>22.715970630058479</v>
       </c>
       <c r="G26" s="127">
         <f>ABS(G18)</f>
-        <v>447.21359549995793</v>
+        <v>276.31623323335776</v>
       </c>
       <c r="H26" s="127" t="e">
         <f>ABS(H18)</f>
@@ -33384,7 +33384,7 @@
       </c>
       <c r="I26" s="127">
         <f>ABS(I18)</f>
-        <v>0</v>
+        <v>8.0499999999999883</v>
       </c>
     </row>
     <row r="27" spans="1:72" ht="15.6" x14ac:dyDescent="0.35">
@@ -33393,22 +33393,22 @@
       </c>
       <c r="B27" s="127">
         <f>B6-ABS(B19)</f>
-        <v>1475</v>
+        <v>1585.6549244426478</v>
       </c>
       <c r="C27" t="s">
         <v>91</v>
       </c>
       <c r="E27" s="127">
         <f>B6-ABS(E19)</f>
-        <v>1463.3249580710799</v>
+        <v>1585.7806603464953</v>
       </c>
       <c r="F27" s="127">
         <f>B6-ABS(F19)</f>
-        <v>1483.484861008832</v>
+        <v>1585.3340293699416</v>
       </c>
       <c r="G27" s="127">
         <f>G26</f>
-        <v>447.21359549995793</v>
+        <v>276.31623323335776</v>
       </c>
       <c r="H27" s="127" t="e">
         <f>H26</f>
@@ -33642,207 +33642,207 @@
       </c>
       <c r="J29" s="127">
         <f>IF(J28&lt;ABS($B$18),$B$3+SIGN($B$18)*J$28*$B$7,IF(J28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(J28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>0</v>
+        <v>0.21609999999999999</v>
       </c>
       <c r="K29" s="127">
         <f t="shared" ref="K29:BH29" si="1">IF(K28&lt;ABS($B$18),$B$3+SIGN($B$18)*K$28*$B$7,IF(K28&lt;$B$6-ABS($B$19),$B$21,$B$21+SIGN($B$19)*(K28-($B$6-ABS($B$19)))*$B$7))</f>
-        <v>1.6E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="L29" s="127">
         <f t="shared" si="1"/>
-        <v>3.2000000000000001E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="M29" s="127">
         <f t="shared" si="1"/>
-        <v>4.8000000000000001E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="N29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="O29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="P29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="Q29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="R29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="S29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="T29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="U29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="V29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="W29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="X29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="Y29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="Z29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AA29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AB29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AC29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AD29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AE29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AF29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AG29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AH29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AI29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AJ29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AK29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AL29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AM29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AN29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AO29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AP29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AQ29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AR29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AS29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AT29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AU29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AV29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AW29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AX29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AY29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="AZ29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="BA29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="BB29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="BC29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="BD29" s="127">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="BE29" s="127">
         <f t="shared" si="1"/>
-        <v>4.8000000000000001E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="BF29" s="127">
         <f t="shared" si="1"/>
-        <v>3.2000000000000001E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="BG29" s="127">
         <f t="shared" si="1"/>
-        <v>1.6E-2</v>
+        <v>0.17130984888529585</v>
       </c>
       <c r="BH29" s="127">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.20000000000000021</v>
       </c>
       <c r="BI29" s="127"/>
       <c r="BJ29" s="127"/>
@@ -33881,203 +33881,203 @@
 IF(K28&lt;$B$27,
 $B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+(K28-$B$26)*$B$21,
 $B$3*$B$26+SIGN($B$18)*0.5*$B$7*$B$26*$B$26+($B$27-$B$26)*$B$21 + $B$21*(K28-$B$27) + SIGN($B$19)*0.5*$B$7*(K28-$B$27)*(K28-$B$27)))</f>
-        <v>0.25600000000000001</v>
+        <v>5.9834545735489755</v>
       </c>
       <c r="L30">
         <f t="shared" si="2"/>
-        <v>1.024</v>
+        <v>11.465369737878442</v>
       </c>
       <c r="M30">
         <f t="shared" si="2"/>
-        <v>2.3040000000000003</v>
+        <v>16.947284902207908</v>
       </c>
       <c r="N30">
         <f t="shared" si="2"/>
-        <v>4.09375</v>
+        <v>22.429200066537376</v>
       </c>
       <c r="O30">
         <f t="shared" si="2"/>
-        <v>6.09375</v>
+        <v>27.911115230866841</v>
       </c>
       <c r="P30">
         <f t="shared" si="2"/>
-        <v>8.09375</v>
+        <v>33.393030395196313</v>
       </c>
       <c r="Q30">
         <f t="shared" si="2"/>
-        <v>10.09375</v>
+        <v>38.874945559525777</v>
       </c>
       <c r="R30">
         <f t="shared" si="2"/>
-        <v>12.09375</v>
+        <v>44.356860723855242</v>
       </c>
       <c r="S30">
         <f t="shared" si="2"/>
-        <v>14.09375</v>
+        <v>49.838775888184713</v>
       </c>
       <c r="T30">
         <f t="shared" si="2"/>
-        <v>16.09375</v>
+        <v>55.320691052514178</v>
       </c>
       <c r="U30">
         <f t="shared" si="2"/>
-        <v>18.09375</v>
+        <v>60.802606216843643</v>
       </c>
       <c r="V30">
         <f t="shared" si="2"/>
-        <v>20.09375</v>
+        <v>66.284521381173121</v>
       </c>
       <c r="W30">
         <f t="shared" si="2"/>
-        <v>22.09375</v>
+        <v>71.766436545502586</v>
       </c>
       <c r="X30">
         <f t="shared" si="2"/>
-        <v>24.09375</v>
+        <v>77.24835170983205</v>
       </c>
       <c r="Y30">
         <f t="shared" si="2"/>
-        <v>26.09375</v>
+        <v>82.730266874161515</v>
       </c>
       <c r="Z30">
         <f t="shared" si="2"/>
-        <v>28.09375</v>
+        <v>88.21218203849098</v>
       </c>
       <c r="AA30">
         <f t="shared" si="2"/>
-        <v>30.09375</v>
+        <v>93.694097202820458</v>
       </c>
       <c r="AB30">
         <f t="shared" si="2"/>
-        <v>32.09375</v>
+        <v>99.176012367149923</v>
       </c>
       <c r="AC30">
         <f t="shared" si="2"/>
-        <v>34.09375</v>
+        <v>104.65792753147939</v>
       </c>
       <c r="AD30">
         <f t="shared" si="2"/>
-        <v>36.09375</v>
+        <v>110.13984269580887</v>
       </c>
       <c r="AE30">
         <f t="shared" si="2"/>
-        <v>38.09375</v>
+        <v>115.62175786013833</v>
       </c>
       <c r="AF30">
         <f t="shared" si="2"/>
-        <v>40.09375</v>
+        <v>121.1036730244678</v>
       </c>
       <c r="AG30">
         <f t="shared" si="2"/>
-        <v>42.09375</v>
+        <v>126.58558818879726</v>
       </c>
       <c r="AH30">
         <f t="shared" si="2"/>
-        <v>44.09375</v>
+        <v>132.06750335312674</v>
       </c>
       <c r="AI30">
         <f t="shared" si="2"/>
-        <v>46.09375</v>
+        <v>137.54941851745619</v>
       </c>
       <c r="AJ30">
         <f t="shared" si="2"/>
-        <v>48.09375</v>
+        <v>143.03133368178567</v>
       </c>
       <c r="AK30">
         <f t="shared" si="2"/>
-        <v>50.09375</v>
+        <v>148.51324884611512</v>
       </c>
       <c r="AL30">
         <f t="shared" si="2"/>
-        <v>52.09375</v>
+        <v>153.9951640104446</v>
       </c>
       <c r="AM30">
         <f t="shared" si="2"/>
-        <v>54.09375</v>
+        <v>159.47707917477408</v>
       </c>
       <c r="AN30">
         <f t="shared" si="2"/>
-        <v>56.09375</v>
+        <v>164.95899433910353</v>
       </c>
       <c r="AO30">
         <f t="shared" si="2"/>
-        <v>58.09375</v>
+        <v>170.44090950343301</v>
       </c>
       <c r="AP30">
         <f t="shared" si="2"/>
-        <v>60.09375</v>
+        <v>175.92282466776246</v>
       </c>
       <c r="AQ30">
         <f t="shared" si="2"/>
-        <v>62.09375</v>
+        <v>181.40473983209191</v>
       </c>
       <c r="AR30">
         <f t="shared" si="2"/>
-        <v>64.09375</v>
+        <v>186.88665499642138</v>
       </c>
       <c r="AS30">
         <f t="shared" si="2"/>
-        <v>66.09375</v>
+        <v>192.36857016075086</v>
       </c>
       <c r="AT30">
         <f t="shared" si="2"/>
-        <v>68.09375</v>
+        <v>197.85048532508031</v>
       </c>
       <c r="AU30">
         <f t="shared" si="2"/>
-        <v>70.09375</v>
+        <v>203.33240048940979</v>
       </c>
       <c r="AV30">
         <f t="shared" si="2"/>
-        <v>72.09375</v>
+        <v>208.81431565373924</v>
       </c>
       <c r="AW30">
         <f t="shared" si="2"/>
-        <v>74.09375</v>
+        <v>214.29623081806872</v>
       </c>
       <c r="AX30">
         <f t="shared" si="2"/>
-        <v>76.09375</v>
+        <v>219.77814598239817</v>
       </c>
       <c r="AY30">
         <f t="shared" si="2"/>
-        <v>78.09375</v>
+        <v>225.26006114672765</v>
       </c>
       <c r="AZ30">
         <f t="shared" si="2"/>
-        <v>80.09375</v>
+        <v>230.74197631105713</v>
       </c>
       <c r="BA30">
         <f t="shared" si="2"/>
-        <v>82.09375</v>
+        <v>236.22389147538658</v>
       </c>
       <c r="BB30">
         <f t="shared" si="2"/>
-        <v>84.09375</v>
+        <v>241.70580663971606</v>
       </c>
       <c r="BC30">
         <f t="shared" si="2"/>
-        <v>86.09375</v>
+        <v>247.18772180404551</v>
       </c>
       <c r="BD30">
         <f t="shared" si="2"/>
-        <v>88.09375</v>
+        <v>252.66963696837499</v>
       </c>
       <c r="BE30">
         <f t="shared" si="2"/>
-        <v>89.883499999999998</v>
+        <v>258.15155213270447</v>
       </c>
       <c r="BF30">
         <f t="shared" si="2"/>
-        <v>91.163499999999999</v>
+        <v>263.63346729703397</v>
       </c>
       <c r="BG30">
         <f t="shared" si="2"/>
-        <v>91.9315</v>
+        <v>269.11538246136342</v>
       </c>
       <c r="BH30">
         <f t="shared" si="2"/>
-        <v>92.1875</v>
+        <v>274.80307881843902</v>
       </c>
     </row>
     <row r="31" spans="1:72" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
bug in kinematic found
</commit_message>
<xml_diff>
--- a/theory/Kinematik.xlsx
+++ b/theory/Kinematik.xlsx
@@ -1814,11 +1814,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="288445160"/>
-        <c:axId val="288445552"/>
+        <c:axId val="325726880"/>
+        <c:axId val="325726096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="288445160"/>
+        <c:axId val="325726880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1856,13 +1856,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288445552"/>
+        <c:crossAx val="325726096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="288445552"/>
+        <c:axId val="325726096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1901,7 +1901,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288445160"/>
+        <c:crossAx val="325726880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="300"/>
@@ -1997,11 +1997,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="288447904"/>
-        <c:axId val="288446336"/>
+        <c:axId val="325728448"/>
+        <c:axId val="325727664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="288447904"/>
+        <c:axId val="325728448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -2013,13 +2013,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288446336"/>
+        <c:crossAx val="325727664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="288446336"/>
+        <c:axId val="325727664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -2032,7 +2032,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288447904"/>
+        <c:crossAx val="325728448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
@@ -2298,11 +2298,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="332643792"/>
-        <c:axId val="332645360"/>
+        <c:axId val="325729624"/>
+        <c:axId val="324298840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="332643792"/>
+        <c:axId val="325729624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2345,12 +2345,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332645360"/>
+        <c:crossAx val="324298840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="332645360"/>
+        <c:axId val="324298840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2401,7 +2401,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332643792"/>
+        <c:crossAx val="325729624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2522,6 +2522,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2933,11 +2934,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="332639088"/>
-        <c:axId val="332639872"/>
+        <c:axId val="324300016"/>
+        <c:axId val="324296880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="332639088"/>
+        <c:axId val="324300016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2988,12 +2989,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332639872"/>
+        <c:crossAx val="324296880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="332639872"/>
+        <c:axId val="324296880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3044,7 +3045,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332639088"/>
+        <c:crossAx val="324300016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3058,6 +3059,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3176,6 +3178,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3598,11 +3601,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="332644576"/>
-        <c:axId val="332641048"/>
+        <c:axId val="324293744"/>
+        <c:axId val="324294136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="332644576"/>
+        <c:axId val="324293744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3658,12 +3661,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332641048"/>
+        <c:crossAx val="324294136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="332641048"/>
+        <c:axId val="324294136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3719,7 +3722,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332644576"/>
+        <c:crossAx val="324293744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3733,6 +3736,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6273,8 +6277,8 @@
       <xdr:rowOff>17929</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2689413" cy="738344"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="Textfeld 11"/>
@@ -6495,18 +6499,6 @@
                               </m:r>
                             </m:e>
                             <m:e>
-                              <m:r>
-                                <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                  <a:solidFill>
-                                    <a:schemeClr val="tx1"/>
-                                  </a:solidFill>
-                                  <a:effectLst/>
-                                  <a:latin typeface="Cambria Math"/>
-                                  <a:ea typeface="+mn-ea"/>
-                                  <a:cs typeface="+mn-cs"/>
-                                </a:rPr>
-                                <m:t>−</m:t>
-                              </m:r>
                               <m:func>
                                 <m:funcPr>
                                   <m:ctrlPr>
@@ -6689,6 +6681,18 @@
                               </m:r>
                             </m:e>
                             <m:e>
+                              <m:r>
+                                <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                  <a:solidFill>
+                                    <a:schemeClr val="tx1"/>
+                                  </a:solidFill>
+                                  <a:effectLst/>
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  <a:ea typeface="+mn-ea"/>
+                                  <a:cs typeface="+mn-cs"/>
+                                </a:rPr>
+                                <m:t>−</m:t>
+                              </m:r>
                               <m:func>
                                 <m:funcPr>
                                   <m:ctrlPr>
@@ -6890,7 +6894,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="Textfeld 11"/>
@@ -6933,7 +6937,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -6945,40 +6949,114 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
                   <a:latin typeface="Cambria Math"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>_0^1=(■8(</a:t>
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>^</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>1=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>(■8(</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="de-DE" sz="1100" i="0">
                   <a:latin typeface="Cambria Math"/>
                 </a:rPr>
-                <a:t>cos⁡〖</a:t>
+                <a:t>cos</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>⁡〖</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="de-DE" sz="1100" i="0">
                   <a:latin typeface="Cambria Math"/>
                   <a:ea typeface="Cambria Math"/>
                 </a:rPr>
-                <a:t>𝜃_</a:t>
+                <a:t>𝜃</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>_</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="de-DE" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math"/>
                 </a:rPr>
                 <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> 〗&amp;</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="de-DE" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math"/>
                   <a:ea typeface="Cambria Math"/>
                 </a:rPr>
-                <a:t> 〗&amp;0</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>&amp;</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -6987,77 +7065,281 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
+                <a:t>sin</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>⁡〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝜃</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> 〗&amp;</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>@</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>sin</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>⁡〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝜃</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> 〗&amp;</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>&amp;−</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>cos</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>⁡〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝜃</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> 〗&amp;</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>@</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
                 <a:t>&amp;</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>−</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>sin</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>⁡〖</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝜃_</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>0 〗</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
                   <a:latin typeface="Cambria Math"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>−1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>&amp;</a:t>
               </a:r>
@@ -7065,125 +7347,59 @@
                 <a:rPr lang="de-DE" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math"/>
                 </a:rPr>
-                <a:t>0@</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>sin</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>&amp;</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>⁡〖</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝜃</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
+                </a:rPr>
+                <a:t>𝑑</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>_</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
+                </a:rPr>
+                <a:t>5</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>@</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>0 〗&amp;0&amp;</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>cos</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>⁡〖</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝜃_</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>0 〗</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>&amp;</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>&amp;</a:t>
               </a:r>
@@ -7191,7 +7407,25 @@
                 <a:rPr lang="de-DE" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math"/>
                 </a:rPr>
-                <a:t>0@0&amp;−1&amp;0&amp;𝑑_5@0&amp;0&amp;0&amp;1))</a:t>
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>&amp;</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>))</a:t>
               </a:r>
               <a:endParaRPr lang="de-DE" sz="1100"/>
             </a:p>
@@ -7209,8 +7443,8 @@
       <xdr:rowOff>7043</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2689413" cy="724622"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="Textfeld 12"/>
@@ -7997,7 +8231,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="Textfeld 12"/>
@@ -8676,8 +8910,8 @@
       <xdr:rowOff>134470</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2689413" cy="736292"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="Textfeld 14"/>
@@ -8884,12 +9118,6 @@
                               </m:r>
                             </m:e>
                             <m:e>
-                              <m:r>
-                                <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                  <a:latin typeface="Cambria Math"/>
-                                </a:rPr>
-                                <m:t>−</m:t>
-                              </m:r>
                               <m:func>
                                 <m:funcPr>
                                   <m:ctrlPr>
@@ -9082,6 +9310,18 @@
                                 </m:funcPr>
                                 <m:fName>
                                   <m:r>
+                                    <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                      <a:solidFill>
+                                        <a:schemeClr val="tx1"/>
+                                      </a:solidFill>
+                                      <a:effectLst/>
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      <a:ea typeface="+mn-ea"/>
+                                      <a:cs typeface="+mn-cs"/>
+                                    </a:rPr>
+                                    <m:t>−</m:t>
+                                  </m:r>
+                                  <m:r>
                                     <m:rPr>
                                       <m:sty m:val="p"/>
                                       <m:brk m:alnAt="7"/>
@@ -9248,7 +9488,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="Textfeld 14"/>
@@ -9402,10 +9642,16 @@
                 <a:t>&amp;</a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
                   <a:latin typeface="Cambria Math"/>
-                </a:rPr>
-                <a:t>−</a:t>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>sin</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="de-DE" sz="1100" i="0">
@@ -9413,10 +9659,82 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>⁡〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
                   <a:latin typeface="Cambria Math"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
+                <a:t>𝜃</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>2</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> 〗&amp;</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>@</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
                 <a:t>sin</a:t>
               </a:r>
               <a:r>
@@ -9489,7 +9807,19 @@
                 <a:rPr lang="de-DE" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>@</a:t>
+                <a:t>&amp;</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>〖−</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="de-DE" sz="1100" i="0">
@@ -9501,7 +9831,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>sin</a:t>
+                <a:t>cos</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="de-DE" sz="1100" i="0">
@@ -9513,91 +9843,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>⁡〖</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝜃</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>_</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>2</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t> 〗&amp;</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math"/>
-                </a:rPr>
-                <a:t>0</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>&amp;</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>cos</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>⁡〖</a:t>
+                <a:t>〗⁡〖</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="de-DE" sz="1100" i="0">
@@ -9771,8 +10017,8 @@
       <xdr:rowOff>5122</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2689413" cy="737959"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="Textfeld 15"/>
@@ -10196,7 +10442,7 @@
                                         <a:schemeClr val="tx1"/>
                                       </a:solidFill>
                                       <a:effectLst/>
-                                      <a:latin typeface="Cambria Math"/>
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                       <a:ea typeface="+mn-ea"/>
                                       <a:cs typeface="+mn-cs"/>
                                     </a:rPr>
@@ -10388,7 +10634,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="Textfeld 15"/>
@@ -10727,19 +10973,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>&amp;〖</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>−</a:t>
+                <a:t>&amp;〖−</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="de-DE" sz="1100" i="0">
@@ -10949,8 +11183,8 @@
       <xdr:rowOff>163285</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2689413" cy="737959"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="17" name="Textfeld 16"/>
@@ -11188,18 +11422,6 @@
                                 </m:funcPr>
                                 <m:fName>
                                   <m:r>
-                                    <a:rPr lang="de-DE" sz="1100" b="0" i="1">
-                                      <a:solidFill>
-                                        <a:schemeClr val="tx1"/>
-                                      </a:solidFill>
-                                      <a:effectLst/>
-                                      <a:latin typeface="Cambria Math"/>
-                                      <a:ea typeface="+mn-ea"/>
-                                      <a:cs typeface="+mn-cs"/>
-                                    </a:rPr>
-                                    <m:t>−</m:t>
-                                  </m:r>
-                                  <m:r>
                                     <m:rPr>
                                       <m:sty m:val="p"/>
                                     </m:rPr>
@@ -11382,6 +11604,18 @@
                                 </m:funcPr>
                                 <m:fName>
                                   <m:r>
+                                    <a:rPr lang="de-DE" sz="1100" b="0" i="1">
+                                      <a:solidFill>
+                                        <a:schemeClr val="tx1"/>
+                                      </a:solidFill>
+                                      <a:effectLst/>
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      <a:ea typeface="+mn-ea"/>
+                                      <a:cs typeface="+mn-cs"/>
+                                    </a:rPr>
+                                    <m:t>−</m:t>
+                                  </m:r>
+                                  <m:r>
                                     <m:rPr>
                                       <m:sty m:val="p"/>
                                       <m:brk m:alnAt="7"/>
@@ -11548,7 +11782,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="17" name="Textfeld 16"/>
@@ -11712,6 +11946,18 @@
                 <a:t>&amp;</a:t>
               </a:r>
               <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>sin</a:t>
+              </a:r>
+              <a:r>
                 <a:rPr lang="de-DE" sz="1100" b="0" i="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
@@ -11721,10 +11967,10 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>〖</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                <a:t>⁡〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -11733,7 +11979,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>−</a:t>
+                <a:t>𝜃</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="de-DE" sz="1100" i="0">
@@ -11741,10 +11987,58 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
                   <a:latin typeface="Cambria Math"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
+                <a:t>4</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> 〗&amp;</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>@</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
                 <a:t>sin</a:t>
               </a:r>
               <a:r>
@@ -11757,187 +12051,103 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
+                <a:t>⁡〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝜃</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>4</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> 〗&amp;</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>&amp;〖−</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>cos</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
                 <a:t>〗⁡〖</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝜃</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>_</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>4</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t> 〗&amp;</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math"/>
-                </a:rPr>
-                <a:t>0</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>@</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>sin</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>⁡〖</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝜃</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>_</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>4</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t> 〗&amp;</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>0</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>&amp;</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>cos</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>⁡〖</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="de-DE" sz="1100" i="0">
@@ -29629,8 +29839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A168" sqref="A168"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32800,7 +33010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BT32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>